<commit_message>
refactor: Split content into chunks when creating vector embeddings
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,81 +463,679 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Giá vàng hôm nay 25-8: Vàng SJC giảm 200.000 đồng/lượng</t>
+          <t>6 người chết do sạt lở đất ở Sa Pa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://tuoitre.vn/gia-vang-hom-nay-25-8-vang-sjc-giam-200-000-dong-luong-20230825085817684.htm</t>
+          <t>https://vnexpress.net/6-nguoi-chet-do-sat-lo-dat-o-sa-pa-4790475.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sáng 25-8, giá vàng SJC giảm 200.000 đồng/lượng so với chốt phiên hôm qua.</t>
+          <t>Lào CaiĐất đá từ trên núi cao sạt xuống khu dân cư ở thị xã Sa Pa, vùi lấp 17 người, làm 6 người chết, 9 người bị thương, trưa 8/9.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Công ty Vàng bạc Đá quý Sài Gòn niêm yết giá vàng SJC mua vào bán ra là 66,8 triệu - 67,5 triệu đồng/lượng, giảm 200.000 đồng/lượng ở chiều mua vào và giảm 100.000 đồng/lượng ở chiều bán ra so với chốt phiên ngày 24-8.</t>
+          <t>Khoảng 13h ngày 8/9, thị xã Sa Pa mưa lớn. Vạt núi cao khoảng 20 m bất ngờ sạt xuống, tràn qua khu ruộng bậc thang và tràn vào khu dân cư thôn Thào Hồng Dến 2, xã Mường Hoa.Nằm cách chân núi khoảng 100 m, khu dân cư có 4 nhà với tổng số 26 người. 9 người kịp chạy thoát ra ngoài. 17 người khác bị bùn đất cùng những cấu kiện trong nhà sập xuống vùi lấp.
+Clip Hiện trường vụ sạt lở ở Lào Cai
+Hiện trường sạt lở đất ở xã Mường Hoa, thị xã Sa Pa. Video: Tân Giang
+Chính quyền thị xã Sa Pa huy động 80 bộ đội, công an tìm kiếm nạn nhân. Đến 15h30, 6 thi thể được tìm thấy, trong đó có bà Vàng Thị Thảo 68 tuổi, Giàng Thị Chú 25 tuổi, cháu Châu Gia Hưng một tuổi và bé sơ sinh Vàng Văn Viên.9 người bị thương được đưa đi cấp cứu tại Bệnh viện Đa khoa thị xã Sa Pa, hiện sức khỏe đã ổn định. Chịu ảnh hưởng của hoàn lưu bão Yagi, lượng mưa từ 7h hôm qua qua đến 13h hôm nay ở Ô Quy Hồ, Hoàng Liên, Mường Hoa gần 150 mm.
+Một trong bốn ngôi nhà sàn bị sạt lở trưa 8/9. Ảnh: CTV
+Trước đó rạng sáng nay, đất đá từ vạt đồi trồng sắn cao hơn 10 m sạt xuống ngôi nhà ở xã Tân Minh, huyện Đà Bắc, tỉnh Hòa Bình, khiến 4 người tử vong.Hoàn lưu bão Yagi khiến miền Bắc mưa lớn hai ngày nay. Cơ quan khí tượng cảnh báo nguy cơ sạt lở đất ở 17/25 tỉnh, gồm: Lai Châu, Điện Biên, Sơn La, Hòa Bình, Lào Cai, Yên Bái, Hà Giang, Tuyên Quang, Vĩnh Phúc, Phú Thọ, Bắc Kạn, Thái Nguyên, Cao Bằng, Lạng Sơn, Quảng Ninh, Bắc Giang và TP Hải Phòng.Gia Chính</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>25/08/2023</t>
+          <t>08/09/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Doanh nghiệp Việt Nam đầu tư vào nước ngoài tăng mạnh</t>
+          <t>Cổ thụ, có nên trồng trên phố?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://tuoitre.vn/doanh-nghiep-viet-nam-dau-tu-vao-nuoc-ngoai-tang-manh-20230825090532564.htm</t>
+          <t>https://vnexpress.net/co-thu-co-nen-trong-tren-pho-4790457.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Trong 8 tháng đầu năm 2023, tổng vốn đầu tư của Việt Nam ra nước ngoài đạt gần 400 triệu USD, tăng 2,5 lần so với cùng kỳ năm ngoái.</t>
+          <t>Nên thay thế dần cổ thụ bằng những loài cây nhỏ, tán rộng, có khả năng chịu gió bão tốt hơn.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Theo số liệu của Cục Đầu tư nước ngoài (Bộ Kế hoạch và Đầu tư), tính đến ngày 20-8, tổng vốn đầu tư của Việt Nam ra nước ngoài (bao gồm vốn cấp mới và tăng thêm) đạt 398,3 triệu USD, tăng 2,5 lần so với cùng kỳ năm 2022.</t>
+          <t>Nhiều người dân Thủ đô sáng nay tan bão, đã dong xe làm một vòng để trở về với nỗi xót xa cho những cái cây vốn đã trở thành một phần linh hồn của đô thị Hà Nội.Cây đổ cũng là một trong những nguyên nhân gây thiệt mạng cho 14 người trong cơn siêu bão vừa qua.Nhưng không chờ đến bão, thỉnh thoảng, nhánh cây già ở đâu đó vẫn thình lình rơi, cướp đi mạng sống của con người. Gần đây nhất, một phụ nữ tử vong khi đang đi trên đường An Dương Vương, quận 5, TP HCM vì nhánh cây đổ vào người.Những thiệt hại nặng nề này khiến một câu hỏi cũ lại được đặt ra: có nên giữ lại cây cổ thụ ven đường hay mạnh dạn thay thế bằng cây nhỏ hơn, phù hợp hơn.Về lâu dài, cổ thụ trên vỉa hè nên được xem xét thay thế bằng cây thấp hơn với tán phủ tốt hơn để đảm bảo an toàn. Các lý do chính bao gồm:Việc trồng cổ thụ cao hàng chục mét trên vỉa hè rất ít gặp ở nhiều quốc gia. Các nước đã thực hiện chương trình thay thế luân phiên cây lớn để đảm bảo an toàn. Cây quá cao thường không che bóng hiệu quả, vì phần lớn thời gian trong ngày, bóng cây sẽ đổ vào nhà dân hơn là lòng đường.Cây cổ thụ với bộ rễ lớn dọc vỉa hè có thể gây hư hại hạ tầng kỹ thuật, bong tróc nền đường và tốn kém chi phí chăm sóc, bảo trì hơn nhiều so với cây nhỏ.Các giống cây lớn nên được trồng và bảo vệ ở công viên, vườn bách thảo hoặc khu vực ít người qua lại để giảm nguy cơ rủi ro từ cành cây gãy. Cây trồng dọc vỉa hè nên là các cây có chiều cao trung bình thấp, thân cành dẻo dai và có tán lá rộng để tạo bóng tâm tốt.Chặt và thay thế cây cổ thụ luôn là vấn đề gây tranh cãi, thậm chí là nhạy cảm ở nhiều quốc gia. Nhưng việc đảm bảo an toàn cho cộng đồng phải được đặt lên hàng đầu. Ở Singapore, cơ quan quản lý cây xanh NPARKS kiểm tra định kỳ những cây đạt kích thước hoặc tuổi nhất định để quyết định giữ lại hay đốn hạ. Việc chặt tỉa và trồng mới được thực hiện luân phiên theo hình thức cuốn chiếu, tức là, cây tới tuổi được đốn bỏ luân phiên và trồng thay cây con mới, để duy trì cảnh quan và bóng mát. Những cây cao trên 20 m chỉ được trồng ở công viên, ngoại ô hoặc ven đô, nơi có không gian đủ lớn để bộ rễ phát triển.
+Cây cổ thụ trên vỉa hè được kiểm tra, cắt tỉa hoặc đốn bỏ. Phần gốc được băm thành mảnh nhỏ (A) và mùn cưa dùng để phủ lên cây non kế bên (B). Cây xanh vỉa hè được trồng luân phiên (C) để duy trì sự xanh mát của trục đường mà không chặt bỏ toàn bộ cùng lúc.
+Ngoài kế hoạch dài hạn là thay thế cổ thụ, một vấn đề khác luôn phải quan tâm định kỳ là làm thế nào để bảo vệ cây xanh đô thị, duy trì cảnh quan và đảm bảo an toàn cho người dân trong mùa mưa bão?Cây xanh đô thị phải chịu nhiều áp lực hơn so với cây cối trong tự nhiên, thường xuyên chịu tác động từ nhiệt độ cao, biến đổi độ ẩm và ô nhiễm không khí. Đất ở khu vực đô thị thường thiếu dinh dưỡng, trong khi các hoạt động xây dựng và giao thông có thể gây hư hại đến rễ, thân, và cành cây, đồng thời hạn chế không gian sinh trưởng. Lưu lượng giao thông cao cũng làm gia tăng nguy cơ du nhập các bệnh cây ngoại lai. Do đó, việc trồng và chăm sóc cây xanh đô thị cần được chú trọng đặc biệt với những biện pháp bảo trì và thay thế kịp thời.Để giảm nguy cơ gãy đổ trong những mùa mưa bão sắp tới, cần rất nhiều biện pháp cùng lúc:Kiểm tra định kỳ: Các chuyên gia cây xanh cần thường xuyên kiểm tra để phát hiện sớm dấu hiệu suy yếu như rễ nổi, thân cây mục nát, cành khô hoặc bị bệnh. Những công nghệ đánh giá hiện đại như VTA, đo điện trở hoặc siêu âm có thể xác định chính xác tình trạng cây.Tỉa cành đúng cách: Tỉa cành giúp loại bỏ cành khô yếu, giảm sức cản gió và tăng độ ổn định. Phương pháp tỉa thưa tán và giảm chiều cao tán có tác dụng giảm tải trọng gió, ngăn ngừa gãy đổ.Cải thiện cấu trúc rễ: Đảm bảo rễ cây không bị tổn thương và có đủ không gian phát triển bằng cách giữ đất thoáng khí, bổ sung dinh dưỡng định kỳ để rễ khỏe mạnh.Hỗ trợ cây trưởng thành: Những cây có giá trị bảo tồn nhưng đã suy yếu cần hỗ trợ thêm bằng cáp, dây chằng, hoặc các hệ thống chống đỡ để tăng khả năng chịu gió bão.Bảo vệ khỏi các yếu tố gây hại: Chăm sóc hợp lý như bón phân, tưới nước và bảo vệ khỏi sâu bệnh sẽ giúp cây phát triển khỏe mạnh và tăng khả năng chống chịu thời tiết.Nỗi xót thương khiến nhiều người đang kêu gọi trồng lại 17.000 cây vừa bị bão Yagi quật ngã. Nhưng việc trồng lại trong phần lớn trường hợp là bất khả thi. Sự mất mát này là cơ hội để thay thế giống cây phù hợp hơn. Đô thị nên ưu tiên những cây có rễ vững chắc và khả năng chịu gió bão tốt, tránh các loài cây gỗ giòn, dễ gãy.Theo nghiên cứu của tôi, hai loại cây rất phù hợp để trồng trên vỉa hè ở Việt Nam là cây Còng (Samanea Saman) và cây Trai Lý (Fagraea fragrans). Cây Còng có tán rộng hình chiếc ô từ 20-30 m, phát triển tốt trong khí hậu nhiệt đới, ít cần chăm sóc và hoa ít mùi. Cây Trai Lý cao từ 10-25 m, phát triển mạnh mẽ trong môi trường đô thị, không đòi hỏi nhiều công chăm sóc và tạo cảnh quan xanh mát cho các tuyến đường.Việc cân bằng giữa an toàn tính mạng con người và cảnh quan, sinh thái, tạo bóng râm cần có sự tính toán và cân đối phù hợp để mang lại lợi ích cho cộng đồng. Đặc biệt yếu tố an toàn phải được đặt lên hàng đầu, nhất là khi hiện tượng thời tiết cực đoan sẽ còn xuất hiện với tần suất càng phổ biến.Trình Phương Quân</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>25/08/2023</t>
+          <t>08/09/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bão Saola mạnh cấp 13 hướng vào Biển Đông</t>
+          <t>Người dân sốc vì phố phường tan hoang sau bão Yagi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://tuoitre.vn/bao-saola-manh-cap-13-huong-vao-bien-dong-20230825080123056.htm</t>
+          <t>https://vnexpress.net/nguoi-dan-soc-vi-pho-phuong-tan-hoang-sau-bao-yagi-4790424.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sáng 25-8, bão Saola đang hoạt động ở phía đông Philippines với sức gió mạnh nhất vùng gần tâm bão mạnh cấp 13.</t>
+          <t>Hà Nội8 tiếng kể từ khi hai cây phượng và xà cừ cổ thụ liên tiếp đổ xuống, đè vào chiếc ôtô đỗ trước cửa nhà, anh Lê Tú, 55 tuổi, vẫn chưa hết bàng hoàng.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Theo Trung tâm Dự báo khí tượng thủy văn quốc gia, hồi 7h ngày 25-8, vị trí tâm bão ở khoảng 19,8 độ vĩ bắc; 127,5 độ kinh đông, cách đảo Lu-dông (Philippines) khoảng 470km về phía đông đông bắc. Sức gió mạnh nhất vùng gần tâm bão mạnh cấp 13 (134-149km/giờ), giật cấp 16.</t>
+          <t>17h30 ngày 7/9, nam tài xế taxi về nhà ở phố Quán Sứ, quận Hoàn Kiếm, sau cuốc xe cuối cùng. Anh đỗ chiếc ôtô sát cửa, cách hai cây cổ thụ trồng trên vỉa hè chừng một mét vì nghĩ cây to, rễ lớn không thể đổ.30 phút sau, một tiếng rắc lớn xé ngang tai, anh Tú thấy cành cây phượng rơi thẳng xuống khiến kính lái của ôtô vỡ vụn. Gia đình khuyên di chuyển xe ra chỗ khác nhưng thấy ngoài trời gió lớn, anh chần chừ. Đúng lúc đó, tiếng uỳnh thứ hai dội đến. Cây xà cừ cổ thụ hơn 40 năm tuổi, thân bằng hai người ôm, bật gốc đè lên khiến chiếc xe bẹp rúm.Không chỉ hai cây cổ thụ trước cửa nhà, hàng chục cây khác trên cùng phố Quán Sứ (quận Hoàn Kiếm) cũng đổ rạp, nhẹ thì gãy cành, nặng thì gãy đôi hoặc bật gốc. "Cảnh tượng hoang tàn như sau một trận bom, lần đầu tôi chứng kiến", anh Tú nói.Đến 12h ngày 8/9, phố Quán Sứ vẫn ngổn ngang cây xanh đổ gãy, nhiều cây nằm ngang đường chưa được dọn dẹp. Người dân phải đi lên vỉa hè.
+Anh Lê Tú, 55 tuổi, đứng bất lực bên cạnh chiếc ôtô của gia đình bị cây đè ngang, bẹp rúm, trưa 8/9. Ảnh: Thanh Nga
+Cách nhà anh Tú chừng một km, tại phố Hàng Trống, quận Hoàn Kiếm, bà Nguyễn Nghĩa, 64 tuổi, cùng người thân đang làm lại đường ống sau khi cây me gần 100 năm tuổi trồng trước cửa nhà bật gốc. "Cái thân cây phải ba người ôm nhưng nay chẳng còn. Khắp nơi đổ nát như thời chiến tranh", bà Nghĩa kể.Cây me đổ khoảng 12h trưa 7/9. Sau tiếng gió rít, họ nghe thấy tiếng đổ ầm, một số nhà cảm nhận được độ rung. Khi chạy ra ngoài mới biết cây đổ ngang đường, nhưng giữa trời giông lốc không thể làm gì, họ đành lui vào trong nhà trú ẩn.
+Một người dân trên phố Hàng Trống sửa lại đường ống nước sau khi cây me trước cửa nhà bật gốc, trưa 8/9. Ảnh: Quỳnh Nguyễn
+6h sáng nay, anh Trần Đức Anh, 42 tuổi, mở cửa nhà tại khu đô thị cách trung tâm Hà Nội hơn 10 km, đập vào mắt là cảnh tượng ''tưởng chỉ có trong phim''. Cây cối hai bên đường đổ rạp. Những cây cổ thụ to từng là nơi ngồi hóng mát, tập thể dục của cư dân đều bị bão quật tan tác.''Hơn 40 năm sống ở Hà Nội, tôi chưa từng thấy cảnh tượng nào như vậy'', anh nói. ''Quá đau lòng khi bao nhiêu cây xanh thân thuộc gục ngã trên đường''.Trưa 8/9, hầu hết tuyến đường tại các quận Hoàn Kiếm, Hai Bà Trưng, Long Biên, Ba Đình, Đống Đa, Cầu Giấy, Nam Từ Liêm, Bắc Từ Liêm cây xanh bị đổ rạp sau bão vẫn đang ngổn ngang. Chủ tịch UBND TP Hà Nội cho biết có khoảng 17.000 cây gãy đổ trên địa bàn.Hà Nội hiện có khoảng 1,8 triệu cây xanh đô thị, chủ yếu là xà cừ, sấu, phượng, muồng, bằng lăng, giáng hương, bàng. Giai đoạn 2016-2020, khoảng 1,6 triệu cây được trồng mới. Hiện trên địa bàn 12 quận nội thành có khoảng 8.000 cây cổ thụ. Các cây này có độ tuổi tối thiểu 50 năm hoặc cây có đường kính từ 50cm trở lên.Nhà nghiên cứu văn hóa, PGS.TS Phạm Ngọc Trung, nguyên trưởng khoa Văn hóa và Phát triển, Học viện Báo chí và Tuyên truyền cho rằng những hàng cây xanh không chỉ che nắng, che mưa cho người dân khi ra đường mà còn tạo cảnh quan, làm đẹp cho thành phố.Trong khi đó, những gốc cây lâu năm còn là một phần ký ức của người Hà Nội, gắn với ký ức của nhiều người. Cây ở các con đường như Hoàng Diệu, Phan Đình Phùng còn mang dấu ấn lịch sử, là hơi thở của thời đại.''Vì lý do cơn bão gây gãy đổ hàng nghìn cây xanh lâu năm, người Hà Nội không khỏi sốc và xót xa'', ông Trung nói.
+Cây đổ gãy trên phố Trích Sài lúc 2h sáng 8/9. Ảnh: Trần Duy Tiệp
+Biết Hà Nội sẽ gánh chịu thiệt hại nặng vì bão nên ngay từ đêm qua, khi gió ngớt đã có một số người dân tình nguyện tham gia dọn dẹp, giải phóng đường.Anh Trần Duy Tiệp, một nhiếp ảnh gia tự do ở Sóc Sơn, đã lên mạng xã hội kêu gọi mọi người cùng hỗ trợ lực lượng chức năng dọn dẹp đường phố, lúc gần 2h sáng. ''Tôi ở nhà cũng không ngủ được nên quyết định làm gì đó có ý nghĩa'', chàng trai Gen Z, nói. Xuất phát từ nhà lúc 1h45 đến 2h30 anh mới có mặt ở phố Thụy Khuê.''Tôi run lên vì không ngờ cảnh hoang tàn, đổ nát đến vậy. Chỉ cần lơ là một giây thôi là có thể tông vào cây đổ'', Tiệp nói.Sau khi tập hợp được gần 10 người, nhóm của Tiệp theo chân cán bộ phường và cảnh sát giao thông dọn dẹp một số khu vực trên đường Nguyễn Đình Thi, Trích Sài (quận Tây Hồ). Đi đến đâu nhóm cũng thấy cây gãy đổ, biển quảng cáo của nhà hàng, doanh nghiệp, cột đèn rơi la liệt bên vệ đường. Có những cây xanh gần chục người mất đến 30 phút mới có thể dọn dẹp xong.Từ sáng sớm nay, Đức Anh lên mạng xã hội kêu gọi cư dân chung tay vì biết với sức có hạn của lực lượng chức năng, nhân viên vệ sinh, không biết khi nào đường phố mới quang đãng trở lại.Một ngày sau cây đổ, bà Nghĩa ở phố Hàng Trống cũng cùng một số hộ dân trên phố đang cùng nhau cắt cành để giải phóng đường. Theo bà, đường ống vỡ thì có thể sửa lại, nhưng cây đổ rồi bà sợ không còn cơ hội trồng cho cây thành cổ thụ như vậy nữa.''Dân trong phố tôi ai cũng xót xa", bà nói.
+Người dân Hà Nội: 'Xót xa khi nghe gió bão rít, cây đổ rầm rầm'
+Video: Lộc Chung - Văn Ngọc - Bá Nam
+Phạm Thanh Nga - Quỳnh Nguyễn</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>25/08/2023</t>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hai sĩ quan hy sinh khi phòng chống bão Yagi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/hai-si-quan-hy-sinh-khi-phong-chong-bao-yagi-4790487.html</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Thượng úy quân đội Nguyễn Đình Khiêm và thiếu tá công an Trần Quốc Hoàng hy sinh khi làm nhiệm vụ phòng chống bão Yagi ở tâm bão Quảng Ninh.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Thượng úy Nguyễn Đình Khiêm, 27 tuổi, là Đại đội trưởng Đại đội 3, Lữ đoàn 513, Quân khu 3. Anh nhập ngũ tháng 9/2015, quê xã Yên Mỹ, huyện Yên Mô, tỉnh Ninh Bình. Trong quá trình phòng chống bão Yagi, đơn vị anh phụ trách đảm bảo an toàn các đơn vị công trình.
+Thượng úy Nguyễn Đình Khiêm.
+Ngày 6/9, Lữ đoàn phát hiện hệ thống lán trại tại công trình thuộc thôn Pạt, xã Lục Hồn, huyện Bình Liêu có nguy cơ mất an toàn trước gió bão. Thượng úy Khiêm được giao chỉ huy lực lượng chuẩn bị vật chất ứng cứu với địa phương và chằng chống lán trại.Trên đường về sau khi lấy vật liệu, thấy đồng đội trượt chân, có thể bị cây đè lên người gây nguy hiểm, thượng úy Khiêm lao vào đỡ và bị ngã. Được đồng đội đưa đi cấp cứu, nhưng anh không qua khỏi.Cũng trong cơn bão Yagi, thiếu tá Trần Quốc Hoàng, 37 tuổi, quê thị xã Mỹ Hào, Hưng Yên, đã hy sinh. Anh Hoàng là cán bộ trại giam Quảng Ninh, thuộc Cục Cảnh sát quản lý trại giam.
+Thiếu tá Trần Quốc Hoàng.
+Rạng sáng 7/9, trong cơn mưa bão, nước lũ dâng cao, có thể nguy hiểm đến tính mạng của phạm nhân tại Phân trại số 2, anh Hoàng đã lao ra cứu người và bị nước lũ cuốn trôi.Trại giam Quảng Ninh cùng với lực lượng cứu nạn cứu hộ đã tìm kiếm trong mưa bão. Đến sáng nay, thi thể của thiếu tá Hoàng được tìm thấy tại bờ suối thôn Đồng Vải, xã Thống Nhất, TP Hạ Long, cách đơn vị khoảng một km.Bão Yagi với sức gió cấp 12-13 đổ bộ vào Quảng Ninh trưa 7/9. Hoàn lưu trước, trong và sau bão gây mưa to, gió mạnh ở khắp miền Bắc. Thống kê của Cục Quản lý đê điều và Phòng chống thiên tai, đến chiều nay bão Yagi và các hiệu ứng liên quan làm 21 người chết, trong đó 9 người do bão, 12 chết do sạt lở đất và một người lũ cuốn, một người mất tích ở Bắc Giang.229 người bị thương, hơn 8.000 ngôi nhà hư hỏng, chìm 25 tàu thuyền. Gần 110.000 ha lúa, gần 18.000 ha hoa màu, gần 7.000 ha cây ăn quả bị ngập úng, hư hại. Hơn 1.100 lồng bè bị cuốn trôi, chủ yếu ở Quảng Ninh.
+Sơn Hà</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Nhiều bệnh viện Quảng Ninh thiệt hại nặng, cạn điện nước sau bão Yagi</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nhieu-benh-vien-quang-ninh-thiet-hai-nang-can-dien-nuoc-sau-bao-yagi-4790425.html</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tất cả bệnh viện, trung tâm y tế tại Quảng Ninh đều bị thiệt hại sau bão Yagi, tốc mái, vỡ kính, hỏng nhiều thiết bị, ảnh hưởng hoạt động khám chữa bệnh.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Chiều 8/9, đại diện Sở Y tế Quảng Ninh cho biết thông tin trên, thêm rằng toàn bộ đơn vị khám bệnh chữa bệnh đều bị thiệt hại nặng nề, nguồn dự trữ năng lượng điện từ máy phát điện dần cạn kiệt. Nguồn nước từ bể dự trữ chỉ duy trì được 12-24 giờ nữa, tùy đơn vị. Trong đó, Bệnh viện Sản Nhi và Bệnh viện Lão khoa - Phục hồi chức năng thiệt hại nặng nề nhất.Tại Bệnh viện Sản nhi Quảng Ninh, đến chiều nay cây cối đổ dài chắn lối đi, nhiều khoa, phòng trống hoác do bị gió lốc thổi bay mái tôn, hỏng nhiều thiết bị quan trọng. Mái tôn Khoa Hồi sức tích cực bị thổi bay. Kính cửa sổ khu vực xét nghiệm bị vỡ gây ẩm, ảnh hưởng máy xét nghiệm.Khu vực phòng DSA (phòng can thiệp - Phẫu thuật tim - mạch) cũng bị hư hỏng nhiều thiết bị quan trọng. Nhiều nội thất như điều hòa, tủ lạnh, tivi, giường, bàn ghế... bị tàn phá. Thiết bị tại khu lưu trữ ngân hàng sữa mẹ, khoa dinh dưỡng cũng bị ảnh hưởng. Nhà xe cho nhân viên, nhà xe cho bệnh nhân cũng bị bay mái.Công tác khám chữa bệnh tại bệnh viện gần như bị đình trệ.
+Khoa Sản, Bệnh viện Sản Nhi Quảng Ninh, bị tốc mái trống hoác, nhiều thiết bị trong phòng bị hỏng. Ảnh: Lê Giang
+Bệnh viện Lão khoa - Phục hồi chức năng bị nứt vỡ kính trần nhà, tốc mái tôn. Bác sĩ phải di chuyển bệnh nhân đến nơi an toàn do mưa lớn hắt vào phòng bệnh. Trung tâm Kiểm soát Bệnh tật (CDC) Quảng Ninh cũng thiệt hại nặng nề.Các đơn vị khác như Bệnh viện Đa khoa Hạ Long, Trung tâm y tế Hải Hà, Tiên Yên, Đầm Hà, Bệnh viện Việt Nam - Thụy Điển Uông Bí, Trung tâm Y tế Hạ Long... trong tình trạng tương tự. Nhiều ôtô bị các tấm tôn, cây ngã đè hỏng.
+Nhiều mái tôn bị tốc mái trong bão bay xuống đất, hư hỏng nặng. Ảnh: Lê Giang
+Tính đến chiều 8/9, các bệnh viện ở Quảng Ninh tiếp nhận điều trị 357 ca tai nạn do bão, ba trường hợp tử vong. Trong đó, 18 ca đa chấn thương nặng, 6 chấn thương sọ não, 19 trường hợp gãy xương và hơn 300 ca chấn thương phần mềm khác.Ngành y tế tiếp nhận 255 cuộc gọi, trong đó 113 cuộc gọi cấp cứu. Trung tâm vận chuyển cấp cứu tiếp cận thành công 11 trường hợp, điều phối 6 chuyển xe cho các đơn vị y tế toàn ngành.Các đơn vị đang cố gắng khắc phục thiệt hại để đảm bảo cấp cứu, điều trị người bệnh.Yagi là cơn bão số 3 đổ bộ vào Việt Nam năm nay, tâm bão quét qua Quảng Ninh và Hải Phòng với sức gió giật trên cấp 14. Đây là cơn bão mạnh nhất trên Biển Đông 30 năm qua, gây thiệt hại nặng nề về người và của.Thùy An</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Người Hải Phòng chạy đôn đáo tìm chỗ sạc điện</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nguoi-hai-phong-chay-don-dao-tim-cho-sac-dien-4790450.html</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Nghe tin một chung cư ở phường Vĩnh Niệm, quận Lê Chân có điện, chị Thu Hà cùng hàng xóm gom 20 chiếc điện thoại, iPad, laptop mang đến sạc nhờ, chiều 8/9.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Nhà chị Hà ở quận Ngô Quyền mất điện từ trưa qua khi bão Yagi đổ bộ, đến nay chưa được cấp lại. Ngoài mất điện, nhiều quận, huyện của thành phố còn mất nước, sóng điện thoại, khiến mọi người không thể liên lạc với người thân."Mất điện hơn một ngày nên mọi thiết bị đều hết pin, con ở xa không liên lạc được lại lo. Tôi dò hỏi khắp nơi, xem chỗ nào có điện để đi sạc nhờ", chị Hà nói.Bà Hồng Hoa, một cư dân khu chung cư ở quận Lê Chân, cho biết gia đình và nhiều hộ khác đã nhận sạc điện thoại, đồ điện tử cho người quen bởi biết hầu hết các khu vực khác đều chưa có điện."Vừa có điện là tôi gọi điện thoại báo cho mọi người ai cần sạc đồ điện tử hay trú ẩn thì qua, cư dân sẽ hỗ trợ hết sức", bà Hoa nói.
+Người dân Hải Phòng ngồi la liệt tại lối vào nhà vệ sinh của trung tâm thương mại Aeon Mall Hải Phòng, quận Lê Chân để sạc điện thoại, chiều 8/9. Ảnh: Duy Anh
+Không có người quen ở khu chung cư nên Minh Ngọc, ở quận Lê Chân, cùng chồng và con con gái đến trung tâm thương mại Aeon Mall Hải Phòng ngay khi biết tin ở đây chạy máy phát điện và có wifi.Đến nơi, Ngọc nhận thấy các hàng quán có ổ cắm điện hoặc khu vực công cộng, thậm chí lối vào nhà vệ sinh có ổ điện đã chật kín người. "Hầu hết điện thoại của mọi người đều đã kiệt pin, chờ sạc được 50% cũng mất cả tiếng. Chắc phải đến tối mới đến lượt tôi", Ngọc nói.Không thể chờ đợi, cô quyết định đội mưa đi tìm các quán cà phê trong thành phố có máy phát để vào sạc nhờ.
+Người Hải Phòng nháo nhác tìm nơi sạc điện
+Người dân Hải Phòng chen chúc tranh chỗ cắm sạc điện thoại tại trung tâm thương mại Aeon Mall quận Lê Chân, 15h ngày 8/9. Nguồn: Duy Anh
+Từ sáng 8/9, Việt Hoàng, 25 tuổi, ở quận Lê Chân đã ra quán cà phê ở quận Hồng Bàng, một trong những nơi được cấp điện trở lại sớm nhất, để sạc điện thoại, đèn pin và làm việc online. Hoàng phải đợi khá lâu mới đến lượt bởi trong quán đã có nhiều người sử dụng. Các quán cà phê khác quanh khu vực anh sống tấp nập người tới ngồi từ sớm.Bốn người trong gia đình Hoàng đã di tản. Bố mẹ cùng em trai tới trung tâm thương mại và cửa hàng tiện lợi trên địa bàn đang chạy máy phát điện với hy vọng có sóng điện thoại hoặc Internet để liên lạc với họ hàng và sạc thiết bị."Trận bão khiến nhà tôi lật mái, kính vỡ, cây đổ chắn lối đi, mất liên lạc cả ngày. Giờ lo sạc điện để kết nối cũng như đề phòng mưa lớn mất điện kéo dài", chàng trai 25 tuổi nói.
+Hầu hết ổ điện tại quán cà phê ở quận Hồng Bàng nơi Việt Hoàng đến đều đang được sử dụng, trưa 8/9. Ảnh: Nhân vật cung cấp
+Quản lý một quán cà phê ở quận Hồng Bàng cho biết đã mở cửa ngay sau khi quán được cấp điện trở lại từ 8h, để phục vụ người dân có nhu cầu tới trú hoặc sử dụng Internet, điện."Từ lúc mở cửa, quán đã có hàng chục người tới sạc điện thoại. Chỉ mong cuộc sống sớm trở lại bình thường", người quản lý nói.Theo Tập đoàn Điện lực Việt Nam (EVN), lưới điện miền Bắc, đặc biệt tại Quảng Ninh, Hải Phòng, Thái Bình và Hải Dương, gặp nhiều khó khăn do sức tàn phá của bão Yagi.Hải Phòng - một trong số địa phương chịu ảnh hưởng nặng nề, bị cắt điện toàn bộ trong ngày 7/9. Ông Nguyễn Hữu Hưởng - Chủ tịch kiêm Tổng giám đốc Công ty TNHH MTV Điện lực Hải Phòng cho biết dự kiến trưa 8/9, 50-60% khách hàng được cấp điện trở lại. Con số này sẽ tăng lên 80% khách hàng vào cuối ngày.Theo khảo sát của VnExpress, đến 15h ngày 8/9, đa số các khu vực dân cư trên địa bàn thành phố như quận Ngô Quyền, Lê Chân, Hồng Bàng chưa được cấp điện trở lại.Thanh Nga - Quỳnh Nguyễn</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tầm nhìn kinh tế ông Trump vạch ra cho nhiệm kỳ tương lai</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/tam-nhin-kinh-te-ong-trump-vach-ra-cho-nhiem-ky-tuong-lai-4789683.html</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ông Trump nhấn mạnh các chính sách như giảm thuế, tăng thuế quan và cắt giảm lãng phí trong bài phát biểu chi tiết về tầm nhìn kinh tế.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ngày 5/9, ông Trump có bài phát biểu kéo dài một giờ tại Câu lạc bộ Kinh tế New York trước những gương mặt nổi tiếng của Phố Wall, vào thời điểm Phó tổng thống Kamala Harris, ứng viên đảng Dân chủ, đã thu hẹp lợi thế của cựu tổng thống trong các cuộc khảo sát cử tri về vấn đề kinh tế. Cả ông Trump và bà Harris đều chịu áp lực phải đưa ra tầm nhìn chính sách cụ thể để giúp thúc đẩy nền kinh tế, vốn bị sa lầy bởi giá cao và lãi suất vay tăng cao, khi có nhiều lo ngại về nguy cơ tăng trưởng chậm."Tôi cam kết thuế thấp, cắt giảm quy định, chi phí năng lượng thấp, lãi suất thấp, biên giới an toàn, tỷ lệ tội phạm cực thấp và thu nhập cao cho công dân bất kể chủng tộc, tôn giáo, màu da hay tín ngưỡng. Kế hoạch của tôi sẽ đẩy lùi lạm phát, nhanh chóng hạ giá và khôi phục mức độ tăng trưởng kinh tế bùng nổ", ứng viên đảng Cộng hòa nói.Ông nêu kế hoạch bổ nhiệm tỷ phú Elon Musk làm lãnh đạo ủy ban "chịu trách nhiệm giám sát tài chính và hiệu suất của toàn bộ chính phủ liên bang, cũng như đưa ra các khuyến nghị cải cách mạnh mẽ". Cựu tổng thống đặt mục tiêu rằng ủy ban này sẽ giúp loại bỏ "hàng nghìn tỷ USD" chi tiêu lãng phí.
+Ứng viên đảng Cộng hòa Donald Trump tại Câu lạc bộ Kinh tế New York ngày 5/9. Ảnh: AP
+Ông Trump ca ngợi thành tựu kinh tế trong nhiệm kỳ đầu của mình, đồng thời chỉ trích các chính sách của chính quyền Biden - Harris về kinh tế và nhập cư. "Chúng tôi đã tạo ra phép màu kinh tế, nhưng Harris và Biden đã biến nó thành thảm họa", ông Trump nói, đổ lỗi cho chính quyền hiện tại về lạm phát cao.Lạm phát đã tăng vọt trong nhiệm kỳ của ông Biden sau khi đại dịch Covid-19 làm tắc nghẽn chuỗi cung ứng, song đã giảm đáng kể sau khi đạt đỉnh vào năm 2022. Lạm phát đang theo đà giảm và dự kiến xuống mức mục tiêu 2%, theo Cục Dự trữ Liên bang Mỹ. Tuy nhiên, ông Trump và các đồng minh vẫn liên tục công kích phe Dân chủ về vấn đề này.Một lời hứa hẹn của ông Trump làm hài lòng giới doanh nghiệp là ông sẽ gia hạn đạo luật cắt giảm thuế mà ông từng thông qua năm 2017. Ông nhấn mạnh sự tương phản giữa mình với bà Harris, khi bà đã nêu kế hoạch tăng thuế doanh nghiệp từ 21 lên 28%.Trump đề xuất giảm thuế doanh nghiệp xuống 15%. Tuy nhiên, mức giảm sẽ chỉ dành cho các công ty sản xuất tại Mỹ, những công ty thuê sản xuất ngoài, chuyển dây chuyền ra nước ngoài hoặc không thuê lao động Mỹ không đủ điều kiện hưởng ưu đãi."Thông điệp của chúng tôi rất đơn giản: hãy tạo ra sản phẩm của bạn ở Mỹ. Chỉ ở Mỹ mà thôi", ông Trump nói.Cựu tổng thống cũng hứa hẹn mang lại "năng lượng dồi dào, độc lập và thậm chí thống trị ngành năng lượng" nếu trở lại Nhà Trắng. Ông dự định tuyên bố tình trạng khẩn cấp quốc gia để cắt giảm các quy định liên quan tới khai thác dầu khí và tăng cường sản xuất năng lượng trong nước.Trump khẳng định những hành động này sẽ làm giảm giá năng lượng ít nhất một nửa trong vòng 12 tháng sau khi ông nhậm chức, cam kết chấm dứt "cuộc thập tự chinh chống năng lượng" của ứng viên đảng Dân chủ. Giá xăng và các chi phí năng lượng khác tại Mỹ hiện cao hơn so với thời Trump còn tại nhiệm.Về thuế quan, Trump đã đề xuất mức thuế chung là 10% với tất cả sản phẩm nhập khẩu vào Mỹ. Tuy nhiên, tại một sự kiện tháng trước ở North Carolina, ông gợi ý thuế suất có thể tăng lên 20%. Với các sản phẩm từ Trung Quốc, ông muốn áp thuế 60%.Trong bài phát biểu ngày 5/9, Trump gọi đây là "chính sách thương mại có lợi cho Mỹ, sử dụng thuế quan để khuyến khích sản xuất trong nước" và sẽ dẫn đến "sự phục hưng kinh tế quốc gia".Trump gợi ý rằng ông có thể sử dụng số tiền thu được từ thuế quan để thành lập một quỹ đầu tư quốc gia, nhằm tài trợ cho dự án cơ sở hạ tầng, chi phí chăm sóc trẻ em hay trả nợ công.
+Người ủng hộ ứng viên tổng thống Donald Trump tại Đại hội toàn quốc đảng Cộng hòa ở Milwaukee, bang Wisconsin ngày 16/7. Ảnh: AFP
+Nhiều nhà kinh tế cảnh báo những mức thuế quan đó có thể phản tác dụng bằng cách làm tăng giá cả cho các gia đình Mỹ, làm mất việc làm và gây ra chiến tranh thương mại toàn cầu. "Đó là chính sách bảo hộ kinh tế khủng khiếp", Douglas Holtz-Eakin, chủ tịch tổ chức tư vấn trung hữu Diễn đàn Hành động Mỹ, nói.Trong khi đó, Trump tin các chính sách của ông sẽ thúc đẩy tăng trưởng, chứ không dẫn tới những hậu quả như làm suy yếu tăng trưởng và khiến giá cả tăng vọt như nhiều nhà kinh tế cảnh báo.Chiến dịch tranh cử của bà Harris cáo buộc ông Trump "nói dối trắng trợn người dân Mỹ, không cho họ biết những hậu quả nghiêm trọng từ kế hoạch kinh tế của ông ấy".Karoline Leavitt, thư ký báo chí chiến dịch của ông Trump, phản bác ý kiến này."Nhiều nhà kinh tế và chuyên gia từng hoài nghi kế hoạch kinh tế của Tổng thống Trump trong nhiệm kỳ đầu. Họ đã sai lầm và sẽ tiếp tục được chứng minh sai lầm một lần nữa. Tổng thống Donald Trump đã áp thành công thuế quan với Trung Quốc trong nhiệm kỳ đầu tiên và cắt giảm thuế cho người Mỹ. Ông ấy sẽ làm điều đó lần nữa trong nhiệm kỳ thứ hai. Kế hoạch của Tổng thống sẽ mang đến hàng triệu việc làm và hàng trăm tỷ USD từ Trung Quốc về Mỹ", Leavitt nói.Người sáng lập Key Square Scott Besent nhận xét bài phát biểu đã cho thấy phần nào chương trình nghị sự chính sách của ông Trump với nhiều mục mới, dự kiến "tăng sức hấp dẫn" cho cựu tổng thống."Ông ấy đã đưa ra cảnh báo về các chính sách hiện tại của chính quyền Tổng thống Biden, sau đó đưa ra giải pháp đầy lạc quan như đã làm năm 2016", Bessent, một trong những đồng minh lớn nhất của ông Trump trong lĩnh vực tài chính, nói.Thùy Lâm (Theo Politico, FT, CNN)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hà Nội sẽ cứu cây xanh gãy đổ do bão Yagi</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/ha-noi-se-cuu-cay-xanh-gay-do-do-bao-yagi-4790498.html</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cây cần bảo tồn, cây quý hiếm có giá trị, cây nhỏ đường kính dưới 25 cm bị gãy đổ sẽ được đánh giá để trồng lại tại chỗ hoặc đưa về vườn ươm chăm sóc.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Trong văn bản khắc phục hậu quả bão Yagi chiều 8/9, Chủ tịch TP Hà Nội Trần Sỹ Thanh yêu cầu các đơn vị liên quan tập trung toàn bộ nhân lực, trang thiết bị để giải tỏa cây đổ, gãy nhằm đảm bảo an toàn giao thông.Trước mắt các lực lượng phải giải tỏa ngay cây gãy đổ trên các tuyến đường phố chính của Thủ đô, xong trước ngày 12/9; sau đó sẽ tiếp tục thu dọn cây đổ, cành cây gãy, dựng lại cây, trồng thay thế và dọn vệ sinh thu hồi củi gỗ theo quy định."Đối với cây xanh cần bảo tồn, cây quý hiếm có giá trị bị nghiêng đổ, cần kiểm tra đánh giá và chống dựng, trồng lại ngay, đảm bảo cây tiếp tục sinh trưởng, phát triển hoặc di chuyển về vườn ươm để chăm sóc, trồng vào vị trí phù hợp trên địa bàn. Công việc này hoàn thành trước ngày 15/9", văn bản nêu.
+Cây sấu lớn trước cửa Bưu điện Hà Nội bật gốc đổ nghiêng về phía tháp Hòa Phong. Ảnh: Ngọc Thành
+Người đứng đầu chính quyền Hà Nội cũng yêu cầu trồng lại các cây xanh đô thị có đường kính nhỏ dưới 25 cm bị gãy đổ. Trước khi trồng lại, phải cắt cành, tán đảm bảo cân đối phù hợp để trồng lại tại chỗ và chăm sóc theo quy định.Ông lưu ý với những cây đổ ra đường sau khi cắt tỉa phải di chuyển lên hè phố, dải phân cách để đảm bảo an toàn giao thông nếu chưa kịp trồng lại. Việc trồng lại các cây xanh nêu trên xong trước ngày 20/9. Với những cây do các quận, huyện thị xã quản lý, việc trồng lại tại chỗ cây đổ hoàn thành trước 30/9.Với những cây gãy đổ không thể trồng lại, củi gỗ thu hồi được đưa về vườn ươm Yên Sở, vườn ươm Cổ Nhuế, bãi tập kết tại dốc La Pho, công viên Tuổi trẻ, sau đó thanh lý. Sở Xây dựng được giao chủ trì xây dựng kế hoạch trồng lại những cây xanh gãy đổ không thể khắc phục, đảm bảo chủng loại, kích thước phù hợp.
+Cây đa cổ thụ ở Vườn hoa Lý Thái Tổ gãy gốc, đổ về phía đường Lê Lai kéo theo cột điện cao áp bên cạnh. Ảnh: Ngọc Thành
+Chủ trương dựng lại cây xanh gãy đổ cũng được Bí thư Thành ủy Bùi Thị Minh Hoài nêu tại buổi kiểm tra công tác khắc phục hậu quả bão Yagi tại quận Nam Từ Liêm và huyện Thanh Oai sáng 8/9. Bà Hoài yêu cầu "cây nào cứu được phải hết sức cứu, dựng lại được phải dựng lại để chăm sóc. Bần cùng bất đắc dĩ mới phải cưa bỏ vì trồng được một cây không dễ, mất rất nhiều thời gian".Hà Nội hiện có khoảng 142.000 cây xanh đô thị do thành phố quản lý. Bão Yagi làm khoảng 17.000 cây gãy đổ trên toàn thành phố, trong đó khoảng 2.000 cây xanh đô thị. Đến nay cơ quan quản lý chưa thông tin phân loại cây đã gãy đổ như cây di sản, cây quý hiếm, cây có đường kính nhỏ...Thủ đô Hà Nội là một trong những địa phương chịu thiệt hại nặng do bão Yagi. Từ 6/9 đến ngày 8/9, thành phố ghi nhận 3 người chết, 10 người bị thương; 13 ôtô và 6 xe máy hư hại; 9 nhà dân bị tốc mái; hàng nghìn ha lúa, hoa màu bị đổ, ngập nước.Võ Hải</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Nga tuyên bố kiểm soát thành phố gần Pokrovsk</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nga-tuyen-bo-kiem-soat-thanh-pho-gan-pokrovsk-4790467.html</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bộ Quốc phòng Nga nói quân đội nước này kiểm soát đô thị gần thành phố chiến lược Pokrovsk, bước tiến mới tại mặt trận phía đông.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>"Nhờ hoạt động tích cực của cánh quân Trung tâm, thành phố Novogrodovka tại Cộng hòa Nhân dân Donetsk đã nằm dưới sự kiểm soát của chúng tôi", Bộ Quốc phòng Nga ngày 8/9 thông báo, đề cập mặt trận Donetsk ở phía đông Ukraine.Cơ quan này cho biết cánh quân Trung tâm còn đánh bại nhân lực, khí tài của ba lữ đoàn và một tiểu đoàn Ukraine ở nhiều khu vực tại tỉnh Donetsk, cũng như chặn 8 cuộc phản công của đối phương, khiến Kiev tổn thất tổng cộng khoảng 560 binh sĩ, một xe tăng cùng nhiều phương tiện, khí tài khác.Bộ Quốc phòng Ukraine chưa bình luận về thông tin.
+Binh sĩ Nga khai hỏa pháo phòng không ZU-23 tại tỉnh Donetsk hồi tháng 8. Ảnh: RIA Novosti
+Thành phố Novogrodovka, được Ukraine gọi là Novohrodivka, có hơn 14.000 cư dân sinh sống trước khi xung đột Nga - Ukraine bùng phát. Nó cách đô thị chiến lược Pokrovsk của Ukraine khoảng 20 km.Pokrovsk là giao điểm giữa nhiều tuyến đường sắt và đường bộ quan trọng, được đánh giá là trung tâm hậu cần chủ chốt giúp ngăn phòng tuyến Ukraine trong khu vực sụp đổ trên diện rộng.Moskva gần đây tuyên bố đạt nhiều bước tiến ở mặt trận Pokrovsk. Bộ Quốc phòng Nga ngày 7/9 thông báo lực lượng nước này đã kiểm soát được làng Kalinovo, cách Pokrovsk khoảng 25 km.Một trong những mục tiêu của Kiev khi mở chiến dịch ở tỉnh Kursk của Nga cách đây một tháng là phân tán bớt lực lượng đối phương và giảm sức ép đối với binh sĩ Ukraine ở mặt trận phía đông. Tuy nhiên, việc Nga tuyên bố đạt nhiều bước tiến ở khu vực này cho thấy chiến lược trên dường như chưa phát huy hiệu quả.Tổng thống Nga Vladimir Putin ngày 5/9 cho biết mục tiêu chính của ông ở Ukraine sau 30 tháng giao tranh là kiểm soát toàn bộ vùng Donbass, trong đó có tỉnh Donetsk, thêm rằng chiến dịch của Kiev ở tỉnh Kursk đang khiến mục tiêu đó trở nên dễ dàng hơn.
+Vị trí Novogrodovka. Đồ họa: RYV
+Phạm Giang (Theo AFP, RIA Novosti)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Thổ Nhĩ Kỳ kêu gọi lập liên minh Hồi giáo đối phó Israel</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/tho-nhi-ky-keu-goi-lap-lien-minh-hoi-giao-doi-pho-israel-4790488.html</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Thổ Nhĩ Kỳ kêu gọi các nước Hồi giáo lập liên minh để ứng phó Israel và "mối đe dọa ngày càng gia tăng từ chủ nghĩa bành trướng".</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>"Động thái duy nhất có thể ngăn chặn sự ngạo mạn, ăn cướp của Israel là thành lập liên minh các nước Hồi giáo", Tổng thống Thổ Nhĩ Kỳ Tayyip Erdogan phát biểu tại sự kiện gần thành phố Istanbul ngày 7/9.Theo ông Erdogan, Thổ Nhĩ Kỳ gần đây đã cải thiện quan hệ với Ai Cập và Syria nhằm thiết lập mặt trận đoàn kết để đối phó "mối đe dọa ngày càng tăng từ chủ nghĩa bành trướng", điều mà ông cho là đang đe dọa Syria và Lebanon.Ngoại trưởng Israel Israel Katz chỉ trích phát biểu của ông Erdogan, mô tả đây là "lời dối trá, kích động nguy hiểm" và cáo buộc Tổng thống Thổ Nhĩ Kỳ đang phối hợp với Iran để làm suy yếu chính quyền các nước Arab trung lập ở khu vực.
+Tổng thống Thổ Nhĩ Kỳ Tayyip Erdogan phát biểu tại Istanbul ngày 6/9. Ảnh: AFP
+Ông Erdogan đưa ra bình luận khi đề cập vụ một phụ nữ Mỹ gốc Thổ Nhĩ Kỳ tên Aysenur Ezgi Eygi bị bắn chết trong lúc biểu tình phản đối mở rộng các khu định cư tại những vùng mà Israel kiểm soát ở Bờ Tây. Giới chức Thổ Nhĩ Kỳ và Palestine cáo buộc binh sĩ Israel là thủ phạm.Nhà Trắng kêu gọi Israel lập tức điều tra sự việc. Quân đội Israel cho biết đang xác minh thông tin về vụ một phụ nữ nước ngoài "thiệt mạng do trúng đạn" ở Bờ Tây.Thổ Nhĩ Kỳ, quốc gia thành viên NATO, ủng hộ giải pháp hai nhà nước cho xung đột Israel - Palestine. Ông Erdogan nhiều lần chỉ trích Tel Aviv về chiến dịch tấn công Dải Gaza và cho rằng giới lãnh đạo Israel phải bị xét xử tại tòa án quốc tế.Chiến sự Israel - Hamas bùng phát sau cuộc đột kích của nhóm vũ trang vào miền nam Israel ngày 7/10/2023 gây thương vong lớn. Chiến dịch đáp trả của Israel vào Gaza đến ngày 8/9 đã khiến gần 41.000 người thiệt mạng, hầu hết là phụ nữ và trẻ em, và hơn 94.700 người bị thương.Như Tâm (Theo Reuters)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Những sản phẩm dự kiến ra mắt tại sự kiện Apple Glowtime</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nhung-san-pham-du-kien-ra-mat-tai-su-kien-apple-glowtime-4790303.html</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ngoài bốn phiên bản iPhone 16, Apple nhiều khả năng sẽ công bố đồng hồ Watch series 10, tai nghe AirPods, iPad và máy Mac thế hệ mới.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sự kiện It's Glowtime của Apple sẽ bắt đầu lúc 10h ngày 9/9 (0h ngày 10/9, giờ Hà Nội) tại nhà hát Steve Jobs trong khuôn viên trụ sở Apple Park ở California (Mỹ).Trong thư mời, Apple thiết kế logo với các quầng sáng màu sắc xung quanh, khiến nhiều người liên tưởng đến bộ tính năng Apple Intelligence và biểu tượng trợ lý ảo Siri mới tích hợp trí tuệ nhân tạo.iPhone 16
+Ảnh dựng iPhone 16 Pro. Ảnh: MacRumors
+iPhone 16 là tâm điểm của sự kiện, với bốn phiên bản gồm iPhone 16, 16 Plus, 16 Pro và 16 Pro Max, trang bị nút chụp riêng với công nghệ cảm biến lực ở cạnh phải.iPhone 16 Pro dự kiến tăng kích cỡ màn hình từ 6,1 lên 6,3 inch, còn 16 Pro Max trang bị tấm nền 6,9 inch. Thay đổi này khiến sản phẩm dài hơn 3 mm và rộng hơn 1 mm so với dòng 15 Pro. Theo Ice Universe, sản phẩm cũng sẽ là smartphone có viền màn hình mỏng nhất thế giới. Máy tích hợp chip A18 Pro, nâng cấp mạnh camera, hỗ trợ kết nối Wi-Fi 7 và 5G Advance, đồng thời sử dụng hệ thống tản nhiệt với chất liệu graphene.iPhone 16 và 16 Plus cũng có một số thay đổi về thiết kế như thêm nút chụp hình điện dung ở cạnh phải, nút gạt chế độ âm thanh đổi thành nút Action. Cụm camera phía sau chuyển sang thiết kế dọc như trên iPhone X.Apple sẽ trang bị chip A18 sản xuất trên tiến trình 3 nm cho hai model tiêu chuẩn, RAM nâng lên 8 GB để hỗ trợ Apple Intelligence. Hãng cũng được cho là sẽ sử dụng công nghệ pin xếp chồng để nâng dung lượng và tuổi thọ pin cao hơn.iPad và iPad mini
+iPad Mini. Ảnh: Tuấn Hưng
+Apple có thể ra mắt iPad mới trong sự kiện này do lần nâng cấp gần nhất là vào 2 năm trước. iPad thế hệ mới dự kiến trang bị dòng chip A series mới hơn.Trong khi đó, iPad mini 6 đã ra mắt từ tháng 9/2021 nên model mới cũng có thể xuất hiện. Camera sau của máy có thể nâng lên 48 megapixel giống iPhone hiện tại.Apple Watch series 10
+Ảnh minh họa về Watch X. Ảnh: 9to5mac
+Smartwatch thế hệ mới của Apple có thể được gọi là Watch X với nâng cấp lớn nhằm kỷ niệm cột mốc 10 năm của dòng sản phẩm này. Máy sẽ được làm mỏng và lớn hơn với kích thước 45 và 49 mm.Apple được cho là sẽ thay đổi thiết kế kết nối gắn dây trên smartwatch thế hệ mới. Sản phẩm có thêm tính năng phát hiện ngưng thở khi ngủ và thông báo để người dùng sớm kiểm tra y tế. Tuy nhiên, tính năng đo nồng độ oxy trong máu vẫn không được trang bị trở lại do vụ kiện pháp lý với Masimo về bằng sáng chế.AirPods 4 và AirPods MaxApple đã công bố nhiều thay đổi về cách AirPods sẽ hoạt động trong iOS 18, nên khả năng cao sản phẩm mới sẽ có mặt trong sự kiện tới.Trong đó, AirPods 4 dự kiến có hai phiên bản, gồm một model giá rẻ với thiết kế mới và hộp sạc có cổng USB-C. Phiên bản thứ hai có giá cao hơn với tính năng ANC và Find My tích hợp trong hộp sạc. Ngoài ra, chất lượng âm thanh cũng tốt hơn thế hệ trước.AirPods Max ra mắt lần đầu vào tháng 12/2020 và chưa được nâng cấp sau 4 năm. Model thế hệ mới có thể chuyển sang dùng cổng kết nối USB-C tương tự các sản phẩm khác của Apple và nâng cấp chip xử lý H2 để cải thiện khả năng chống ồn và kéo dài thời lượng pin.Mac mini và iMacVới việc ra mắt chip xử lý M4 vào tháng 5, nhiều nguồn tin cho rằng Apple sẽ công bố bản nâng cấp của Mac mini và iMac vào ngày mai.Mac mini được cho là sẽ có thiết kế mới nhỏ gọn hơn phiên bản hiện tại, trang bị cả chip M4 và M4 Pro. Còn iMac cũng sử dụng chip M4, kích thước màn hình lên 32 inch so với 24 inch hiện tại.MacBook Pro
+MacBook Pro. Ảnh: Tuấn Hưng
+Với chu kỳ nâng cấp thường niên, nhiều khả năng hai model MacBook Pro 14 inch và MacBook Pro 16 inch sẽ xuất hiện trong sự kiện. Tuy nhiên, Macbook Pro mới sẽ không có nhiều thay đổi về thiết kế, chỉ nâng cấp phần cứng với chip M4 mới.
+Huy Đức</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sa Pa dừng mọi hoạt động du lịch vì bão Yagi</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/sa-pa-dung-moi-hoat-dong-du-lich-vi-bao-yagi-4790470.html</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Lào CaiSa Pa quyết định dừng mọi hoạt động tham quan, du lịch từ hôm nay, do nhiều nơi bị sạt lở trong mưa bão Yagi.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>UBND thị xã Sa Pa ngày 8/9 thông báo dừng các hoạt động du lịch ngoài trời; đón khách tham quan tại các điểm di tích, danh thắng trên địa bàn đến khi có thông báo mới. Do ảnh hưởng của bão Yagi, hiện nhiều tuyến đường và các đập tràn ở Sa Pa bị hư hỏng, không đảm bảo an toàn giao thông.
+Khu vực cầu 32, cửa ngõ vào Sa Pa, ngày 8/9. Ảnh: NVCC
+Ông Nguyễn Trung Kiên, đại diện khu du lịch Cát Cát, cho biết mưa lớn từ 7/9 làm đường DH92 từ thị xã xuống khu du lịch sạt lở nghiêm trọng. Đơn vị đã dừng các hoạt động tại đây vào sáng 8/9.Theo ông Kiên, bản Cát Cát vẫn an toàn nhưng lượng nước tại các suối hồ có khả năng dâng cao từ đêm nay. Đại diện UBND xã Tả Van nói đơn vị đang khắc phục các điểm sạt lở. Hiện tại, giao thông bên trong xã vẫn ổn, một số cơ sở homestay vẫn còn khách lưu trú.Nhiều du khách đã hủy dịch vụ du lịch ở Sa Pa từ 5/9 sau khi nghe thông tin về bão. Chị Phạm Thùy Giang, chủ homestay PaVi, cho biết cơ sở của mình và các khu lưu trú lân cận hầu như không có du khách. Đối với những khách đã đặt tour trước đó, homestay cũng chủ động dời ngày để khách có trải nghiệm an toàn hơn khi đến Sa Pa.
+Sạt lở ở đường vào bản Cát Cát
+Sạt lở ở đường vào bản Cát Cát ngày 8/9. Ảnh: Ban quản lý bản Cát Cát
+Nhà xe Interbuslines ghi nhận lượng hủy dịch vụ xe đưa đón từ Hà Nội lên Sa Pa gần 100% trong ngày 7/9. Trong ngày 8/9, hầu hết khách Việt đặt chỗ đều đã hủy vé hoặc báo dời ngày. Hai xe 30 chỗ từ Hà Nội lên Sa Pa chủ yếu chở khách nước ngoài đã mua tour từ trước. Đường đi có một số đoạn sạt lở, phải dừng khoảng 30 phút nhưng không gặp vấn đề lớn.Một số đơn vị lữ hành cho biết đã dừng tất cả hoạt động du lịch từ 5/9 khi được dự báo thời tiết xấu. Theo Bà Mai Thanh Hoa, Giám đốc Công ty Du lịch Tinh thần Cộng đồng, khách du lịch nước ngoài gặp hạn chế về việc tiếp cận thông tin nên đơn vị du lịch cần chủ động thông báo, đặt an toàn lên hàng đầu.Tú Nguyễn - Tuấn Anh</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bộ đội, công an giúp dân khắc phục hậu quả bão Yagi</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/bo-doi-cong-an-giup-dan-khac-phuc-hau-qua-bao-yagi-4790269.html</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bộ đội giúp dân sơ tán đến nơi an toàn, xử lý cổ thụ gãy đổ và cùng người dân dọn dẹp phố phường, khôi phục cuộc sống bình thường sau bão.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Ảnh hưởng của bão Yagi, Lạng Sơn mưa lớn, một số khu vực ở huyện Bắc Sơn, Chi Lăng bị ngập. Bộ đội Biên phòng và Cảnh sát cứu hộ cứu nạn đã hỗ trợ sơ tán người dân và tài sản đến nơi an toàn từ chiều 7/9. 
+Ảnh hưởng của bão Yagi, Lạng Sơn mưa lớn, một số khu vực ở huyện Bắc Sơn, Chi Lăng bị ngập. Bộ đội Biên phòng và Cảnh sát cứu hộ cứu nạn đã hỗ trợ sơ tán người dân và tài sản đến nơi an toàn từ chiều 7/9. 
+Chiến sĩ Biên phòng cõng cụ ông tới nơi tránh trú mưa bão. Bộ đội Biên phòng Lạng Sơn cho biết hơn 150 lượt cán bộ, chiến sĩ của đơn vị đã giúp 18 hộ gia đình sơ tán và di dời tài sản gồm tivi, tủ lạnh, thóc lúa đến nơi an toàn. Bộ đội cũng giúp hơn 35 hộ dân chằng néo nhà cửa phòng chống mưa, bão; di dời cây đổ ảnh hưởng đến giao thông; bố trí người canh gác tại các điểm nguy hiểm có nguy cơ sạt lở. 
+Chiến sĩ Biên phòng cõng cụ ông tới nơi tránh trú mưa bão. Bộ đội Biên phòng Lạng Sơn cho biết hơn 150 lượt cán bộ, chiến sĩ của đơn vị đã giúp 18 hộ gia đình sơ tán và di dời tài sản gồm tivi, tủ lạnh, thóc lúa đến nơi an toàn. Bộ đội cũng giúp hơn 35 hộ dân chằng néo nhà cửa phòng chống mưa, bão; di dời cây đổ ảnh hưởng đến giao thông; bố trí người canh gác tại các điểm nguy hiểm có nguy cơ sạt lở. 
+Hàng chục cán bộ, chiến sĩ cũng được huy động xuống đồng giúp người dân gặt lúa chạy bão. 
+Hàng chục cán bộ, chiến sĩ cũng được huy động xuống đồng giúp người dân gặt lúa chạy bão. 
+Tại Hà Nội, Cảnh sát phòng cháy chữa cháy và cứu hộ cứu nạn tham gia xử lý, dọn dẹp nhiều cổ thụ gãy đổ. Số lượng cây gãy đổ của Hà Nội rất lớn, khoảng 17.000 nên cần nhiều người, nhiều thời gian thu dọn. 
+Tại Hà Nội, Cảnh sát phòng cháy chữa cháy và cứu hộ cứu nạn tham gia xử lý, dọn dẹp nhiều cổ thụ gãy đổ. Số lượng cây gãy đổ của Hà Nội rất lớn, khoảng 17.000 nên cần nhiều người, nhiều thời gian thu dọn. 
+Nhiều xe chuyên dụng được điều đến hiện trường. Thống kê sơ bộ đến sáng 8/9, Cảnh sát Phòng cháy chữa cháy và Cứu hộ cứu nạn Công an TP Hà Nội và công an quận, huyện, thị xã đã điều gần 300 lượt phương tiện cùng gần 2.000 cán bộ, chiến sĩ phối hợp cứu nạn, cứu hộ góp phần giảm thiểu thiệt hại do mưa bão. 
+Nhiều xe chuyên dụng được điều đến hiện trường. Thống kê sơ bộ đến sáng 8/9, Cảnh sát Phòng cháy chữa cháy và Cứu hộ cứu nạn Công an TP Hà Nội và công an quận, huyện, thị xã đã điều gần 300 lượt phương tiện cùng gần 2.000 cán bộ, chiến sĩ phối hợp cứu nạn, cứu hộ góp phần giảm thiểu thiệt hại do mưa bão. 
+Nhân viên Công ty Công viên cây xanh Hà Nội tất bật dọn dẹp khu vực công viên Lênin, đường Trần Phú do nhiều cây gãy đổ.
+Tối 7/9, tâm bão Yagi quét qua Thủ đô gây mưa to, gió mạnh suốt 7 tiếng. Gió bão giật cấp 10 khiến cây đổ la liệt khắp thành phố. 
+Nhân viên Công ty Công viên cây xanh Hà Nội tất bật dọn dẹp khu vực công viên Lênin, đường Trần Phú do nhiều cây gãy đổ.
+Tối 7/9, tâm bão Yagi quét qua Thủ đô gây mưa to, gió mạnh suốt 7 tiếng. Gió bão giật cấp 10 khiến cây đổ la liệt khắp thành phố. 
+Hàng trăm bộ đội công an dọn cây cối đổ trên đường Hoàng Quốc Việt
+Bộ đội, công an dọn cây đổ trên đường Hoàng Quốc Việt, quận Cầu Giấy, Hà Nội. Video: Lộc Chung 
+Tại Quảng Ninh, gió bão trưa 7/9 khiến xe tải chở hàng đang đỗ trên đường bêtông trong khu dân cư ở phường Cẩm Sơn, TP Cẩm Phả bị lật nghiêng. Sau khi bão tan, 16 người hợp sức dùng dây cáp giúp tài xế kéo ôtô đứng dậy. 
+Tại Quảng Ninh, gió bão trưa 7/9 khiến xe tải chở hàng đang đỗ trên đường bêtông trong khu dân cư ở phường Cẩm Sơn, TP Cẩm Phả bị lật nghiêng. Sau khi bão tan, 16 người hợp sức dùng dây cáp giúp tài xế kéo ôtô đứng dậy. 
+Hai người đàn ông lợp tạm mái nhà bằng bạt để phòng mưa ở TP Cẩm Phả. Do ảnh hưởng của bão Yagi, từ chiều đến tối hôm qua, tỉnh Quảng Ninh có gió bão cấp 12-13, giật cấp 17 và mưa 100-250 mm. Theo báo cáo của UBND tỉnh Quảng Ninh, toàn tỉnh có 2.083 nhà bị tốc mái, 254 cột điện bị gãy đổ. Một số nhà dân bị cột điện gãy đè trúng, hư hại. 
+Hai người đàn ông lợp tạm mái nhà bằng bạt để phòng mưa ở TP Cẩm Phả. Do ảnh hưởng của bão Yagi, từ chiều đến tối hôm qua, tỉnh Quảng Ninh có gió bão cấp 12-13, giật cấp 17 và mưa 100-250 mm. Theo báo cáo của UBND tỉnh Quảng Ninh, toàn tỉnh có 2.083 nhà bị tốc mái, 254 cột điện bị gãy đổ. Một số nhà dân bị cột điện gãy đè trúng, hư hại. 
+Chị Nguyễn Thị Chi ở phường Quang Anh, TP Cẩm Phả thu gom những vật dụng còn sót lại sau bão, sáng 8/9. Tầng 1 là quán phở bò, tầng 2 là nơi ở của 5 người trong gia đình, đã bị gió thổi bay toàn bộ mái tôn. "Chỉ trong hơn một phút, mái nhà bị cuốn bay, cả gia đình sợ hãi kéo nhau trốn trong nhà vệ sinh", chị kể, cho biết vợ chồng và 3 đứa con nhỏ phải khăn gói sang nhà người thân ở nhờ. 
+Chị Nguyễn Thị Chi ở phường Quang Anh, TP Cẩm Phả thu gom những vật dụng còn sót lại sau bão, sáng 8/9. Tầng 1 là quán phở bò, tầng 2 là nơi ở của 5 người trong gia đình, đã bị gió thổi bay toàn bộ mái tôn. "Chỉ trong hơn một phút, mái nhà bị cuốn bay, cả gia đình sợ hãi kéo nhau trốn trong nhà vệ sinh", chị kể, cho biết vợ chồng và 3 đứa con nhỏ phải khăn gói sang nhà người thân ở nhờ. 
+Chị Đỗ Thị Nhung 35 tuổi, ở xã Vũ Oai, TP Hạ Long, dọn dẹp nhà sau khi bị bão đánh sập trần. 
+Chị Đỗ Thị Nhung 35 tuổi, ở xã Vũ Oai, TP Hạ Long, dọn dẹp nhà sau khi bị bão đánh sập trần. 
+Tại thị trấn Cái Rồng, huyện Vân Đồn, từ chiều 7/9, ngay khi trời ngớt mưa, bớt gió, nhà chức trách huy động người và phương tiện cắt tỉa, giải phóng những cây bị đổ để tránh cản trở giao thông.
+Khắp các ngả đường ở thị trấn Cái Rồng, xã Hạ Long và nhiều khu vực khác của huyện Vân Đồn tan hoang trong bão. Nhiều biển quảng cáo, cột đèn, biển báo giao thông gãy gập. Hàng trăm mái tôn bị gió thổi bay văng xa hàng trăm mét. 
+Tại thị trấn Cái Rồng, huyện Vân Đồn, từ chiều 7/9, ngay khi trời ngớt mưa, bớt gió, nhà chức trách huy động người và phương tiện cắt tỉa, giải phóng những cây bị đổ để tránh cản trở giao thông.
+Khắp các ngả đường ở thị trấn Cái Rồng, xã Hạ Long và nhiều khu vực khác của huyện Vân Đồn tan hoang trong bão. Nhiều biển quảng cáo, cột đèn, biển báo giao thông gãy gập. Hàng trăm mái tôn bị gió thổi bay văng xa hàng trăm mét. 
+Những tấm tôn bị bay xuống đường được người dân thị trấn Cái Rồng thu gom, tập kết một chỗ.
+Bão Yagi quét qua nhiều tỉnh thành như Quảng Ninh, Hải Phòng, Thái Bình, Hải Dương, Hà Nội... làm 14 người chết, trong đó Hà Nội 3 người, 176 người khác bị thương. 
+Những tấm tôn bị bay xuống đường được người dân thị trấn Cái Rồng thu gom, tập kết một chỗ.
+Bão Yagi quét qua nhiều tỉnh thành như Quảng Ninh, Hải Phòng, Thái Bình, Hải Dương, Hà Nội... làm 14 người chết, trong đó Hà Nội 3 người, 176 người khác bị thương. 
+Giang Huy - Phạm Dự - Duy Anh - Phạm Chiểu</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Người dân xếp hàng mua xăng tại Quảng Ninh</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nguoi-dan-xep-hang-mua-xang-tai-quang-ninh-4790434.html</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Nhiều cây xăng tại các địa phương bị ảnh hưởng do siêu bão Yagi, có nơi người dân phải xếp hàng, chờ gần 30 phút để mua nhiên liệu.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sáng 8/9, hàng trăm người dân mang chai nhựa, can, đứng xếp hàng dài ở cửa hàng 125 - Petrolimex ở phường Hà Tu, thành phố Hạ Long để mua xăng dầu. Sau một ngày bị cắt điện toàn thành phố do bão Yagi, các cây xăng cũng tạm dừng hoạt động để đảm bảo an toàn.
+Anh Hoàng Quang Huy, trú thành phố Hạ Long, cho biết xếp hàng gần 30 phút để mua 10 lít dầu về chạy máy phát điện và 5 lít xăng để đổ cho 3 xe máy của gia đình.
+Người dân xếp hàng chờ mua tại một cây xăng ở Hà Tu, Hạ Long, Quảng Ninh, sáng 8/9. Ảnh: Phạm Dự
+Theo một đại diện của Petrolimex, nhiều cửa hàng xăng dầu trên địa bàn Quảng Ninh chưa khắc phục sau bão, trong khi nhu cầu tăng. Do đó, tại các cửa hàng được mở cửa lại, lượng khách vào đông, nhiều thời điểm có thể phải xếp hàng. Tuy nhiên, ông cho biết hiện chỉ còn một số cây xăng bị thiệt hại nặng, dự kiến được khắc phục để hoạt động trở lại vào ngày mai.Báo cáo của các đơn vị chức năng tại cuộc họp của Bộ Công Thương sáng nay cũng ghi nhận nhiều cơ sở kinh doanh xăng dầu bị thiệt hại do siêu bão Yagi. Trong đó, Công ty Xăng dầu B12 (đầu mối cung cấp xăng dầu lớn nhất miền Bắc, thuộc Petrolimex) bị sạt lở 100 m bờ kè và chìm 2 tàu kéo phao khi đang neo đậu tại kho cảng. Các kho xăng dầu Cái Lân (Quảng Ninh), An Hải và Đình Vũ (Hải Phòng) cũng bị ảnh hưởng.
+Video xếp hàng mua xăng chạy máy phát Hạ Long
+Người dân xếp hàng chờ mua xăng tại Quảng Ninh, sáng 8/9. Video: Huy Mạnh
+Tại Hải Phòng và Quảng Ninh, nhiều cửa hàng xăng dầu bị tốc mái. Tình trạng mất điện diện rộng, không có kết nối Internet cũng ảnh hưởng tới các cơ sở bán hàng tự động và kết nối dữ liệu hóa đơn điện tử.Tại Bắc Giang, sáng nay các cửa hàng kinh doanh xăng dầu vẫn mở cửa bán. Hệ thống cửa hàng trên địa bàn tỉnh chưa ghi nhận thêm thiệt hại đáng kể nào. Dự kiến, hoạt động cung ứng xăng dầu diễn ra bình thường.Tại Hà Nội, báo cáo nhanh của Sở Công Thương cập nhật đến 9h cho thấy, thành phố không có thiệt hại về người và các trang thiết bị phục vụ bán hàng tại các cửa hàng xăng dầu. Đa số các cửa hàng bị hư hại như bong tróc hệ thống quảng cáo, rơi biển hiệu, vỡ cửa kính, tốc mái, đứt, chập dây điện, cây đổ gần vị trí cửa hàng. Sáng sớm, các doanh nghiệp đã dọn dẹp, khắc phục hậu quả. Hiện, cơ bản các cửa hàng hoạt động bình thường.Chỉ một số cây xăng tạm dừng do sự cố mất điện lưới, chờ cơ quan điện khắc phục, xử lý sự cố đứt đường dây, dọn dẹp cây đổ... Một số cửa hàng chỉ thanh toán được bằng tiền mặt do mất tín hiệu viễn thông.Vụ Thị trường trong nước (Bộ Công thương) đề nghị EVN, EVNNPC ưu tiên cấp điện cho xăng dầu, các hệ thống cung cấp hàng hóa thiết yếu, nhất là khắc phục điện cho khu vực B12 để bơm xăng dầu với khu vực 1 và miền Bắc.Tại cuộc họp sáng nay, Bộ trưởng Công Thương Nguyễn Hồng Diên cũng đề nghị chính quyền địa phương phối hợp với các bộ ngành chỉ đạo thương nhân đầu mối, phân phối bảo đảm duy trì nguồn cung xăng dầu trong mọi tình huống. Bộ Thông tin và Truyền thông khắc phục, khôi phục cung cấp dịch vụ viễn thông, mạng Internet để phục vụ hoạt động cung cấp điện, xăng dầu...Phạm Dự - Phương Dung</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tháo dỡ bãi nuôi hàu trái phép trên sông Rác</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/thao-do-bai-nuoi-hau-trai-phep-tren-song-rac-4790455.html</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hà TĩnhChính quyền huy động hơn 150 lượt người tháo dỡ hàng nghìn cọc bêtông, cọc tre, lốp xe dùng để nuôi hàu trên sông Rác ở huyện Cẩm Xuyên.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Ngày 8/9, lãnh đạo huyện Cẩm Xuyên cho biết cuối tháng 8 và đầu tháng 9 đã thành lập các đoàn liên ngành kiểm tra, rà soát, thống kê được 78 hộ dân tự ý nuôi trồng thủy sản trái phép trên sông Rác đoạn qua xã Cẩm Lĩnh và bãi bồi cửa biển. Nhà chức trách đã làm việc với các chủ bãi hàu, tuyên truyền vận động họ tháo dỡ, trả lại hiện trạng ban đầu cho sông, nhưng đa số không chấp hành.
+Nhiều lực lượng tháo dỡ bãi nuôi hàu trái phép trên sông Rác hồi cuối tháng 8. Ảnh: Hùng Lê
+Những ngày sau đó, xã Cẩm Lĩnh đã huy động 150 lượt người gồm cán bộ xã, thôn xóm, dân quân, đoàn thanh niên... xuống sông Rác tháo dỡ được hơn 2.000 cọc bêtông, cọc tre, dây néo trên diện tích 5 ha, lập biên bản xử lý 7 hộ.Lãnh đạo xã Cẩm Lĩnh cho hay việc tháo dỡ được tập trung vào các vị trí quan trọng, ảnh hưởng đến cảnh quan, dòng chảy tiêu thoát lũ, cản trở giao thông đường thủy... Quá trình làm việc gặp nhiều khó khăn do khối lượng cọc bêtông và các vật liệu khác lớn, cắm sâu dưới đáy sông nên không thể sử dụng sức người thu gom hết, huy động máy móc cũng tốn kém."Nhiều vị trí liên quan đến việc cho thuê đất trái thẩm quyền kéo dài hàng chục năm nay chưa giải quyết xong, người dân vẫn đầu tư nuôi thủy sản, vì thế gây khó khăn cho quá trình xử lý", lãnh đạo nói.
+Cọc bêtông, lốp xe dày đặc trên sông Rác đoạn tiếp giáp với cầu Cửa Nhượng, huyện Cẩm Xuyên hồi giữa tháng 8. Ảnh: Đức Hùng
+Thời gian tới, nhà chức trách huyện Cẩm Xuyên tiếp tục huy động lực lượng tháo dỡ các bãi nuôi hàu trái phép trên sông Rác, tuyên truyền người dân nuôi đúng quy hoạch, không ảnh hưởng đến dòng chảy, môi trường, cảnh quan.Sông Rác dài 35-40 km, chảy qua hai huyện Kỳ Anh và Cẩm Xuyên. Tại đoạn hai km qua xã Cẩm Lĩnh và Cẩm Trung, huyện Cẩm Xuyên, người dân cắm hàng nghìn trụ bêtông và cọc tre xuống đáy, cố định dây thừng và lốp xe để làm giá nuôi hàu khi chưa được chính quyền cho phép thuê đất, thuê mặt nước.
+Hiện trạng các bãi nuôi hàu trái phép ở huyện Cẩm Xuyên
+Bãi nuôi hàu trái phép ở huyện Cẩm Xuyên hồi giữa tháng 8. Video: Đức Hùng
+Theo thống kê, dọc bờ sông Rác đoạn qua huyện Cẩm Xuyên có gần 30 ha mặt nước bị người dân chiếm dụng để nuôi hàu tự phát. Tình trạng này xảy ra từ nhiều năm, lực lượng chức năng đã tới gặp các hộ dân tuyên truyền tháo dỡ, nhưng chưa thể chấm dứt.Theo các chủ bãi hàu, trước đây chính quyền cho họ thuê mặt nước để nuôi trồng thủy sản trên sông Rác, nhưng sau đó chấm dứt hợp đồng. Nhiều năm qua, vì "tiếc tiền" đã bỏ ra đầu tư, nhiều gia đình vẫn cố làm dù biết là không đúng.
+Đức Hùng</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Giá rau xanh tăng sau bão</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/gia-rau-xanh-tang-sau-bao-4790435.html</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Tại nhiều chợ dân sinh ở Hà Nội, Hải Phòng, các loại rau muống, mồng tơi, cải đều có giá 15.000 đồng một bó, tăng khoảng 30% so với hai ngày trước.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sáng 8/9, các khu chợ ở Hà Nội, Hải Phòng, Quảng Ninh đã hoạt động lại sau cơn bão Yagi, nhưng lượng người bán và mua vắng hơn mọi ngày. Giá thực phẩm như thịt, cá không biến động nhiều, dẫu vậy rau xanh tăng mạnh. Trong đó, nhiều loại như mồng tơi, cải, ngót... đều có giá 15.000 đồng một bó.
+Một quầy rau xanh (chủ yếu củ, quả) ở Nam Từ Liêm, Hà Nội sau ngày bão tấn công. Ảnh: Anh Tú
+Theo một tiểu thương kinh doanh ở chợ Nghĩa Tân (Cầu Giấy), giá rau củ đã tăng dần từ mấy ngày trước bão khi nhu cầu tích trữ của người dân lên cao. "Giá rau hôm nay tăng tiếp 20-30% so với hai ngày trước", người này nói.Chị Thu Thanh, trú phường Kênh Dương, quận Lê Chân, Hải Phòng cho biết các chợ dân sinh ở khu vực này đã mở cửa, nhưng số lượng sản phẩm không nhiều. Nhiều loại rau xanh cũng được bán 15.000 đồng một bó, chỉ có rau dền rẻ hơn, khoảng 12.000-13.000 đồng. Các loại củ quả khác tăng nhẹ như su su, bắp cải 20.000 đồng một kg...Tại Quảng Ninh, theo báo cáo của Sở Công Thương tỉnh, một số mặt hàng rau, củ, quả cũng có xu hướng tăng 5-10% so với những ngày trước đó, tập trung tại các chợ, cửa hàng nhỏ.Lý giải giá rau tăng, các tiểu thương cho biết do giá mua vào tăng cao, việc nhập hàng, di chuyển cũng khó khăn hơn nhiều do ảnh hưởng mưa bão. Dự kiến giá rau vài ngày tới khó giảm vì mưa to, gió lớn gây thiệt hại nhiều hoa màu.
+Quầy hàng rau, củ tại một siêu thị lớn trên đường Trần Đăng Ninh, Cầu Giấy lúc 12h trưa 8/9. Ảnh: Anh Tú
+Trong khi đó tại siêu thị, giá các loại rau, củ vẫn được giữ ở mức ổn định. Ghi nhận trưa 8/9, các kệ thực phẩm, rau củ ở nhiều siêu thị Hà Nội đầy ắp, không còn cảnh cháy hàng như hai ngày trước. Tại một siêu thị lớn trên đường Trần Đăng Ninh (Cầu Giấy), các loại rau như cải, muống có giá từ 13.000-15.000 đồng một bó, nặng 0,45-0,5 kg, bắp cải từ 22.000 đồng một kg.Còn ở Hải Phòng, người dân đến các siêu thị ngay từ sáng sớm để mua bánh mỳ, nước lọc khi nhiều khu vực thành phố này vẫn chưa có điện và nước. Đến giờ trưa, một số điểm bán hết nước lọc trên kệ hàng. Đồng thời, nhiều người cũng đến siêu thị để tranh thủ sạc điện thoại, thiết bị điện tử.
+Người dân Hải Phòng đổ đến trung tâm thương mại Aeon Mall ở quận Lê Chân lúc đầu giờ chiều 8/9. Ảnh: Dương Thanh
+Đại diện Aeon Việt Nam cho biết sáng nay, sau cơn bão người dân đã bắt đầu đi mua sắm trở lại, chủ yếu vẫn là các mặt hàng thiết yếu. Hệ thống này sẽ bổ sung đầy đủ hàng hóa, ổn định giá để đáp ứng nhu cầu.Tương tự bà Nguyễn Thị Kim Dung, Giám đốc siêu thị Co.opmart Hà Nội, cho hay hiện tại hàng hóa tại siêu thị vẫn đầy đủ, giá cả ổn định. "Một số nhà cung cấp không giao hàng hôm nay nhưng chúng tôi đã có dự trữ đủ hàng để phục vụ người dân", bà Dung nói.Hôm nay, toàn bộ siêu thị WinMart hoạt động bình thường. Các cửa hàng nhỏ hơn như WinMart+/ Win cũng mở cửa trừ một số cơ sở bị thiệt hại (vỡ kính, bay mái tôn) hay nằm trong khu vực lụt, cây đổ gây cản trở giao thông.Vụ Thị trường trong nước (Bộ Công Thương) cho rằng nhu cầu tiêu dùng trên thị trường sẽ giảm do hàng hóa thiết yếu đã được mua từ ngày 6/9. Tình hình cung ứng hàng hóa, lương thực, thực phẩm, xăng dầu cơ bản đảm bảo. Bộ Công Thương sẽ tiếp tục bám sát, cập nhật tình hình để có chỉ đạo.Anh Tú - Phương Dung</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Hoàn thành nâng cấp đường nối cù lao phía Đông TP HCM</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/hoan-thanh-nang-cap-duong-noi-cu-lao-phia-dong-tp-hcm-4790430.html</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tuyến đường 6 km kết nối cù lao Long Phước qua trung tâm Thủ Đức hoàn thành nâng cấp tạo diện mạo mới cho khu vực, người dân thuận tiện đi lại.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Chiều 8/9, đại diện Ban Quản lý dự án đầu tư xây dựng khu vực TP Thủ Đức (chủ đầu tư), cho biết dự án nâng cấp đường Long Phước dài gần 6 km, thuộc phường Long Phước, đã cơ bản hoàn thành sau gần hai năm khởi động trở lại.Tuyến đường được chỉnh trang, mở rộng lên 9-12 m kết hợp các hạng mục thoát nước, chiếu sáng, vỉa hè... Trong tổng mức đầu tư hơn 260 tỷ đồng, kinh phí xây lắp của dự án chiếm phần ít với khoảng 75 tỷ đồng, còn lại chủ yếu là tiền đền bù, giải phóng mặt bằng.
+Đường Long Phước kết nối vào cầu Long Đại, phía trước là khu dân cư Vinhome Grand Park, tháng 9/2024. Ảnh: Gia Minh
+Dự án nâng cấp đường Long Phước khởi công cuối năm 2017, nhưng hai năm sau dừng do vướng mặt bằng. Thủ tục đền bù cho các hộ tiếp tục gặp khó khăn trong hai năm đại dịch, phải tới cuối năm 2022 dự án mới thi công trở lại. Đến nay, toàn bộ dự án chỉ còn một số hạng mục nhỏ như vỉa hè đang hoàn thiện.Được bao bọc bởi sông Đồng Nai, sông Tắc, vùng đất Long Phước còn được gọi là cù lao, giao thông cách trở, đi lại khó khăn. Đường Long Phước cũng là tuyến nối vào cầu Long Đại mới đưa vào khai thác cuối năm 2023. Trục đường này sau khi hoàn thành nâng cấp giúp người dân thuận tiện đi lại, rút ngắn hành trình sang phường Long Bình, vào trung tâm TP Thủ Đức còn hơn 500 m thay vì phải chạy vòng khoảng 10 km như trước.
+Đường Long Phước nằm dưới cao tốc TP HCM - Long Thành - Giây. Ảnh: Gia Minh
+Ngoài ra, đường Long Phước còn là một trong những tuyến quan trọng khi có các trục giao thông lớn cắt qua là cao tốc TP HCM - Long Thành - Dầu Giây (đã khai thác) và Vành đai 3 (đang xây dựng).Trước đó, ngành giao thông thành phố từng đề xuất xây dựng nút giao kết nối đường Long Phước với cao tốc trong phương án mở rộng tuyến đường này. Khi hai tuyến được kết nối, người dân ở khu vực thuận tiện ra vào nội thành, giảm áp lực cho trục đường hiện hữu là Long Phước - Long Thuận - Nguyễn Duy Trinh.
+ Hướng tuyến đường Long Phước. Đồ hoạ: Đăng Hiếu
+Ngoài đường Long Phước, nhiều công trình giao thông trọng điểm khác ở TP Thủ Đức sau thời gian dài vướng mặt bằng được triển khai trở lại. Trong đó, tháng 9 này ở địa phương dự kiến có thêm cầu Nam Lý được thông xe, giảm ùn tắc đường Đỗ Xuân Hợp, góp phần hoàn thiện mạng lưới giao thông khu đông TP HCM.Gia Minh</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hơn 20 tàu du lịch Hạ Long chìm vì bão Yagi</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/hon-20-tau-du-lich-ha-long-chim-vi-bao-yagi-4790415.html</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Quảng NinhBão Yagi đánh chìm hơn 20 tàu ở bến cảng Tuần Châu, nơi đưa khách tham quan vịnh Hạ Long, khiến chủ tàu thiệt hại hàng tỷ đồng.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Đại diện Cảng tàu khách Quốc tế Tuần Châu cho biết hơn 20 tàu du lịch bị siêu bão Yagi đánh chìm, theo thống kê đến sáng nay. Hiện tại, công tác thống kê, xác minh chủ phương tiện vẫn chưa hoàn tất do sóng viễn thông kém, mất điện, nhiều phương tiện đi tránh trú chưa liên lạc được.Cảng Tuần Châu là một trong ba bến cảng được phép đón trả khách du lịch tham quan trên vịnh Hạ Long, diện tích hơn 1,7 triệu m2 và sức chứa trên 2.000 tàu. Đây cũng là nơi đặt nhà chờ của nhiều đơn vị kinh doanh dịch vụ du thuyền ngủ đêm trên vịnh Lan Hạ.
+video hiện trường tàu Tuần Châu
+Nhiều tàu bị đánh chìm, va đập hư hỏng tại Tuần Châu. Video: Huy Mạnh
+Theo tìm hiểu, chi phí đóng tàu du lịch chở khách tham quan vịnh trong ngày thường khoảng hai tỷ đồng, tàu ngủ đêm, vỏ thép khoảng 35 tỷ đồng. Ông Duy Anh, chủ 5 tàu du lịch hoạt động trên vịnh Lan Hạ, ước tính ban đầu đơn vị ông bị thiệt hại khoảng 5 tỷ đồng."May mắn tàu không chìm nhưng hệ thống cầu tàu, nhà chờ, kho bãi và các vật dụng phục vụ du lịch bị bão san thành bình địa", ông nói.Trước khi Hải Phòng có lệnh cấm biển, ông đã đưa hết tàu về bến, hủy tour của khách, để có chỗ neo đậu an toàn.
+Tàu chở khách tham quan trong ngày bị sóng đánh tấp vào cầu tàu của công ty ông Duy Anh và chìm sau đó, cầu tàu hư hỏng nặng. Ảnh: NVCC
+CEO Phạm Hà của Lux Group - đơn vị kinh doanh du thuyền trên vịnh Lan Hạ - nói hai xuồng chở khách từ cảng ra tàu lớn bị chìm, cần trục vớt để sửa chữa. Tàu du lịch chở khách ngủ đêm của đơn vị cũng bị gió bão đánh va đập nhưng cơ bản vẫn hoạt động được. Đại diện đơn vị này nói do cột sóng viễn thông bị đổ nên nhiều chủ tàu mất liên lạc với thuyền viên, công tác thống kê thiệt hại còn khó khăn.Tại Hạ Long, nhiều khách sạn ghi nhận thiệt hại nặng vì bão Yagi trong ngày 7/9. Khách sạn Novotel Hạ Long cho biết hàng loạt cửa kính của bị vỡ, khuôn viên cây cảnh gãy đổ. Tới sáng 8/9 Hạ Long vẫn mưa to nên khách sạn chưa thống kê được đầy đủ thiệt hại. Khách sạn Diamond ở Hạ Long cho biết "thiệt hại rất nhiều" về tài sản khi loạt cửa kính, mái hiên bị gió giật đổ.Hannah McEvoy, khách lưu trú dài hạn ở tầng cao khách sạn Best Western Premier Sapphire Halong, nói những gì đã trải qua trong ngày 7/9 "thực sự đáng sợ". Cô cảm giác tòa nhà lắc lư và phòng của mình rung lên vì gió. Do sợ cửa kính có thể vỡ, trong tối cùng ngày, cô được nhân viên khách sạn bố trí vào ở một phòng thấp hơn cùng một số khách khác còn lưu trú.Tới sáng 8/9, McEvoy mới trở lại phòng cũ, nơi chỉ bị nước tràn ướt sàn nhà. Tuy nhiên, nữ du khách cho biết khu vực sảnh và xung quanh khách sạn có nhiều kính vỡ, cây đổ.
+Bên ngoài khách sạn McEvoy thuê. Ảnh: NVCC
+Quan Lạn, Quảng Ninh, cũng là điểm chịu thiệt hại nặng nề vì bão. Tới khoảng 9h ngày 8/9, sóng viễn thông trên đảo vẫn gặp vấn đề, đường phố tan hoang vì cây đổ, nhà tốc mái. Anh Phương Nam, chủ một khách sạn trên đảo, nói cơ sở không bị tàn phá nặng nhưng bị tốc mái, khiến nước tràn ngập 5 tầng. Chủ khách sạn quan ngại khó đón khách trong tuần tới khi hệ thống điện còn gặp vấn đề và cơ sở vật chất phục vụ du lịch bị thiệt hại.Tại Đồ Sơn, Hải Phòng, hàng chục cửa hàng, nhà dân bị tốc mái, hư hỏng nặng sau bão Yagi. Cây cối, tôn, tường bao ngổn ngang khắp nơi tại bãi biển Đồ Sơn. Anh Vũ Văn Khánh, chủ kinh doanh dịch vụ ăn uống, nhà nghỉ cho biết nhà anh "gần như bị xóa sổ", thiệt hại ước tính hơn 3 tỷ đồng.Tâm bão Quảng Ninh hôm qua hứng chịu sức gió mạnh nhất ở Bãi Cháy, lên tới cấp 14, các khu vực cấp 12-13. Thống kê đến sáng nay, tỉnh có 38 tàu, thuyền bị chìm, mất tích; 1.000 lồng bè nuôi trồng thủy sản bị hư hại, chìm, mất tích. Số nhà bị tốc mái, hư hại lên đến hàng nghìn.
+Nhà nghỉ của anh Vũ Văn Khánh tại Đồ Sơn, Hải Phòng. Ảnh: Anh Phú
+Từ chiều đến tối qua, toàn tỉnh Quảng Ninh, TP Hải Phòng và Thái Bình phải cắt điện để khắc phục sự cố và đảm bảo an toàn trong mưa bão. Đến sáng nay, nhiều khu vực vẫn mất điện.Nhiều công ty lữ hành có đoàn khởi hành du lịch tuyến miền Bắc, qua Hà Nội, Hạ Long tuần tới quan ngại về khả năng cung ứng dịch vụ.Công ty CP Truyền thông Du Lịch Việt, có hai đoàn khởi hành từ phía TP HCM, tham quan tuyến du lịch miền Bắc từ 10/9, lo ngại khả năng cung ứng thực phẩm của các đối tác nhà hàng và tính khả thi của lịch trình du lịch Hạ Long - một trong những điểm chịu ảnh hưởng nặng nhất của bão Yagi. Hiện tại, các đối tác chưa thể cập nhật đủ thông tin do nhiều nhân viên còn nghỉ làm, lo dọn dẹp nhà cửa và sóng viễn thông chưa ổn định.Đại diện Vietluxtour nói theo lịch dự kiến, công ty có khoảng 10 đoàn du lịch miền Bắc và ba đoàn sẽ tới Hạ Long. Tuy nhiên, với việc các cơ sở phục vụ du lịch bị ảnh hưởng, một số đoàn có thể phải chuyển hướng tour, dời lịch khởi hành.Tuấn Anh - Tú Nguyễn</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Khoảnh khắc rocket Hezbollah bay tới tấp vào Israel</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/khoanh-khac-rocket-hezbollah-bay-toi-tap-vao-israel-4790405.html</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hezbollah phóng 50 rocket nhằm vào lãnh thổ Israel để đáp trả vụ ba nhân viên ứng phó khẩn cấp bị đối phương "sát hại" ở Lebanon.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Lực lượng Phòng vệ Israel (IDF) thông báo hơn 50 rocket rạng sáng nay bay từ lãnh thổ Lebanon về hướng thành phố Kiryat Shmona ở miền bắc nước này. Khoảng 20 quả được phóng lúc 1h30 và 2h30, phần lớn bị lưới phòng không Israel đánh chặn, song một số đã gây ra thiệt hại vật chất. Một rocket đã bắn trúng một tòa nhà, còn một quả khác rơi xuống vỉa hè.Khoảng 30 quả rocket còn lại được khai hỏa vào lúc 5h30, một số bị đánh chặn, số còn lại rơi xuống khu vực trống trải. Không ai bị thương sau các vụ tấn công.Video đăng trên mạng xã hội cho thấy hàng loạt rocket bay liên tục về hướng thành phố Kiryat Shmona khi trời vẫn tối đen, tạo thành các vệt sáng lớn trên bầu trời.
+Khoảnh khắc loạt rocket Hezbollah bay tới tấp vào Israel
+Rocket Hezbollah bay vào lãnh thổ Israel rạng sáng 8/9. Video: X/OSINTdefender
+Nhóm vũ trang Hezbollah tại Lebanon ngày 8/9 thông báo sáng cùng ngày đã phóng "loạt rocket Falaq" nhằm "đáp trả các vụ tấn công của đối phương", đặc biệt là cuộc tập kích khiến các nhân viên cứu hộ thiệt mạng ở làng Froun.Bộ Y tế Lebanon cáo buộc Israel hôm 7/9 "nhắm mục tiêu vào một tổ phòng vệ dân sự đang làm nhiệm vụ dập hỏa hoạn, vốn do các cuộc tập kích gần đây của Tel Aviv gây ra tại làng Froun". Cuộc tập kích của Israel "khiến ba nhân viên ứng phó khẩn cấp thiệt mạng".Cơ quan này lên án sự việc, gọi đây là "vụ tấn công trắng trợn nhằm vào lực lượng thuộc cơ quan chính thức của nhà nước Lebanon".Phong trào Amal, đồng minh của Hezbollah, cho biết hai thành viên của nhóm nằm trong số những người chết trong vụ tập kích ngày 7/9 của Israel, thêm rằng họ "đang làm nhiệm vụ nhân đạo và quốc gia để bảo vệ Lebanon" khi thiệt mạng.Trong khi đó, Israel tuyên bố đã hạ các thành viên Amal trực thuộc "một cơ cấu quân sự của Hezbollah".Sau vụ tấn công sáng 8/9 của Hezbollah, quân đội Israel không kích đáp trả nhằm vào các cơ sở quân sự của nhóm vũ trang tại miền nam Lebanon.
+Vị trí Israel và Lebanon. Đồ họa: AFP
+Giao tranh xuyên biên giới giữa Israel và Hezbollah diễn ra gần như hàng ngày sau khi xung đột tại Dải Gaza bùng phát tháng 10 năm ngoái. Hezbollah tuyên bố họ tập kích Israel nhằm thể hiện ủng hộ với đồng minh Hamas tại Dải Gaza.Các cuộc đụng độ đã khiến 614 người thiệt mạng ở Lebanon, phần lớn là các tay súng, song cũng bao gồm 138 dân thường, theo số liệu của AFP. Bộ trưởng Y tế Lebanon Firass Abiad cho biết 27 nhân viên ứng phó khẩn cấp và nhân viên y tế đã tử vong, bên cạnh 94 người bị thương, do "hành động gây hấn của Israel".Hai bệnh viện và 21 trung tâm y tế đã bị nhắm mục tiêu, trong khi 32 xe cứu hỏa, cứu thương đã bị hư hỏng một phần hoặc không thể hoạt động tiếp, ông cho hay.Trong khi đó, giới chức Israel cho biết ít nhất 24 binh sĩ và 26 dân thường nước này đã thiệt mạng do xung đột với Hezbollah.Phạm Giang (Theo AFP, Times of Israel)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bão Yagi làm 14 người chết</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/bao-yagi-lam-14-nguoi-chet-4790367.html</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bão Yagi đổ bộ Quảng Ninh - Hải Phòng với sức gió cấp 12-13 làm 14 người chết, trong đó Quảng Ninh 4, Hà Nội 3 người, 176 người khác bị thương.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Theo Cục Cứu hộ - Cứu nạn, Bộ Quốc phòng, tổng hợp đến 10h sáng nay bão Yagi đã làm 4 người ở Quảng Ninh, 4 người ở Hòa Bình, 3 người ở Hà Nội, Hải Phòng, Hải Dương, Quân khu 3 mỗi nơi có một người chết. Ngoài ra, 176 người, chủ yếu ở Quảng Ninh bị thương. Các nạn nhân chủ yếu do bị cây đổ đè vào người, sạt lở đất và tàu bè trôi, mất tích.Tâm bão Quảng Ninh hứng chịu sức gió mạnh nhất ở Bãi Cháy lên tới cấp 14, các khu vực cấp 12-13 chịu nhiều tổn thất nhất về tài sản. Thống kê đến sáng nay, tỉnh có 38 tàu, thuyền bị chìm, mất tích; 1.000 lồng bè nuôi trồng thủy sản bị hư hại, chìm, mất tích. Số nhà bị tốc mái, hư hại lên đến hàng nghìn.
+Cột điện gãy đổ ở Đồ Sơn, Hải Phòng. Ảnh: Anh Phú
+Mạng lưới điện chịu thiệt hại với 401 cột điện bị gãy đổ, 27 trạm biến áp hư hỏng. Từ chiều đến tối qua, toàn tỉnh Quảng Ninh, TP Hải Phòng và Thái Bình phải cắt điện để khắc phục sự cố và đảm bảo an toàn trong mưa bão, làm hơn 3 triệu khách hàng (hộ gia đình, doanh nghiệp) bị ảnh hưởng. Đến sáng nay, nhiều khu vực vẫn mất điện.Sóng di động cũng gián đoạn từ chiều qua do 7 tuyến cáp quang liên tỉnh đứt, 27 cột phát sóng gãy đổ, 6.285 trạm mất điện trong bão Yagi, theo Cục Viễn thông, Bộ Thông tin và Truyền thông. Đến sáng nay, tại một khu vực ở Hải Phòng, Quảng Ninh và Hải Dương, nhiều người phản ánh chưa bắt được sóng di động.121.500 ha lúa và hoa màu bị ngập, hư hại sau bão, tập trung tại Thái Bình, Hải Phòng, Hải Dương, Bắc Ninh, Hà Nội, Nam Định, Hưng Yên, Hà Nam. 5.000 ha cây ăn quả tại Hải Phòng, Thái Bình, Hưng Yên bị hư hại. Cây xanh ở miền Bắc gãy đổ rất nhiều, địa phương đang thống kê, riêng Hà Nội khoảng 17.000 cây.
+Một chiếc ôtô bị cây đổ đè bẹp ở bán đảo Linh Đàm, Hà Nội. Ảnh: Lộc Chung
+Sáng 8/9, Thủ tướng Phạm Minh Chính chủ trì hội nghị trực tuyến với 26 địa phương từ Thanh Hóa trở ra để đánh giá công tác chỉ đạo ứng phó, triển khai các biện pháp cấp bách khắc phục hậu quả bão Yagi.Phát biểu mở đầu hội nghị, Thủ tướng Phạm Minh Chính nói bão Yagi hoành hành trên đất liền hơn một ngày gây hậu quả nghiêm trọng. Hoàn lưu bão sẽ tiếp tục gây mưa lũ, nhất là các tỉnh miền núi phía Bắc.Thủ tướng yêu cầu cần rà soát ngay, hỗ trợ cho các địa phương bị thiệt hại, các gia đình có người thiệt mạng. Trong lúc này, người dân đang phải chịu thiệt hại, phải bàn với tinh thần khẩn trương; tiếp tục triển khai ngay các công việc khắc phục hậu quả bão; kịp thời xử lý các vấn đề liên quan tới đời sống người dân, sản xuất, kinh doanh, ứng phó sạt lở, sụt lún.Bão giảm cấp không theo quy luật thông thườngTại hội nghị, Bộ Tài nguyên và Môi trường đánh giá bão Yagi "rất đặc biệt", hình thành phía đông Philippines, mạnh lên thành siêu bão trên Biển Đông và là cơn bão mạnh nhất tại đây trong 30 năm qua. Yagi tăng cường độ rất nhanh, trong 24 giờ đã tăng 8 cấp lên cấp 16 siêu bão và duy trì cấp này trong thời gian dài. Kể cả khi đổ bộ đảo Hải Nam của Trung Quốc đêm 6/9, bão vẫn đạt cấp siêu bão.Mức độ giảm cấp trên đường đi của Yagi "không theo quy luật thông thường". Bình thường các cơn bão đi qua đảo Hải Nam vào vịnh Bắc Bộ do ma sát với đảo sẽ yếu đi nhanh, nhưng Yagi chỉ giảm 2 cấp, còn 14. Khi áp sát bờ biển Quảng Ninh - Hải Phòng vào trưa qua, bão vẫn giữ cấp 12-13.Thời gian Yagi lưu trên đất liền kéo dài 12 giờ, trong đó nhiều giờ sau khi đổ bộ Quảng Ninh - Hải Phòng bão vẫn giữ cấp 12-13. Đến 4h sáng nay, Yagi suy yếu thành áp thấp nhiệt đới ở Tây Bắc Bộ, dự báo trong 12-24 giờ tới suy yếu thành vùng thấp và tan dần.Hôm qua, lý giải vì sao bão chậm giảm cấp dù đã đổ bộ, ông Mai Văn Khiêm, Giám đốc Trung tâm Dự báo Khí tượng Thủy văn quốc gia, cho biết hoàn lưu của bão Yagi rất rộng, bao trùm cả Bắc Bộ, Bắc Trung Bộ và có tính chất đối xứng khiến việc giảm cấp nhanh rất khó. Bề mặt đệm ở Bắc Bộ nóng, ẩm, là nguồn cung cấp năng lượng cho bão.
+Người dân Hà Nội: 'Xót xa khi nghe gió bão rít, cây đổ rầm rầm'
+Hà Nội tan hoang sau bão Yagi. Video: Lộc Chung - Văn Ngọc - Bá Nam
+Bộ Tài nguyên và Môi trường đánh giá dự báo của Việt Nam về cường độ, hướng đi của bão Yagi sát với thực tế từ khi ở vịnh Bắc Bộ cũng như khi vào đất liền. Dự báo hai ngày tới hoàn lưu bão Yagi sẽ gây mưa lớn cho đồng bằng, trung du và miền núi phía Bắc, lượng mưa trung bình 24 giờ có thể lên tới 100-150 mm, có nơi lên đến hơn 200 mm.Trên các sông nhỏ ở Quảng Ninh, Lạng Sơn, Cao Bằng, Hòa Bình, lũ có thể lên mức báo động 2-3. Các tỉnh thành Quảng Ninh, Hải Phòng, Lạng Sơn, Thái Nguyên, Cao Bằng, Hà Giang, Yên Bái, Bắc Kạn, Nam Định, Thái Bình, Hà Nam, Hà Nội có nguy cơ cao ngập lụt do mưa lớn.Nhiều địa phương như Quảng Ninh, Lạng Sơn, Bắc Kạn, Thái Nguyên, Bắc Giang, Vĩnh Phúc, Hòa Bình, Phú Thọ, Tuyên Quang, Yên Bái, Sơn La, Lai Châu, Lào Cai, Thanh Hòa đối diện nguy cơ lũ ống, lũ quét, sạt lở đất.Viết Tuân - Gia Chính</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: Update history.py to include conversation history and prompt update function
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -463,681 +463,650 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6 người chết do sạt lở đất ở Sa Pa</t>
+          <t>Nghi phạm âm mưu ám sát ông Trump từng làm gì ở Ukraine?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/6-nguoi-chet-do-sat-lo-dat-o-sa-pa-4790475.html</t>
+          <t>https://vnexpress.net/nghi-pham-am-muu-am-sat-ong-trump-tung-lam-gi-o-ukraine-4793710.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lào CaiĐất đá từ trên núi cao sạt xuống khu dân cư ở thị xã Sa Pa, vùi lấp 17 người, làm 6 người chết, 9 người bị thương, trưa 8/9.</t>
+          <t>Ryan Routh từng đến Ukraine ngay sau khi xung đột nổ ra, cố gắng tuyển mộ quân nhân Afghanistan đến chiến đấu cho Kiev, nhưng bị mô tả là "lập dị" và gây nhiều nghi ngại.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Khoảng 13h ngày 8/9, thị xã Sa Pa mưa lớn. Vạt núi cao khoảng 20 m bất ngờ sạt xuống, tràn qua khu ruộng bậc thang và tràn vào khu dân cư thôn Thào Hồng Dến 2, xã Mường Hoa.Nằm cách chân núi khoảng 100 m, khu dân cư có 4 nhà với tổng số 26 người. 9 người kịp chạy thoát ra ngoài. 17 người khác bị bùn đất cùng những cấu kiện trong nhà sập xuống vùi lấp.
-Clip Hiện trường vụ sạt lở ở Lào Cai
-Hiện trường sạt lở đất ở xã Mường Hoa, thị xã Sa Pa. Video: Tân Giang
-Chính quyền thị xã Sa Pa huy động 80 bộ đội, công an tìm kiếm nạn nhân. Đến 15h30, 6 thi thể được tìm thấy, trong đó có bà Vàng Thị Thảo 68 tuổi, Giàng Thị Chú 25 tuổi, cháu Châu Gia Hưng một tuổi và bé sơ sinh Vàng Văn Viên.9 người bị thương được đưa đi cấp cứu tại Bệnh viện Đa khoa thị xã Sa Pa, hiện sức khỏe đã ổn định. Chịu ảnh hưởng của hoàn lưu bão Yagi, lượng mưa từ 7h hôm qua qua đến 13h hôm nay ở Ô Quy Hồ, Hoàng Liên, Mường Hoa gần 150 mm.
-Một trong bốn ngôi nhà sàn bị sạt lở trưa 8/9. Ảnh: CTV
-Trước đó rạng sáng nay, đất đá từ vạt đồi trồng sắn cao hơn 10 m sạt xuống ngôi nhà ở xã Tân Minh, huyện Đà Bắc, tỉnh Hòa Bình, khiến 4 người tử vong.Hoàn lưu bão Yagi khiến miền Bắc mưa lớn hai ngày nay. Cơ quan khí tượng cảnh báo nguy cơ sạt lở đất ở 17/25 tỉnh, gồm: Lai Châu, Điện Biên, Sơn La, Hòa Bình, Lào Cai, Yên Bái, Hà Giang, Tuyên Quang, Vĩnh Phúc, Phú Thọ, Bắc Kạn, Thái Nguyên, Cao Bằng, Lạng Sơn, Quảng Ninh, Bắc Giang và TP Hải Phòng.Gia Chính</t>
+          <t>Hai tháng sau vụ ám sát hụt tại sự kiện tranh cử ở Bulter, bang Pennsylvania, cựu tổng thống Donald Trump ngày 15/9 đối mặt âm mưu ám sát tại câu lạc bộ golf ở West Palm Beach, bang Florida. Nghi phạm được xác định là người đàn ông 58 tuổi Ryan Wesley Routh.Routh là người ủng hộ nhiệt thành cho Ukraine, nhưng từng có nhiều hành động thất thường đến nỗi một số người Mỹ phải báo cáo hành vi của ông ta với giới chức.Routh đã tới Ukraine ngay sau khi Nga bắt đầu chiến dịch cuối tháng 2/2022 với hy vọng được tham chiến. Tại Kiev, Routh nhuộm tóc màu xanh và vàng như màu cờ của Ukraine và thường xuyên mặc áo phông có ba màu cờ Mỹ gồm đỏ, trắng và xanh dương. Routh dán áp phích khắp Kiev để kêu gọi người nước ngoài muốn hỗ trợ Ukraine nhắn tin cho ông ta.Chelsea Walsh, y tá ở West Palm Beach, nói cô đã nhắn tin tới số điện thoại trên áp phích khi mới đến Kiev, nghĩ rằng nó sẽ giúp cô kết nối với một tổ chức tình nguyện.Tuy nhiên, Routh đã yêu cầu cô gặp ông ta và những người khác tại quảng trường trung tâm ở Kiev vào ngày hôm sau để giương cờ các quốc gia và tuyên bố về sự hỗ trợ toàn cầu dành cho Ukaine. Walsh đã tới và giơ cao lá cờ của Ireland. Lúc đó, Walsh cảm thấy Routh lập dị nhưng không nguy hiểm.
+Ryan Wesley Routh tham gia cuộc biểu tình ở Kiev, Ukraine hồi tháng 4/2022. Ảnh: AP
+Quan điểm của cô về ông này thay đổi sau hàng chục cuộc gặp gỡ ở Kiev. Walsh kể ông ta đã nói về việc muốn ám sát Tổng thống Nga Putin và lãnh đạo Triều Tiên Kim Jong-un. Routh cũng đề cập tới cựu tổng thống Trump và Tổng thống Joe Biden, song Walsh không nhớ liệu ông ta có nói điều gì đe dọa về họ hay không.Những lời đe dọa bạo lực của Routh khiến Walsh lo lắng đến mức phải chia sẻ những lo ngại của mình với sĩ quan Cơ quan Hải quan và Biên phòng Mỹ (CBP) trong cuộc nói chuyện kéo dài một giờ ở sân bay Dulles, Washington, hồi tháng 6/2022.Walsh nói rằng Routh là một trong những người Mỹ nguy hiểm nhất mà cô gặp trong một tháng rưỡi ở Ukraine. Cô cũng cho sĩ quan CBP xem cuốn sổ liệt kê hơn chục cái tên người Mỹ và những người khác có hành động khiến cô hoảng sợ. Mục những người có đặc điểm chống đối xã hội gồm 4 cái tên, trong đó Routh đứng đầu danh sách.Khi nghe tin Routh cố chiêu mộ người tị nạn Syria đến chiến đấu ở Ukraine năm 2023, Walsh đã gửi cảnh báo trực tuyến cho FBI và Interpol, nêu rõ những lo ngại về Routh. Cả CBP và FBI đều không hồi đáp.Routh nổi lên trong các nhóm tình nguyện cứu trợ ở Ukraine như "kẻ lừa đảo" và "lập dị", theo Sarah Adams, cựu sĩ quan CIA từng giúp vận hành mạng lưới 50 nhóm cứu trợ để chia sẻ thông tin, điều phối hoạt động nhân đạo. Adams cho biết Routh từng tuyên bố đang làm việc với chính phủ Ukraine để tuyển mộ binh sĩ nước ngoài, nhưng điều này không đúng.Routh gửi tin nhắn tới các binh sĩ Afghanistan trên ứng dụng Signal và WhatsApp, giới thiệu mình là người Mỹ và đã giúp "quân đội Ukraine nhận thử một số lính Afghanistan".Routh cũng từng xuất hiện trong video đứng trước Đồi Capitol, bày tỏ thất vọng rằng Ukraine không tiếp nhận nhiều hơn những người lính Afghanistan mà ông ta chiêu mộ. Routh sau đó nói với Semafor năm 2023 rằng Ukraine lo sợ họ là "gián điệp".Tuy nhiên, Cục Điều phối người nước ngoài thuộc Bộ Tư lệnh Lục quân Ukraine cho biết Routh chưa từng phục vụ trong quân đội Ukraine hay hợp tác với họ. Oleksandr Shahuri, đại diện cục điều phối, cho hay Routh thường xuyên liên lạc với Quân đoàn Quốc tế Ukraine để đưa ra "những ý tưởng vô nghĩa và thậm chí là ảo tưởng".Cảnh giác với các tin nhắn kêu gọi của Routh, các nhóm cứu trợ khác đã cấm ông ta tham gia hoạt động của họ trên Signal. Họ cũng báo cáo hoạt động của Routh với Bộ Ngoại giao Mỹ, bày tỏ lo ngại rằng ông ta có thể dính dáng tới hành vi buôn người hoặc nhập cư trái phép, theo Adams."Hãy cẩn thận với Ryan Routh", Adams gửi tin nhắn cảnh báo các nhóm cứu trợ Ukraine hồi tháng 6/2023.Adams thêm rằng rất nhiều người đã cố gắng ngăn cản hoạt động của Routh hoặc ít nhất ngăn mọi người "rơi vào những trò lừa đảo" của ông ta.
+Mỹ công bố video bắt nghi phạm định ám sát ông Trump ở Florida
+Cảnh sát khống chế Ryan Routh. Video: Martin County Sheriff's Office
+Mặc dù giới chức Ukraine phủ nhận liên quan đến Routh, một người đàn ông Pháp tới Ukraine với ý định tham chiến cho biết Routh đã giúp anh ta được tuyển vào một đơn vị quân đội Ukraine. Anh kể rằng Routh đã bày tỏ phẫn nộ về ông Trump khi hai người gặp nhau tại một quán bia ở Kiev năm 2022."Ryan rất thất vọng về việc ông Trump cố gắng đàm phán thỏa thuận với ông Putin thay vì thực sự ủng hộ Ukraine", người đàn ông này nói.Vài năm gần đây, Routh có quan điểm ngày càng tệ về Trump. Trong cuốn sách tự xuất bản năm 2023 mang tên Cuộc chiến không thể thắng của Ukraine, Routh viết rằng "Iran có thể thoải mái ám sát ông Trump", mô tả cựu tổng thống là "kẻ ngốc" vì cuộc bạo loạn Đồi Capitol hồi tháng 1/2021 và "mắc sai lầm lớn" khi rút khỏi thỏa thuận hạt nhân với Iran.Routh nói ông từng bỏ phiếu bầu cho Trump và phải chịu trách nhiệm với "người mà chúng tôi đã bầu làm tổng thống tiếp theo, nhưng cuối cùng hóa ra chỉ là kẻ ngốc". Ông ta bày tỏ ủng hộ đối với Tổng thống Biden và Phó tổng thống Kamala Harris. "Đảng Dân chủ là lựa chọn của tôi và chúng tôi không thể thua", ông viết trên X hồi tháng 4.Vào tháng 7, sau vụ ông Trump bị ám sát hụt tại Pennsylvania, Routh viết trên mạng xã hội rằng ông Biden và bà Harris nên tới thăm những người bị thương trong vụ xả súng và tham dự đám tang của người lính cứu hỏa thiệt mạng. "Trump sẽ không bao giờ làm bất kỳ điều gì cho họ", Routh bình luận.Routh cũng viết trong sách của ông ta rằng thế giới sẽ tốt đẹp hơn nếu do phụ nữ lãnh đạo, bởi vì "dường như toàn bộ vấn đề của thế giới xoay quanh những người đàn ông bất ổn, với trí thông minh và hành vi như trẻ con".
+Vị trí của ông Trump và nơi nghi phạm bị phát hiện ở sân golf tại West Palm Beach, Florida ngày 15/9. Đồ họa: AP
+Sau khi bị bắt vì âm mưu ám sát ông Trump, Routh ngày 16/9 đã hầu tòa với hai tội danh "sở hữu súng dù là người từng bị kết án trọng tội" và "sở hữu khẩu súng bị xóa số seri". Nếu bị kết án cả hai tội, Routh sẽ đối mặt với mức án tù lên tới 20 năm. Giới chức có thể đưa ra thêm cáo buộc với Routh.Dù nhiều người từng bày tỏ lo ngại về Routh, vẫn có người nói tốt về ông này. Hàng xóm Christopher Tam mô tả Routh rất kín tiếng, tôn trọng người khác, thân thiện và tử tế."Những điều anh ta bị cáo buộc thực sự rất đáng ngạc nhiên. Chúng tôi thực sự bị sốc", Tam nói.Thùy Lâm (Theo AP, WSJ, CBS News)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cổ thụ, có nên trồng trên phố?</t>
+          <t>Ngộ nhận 'Tây là tốt'</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/co-thu-co-nen-trong-tren-pho-4790457.html</t>
+          <t>https://vnexpress.net/ngo-nhan-tay-la-tot-4793739.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nên thay thế dần cổ thụ bằng những loài cây nhỏ, tán rộng, có khả năng chịu gió bão tốt hơn.</t>
+          <t>Giáo dục các nước phương Tây cũng đối mặt với những vấn đề mà giáo dục Việt Nam gặp phải.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nhiều người dân Thủ đô sáng nay tan bão, đã dong xe làm một vòng để trở về với nỗi xót xa cho những cái cây vốn đã trở thành một phần linh hồn của đô thị Hà Nội.Cây đổ cũng là một trong những nguyên nhân gây thiệt mạng cho 14 người trong cơn siêu bão vừa qua.Nhưng không chờ đến bão, thỉnh thoảng, nhánh cây già ở đâu đó vẫn thình lình rơi, cướp đi mạng sống của con người. Gần đây nhất, một phụ nữ tử vong khi đang đi trên đường An Dương Vương, quận 5, TP HCM vì nhánh cây đổ vào người.Những thiệt hại nặng nề này khiến một câu hỏi cũ lại được đặt ra: có nên giữ lại cây cổ thụ ven đường hay mạnh dạn thay thế bằng cây nhỏ hơn, phù hợp hơn.Về lâu dài, cổ thụ trên vỉa hè nên được xem xét thay thế bằng cây thấp hơn với tán phủ tốt hơn để đảm bảo an toàn. Các lý do chính bao gồm:Việc trồng cổ thụ cao hàng chục mét trên vỉa hè rất ít gặp ở nhiều quốc gia. Các nước đã thực hiện chương trình thay thế luân phiên cây lớn để đảm bảo an toàn. Cây quá cao thường không che bóng hiệu quả, vì phần lớn thời gian trong ngày, bóng cây sẽ đổ vào nhà dân hơn là lòng đường.Cây cổ thụ với bộ rễ lớn dọc vỉa hè có thể gây hư hại hạ tầng kỹ thuật, bong tróc nền đường và tốn kém chi phí chăm sóc, bảo trì hơn nhiều so với cây nhỏ.Các giống cây lớn nên được trồng và bảo vệ ở công viên, vườn bách thảo hoặc khu vực ít người qua lại để giảm nguy cơ rủi ro từ cành cây gãy. Cây trồng dọc vỉa hè nên là các cây có chiều cao trung bình thấp, thân cành dẻo dai và có tán lá rộng để tạo bóng tâm tốt.Chặt và thay thế cây cổ thụ luôn là vấn đề gây tranh cãi, thậm chí là nhạy cảm ở nhiều quốc gia. Nhưng việc đảm bảo an toàn cho cộng đồng phải được đặt lên hàng đầu. Ở Singapore, cơ quan quản lý cây xanh NPARKS kiểm tra định kỳ những cây đạt kích thước hoặc tuổi nhất định để quyết định giữ lại hay đốn hạ. Việc chặt tỉa và trồng mới được thực hiện luân phiên theo hình thức cuốn chiếu, tức là, cây tới tuổi được đốn bỏ luân phiên và trồng thay cây con mới, để duy trì cảnh quan và bóng mát. Những cây cao trên 20 m chỉ được trồng ở công viên, ngoại ô hoặc ven đô, nơi có không gian đủ lớn để bộ rễ phát triển.
-Cây cổ thụ trên vỉa hè được kiểm tra, cắt tỉa hoặc đốn bỏ. Phần gốc được băm thành mảnh nhỏ (A) và mùn cưa dùng để phủ lên cây non kế bên (B). Cây xanh vỉa hè được trồng luân phiên (C) để duy trì sự xanh mát của trục đường mà không chặt bỏ toàn bộ cùng lúc.
-Ngoài kế hoạch dài hạn là thay thế cổ thụ, một vấn đề khác luôn phải quan tâm định kỳ là làm thế nào để bảo vệ cây xanh đô thị, duy trì cảnh quan và đảm bảo an toàn cho người dân trong mùa mưa bão?Cây xanh đô thị phải chịu nhiều áp lực hơn so với cây cối trong tự nhiên, thường xuyên chịu tác động từ nhiệt độ cao, biến đổi độ ẩm và ô nhiễm không khí. Đất ở khu vực đô thị thường thiếu dinh dưỡng, trong khi các hoạt động xây dựng và giao thông có thể gây hư hại đến rễ, thân, và cành cây, đồng thời hạn chế không gian sinh trưởng. Lưu lượng giao thông cao cũng làm gia tăng nguy cơ du nhập các bệnh cây ngoại lai. Do đó, việc trồng và chăm sóc cây xanh đô thị cần được chú trọng đặc biệt với những biện pháp bảo trì và thay thế kịp thời.Để giảm nguy cơ gãy đổ trong những mùa mưa bão sắp tới, cần rất nhiều biện pháp cùng lúc:Kiểm tra định kỳ: Các chuyên gia cây xanh cần thường xuyên kiểm tra để phát hiện sớm dấu hiệu suy yếu như rễ nổi, thân cây mục nát, cành khô hoặc bị bệnh. Những công nghệ đánh giá hiện đại như VTA, đo điện trở hoặc siêu âm có thể xác định chính xác tình trạng cây.Tỉa cành đúng cách: Tỉa cành giúp loại bỏ cành khô yếu, giảm sức cản gió và tăng độ ổn định. Phương pháp tỉa thưa tán và giảm chiều cao tán có tác dụng giảm tải trọng gió, ngăn ngừa gãy đổ.Cải thiện cấu trúc rễ: Đảm bảo rễ cây không bị tổn thương và có đủ không gian phát triển bằng cách giữ đất thoáng khí, bổ sung dinh dưỡng định kỳ để rễ khỏe mạnh.Hỗ trợ cây trưởng thành: Những cây có giá trị bảo tồn nhưng đã suy yếu cần hỗ trợ thêm bằng cáp, dây chằng, hoặc các hệ thống chống đỡ để tăng khả năng chịu gió bão.Bảo vệ khỏi các yếu tố gây hại: Chăm sóc hợp lý như bón phân, tưới nước và bảo vệ khỏi sâu bệnh sẽ giúp cây phát triển khỏe mạnh và tăng khả năng chống chịu thời tiết.Nỗi xót thương khiến nhiều người đang kêu gọi trồng lại 17.000 cây vừa bị bão Yagi quật ngã. Nhưng việc trồng lại trong phần lớn trường hợp là bất khả thi. Sự mất mát này là cơ hội để thay thế giống cây phù hợp hơn. Đô thị nên ưu tiên những cây có rễ vững chắc và khả năng chịu gió bão tốt, tránh các loài cây gỗ giòn, dễ gãy.Theo nghiên cứu của tôi, hai loại cây rất phù hợp để trồng trên vỉa hè ở Việt Nam là cây Còng (Samanea Saman) và cây Trai Lý (Fagraea fragrans). Cây Còng có tán rộng hình chiếc ô từ 20-30 m, phát triển tốt trong khí hậu nhiệt đới, ít cần chăm sóc và hoa ít mùi. Cây Trai Lý cao từ 10-25 m, phát triển mạnh mẽ trong môi trường đô thị, không đòi hỏi nhiều công chăm sóc và tạo cảnh quan xanh mát cho các tuyến đường.Việc cân bằng giữa an toàn tính mạng con người và cảnh quan, sinh thái, tạo bóng râm cần có sự tính toán và cân đối phù hợp để mang lại lợi ích cho cộng đồng. Đặc biệt yếu tố an toàn phải được đặt lên hàng đầu, nhất là khi hiện tượng thời tiết cực đoan sẽ còn xuất hiện với tần suất càng phổ biến.Trình Phương Quân</t>
+          <t>Tuy nhiên, khi di cư tới một nước phương Tây, chị lại cho rằng giáo dục phương Tây rất kém. Học sinh không biết làm toán, không thể đọc hiểu... Vì vậy, phương Tây đang phải thu hút nhân tài từ các nước đang phát triển như Việt Nam để lấp chỗ trống này. Thực tế, đây cũng là những luồng ý kiến thường được bàn luận khi nói về giáo dục.Theo tôi cả hai trường phái đều là cực đoan và ngộ nhận. Những nền giáo dục tiên tiến của phương Tây không hoàn hảo, nhưng cũng không hề kém.Bắt đầu từ năm 2000, Tổ chức Hợp tác và Phát triển Kinh tế OECD (Organisation for Economic Co-operation and Development) thực hiện Chương trình Đánh giá học sinh quốc tế (Programme for International Student Assessment - PISA) để đo lường khả năng của học sinh 15 tuổi ở các nước và vùng lãnh thổ trong và ngoài OECD, về toán, khoa học và đọc hiểu.Kết quả PISA 2022 cho thấy những nước bị xem là lười học toán như Australia (487 điểm), Canada (497) có khoảng cách nhất định với Trung Quốc (552), Nhật Bản (536) nhưng lại tốt hơn nước chăm học toán là Việt Nam (469). Kết quả đọc hiểu cũng tương tự.Việc bạn tôi cảm thấy Tây dốt toán là do hai hiệu ứng. Thứ nhất, chị đang lấy bản thân (là học sinh ưu tú của Việt Nam) để so sánh với môi trường xung quanh (có thể không phải môi trường ưu tú của nước bạn). Thứ hai là con người thường có xu hướng quy chụp suy rộng. Giống như việc tôi từng gặp một số người Australia cho rằng không nói được tiếng Anh thành thạo là có học thức thấp.Còn chuyện các nước thu hút nhân tài là một chính sách khôn ngoan, không có nghĩa nền giáo dục của họ không có khả năng đào tạo nhân tài. Nếu nhìn vào danh sách người đoạt các giải thưởng danh giá như Nobel, Fields... chúng ta có thể bắt gặp một số người gốc Á, và nhiều người trong số này cũng được đào tạo từ nhỏ ở phương Tây.Nói như vậy, nhưng giáo dục phương Tây cũng có ưu khuyết riêng. Nhìn về tổng thể, các nền giáo dục này chưa chắc đã hiệu quả hơn Việt Nam, nếu tính tới nguồn lực khổng lồ mà các nước tiên tiến đầu tư vào. Năm 2022, Australia chi 88,4 tỷ USD cho bốn triệu học sinh, trong khi Việt Nam chỉ đầu tư 12 tỷ USD cho 18 triệu học sinh. Tất nhiên, mọi so sánh đều là khập khiễng. Tuy nhiên, người làm giáo dục ở các nước tiên tiến vẫn hiểu rằng họ còn ở rất xa mức hoàn thiện và có những vấn đề cần đối mặt. Ví dụ, kết quả PISA của Australia trong hơn 20 năm qua thực tế là đi xuống đáng kể, chứ không đi lên.Giáo dục các nước phương Tây thậm chí cũng phải đối mặt với những vấn đề mà giáo dục Việt Nam gặp phải. Ví dụ, Australia cũng có tình trạng thiếu giáo viên, và đầu vào ngành sư phạm quá thấp. Các nhà giáo từng cảnh báo việc này sẽ kéo chất lượng giảng dạy đi xuống, vì giáo viên ngoài truyền đạt kiến thức, còn cần truyền đạt niềm đam mê với kiến thức cho các em. Năm 2019, trong chiến dịch tranh cử thủ tướng Australia, ứng viên lưỡng đảng đều khẳng định giáo dục Australia có sự thiếu công bằng và còn xa mới đạt tới nền giáo dục tốt nhất thế giới.Thế nhưng nền giáo dục tốt nhất thế giới được nhiều học giả tán dương và diễn đàn kinh tế công nhận vào năm 2018 là Phần Lan cũng không công bằng. Dựa trên kết quả tốt nghiệp trung học của hơn 400 trường trung học, tôi thấy phổ điểm của Phần Lan bình thường như bao nước khác, kể cả Việt Nam. Trường tốt nhất có điểm trung bình tốt nghiệp gần gấp đôi trường kém nhất (5,98/7 so với 3,13/7).
+Nếu ở Việt Nam có phụ huynh đạp hàng rào cổng trường để cho con học trường điểm, thì ở Phần Lan cũng có một số phụ huynh chuyển hoặc thuê nhà để con được vào học trường tốt; mặc kệ chính phủ và nhiều nhà quản lý giáo dục đều cố gắng thuyết phục mọi người rằng không có sự khác biệt nào giữa các trường, trường tốt nhất là trường gần nhà nhất...Vậy nên, khi học hỏi nền giáo dục tiên tiến, cần một sự tỉnh táo nhất định. Nếu không học hỏi thì không tiến bộ. Mà nếu học, thì cần biết cách chọn lọc phù hợp, hơn là kêu gọi sao chép mù quáng chỉ vì điều đó có ở phương Tây. Tôi cho rằng cả hai ngộ nhận trên đều nên được loại bỏ khỏi tâm thế khi chúng ta cắp sách đi học những nền giáo dục tiên tiến.Thế mạnh lớn nhất của Việt Nam là hiếu học. Từ ngàn đời nay, người Việt Nam thức khuya dậy sớm học tập để có tri thức, có sức mạnh, có khả năng làm chủ cuộc sống của mình. Điều chúng ta còn chưa có đầy đủ là một nền giáo dục thực dụng hiệu quả cao, giúp người học tiết kiệm thời gian và có năng lực tốt.Tô Thức</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Người dân sốc vì phố phường tan hoang sau bão Yagi</t>
+          <t>27 cơ thủ Việt Nam bị cấm một năm</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-dan-soc-vi-pho-phuong-tan-hoang-sau-bao-yagi-4790424.html</t>
+          <t>https://vnexpress.net/27-co-thu-viet-nam-bi-cam-mot-nam-4793840.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hà Nội8 tiếng kể từ khi hai cây phượng và xà cừ cổ thụ liên tiếp đổ xuống, đè vào chiếc ôtô đỗ trước cửa nhà, anh Lê Tú, 55 tuổi, vẫn chưa hết bàng hoàng.</t>
+          <t>Các cơ thủ dự giải carom 3 băng PBA Hanoi Open 2024 hồi cuối tháng 8 đều bị Liên đoàn Billiards Carom Thế giới (UMB) cấm thi đấu trong một năm.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17h30 ngày 7/9, nam tài xế taxi về nhà ở phố Quán Sứ, quận Hoàn Kiếm, sau cuốc xe cuối cùng. Anh đỗ chiếc ôtô sát cửa, cách hai cây cổ thụ trồng trên vỉa hè chừng một mét vì nghĩ cây to, rễ lớn không thể đổ.30 phút sau, một tiếng rắc lớn xé ngang tai, anh Tú thấy cành cây phượng rơi thẳng xuống khiến kính lái của ôtô vỡ vụn. Gia đình khuyên di chuyển xe ra chỗ khác nhưng thấy ngoài trời gió lớn, anh chần chừ. Đúng lúc đó, tiếng uỳnh thứ hai dội đến. Cây xà cừ cổ thụ hơn 40 năm tuổi, thân bằng hai người ôm, bật gốc đè lên khiến chiếc xe bẹp rúm.Không chỉ hai cây cổ thụ trước cửa nhà, hàng chục cây khác trên cùng phố Quán Sứ (quận Hoàn Kiếm) cũng đổ rạp, nhẹ thì gãy cành, nặng thì gãy đôi hoặc bật gốc. "Cảnh tượng hoang tàn như sau một trận bom, lần đầu tôi chứng kiến", anh Tú nói.Đến 12h ngày 8/9, phố Quán Sứ vẫn ngổn ngang cây xanh đổ gãy, nhiều cây nằm ngang đường chưa được dọn dẹp. Người dân phải đi lên vỉa hè.
-Anh Lê Tú, 55 tuổi, đứng bất lực bên cạnh chiếc ôtô của gia đình bị cây đè ngang, bẹp rúm, trưa 8/9. Ảnh: Thanh Nga
-Cách nhà anh Tú chừng một km, tại phố Hàng Trống, quận Hoàn Kiếm, bà Nguyễn Nghĩa, 64 tuổi, cùng người thân đang làm lại đường ống sau khi cây me gần 100 năm tuổi trồng trước cửa nhà bật gốc. "Cái thân cây phải ba người ôm nhưng nay chẳng còn. Khắp nơi đổ nát như thời chiến tranh", bà Nghĩa kể.Cây me đổ khoảng 12h trưa 7/9. Sau tiếng gió rít, họ nghe thấy tiếng đổ ầm, một số nhà cảm nhận được độ rung. Khi chạy ra ngoài mới biết cây đổ ngang đường, nhưng giữa trời giông lốc không thể làm gì, họ đành lui vào trong nhà trú ẩn.
-Một người dân trên phố Hàng Trống sửa lại đường ống nước sau khi cây me trước cửa nhà bật gốc, trưa 8/9. Ảnh: Quỳnh Nguyễn
-6h sáng nay, anh Trần Đức Anh, 42 tuổi, mở cửa nhà tại khu đô thị cách trung tâm Hà Nội hơn 10 km, đập vào mắt là cảnh tượng ''tưởng chỉ có trong phim''. Cây cối hai bên đường đổ rạp. Những cây cổ thụ to từng là nơi ngồi hóng mát, tập thể dục của cư dân đều bị bão quật tan tác.''Hơn 40 năm sống ở Hà Nội, tôi chưa từng thấy cảnh tượng nào như vậy'', anh nói. ''Quá đau lòng khi bao nhiêu cây xanh thân thuộc gục ngã trên đường''.Trưa 8/9, hầu hết tuyến đường tại các quận Hoàn Kiếm, Hai Bà Trưng, Long Biên, Ba Đình, Đống Đa, Cầu Giấy, Nam Từ Liêm, Bắc Từ Liêm cây xanh bị đổ rạp sau bão vẫn đang ngổn ngang. Chủ tịch UBND TP Hà Nội cho biết có khoảng 17.000 cây gãy đổ trên địa bàn.Hà Nội hiện có khoảng 1,8 triệu cây xanh đô thị, chủ yếu là xà cừ, sấu, phượng, muồng, bằng lăng, giáng hương, bàng. Giai đoạn 2016-2020, khoảng 1,6 triệu cây được trồng mới. Hiện trên địa bàn 12 quận nội thành có khoảng 8.000 cây cổ thụ. Các cây này có độ tuổi tối thiểu 50 năm hoặc cây có đường kính từ 50cm trở lên.Nhà nghiên cứu văn hóa, PGS.TS Phạm Ngọc Trung, nguyên trưởng khoa Văn hóa và Phát triển, Học viện Báo chí và Tuyên truyền cho rằng những hàng cây xanh không chỉ che nắng, che mưa cho người dân khi ra đường mà còn tạo cảnh quan, làm đẹp cho thành phố.Trong khi đó, những gốc cây lâu năm còn là một phần ký ức của người Hà Nội, gắn với ký ức của nhiều người. Cây ở các con đường như Hoàng Diệu, Phan Đình Phùng còn mang dấu ấn lịch sử, là hơi thở của thời đại.''Vì lý do cơn bão gây gãy đổ hàng nghìn cây xanh lâu năm, người Hà Nội không khỏi sốc và xót xa'', ông Trung nói.
-Cây đổ gãy trên phố Trích Sài lúc 2h sáng 8/9. Ảnh: Trần Duy Tiệp
-Biết Hà Nội sẽ gánh chịu thiệt hại nặng vì bão nên ngay từ đêm qua, khi gió ngớt đã có một số người dân tình nguyện tham gia dọn dẹp, giải phóng đường.Anh Trần Duy Tiệp, một nhiếp ảnh gia tự do ở Sóc Sơn, đã lên mạng xã hội kêu gọi mọi người cùng hỗ trợ lực lượng chức năng dọn dẹp đường phố, lúc gần 2h sáng. ''Tôi ở nhà cũng không ngủ được nên quyết định làm gì đó có ý nghĩa'', chàng trai Gen Z, nói. Xuất phát từ nhà lúc 1h45 đến 2h30 anh mới có mặt ở phố Thụy Khuê.''Tôi run lên vì không ngờ cảnh hoang tàn, đổ nát đến vậy. Chỉ cần lơ là một giây thôi là có thể tông vào cây đổ'', Tiệp nói.Sau khi tập hợp được gần 10 người, nhóm của Tiệp theo chân cán bộ phường và cảnh sát giao thông dọn dẹp một số khu vực trên đường Nguyễn Đình Thi, Trích Sài (quận Tây Hồ). Đi đến đâu nhóm cũng thấy cây gãy đổ, biển quảng cáo của nhà hàng, doanh nghiệp, cột đèn rơi la liệt bên vệ đường. Có những cây xanh gần chục người mất đến 30 phút mới có thể dọn dẹp xong.Từ sáng sớm nay, Đức Anh lên mạng xã hội kêu gọi cư dân chung tay vì biết với sức có hạn của lực lượng chức năng, nhân viên vệ sinh, không biết khi nào đường phố mới quang đãng trở lại.Một ngày sau cây đổ, bà Nghĩa ở phố Hàng Trống cũng cùng một số hộ dân trên phố đang cùng nhau cắt cành để giải phóng đường. Theo bà, đường ống vỡ thì có thể sửa lại, nhưng cây đổ rồi bà sợ không còn cơ hội trồng cho cây thành cổ thụ như vậy nữa.''Dân trong phố tôi ai cũng xót xa", bà nói.
-Người dân Hà Nội: 'Xót xa khi nghe gió bão rít, cây đổ rầm rầm'
-Video: Lộc Chung - Văn Ngọc - Bá Nam
-Phạm Thanh Nga - Quỳnh Nguyễn</t>
+          <t>Lệnh cấm của UMB đã được Liên đoàn Billiards &amp; Snooker Việt Nam (VBSF) thông báo tới Sở Văn hóa, Thể thao và Du lịch các tỉnh, thành phố cùng các liên đoàn địa phương, có VĐV liên quan. Theo đó, 128 cơ thủ nam và 64 cơ thủ nữ vừa dự giải này sẽ bị cấm thi đấu một năm trên các giải thuộc UMB và quốc gia của cơ thủ đó, từ ngày 27/8/2024 đến ngày 27/8/2025.Hanoi Open 2024 tổ chức từ ngày 19/8 đến 26/8 tại Hà Nội. Giải đấu thuộc hệ thống của Hiệp hội Billiards Chuyên nghiệp (PBA) – là tổ chức đối trọng và không được UMB công nhận.
+Cơ thủ carom 3 băng Nguyễn Quốc Nguyện. Ảnh: PBA
+Việt Nam không có cơ thủ nữ, nhưng có 32 cơ thủ nam tham dự Hanoi Open 2024. Trong đó, năm cơ thủ nổi tiếng đã bị UMB cấm từ trước, do chuyển hẳn sang chơi cho PBA, gồm Nguyễn Quốc Nguyện, Ngô Đình Nại, Mã Minh Cẩm, Nguyễn Huỳnh Phương Linh và Nguyễn Đức Anh Chiến.27 cơ thủ còn lại gồm Huỳnh Phi Long, Trương Văn Đức, Tô Minh Thiện, Trương Thái Duy, Huỳnh Thanh Hiền, Đỗ Đức Hiền, Huỳnh Đức, Huỳnh Lê Trương Hưng, Trần Quốc Vinh, Nguyễn Công Thành, Ngô Văn Đức, Cao Ngọc Bảo Kha, Nguyễn Đình Núi, Trần Đình Phương Vũ, Ken Vĩnh, Nguyễn Mạnh Phát, Trần Tiến Phong, Đặng Mai Phú, Trương Bé Năm, Nguyễn Ngọc Trị, Lâm Hán Thành, Nguyễn Văn Phước Hiếu, Nguyễn Văn Long, Huỳnh Tấn Mỹ, Nguyễn Quốc Thắng, Nguyễn Vũ Quang Trường, Trần Văn Ngân.15 trong 27 tay cơ kể trên đã có mã định danh trên bảng thứ bậc UMB. Một số tay cơ đã để lại tên tuổi trong làng carom 3 băng Việt Nam, như Ngọc Trị, Trần Văn Ngân, Đỗ Đức Hiền, Đình Núi. Những VĐV này giành quyền tham dự Hanoi Open 2024 sau khi thi đấu vòng loại tại TP HCM.Ngoài Việt Nam, VĐV dự Hanoi Open 2024 phần lớn đến từ Hàn Quốc, một số đến từ Nhật Bản, Tây Ban Nha, Bỉ, Thổ Nhĩ Kỳ.
+Cơ thủ carom 3 băng Trần Văn Ngân.
+Trao đổi với VnExpress, Nguyễn Quốc Nguyện thấu hiểu luật cấm của UMB, vì chỉ khi các thành viên tuân thủ quy định thì hiệp hội mới có thể duy trì và phát triển. Nhưng cơ thủ 42 tuổi người Gia Lai cũng mong rằng các cơ quan quản lý như PBA hay UMB tìm tiếng nói chung để xóa bỏ lệnh cấm hoặc giảm bớt mức độ, giúp VĐV được dự nhiều giải, qua đó làm môn thể thao phát triển hơn nữa.Lệnh cấm của UMB cũng không ảnh hưởng đến giải carom 3 băng vô địch thế giới 2024 sẽ tổ chức tại Bình Thuận, từ ngày 25/9 đến 29/9, khi không có tay cơ nào trong danh sách cấm tham dự. Tuy nhiên, giải này vẫn sẽ quy tụ những cơ thủ 3 băng hàng đầu Việt Nam khác như Bao Phương Vinh, Trần Quyết Chiến, Trần Đức Minh.PBA thành lập từ năm 2019 tại Hàn Quốc, và tạo nên hệ thống PBA Tour thi đấu carom 3 băng. Hanoi Open 2024 là lần đầu tiên PBA Tour tổ chức ở nước ngoài.PBA không cấm các VĐV đã ký hợp đồng tham dự các giải của UMB, nhưng UMB thì ngược lại. Các VĐV Việt Nam đến Hanoi Open đều biết có thể nhận án cấm từ UMB, nhưng vẫn tham gia. Họ sẽ không được dự các giải của UMB, hoặc đơn vị trực thuộc như VBSF, Liên đoàn Billiards châu Á (ACBS) tổ chức.Sức hấp dẫn của PBA đến từ thể thức thi đấu đánh theo set và tạo nhiều cơ hội cho VĐV nữ, VĐV trẻ dưới 18 tuổi tham dự. Tiền thưởng vô địch nam một chặng PBA Tour là khoảng 75.000 USD, cao hơn ba lần so với một chặng UMB World Cup. Trên các diễn đàn billiards, người hâm mộ Việt Nam cho rằng việc tiếp cận xem PBA Tour dễ hơn UMB.Trước đó, ngày 30/7, VBSF cho biết các thành viên bị cấm tham dự các giải của ACBS, Liên đoàn Pool Thế giới (WPA) và Liên đoàn Billiards &amp; Snooker Quốc tế (ISBF) trong sáu tháng, từ 13/7/2024 đến 12/1/2025. Lý do được đưa ra là Việt Nam đã tổ chức giải pool Hanoi Open vào tháng 10/2023. Giải đấu không được ACBS, WPA cấp phép, do thuộc hệ thống World Nineball Tour (WNT) của Matchroom Pool – một tổ chức đối lập với WPA.Lệnh cấm của ACBS, WPA và ISBF dẫn đến cuộc tranh luận lớn trong giới billiards Việt Nam lẫn thế giới. Nhiều cơ thủ pool nổi tiếng như Shane Van Boening, Jyson Shaw, Francisco Sanchez... đòi dỡ lệnh cấm và có thể tẩy chay không tham dự các giải của WPA. Điều này khiến WPA phải lên tiếng trấn an, cho biết sẽ có cuộc gặp gỡ trực tuyến để lắng nghe nguyện vọng của các cơ thủ. Matchroom và PBA thất vọng, cho rằng ACBS vượt quyền và kìm hãm sự phát triển của billiards Việt Nam.Hiếu Lương</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hai sĩ quan hy sinh khi phòng chống bão Yagi</t>
+          <t>Phu nhân đại tướng Võ Nguyên Giáp qua đời</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hai-si-quan-hy-sinh-khi-phong-chong-bao-yagi-4790487.html</t>
+          <t>https://vnexpress.net/phu-nhan-dai-tuong-vo-nguyen-giap-qua-doi-4793935.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Thượng úy quân đội Nguyễn Đình Khiêm và thiếu tá công an Trần Quốc Hoàng hy sinh khi làm nhiệm vụ phòng chống bão Yagi ở tâm bão Quảng Ninh.</t>
+          <t>Bà Đặng Bích Hà, phu nhân cố đại tướng Võ Nguyên Giáp, qua đời rạng sáng ngày 17/9, hưởng thọ 96 tuổi.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Thượng úy Nguyễn Đình Khiêm, 27 tuổi, là Đại đội trưởng Đại đội 3, Lữ đoàn 513, Quân khu 3. Anh nhập ngũ tháng 9/2015, quê xã Yên Mỹ, huyện Yên Mô, tỉnh Ninh Bình. Trong quá trình phòng chống bão Yagi, đơn vị anh phụ trách đảm bảo an toàn các đơn vị công trình.
-Thượng úy Nguyễn Đình Khiêm.
-Ngày 6/9, Lữ đoàn phát hiện hệ thống lán trại tại công trình thuộc thôn Pạt, xã Lục Hồn, huyện Bình Liêu có nguy cơ mất an toàn trước gió bão. Thượng úy Khiêm được giao chỉ huy lực lượng chuẩn bị vật chất ứng cứu với địa phương và chằng chống lán trại.Trên đường về sau khi lấy vật liệu, thấy đồng đội trượt chân, có thể bị cây đè lên người gây nguy hiểm, thượng úy Khiêm lao vào đỡ và bị ngã. Được đồng đội đưa đi cấp cứu, nhưng anh không qua khỏi.Cũng trong cơn bão Yagi, thiếu tá Trần Quốc Hoàng, 37 tuổi, quê thị xã Mỹ Hào, Hưng Yên, đã hy sinh. Anh Hoàng là cán bộ trại giam Quảng Ninh, thuộc Cục Cảnh sát quản lý trại giam.
-Thiếu tá Trần Quốc Hoàng.
-Rạng sáng 7/9, trong cơn mưa bão, nước lũ dâng cao, có thể nguy hiểm đến tính mạng của phạm nhân tại Phân trại số 2, anh Hoàng đã lao ra cứu người và bị nước lũ cuốn trôi.Trại giam Quảng Ninh cùng với lực lượng cứu nạn cứu hộ đã tìm kiếm trong mưa bão. Đến sáng nay, thi thể của thiếu tá Hoàng được tìm thấy tại bờ suối thôn Đồng Vải, xã Thống Nhất, TP Hạ Long, cách đơn vị khoảng một km.Bão Yagi với sức gió cấp 12-13 đổ bộ vào Quảng Ninh trưa 7/9. Hoàn lưu trước, trong và sau bão gây mưa to, gió mạnh ở khắp miền Bắc. Thống kê của Cục Quản lý đê điều và Phòng chống thiên tai, đến chiều nay bão Yagi và các hiệu ứng liên quan làm 21 người chết, trong đó 9 người do bão, 12 chết do sạt lở đất và một người lũ cuốn, một người mất tích ở Bắc Giang.229 người bị thương, hơn 8.000 ngôi nhà hư hỏng, chìm 25 tàu thuyền. Gần 110.000 ha lúa, gần 18.000 ha hoa màu, gần 7.000 ha cây ăn quả bị ngập úng, hư hại. Hơn 1.100 lồng bè bị cuốn trôi, chủ yếu ở Quảng Ninh.
-Sơn Hà</t>
+          <t>Bà Đặng Bích Hà sinh năm 1928 tại Nghệ An, là con gái của Giáo sư Đặng Thai Mai, nguyên Bộ trưởng Giáo dục, Viện trưởng Viện Văn học Việt Nam. Bà gắn bó với đại tướng Võ Nguyên Giáp từ những năm thiếu thời, khi ông sống tại nhà giáo sư Đặng Thai Mai trong 10 năm, từ 1931 đến 1941.Năm 1943, bà Bích Hà theo trường tản cư về Thanh Hóa, hai năm sau mới quay về Hà Nội. Bà từng kể khi 6-7 tuổi, thường được ông Giáp chở đến sân vận động Hàng Đẫy (khi đó gọi là Septo) tập thể thao. Năm 1945, hai người gặp lại nhau. Lúc này, đại tướng đang chịu nỗi đau mất vợ, khi bà Nguyễn Thị Quang Thái bị bắt và mất trong nhà tù Hỏa Lò đầu năm 1944.Cuối năm 1946, lễ cưới giản dị giữa đại tướng Võ Nguyên Giáp và bà Đặng Bích Hà được tổ chức. Hai người gắn bó với nhau đến khi đại tướng Võ Nguyên Giáp qua đời năm 2013.Dù bận rộn với công việc, đại tướng Võ Nguyên Giáp luôn dành những khoảnh khắc đặc biệt cho gia đình. Mỗi dịp kỷ niệm ngày cưới 27/11, ông đều nhờ con gái mua một bó hoa tặng bà Đặng Bích Hà. Những năm cuối đời, sức khỏe tướng Giáp ngày càng yếu, hầu hết thời gian nằm trong bệnh viện. Bà Hà luôn chăm sóc, đồng hành, chuyện trò cùng ông.
+Đại tướng Võ Nguyên Giáp và phu nhân Đặng Bích Hà. Ảnh: Trần Hồng 
+Sinh năm 1911 tại Lệ Thủy, Quảng Bình, đại tướng Võ Nguyên Giáp từ một thầy giáo dạy sử đã trở thành nhà quân sự tài ba. Là đại tướng đầu tiên và Tổng Tư lệnh tối cao của Quân đội nhân dân Việt Nam, ông đã có những đóng góp to lớn vào sự nghiệp giải phóng dân tộc.Trong kháng chiến chống Pháp và chống Mỹ, đại tướng trực tiếp chỉ huy nhiều chiến dịch lớn. Tên tuổi của ông gắn liền với chiến thắng trong Chiến dịch Điện Biên Phủ (1954) và Hồ Chí Minh (1975) - những bước ngoặt trong lịch sử dân tộc.Sau khi đất nước thống nhất, ông làm Phó thủ tướng kiêm Bộ trưởng Quốc phòng (đến 1980); Phó chủ tịch Hội đồng Bộ trưởng (1981-1991). Ông cũng là đại biểu Quốc hội các khóa 1-7.Đại tướng Võ Nguyên Giáp kết hôn lần đầu năm 1934 với nhà cách mạng Nguyễn Thị Quang Thái. Hai người có một người con là bà Võ Hồng Anh (1941-2009).Ông tái hôn với giáo sư Đặng Bích Hà năm 1946, sau khi bà Thái hy sinh. Ông bà có 4 người con là Võ Hòa Bình, Võ Hạnh Phúc, Võ Điện Biên và Võ Hồng Nam.
+Viết Tuân</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Nhiều bệnh viện Quảng Ninh thiệt hại nặng, cạn điện nước sau bão Yagi</t>
+          <t>Meta cấm các hãng truyền thông nhà nước Nga</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhieu-benh-vien-quang-ninh-thiet-hai-nang-can-dien-nuoc-sau-bao-yagi-4790425.html</t>
+          <t>https://vnexpress.net/meta-cam-cac-hang-truyen-thong-nha-nuoc-nga-4793974.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tất cả bệnh viện, trung tâm y tế tại Quảng Ninh đều bị thiệt hại sau bão Yagi, tốc mái, vỡ kính, hỏng nhiều thiết bị, ảnh hưởng hoạt động khám chữa bệnh.</t>
+          <t>Meta, công ty mẹ của Facebook và Instagram, cho biết sẽ cấm các hãng truyền thông Rossiya Segodnya và RT của Nga do liên quan "hoạt động can thiệp của nước ngoài".</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Chiều 8/9, đại diện Sở Y tế Quảng Ninh cho biết thông tin trên, thêm rằng toàn bộ đơn vị khám bệnh chữa bệnh đều bị thiệt hại nặng nề, nguồn dự trữ năng lượng điện từ máy phát điện dần cạn kiệt. Nguồn nước từ bể dự trữ chỉ duy trì được 12-24 giờ nữa, tùy đơn vị. Trong đó, Bệnh viện Sản Nhi và Bệnh viện Lão khoa - Phục hồi chức năng thiệt hại nặng nề nhất.Tại Bệnh viện Sản nhi Quảng Ninh, đến chiều nay cây cối đổ dài chắn lối đi, nhiều khoa, phòng trống hoác do bị gió lốc thổi bay mái tôn, hỏng nhiều thiết bị quan trọng. Mái tôn Khoa Hồi sức tích cực bị thổi bay. Kính cửa sổ khu vực xét nghiệm bị vỡ gây ẩm, ảnh hưởng máy xét nghiệm.Khu vực phòng DSA (phòng can thiệp - Phẫu thuật tim - mạch) cũng bị hư hỏng nhiều thiết bị quan trọng. Nhiều nội thất như điều hòa, tủ lạnh, tivi, giường, bàn ghế... bị tàn phá. Thiết bị tại khu lưu trữ ngân hàng sữa mẹ, khoa dinh dưỡng cũng bị ảnh hưởng. Nhà xe cho nhân viên, nhà xe cho bệnh nhân cũng bị bay mái.Công tác khám chữa bệnh tại bệnh viện gần như bị đình trệ.
-Khoa Sản, Bệnh viện Sản Nhi Quảng Ninh, bị tốc mái trống hoác, nhiều thiết bị trong phòng bị hỏng. Ảnh: Lê Giang
-Bệnh viện Lão khoa - Phục hồi chức năng bị nứt vỡ kính trần nhà, tốc mái tôn. Bác sĩ phải di chuyển bệnh nhân đến nơi an toàn do mưa lớn hắt vào phòng bệnh. Trung tâm Kiểm soát Bệnh tật (CDC) Quảng Ninh cũng thiệt hại nặng nề.Các đơn vị khác như Bệnh viện Đa khoa Hạ Long, Trung tâm y tế Hải Hà, Tiên Yên, Đầm Hà, Bệnh viện Việt Nam - Thụy Điển Uông Bí, Trung tâm Y tế Hạ Long... trong tình trạng tương tự. Nhiều ôtô bị các tấm tôn, cây ngã đè hỏng.
-Nhiều mái tôn bị tốc mái trong bão bay xuống đất, hư hỏng nặng. Ảnh: Lê Giang
-Tính đến chiều 8/9, các bệnh viện ở Quảng Ninh tiếp nhận điều trị 357 ca tai nạn do bão, ba trường hợp tử vong. Trong đó, 18 ca đa chấn thương nặng, 6 chấn thương sọ não, 19 trường hợp gãy xương và hơn 300 ca chấn thương phần mềm khác.Ngành y tế tiếp nhận 255 cuộc gọi, trong đó 113 cuộc gọi cấp cứu. Trung tâm vận chuyển cấp cứu tiếp cận thành công 11 trường hợp, điều phối 6 chuyển xe cho các đơn vị y tế toàn ngành.Các đơn vị đang cố gắng khắc phục thiệt hại để đảm bảo cấp cứu, điều trị người bệnh.Yagi là cơn bão số 3 đổ bộ vào Việt Nam năm nay, tâm bão quét qua Quảng Ninh và Hải Phòng với sức gió giật trên cấp 14. Đây là cơn bão mạnh nhất trên Biển Đông 30 năm qua, gây thiệt hại nặng nề về người và của.Thùy An</t>
+          <t>"Sau khi cân nhắc kỹ lưỡng, chúng tôi mở rộng hạn chế đang được áp dụng đối với các cơ quan truyền thông nhà nước Nga", Meta ngày 16/9 cho hay. "Rossiya Segodnya, RT và các thực thể liên quan hiện bị cấm khỏi các ứng dụng của chúng tôi trên toàn cầu vì tiến hành hoạt động can thiệp của nước ngoài".Meta, công ty có trụ sở tại Mỹ, sở hữu các ứng dụng bao gồm Facebook, Instagram, WhatsApp và Threads.Rossiya Segodnya là tập đoàn truyền thông hàng đầu của Nga, sở hữu nhiều kênh lớn, trong đó có RIA Novosti, Sputnik, phát hành tại 19 quốc gia với 32 ngôn ngữ. RT ra mắt vào năm 2005 với tên gọi "Russia Today", từ đó mở rộng với các kênh truyền hình và trang web bằng các ngôn ngữ bao gồm tiếng Anh, Pháp, Tây Ban Nha và Arab.Nga chỉ trích gay gắt động thái của Meta. "Meta đang tự làm mất uy tín của chính mình bằng hành động này. Những việc làm chống lại truyền thông Nga là không thể chấp nhận được và làm phức tạp triển vọng bình thường hóa quan hệ của chúng tôi với Meta", người phát ngôn Điện Kremlin Dmitry Peskov nói tại cuộc họp báo ở Moskva ngày 17/9.
+Các ứng dụng thuộc sở hữu của Meta trên màn hình điện thoại ở Chania, Hy Lạp ngày 9/8. Ảnh: AFP
+Lệnh cấm được đưa ra sau khi Mỹ cáo buộc RT và các nhân viên của đài này chuyển 10 triệu USD thông qua những "thực thể bình phong" để bí mật tài trợ cho các chiến dịch gây ảnh hưởng trên mạng xã hội TikTok, Instagram, X và YouTube, AFP dẫn nội dung một bản cáo trạng chưa được công bố.RT đã buộc phải ngừng hoạt động tại Anh, Canada, Liên minh châu Âu và Mỹ do các lệnh trừng phạt sau khi Nga mở chiến dịch ở Ukraine tháng 2/2022.Bộ Ngoại giao Mỹ gần đây cho biết năng lực của RT đã được mở rộng vào đầu năm ngoái, với việc chính phủ Nga tăng cường "năng lực hoạt động mạng và mối quan hệ với tình báo Nga". Mỹ khẳng định thông tin thu thập được từ hoạt động bí mật của RT sẽ được chuyển đến các cơ quan tình báo, truyền thông Nga.Tổng biên tập RT Margarita Simonyan mỉa mai những cáo buộc này, nói đùa rằng RT đã học theo người Mỹ, chứ không phải từ các sĩ quan tình báo Nga. "Thật sao? Các anh hết gương rồi à?", bà nói.Nhà Trắng từ chối bình luận về động thái của Meta. Ngoại trưởng Antony Blinken cuối tuần qua cho rằng các quốc gia nên coi hoạt động của RT như "hoạt động tình báo bí mật".Nga hồi năm 2022 coi Meta là tổ chức "cực đoan" và chặn Instagram, Facebook.
+Moskva cũng chỉ trích những nỗ lực trước đây của Meta trong việc hạn chế năng lực tiếp cận của truyền thông Nga và nhiều lần phạt công ty này vì không xóa nội dung bị cho là bất hợp pháp ở Nga. WhatsApp, ứng dụng chưa bị Nga cấm, hiện vẫn có hàng triệu người sử dụng ở quốc gia này.Huyền Lê (Theo AFP, Reuters, RT)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Người Hải Phòng chạy đôn đáo tìm chỗ sạc điện</t>
+          <t>Trương Thế Vinh: 'Tôi không đánh đổi sức khỏe vì tiền'</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-hai-phong-chay-don-dao-tim-cho-sac-dien-4790450.html</t>
+          <t>https://vnexpress.net/truong-the-vinh-toi-khong-danh-doi-suc-khoe-vi-tien-4792567.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nghe tin một chung cư ở phường Vĩnh Niệm, quận Lê Chân có điện, chị Thu Hà cùng hàng xóm gom 20 chiếc điện thoại, iPad, laptop mang đến sạc nhờ, chiều 8/9.</t>
+          <t>Ca sĩ kiêm diễn viên Trương Thế Vinh nói chọn sống bình tĩnh, dành thời gian cho người thân, gia đình chứ không lao vào kiếm tiền bất chấp.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Nhà chị Hà ở quận Ngô Quyền mất điện từ trưa qua khi bão Yagi đổ bộ, đến nay chưa được cấp lại. Ngoài mất điện, nhiều quận, huyện của thành phố còn mất nước, sóng điện thoại, khiến mọi người không thể liên lạc với người thân."Mất điện hơn một ngày nên mọi thiết bị đều hết pin, con ở xa không liên lạc được lại lo. Tôi dò hỏi khắp nơi, xem chỗ nào có điện để đi sạc nhờ", chị Hà nói.Bà Hồng Hoa, một cư dân khu chung cư ở quận Lê Chân, cho biết gia đình và nhiều hộ khác đã nhận sạc điện thoại, đồ điện tử cho người quen bởi biết hầu hết các khu vực khác đều chưa có điện."Vừa có điện là tôi gọi điện thoại báo cho mọi người ai cần sạc đồ điện tử hay trú ẩn thì qua, cư dân sẽ hỗ trợ hết sức", bà Hoa nói.
-Người dân Hải Phòng ngồi la liệt tại lối vào nhà vệ sinh của trung tâm thương mại Aeon Mall Hải Phòng, quận Lê Chân để sạc điện thoại, chiều 8/9. Ảnh: Duy Anh
-Không có người quen ở khu chung cư nên Minh Ngọc, ở quận Lê Chân, cùng chồng và con con gái đến trung tâm thương mại Aeon Mall Hải Phòng ngay khi biết tin ở đây chạy máy phát điện và có wifi.Đến nơi, Ngọc nhận thấy các hàng quán có ổ cắm điện hoặc khu vực công cộng, thậm chí lối vào nhà vệ sinh có ổ điện đã chật kín người. "Hầu hết điện thoại của mọi người đều đã kiệt pin, chờ sạc được 50% cũng mất cả tiếng. Chắc phải đến tối mới đến lượt tôi", Ngọc nói.Không thể chờ đợi, cô quyết định đội mưa đi tìm các quán cà phê trong thành phố có máy phát để vào sạc nhờ.
-Người Hải Phòng nháo nhác tìm nơi sạc điện
-Người dân Hải Phòng chen chúc tranh chỗ cắm sạc điện thoại tại trung tâm thương mại Aeon Mall quận Lê Chân, 15h ngày 8/9. Nguồn: Duy Anh
-Từ sáng 8/9, Việt Hoàng, 25 tuổi, ở quận Lê Chân đã ra quán cà phê ở quận Hồng Bàng, một trong những nơi được cấp điện trở lại sớm nhất, để sạc điện thoại, đèn pin và làm việc online. Hoàng phải đợi khá lâu mới đến lượt bởi trong quán đã có nhiều người sử dụng. Các quán cà phê khác quanh khu vực anh sống tấp nập người tới ngồi từ sớm.Bốn người trong gia đình Hoàng đã di tản. Bố mẹ cùng em trai tới trung tâm thương mại và cửa hàng tiện lợi trên địa bàn đang chạy máy phát điện với hy vọng có sóng điện thoại hoặc Internet để liên lạc với họ hàng và sạc thiết bị."Trận bão khiến nhà tôi lật mái, kính vỡ, cây đổ chắn lối đi, mất liên lạc cả ngày. Giờ lo sạc điện để kết nối cũng như đề phòng mưa lớn mất điện kéo dài", chàng trai 25 tuổi nói.
-Hầu hết ổ điện tại quán cà phê ở quận Hồng Bàng nơi Việt Hoàng đến đều đang được sử dụng, trưa 8/9. Ảnh: Nhân vật cung cấp
-Quản lý một quán cà phê ở quận Hồng Bàng cho biết đã mở cửa ngay sau khi quán được cấp điện trở lại từ 8h, để phục vụ người dân có nhu cầu tới trú hoặc sử dụng Internet, điện."Từ lúc mở cửa, quán đã có hàng chục người tới sạc điện thoại. Chỉ mong cuộc sống sớm trở lại bình thường", người quản lý nói.Theo Tập đoàn Điện lực Việt Nam (EVN), lưới điện miền Bắc, đặc biệt tại Quảng Ninh, Hải Phòng, Thái Bình và Hải Dương, gặp nhiều khó khăn do sức tàn phá của bão Yagi.Hải Phòng - một trong số địa phương chịu ảnh hưởng nặng nề, bị cắt điện toàn bộ trong ngày 7/9. Ông Nguyễn Hữu Hưởng - Chủ tịch kiêm Tổng giám đốc Công ty TNHH MTV Điện lực Hải Phòng cho biết dự kiến trưa 8/9, 50-60% khách hàng được cấp điện trở lại. Con số này sẽ tăng lên 80% khách hàng vào cuối ngày.Theo khảo sát của VnExpress, đến 15h ngày 8/9, đa số các khu vực dân cư trên địa bàn thành phố như quận Ngô Quyền, Lê Chân, Hồng Bàng chưa được cấp điện trở lại.Thanh Nga - Quỳnh Nguyễn</t>
+          <t>Sau nhiều năm ngưng ca hát, Trương Thế Vinh gây chú ý khi trở lại tại show âm nhạc Anh trai vượt ngàn chông gai. Anh nói tìm thấy nhiều niềm hứng khởi, được khơi dậy tình yêu nghề.
+Trương Thế Vinh: 'Sợ nhất là không thể lo cho gia đình'
+Trương Thế Vinh: "Tôi không lo già, chỉ sợ cô đơn"
+Trương Thế Vinh tự nhận bản thân không quá giàu nhưng hài lòng về sự bình yên đang có. "Nhiều năm qua, tôi chọn cách sống bình tĩnh nhưng vẫn đặt ra mục tiêu rõ ràng để phấn đấu. Điều tôi chú trọng là sức khỏe. Tôi sợ nhất nếu một ngày không còn được thể hiện sự yêu thương, trách nhiệm với gia đình", anh nói.
+Với Trương Thế Vinh, gia đình có ý nghĩa quan trọng trong việc bồi đắp tình yêu nghề, đồng thời giúp anh tránh khỏi những cám dỗ, dần trở thành trụ cột như hiện tại. Anh thấm thía về tình thân rõ ràng nhất sau khi bố qua đời. Hiện ca sĩ muốn làm chỗ dựa tinh thần, mang đến niềm vui cho mẹ.
+Trương Thế Vinh tên thật là Nguyễn Xuân Vinh, 40 tuổi, sinh ở Đà Nẵng. Năm 2001, anh cùng Khánh Phương, Trần Tuyên và Phương Tài thành lập nhóm nhạc MP5. Nhóm hoạt động được ba năm thì tan rã. Thế Vinh sau đó chuyển sang solo, ghi dấu ấn với khán giả qua nhiều nhạc phẩm như Tình yêu hoa gió, Anh sẽ trở về, Bức tranh trong tim.
+Với diễn xuất, anh từng đóng các phim Hoán đổi thân xác (2011), Nhà có năm nàng tiên (2013), Cha và con và... (2015), Người bất tử, Cây táo nở hoa (2018). Gần nhất, Trương Thế Vinh tham gia dự án điện ảnh Án mạng lầu 4, đóng cùng Lương Bích Hữu.
+Tân Cao - Tuấn Việt</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tầm nhìn kinh tế ông Trump vạch ra cho nhiệm kỳ tương lai</t>
+          <t>Người đập vỡ kính, tấn công tài xế ôtô sau va chạm giao thông bị bắt</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tam-nhin-kinh-te-ong-trump-vach-ra-cho-nhiem-ky-tuong-lai-4789683.html</t>
+          <t>https://vnexpress.net/nguoi-dap-vo-kinh-tan-cong-tai-xe-oto-sau-va-cham-giao-thong-bi-bat-4793991.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ông Trump nhấn mạnh các chính sách như giảm thuế, tăng thuế quan và cắt giảm lãng phí trong bài phát biểu chi tiết về tầm nhìn kinh tế.</t>
+          <t>TP HCMNgô Đức Giang, 43 tuổi, bị bắt về hành vi đập vỡ kính, hành hung tài xế ôtô sau va quẹt trên đường Kha Vạn Cân, TP Thủ Đức.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ngày 5/9, ông Trump có bài phát biểu kéo dài một giờ tại Câu lạc bộ Kinh tế New York trước những gương mặt nổi tiếng của Phố Wall, vào thời điểm Phó tổng thống Kamala Harris, ứng viên đảng Dân chủ, đã thu hẹp lợi thế của cựu tổng thống trong các cuộc khảo sát cử tri về vấn đề kinh tế. Cả ông Trump và bà Harris đều chịu áp lực phải đưa ra tầm nhìn chính sách cụ thể để giúp thúc đẩy nền kinh tế, vốn bị sa lầy bởi giá cao và lãi suất vay tăng cao, khi có nhiều lo ngại về nguy cơ tăng trưởng chậm."Tôi cam kết thuế thấp, cắt giảm quy định, chi phí năng lượng thấp, lãi suất thấp, biên giới an toàn, tỷ lệ tội phạm cực thấp và thu nhập cao cho công dân bất kể chủng tộc, tôn giáo, màu da hay tín ngưỡng. Kế hoạch của tôi sẽ đẩy lùi lạm phát, nhanh chóng hạ giá và khôi phục mức độ tăng trưởng kinh tế bùng nổ", ứng viên đảng Cộng hòa nói.Ông nêu kế hoạch bổ nhiệm tỷ phú Elon Musk làm lãnh đạo ủy ban "chịu trách nhiệm giám sát tài chính và hiệu suất của toàn bộ chính phủ liên bang, cũng như đưa ra các khuyến nghị cải cách mạnh mẽ". Cựu tổng thống đặt mục tiêu rằng ủy ban này sẽ giúp loại bỏ "hàng nghìn tỷ USD" chi tiêu lãng phí.
-Ứng viên đảng Cộng hòa Donald Trump tại Câu lạc bộ Kinh tế New York ngày 5/9. Ảnh: AP
-Ông Trump ca ngợi thành tựu kinh tế trong nhiệm kỳ đầu của mình, đồng thời chỉ trích các chính sách của chính quyền Biden - Harris về kinh tế và nhập cư. "Chúng tôi đã tạo ra phép màu kinh tế, nhưng Harris và Biden đã biến nó thành thảm họa", ông Trump nói, đổ lỗi cho chính quyền hiện tại về lạm phát cao.Lạm phát đã tăng vọt trong nhiệm kỳ của ông Biden sau khi đại dịch Covid-19 làm tắc nghẽn chuỗi cung ứng, song đã giảm đáng kể sau khi đạt đỉnh vào năm 2022. Lạm phát đang theo đà giảm và dự kiến xuống mức mục tiêu 2%, theo Cục Dự trữ Liên bang Mỹ. Tuy nhiên, ông Trump và các đồng minh vẫn liên tục công kích phe Dân chủ về vấn đề này.Một lời hứa hẹn của ông Trump làm hài lòng giới doanh nghiệp là ông sẽ gia hạn đạo luật cắt giảm thuế mà ông từng thông qua năm 2017. Ông nhấn mạnh sự tương phản giữa mình với bà Harris, khi bà đã nêu kế hoạch tăng thuế doanh nghiệp từ 21 lên 28%.Trump đề xuất giảm thuế doanh nghiệp xuống 15%. Tuy nhiên, mức giảm sẽ chỉ dành cho các công ty sản xuất tại Mỹ, những công ty thuê sản xuất ngoài, chuyển dây chuyền ra nước ngoài hoặc không thuê lao động Mỹ không đủ điều kiện hưởng ưu đãi."Thông điệp của chúng tôi rất đơn giản: hãy tạo ra sản phẩm của bạn ở Mỹ. Chỉ ở Mỹ mà thôi", ông Trump nói.Cựu tổng thống cũng hứa hẹn mang lại "năng lượng dồi dào, độc lập và thậm chí thống trị ngành năng lượng" nếu trở lại Nhà Trắng. Ông dự định tuyên bố tình trạng khẩn cấp quốc gia để cắt giảm các quy định liên quan tới khai thác dầu khí và tăng cường sản xuất năng lượng trong nước.Trump khẳng định những hành động này sẽ làm giảm giá năng lượng ít nhất một nửa trong vòng 12 tháng sau khi ông nhậm chức, cam kết chấm dứt "cuộc thập tự chinh chống năng lượng" của ứng viên đảng Dân chủ. Giá xăng và các chi phí năng lượng khác tại Mỹ hiện cao hơn so với thời Trump còn tại nhiệm.Về thuế quan, Trump đã đề xuất mức thuế chung là 10% với tất cả sản phẩm nhập khẩu vào Mỹ. Tuy nhiên, tại một sự kiện tháng trước ở North Carolina, ông gợi ý thuế suất có thể tăng lên 20%. Với các sản phẩm từ Trung Quốc, ông muốn áp thuế 60%.Trong bài phát biểu ngày 5/9, Trump gọi đây là "chính sách thương mại có lợi cho Mỹ, sử dụng thuế quan để khuyến khích sản xuất trong nước" và sẽ dẫn đến "sự phục hưng kinh tế quốc gia".Trump gợi ý rằng ông có thể sử dụng số tiền thu được từ thuế quan để thành lập một quỹ đầu tư quốc gia, nhằm tài trợ cho dự án cơ sở hạ tầng, chi phí chăm sóc trẻ em hay trả nợ công.
-Người ủng hộ ứng viên tổng thống Donald Trump tại Đại hội toàn quốc đảng Cộng hòa ở Milwaukee, bang Wisconsin ngày 16/7. Ảnh: AFP
-Nhiều nhà kinh tế cảnh báo những mức thuế quan đó có thể phản tác dụng bằng cách làm tăng giá cả cho các gia đình Mỹ, làm mất việc làm và gây ra chiến tranh thương mại toàn cầu. "Đó là chính sách bảo hộ kinh tế khủng khiếp", Douglas Holtz-Eakin, chủ tịch tổ chức tư vấn trung hữu Diễn đàn Hành động Mỹ, nói.Trong khi đó, Trump tin các chính sách của ông sẽ thúc đẩy tăng trưởng, chứ không dẫn tới những hậu quả như làm suy yếu tăng trưởng và khiến giá cả tăng vọt như nhiều nhà kinh tế cảnh báo.Chiến dịch tranh cử của bà Harris cáo buộc ông Trump "nói dối trắng trợn người dân Mỹ, không cho họ biết những hậu quả nghiêm trọng từ kế hoạch kinh tế của ông ấy".Karoline Leavitt, thư ký báo chí chiến dịch của ông Trump, phản bác ý kiến này."Nhiều nhà kinh tế và chuyên gia từng hoài nghi kế hoạch kinh tế của Tổng thống Trump trong nhiệm kỳ đầu. Họ đã sai lầm và sẽ tiếp tục được chứng minh sai lầm một lần nữa. Tổng thống Donald Trump đã áp thành công thuế quan với Trung Quốc trong nhiệm kỳ đầu tiên và cắt giảm thuế cho người Mỹ. Ông ấy sẽ làm điều đó lần nữa trong nhiệm kỳ thứ hai. Kế hoạch của Tổng thống sẽ mang đến hàng triệu việc làm và hàng trăm tỷ USD từ Trung Quốc về Mỹ", Leavitt nói.Người sáng lập Key Square Scott Besent nhận xét bài phát biểu đã cho thấy phần nào chương trình nghị sự chính sách của ông Trump với nhiều mục mới, dự kiến "tăng sức hấp dẫn" cho cựu tổng thống."Ông ấy đã đưa ra cảnh báo về các chính sách hiện tại của chính quyền Tổng thống Biden, sau đó đưa ra giải pháp đầy lạc quan như đã làm năm 2016", Bessent, một trong những đồng minh lớn nhất của ông Trump trong lĩnh vực tài chính, nói.Thùy Lâm (Theo Politico, FT, CNN)</t>
+          <t>Chiều 17/9, Giang bị Công an TP Thủ Đức bắt tạm giam về tội Gây rối trật tự công cộng. Bị can còn bị điều tra về các dấu hiệu hành vi Hủy hoại tài sản và Cố ý gây thương tích. 
+Đập kính, hành hung tài xế ôtô sau va chạm giao thông
+Video ghi lại cảnh Ngô Đức Giang đập vỡ kính xe, tấn công tài xế. Video: Người dân cung cấp
+Theo điều tra, tối hai hôm trước, Giang lái ôtô trên đường Kha Vạn Cân, TP Thủ Đức, thì xảy ra va chạm với ôtô đi ngược chiều do anh Nguyễn Ngọc Sơn, 35 tuổi, cầm lái. Hai xe dừng lại giữa đường, Giang bước xuống chửi bới anh Sơn, la lớn: "Bước xuống đây, xuống đây".Giang đến chỗ ghế lái của anh Sơn, đánh anh này qua cửa kính đang mở, bẻ kính xe. Tiếp đó, người này về xe lấy cây cờ lê đánh liên tiếp vào cằm, bụng, chân, tay của anh Sơn; mặc nạn nhân và vợ van xin.
+Ngô Đức Giang tại cơ quan điều tra. Ảnh: Công an cung cấp
+Sự việc xảy ra gây ồn ào khu vực, nhiều người chứng kiến. Người dân đã quay video và đăng lên mạng xã hội.Bị cảnh sát triệu tập, Giang thừa nhận hành vi, cho biết mình đi đúng đường nhưng do bị xe anh Sơn va chạm nên bực tức.Cơ quan điều tra đang mở rộng điều tra.Quốc Thắng</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hà Nội sẽ cứu cây xanh gãy đổ do bão Yagi</t>
+          <t>Chứng khoán tăng mạnh nhất một tháng</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ha-noi-se-cuu-cay-xanh-gay-do-do-bao-yagi-4790498.html</t>
+          <t>https://vnexpress.net/chung-khoan-17-9-vn-index-tang-manh-nhat-mot-thang-4793917.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cây cần bảo tồn, cây quý hiếm có giá trị, cây nhỏ đường kính dưới 25 cm bị gãy đổ sẽ được đánh giá để trồng lại tại chỗ hoặc đưa về vườn ươm chăm sóc.</t>
+          <t>Bộ ba dẫn dắt dòng tiền gồm bất động sản, chứng khoán và ngân hàng giúp kéo VN-Index hôm nay tăng gần 20 điểm, mạnh nhất một tháng qua.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Trong văn bản khắc phục hậu quả bão Yagi chiều 8/9, Chủ tịch TP Hà Nội Trần Sỹ Thanh yêu cầu các đơn vị liên quan tập trung toàn bộ nhân lực, trang thiết bị để giải tỏa cây đổ, gãy nhằm đảm bảo an toàn giao thông.Trước mắt các lực lượng phải giải tỏa ngay cây gãy đổ trên các tuyến đường phố chính của Thủ đô, xong trước ngày 12/9; sau đó sẽ tiếp tục thu dọn cây đổ, cành cây gãy, dựng lại cây, trồng thay thế và dọn vệ sinh thu hồi củi gỗ theo quy định."Đối với cây xanh cần bảo tồn, cây quý hiếm có giá trị bị nghiêng đổ, cần kiểm tra đánh giá và chống dựng, trồng lại ngay, đảm bảo cây tiếp tục sinh trưởng, phát triển hoặc di chuyển về vườn ươm để chăm sóc, trồng vào vị trí phù hợp trên địa bàn. Công việc này hoàn thành trước ngày 15/9", văn bản nêu.
-Cây sấu lớn trước cửa Bưu điện Hà Nội bật gốc đổ nghiêng về phía tháp Hòa Phong. Ảnh: Ngọc Thành
-Người đứng đầu chính quyền Hà Nội cũng yêu cầu trồng lại các cây xanh đô thị có đường kính nhỏ dưới 25 cm bị gãy đổ. Trước khi trồng lại, phải cắt cành, tán đảm bảo cân đối phù hợp để trồng lại tại chỗ và chăm sóc theo quy định.Ông lưu ý với những cây đổ ra đường sau khi cắt tỉa phải di chuyển lên hè phố, dải phân cách để đảm bảo an toàn giao thông nếu chưa kịp trồng lại. Việc trồng lại các cây xanh nêu trên xong trước ngày 20/9. Với những cây do các quận, huyện thị xã quản lý, việc trồng lại tại chỗ cây đổ hoàn thành trước 30/9.Với những cây gãy đổ không thể trồng lại, củi gỗ thu hồi được đưa về vườn ươm Yên Sở, vườn ươm Cổ Nhuế, bãi tập kết tại dốc La Pho, công viên Tuổi trẻ, sau đó thanh lý. Sở Xây dựng được giao chủ trì xây dựng kế hoạch trồng lại những cây xanh gãy đổ không thể khắc phục, đảm bảo chủng loại, kích thước phù hợp.
-Cây đa cổ thụ ở Vườn hoa Lý Thái Tổ gãy gốc, đổ về phía đường Lê Lai kéo theo cột điện cao áp bên cạnh. Ảnh: Ngọc Thành
-Chủ trương dựng lại cây xanh gãy đổ cũng được Bí thư Thành ủy Bùi Thị Minh Hoài nêu tại buổi kiểm tra công tác khắc phục hậu quả bão Yagi tại quận Nam Từ Liêm và huyện Thanh Oai sáng 8/9. Bà Hoài yêu cầu "cây nào cứu được phải hết sức cứu, dựng lại được phải dựng lại để chăm sóc. Bần cùng bất đắc dĩ mới phải cưa bỏ vì trồng được một cây không dễ, mất rất nhiều thời gian".Hà Nội hiện có khoảng 142.000 cây xanh đô thị do thành phố quản lý. Bão Yagi làm khoảng 17.000 cây gãy đổ trên toàn thành phố, trong đó khoảng 2.000 cây xanh đô thị. Đến nay cơ quan quản lý chưa thông tin phân loại cây đã gãy đổ như cây di sản, cây quý hiếm, cây có đường kính nhỏ...Thủ đô Hà Nội là một trong những địa phương chịu thiệt hại nặng do bão Yagi. Từ 6/9 đến ngày 8/9, thành phố ghi nhận 3 người chết, 10 người bị thương; 13 ôtô và 6 xe máy hư hại; 9 nhà dân bị tốc mái; hàng nghìn ha lúa, hoa màu bị đổ, ngập nước.Võ Hải</t>
+          <t>Chỉ số của sàn HoSE lình xình quanh tham chiếu trong cả buổi sáng với biên độ dưới 5 điểm. Phần lớn thời gian giao dịch, đồ thị đạt sắc xanh nhưng thị trường giao dịch trầm lắng. Thanh khoản hết buổi sáng chỉ đạt gần 3.900 tỷ đồng. Không xuất hiện cổ phiếu hay nhóm ngành nào dẫn dắt thị trường, nhà đầu tư cũng chỉ tham gia ở mức thăm dò, cầm chừng.Sang buổi chiều, VN-Index bắt đầu tăng tốc khi các lệnh giao dịch được đổ lên hệ thống nhiều hơn. Lực cầu chiếm ưu thế giúp chỉ số này lấy lại mốc tâm lý quan trọng 1.250 điểm vào khoảng 14h20. Lệnh mua chủ động xuất hiện nhiều hơn, thị trường tiếp tục tích lũy trong phiên ATC.Chốt phiên, VN-Index đóng cửa ở sát 1.259 điểm, tăng gần 19,7 điểm so với hôm qua. Đây là mức tích lũy mạnh nhất kể từ phiên 16/8, đưa chứng khoán trở lại gần với vùng giá đầu tuần trước.Số lượng cổ phiếu tăng giá áp đảo so với bên giảm, lần lượt đạt 312 mã và 88 mã. Đóng góp tích cực nhất là VHM, VCB, BID, TCB, VIC. Ba nhóm cổ phiếu dẫn dắt dòng tiền cũng là các ngành góp điểm nhiều nhất cho chỉ số chung, gồm bất động sản, chứng khoán và ngân hàng.Bảng điện bất động sản hôm nay được phủ hầu hết sắc xanh. Nổi bật nhất là VHM và PDR khi lần lượt tăng 5,4% và 5,1%. Ngoài ra nhiều mã có thanh khoản tốt như DIG, DXG, VRE, HDG, VIC, VCG... cũng tích lũy khoảng 2-4%.Trong các mã hút dòng tiền nhất ngành địa ốc, NVL có diễn biến trái chiều. Cổ phiếu này diễn biến tiêu cực trong nửa cuối buổi sáng, có lúc thấp hơn tham chiếu 4,9%. Tuy nhiên sang buổi chiều, lực cầu trở lại đã hỗ trợ cho thị giá NVL và chốt phiên ở mức tham chiếu 11.200 đồng.Diễn biến trên xảy ra sau khi Sở Giao dịch chứng khoán TP HCM (HoSE) quyết định đưa cổ phiếu NVL vào diện cảnh báo. Nguyên nhân là doanh nghiệp này chậm công bố báo cáo tài chính bán niên đã soát xét quá 15 ngày so với thời hạn quy định. Tuần trước, HoSE cũng đưa cổ phiếu này vào danh sách không đủ điều kiện giao dịch ký quỹ (margin).Novaland cho biết trong 6 tháng đầu năm, doanh nghiệp này triển khai nhiều kế hoạch, chương trình hoạt động cùng lúc như tái khởi động các dự án, hoàn thiện và bàn giao sản phẩm, bàn giao giấy chứng nhận cho cư dân. Do đó, giao dịch và số lượng hồ sơ chứng từ tăng cao giữa công ty mẹ và các công ty con, làm chậm quá trình hoàn thiện báo cáo tài chính. Novaland nói đang nỗ lực làm việc với đơn vị kiểm toán để sớm công bố thông tin.Ở nhóm chứng khoán và ngân hàng, tất cả mã đạt thanh khoản trăm tỷ đều tăng giá. Nổi bật nhất là HCM, VCI, FTS, MBB, VPB, TCB...Thanh khoản cải thiện trong buổi chiều nhưng tổng lại chỉ nhích nhẹ so với hôm qua, đạt trên 13.500 tỷ đồng. Điểm tích cực là nhà đầu tư nước ngoài tăng giá trị mua ròng, ghi nhận khoảng 525 tỷ đồng, tâm điểm nằm ở VHM và FPT.Tất Đạt</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nga tuyên bố kiểm soát thành phố gần Pokrovsk</t>
+          <t>Nga tăng quy mô quân đội lên 1,5 triệu người</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nga-tuyen-bo-kiem-soat-thanh-pho-gan-pokrovsk-4790467.html</t>
+          <t>https://vnexpress.net/nga-tang-quy-mo-quan-doi-len-1-5-trieu-nguoi-4793792.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bộ Quốc phòng Nga nói quân đội nước này kiểm soát đô thị gần thành phố chiến lược Pokrovsk, bước tiến mới tại mặt trận phía đông.</t>
+          <t>Ông Putin ký lệnh nâng trần quân số chiến đấu của Nga lên 1,5 triệu người, đánh dấu lần thứ ba động thái này diễn ra kể từ năm 2022.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>"Nhờ hoạt động tích cực của cánh quân Trung tâm, thành phố Novogrodovka tại Cộng hòa Nhân dân Donetsk đã nằm dưới sự kiểm soát của chúng tôi", Bộ Quốc phòng Nga ngày 8/9 thông báo, đề cập mặt trận Donetsk ở phía đông Ukraine.Cơ quan này cho biết cánh quân Trung tâm còn đánh bại nhân lực, khí tài của ba lữ đoàn và một tiểu đoàn Ukraine ở nhiều khu vực tại tỉnh Donetsk, cũng như chặn 8 cuộc phản công của đối phương, khiến Kiev tổn thất tổng cộng khoảng 560 binh sĩ, một xe tăng cùng nhiều phương tiện, khí tài khác.Bộ Quốc phòng Ukraine chưa bình luận về thông tin.
-Binh sĩ Nga khai hỏa pháo phòng không ZU-23 tại tỉnh Donetsk hồi tháng 8. Ảnh: RIA Novosti
-Thành phố Novogrodovka, được Ukraine gọi là Novohrodivka, có hơn 14.000 cư dân sinh sống trước khi xung đột Nga - Ukraine bùng phát. Nó cách đô thị chiến lược Pokrovsk của Ukraine khoảng 20 km.Pokrovsk là giao điểm giữa nhiều tuyến đường sắt và đường bộ quan trọng, được đánh giá là trung tâm hậu cần chủ chốt giúp ngăn phòng tuyến Ukraine trong khu vực sụp đổ trên diện rộng.Moskva gần đây tuyên bố đạt nhiều bước tiến ở mặt trận Pokrovsk. Bộ Quốc phòng Nga ngày 7/9 thông báo lực lượng nước này đã kiểm soát được làng Kalinovo, cách Pokrovsk khoảng 25 km.Một trong những mục tiêu của Kiev khi mở chiến dịch ở tỉnh Kursk của Nga cách đây một tháng là phân tán bớt lực lượng đối phương và giảm sức ép đối với binh sĩ Ukraine ở mặt trận phía đông. Tuy nhiên, việc Nga tuyên bố đạt nhiều bước tiến ở khu vực này cho thấy chiến lược trên dường như chưa phát huy hiệu quả.Tổng thống Nga Vladimir Putin ngày 5/9 cho biết mục tiêu chính của ông ở Ukraine sau 30 tháng giao tranh là kiểm soát toàn bộ vùng Donbass, trong đó có tỉnh Donetsk, thêm rằng chiến dịch của Kiev ở tỉnh Kursk đang khiến mục tiêu đó trở nên dễ dàng hơn.
-Vị trí Novogrodovka. Đồ họa: RYV
-Phạm Giang (Theo AFP, RIA Novosti)</t>
+          <t>Điện Kremlin ngày 16/9 công bố sắc lệnh của Tổng thống Vladmir Putin, trong đó quy định quân số chiến đấu tối đa của lực lượng vũ trang Nga sẽ được tăng thêm 180.000 người, lên 1.500.000 binh sĩ. Sắc lệnh sẽ có hiệu lực từ ngày 1/12.Con số này bao gồm quân nhân chuyên nghiệp ký hợp đồng dài hạn với lực lượng vũ trang và lính nghĩa vụ có thời hạn phục vụ 12 tháng. Thống kê của Statista năm 2023 cho thấy Nga biên chế khoảng 277.000 lính nghĩa vụ, lực lượng này bị cấm tham gia nhiệm vụ tác chiến ngoài lãnh thổ và không tham gia chiến dịch tại Ukraine.Viện Nghiên cứu Chiến lược Quốc tế (IISS) có trụ sở tại Anh nói rằng quân đội Nga đang xếp thứ tư thế giới về quân số chiến đấu, sau Trung Quốc, Ấn Độ và Mỹ. Đợt nâng trần sẽ khiến Nga vượt qua Ấn Độ và Mỹ, trở thành quốc gia biên chế số lượng binh sĩ chiến đấu nhiều thứ hai thế giới.Nếu tính cả binh sĩ không đảm nhiệm vai trò chiến đấu, lực lượng vũ trang Nga sẽ có tổng cộng gần 2,4 triệu quân nhân.Chủ tịch Ủy ban Quốc phòng Hạ viện Nga Andrei Kartapolov nói rằng động thái nằm trong kế hoạch cải cách toàn diện lực lượng vũ trang, trong đó có tăng dần quy mô quân số để ứng phó với "tình hình quốc tế và hành động của những nước từng là đối tác của Nga".
+Quân nhân Nga tại lễ Duyệt binh Chiến thắng ở Quảng trường Đỏ hồi tháng 5. Ảnh: RIA Novosti
+Đây là lần thứ ba ông Putin ra lệnh mở rộng quy mô lực lượng vũ trang kể từ khi xung đột Ukraine bùng phát đầu năm 2022. Tổng thống Nga tháng 8/2022 yêu cầu bổ sung 137.000 binh sĩ vào đầu năm 2023, nâng tổng số quân nhân đảm nhận vai trò chiến đấu của nước này lên 1,15 triệu người.Tháng 12/2023, ông chủ Điện Kremlin tiếp tục ra lệnh tăng thêm 170.000 binh sĩ trong biên chế quân đội, nâng quy mô lực lượng chiến đấu của nước này lên 1,32 triệu người.Bên cạnh đó, Nga cũng tiến hành động viên một phần hồi tháng 9/2022, triệu tập lực lượng dự bị khoảng 300.000 người, chủ yếu là quân nhân giải ngũ, có chuyên môn và kinh nghiệm quân sự, nhằm đối phó chiến dịch phản công chớp nhoáng của Ukraine tại tỉnh Kharkov.Đợt động viên quân kết thúc vào tháng 11/2022, sau khi giới chức Nga tuyên bố đã huy động đủ 300.000 binh sĩ như mục tiêu đề ra.Sắc lệnh tăng quân được ông Putin phê duyệt sau khi Ukraine tháng trước bất ngờ tấn công tỉnh Kursk, đánh dấu lần đầu lãnh thổ Nga bị quân đội nước ngoài xâm nhập từ sau Thế chiến II. Kiev tuyên bố chiếm 100 ngôi làng và kiểm soát 1.300 km2 lãnh thổ tại Kursk, nhưng chiến dịch dường như đã đình trệ và không đạt mục tiêu chiến lược là buộc Moskva rút lực lượng từ mặt trận Donbass.Quân đội Nga tuần trước mở chiến dịch phản công và tuyên bố đã giành lại được 12 khu dân cư ở tỉnh Kursk. Lực lượng Nga cũng đẩy mạnh tiến công trên mặt trận Donbass và đang áp sát thành trì chiến lược Pokrovsk tại tỉnh Donetsk.Hiện không rõ thương vong của quân đội Nga sau hơn hai năm xung đột. Tháng 9/2022, ông Sergey Shoigu, khi đó là Bộ trưởng Quốc phòng Nga, cho biết gần 6.000 binh sĩ đã thiệt mạng tại Ukraine, song Moskva từ đó tới nay không cập nhật số liệu.Quân đội Ukraine hôm 1/9 cho biết hơn 616.000 binh sĩ Nga đã thiệt mạng và bị thương kể từ đầu xung đột. Bộ Quốc phòng Anh hồi đầu tháng cũng đưa ra con số gần như tương tự, đồng thời dự đoán quân đội Nga sẽ hứng chịu tổn thất trung bình 1.000 người mỗi ngày trong tháng này.Phạm Giang (Theo CNN, Reuters, AFP)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Thổ Nhĩ Kỳ kêu gọi lập liên minh Hồi giáo đối phó Israel</t>
+          <t>Áp thấp nhiệt đới vào Biển Đông</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tho-nhi-ky-keu-goi-lap-lien-minh-hoi-giao-doi-pho-israel-4790488.html</t>
+          <t>https://vnexpress.net/ap-thap-nhiet-doi-vao-bien-dong-4793655.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Thổ Nhĩ Kỳ kêu gọi các nước Hồi giáo lập liên minh để ứng phó Israel và "mối đe dọa ngày càng gia tăng từ chủ nghĩa bành trướng".</t>
+          <t>10h hôm nay, áp thấp nhiệt đới vượt qua đảo Luzon của Philippines vào Biển Đông, sức gió mạnh nhất 61 km/h (cấp 7), dự kiến mạnh lên bão vào ngày mai.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>"Động thái duy nhất có thể ngăn chặn sự ngạo mạn, ăn cướp của Israel là thành lập liên minh các nước Hồi giáo", Tổng thống Thổ Nhĩ Kỳ Tayyip Erdogan phát biểu tại sự kiện gần thành phố Istanbul ngày 7/9.Theo ông Erdogan, Thổ Nhĩ Kỳ gần đây đã cải thiện quan hệ với Ai Cập và Syria nhằm thiết lập mặt trận đoàn kết để đối phó "mối đe dọa ngày càng tăng từ chủ nghĩa bành trướng", điều mà ông cho là đang đe dọa Syria và Lebanon.Ngoại trưởng Israel Israel Katz chỉ trích phát biểu của ông Erdogan, mô tả đây là "lời dối trá, kích động nguy hiểm" và cáo buộc Tổng thống Thổ Nhĩ Kỳ đang phối hợp với Iran để làm suy yếu chính quyền các nước Arab trung lập ở khu vực.
-Tổng thống Thổ Nhĩ Kỳ Tayyip Erdogan phát biểu tại Istanbul ngày 6/9. Ảnh: AFP
-Ông Erdogan đưa ra bình luận khi đề cập vụ một phụ nữ Mỹ gốc Thổ Nhĩ Kỳ tên Aysenur Ezgi Eygi bị bắn chết trong lúc biểu tình phản đối mở rộng các khu định cư tại những vùng mà Israel kiểm soát ở Bờ Tây. Giới chức Thổ Nhĩ Kỳ và Palestine cáo buộc binh sĩ Israel là thủ phạm.Nhà Trắng kêu gọi Israel lập tức điều tra sự việc. Quân đội Israel cho biết đang xác minh thông tin về vụ một phụ nữ nước ngoài "thiệt mạng do trúng đạn" ở Bờ Tây.Thổ Nhĩ Kỳ, quốc gia thành viên NATO, ủng hộ giải pháp hai nhà nước cho xung đột Israel - Palestine. Ông Erdogan nhiều lần chỉ trích Tel Aviv về chiến dịch tấn công Dải Gaza và cho rằng giới lãnh đạo Israel phải bị xét xử tại tòa án quốc tế.Chiến sự Israel - Hamas bùng phát sau cuộc đột kích của nhóm vũ trang vào miền nam Israel ngày 7/10/2023 gây thương vong lớn. Chiến dịch đáp trả của Israel vào Gaza đến ngày 8/9 đã khiến gần 41.000 người thiệt mạng, hầu hết là phụ nữ và trẻ em, và hơn 94.700 người bị thương.Như Tâm (Theo Reuters)</t>
+          <t>Trung tâm Dự báo Khí tượng Thủy văn quốc gia cho biết lúc 10h, tâm áp thấp nhiệt đới trên vùng biển phía đông khu vực Bắc Biển Đông, duy trì cấp 7 dù vừa ma sát với đảo, giật tăng hai cấp. Với tốc độ 20 km/h và theo hướng tây, đến 10h ngày mai nó sẽ mạnh lên thành bão với sức gió 74 km/h (cấp 8) khi cách quần đảo Hoàng Sa khoảng 320 km. Bão sau đó chếch xuống phía nam, tốc độ nhanh hơn (25 km/h), đến 10h ngày 19/9 khi ở phía tây quần đảo Hoàng Sa thì mạnh lên cấp 9, sức gió tối đa 88 km/h, giật tăng hai cấp. Trong 48 đến 72 giờ tiếp theo, bão có khả năng đổi hướng chếch lên bắc, tốc độ chậm hơn 10 km/h. Đài khí tượng Nhật Bản nhận định vào Biển Đông áp thấp nhiệt đới sẽ mạnh lên thành bão. Bão đi ngang theo hướng tây đến giữa Biển Đông rồi chếch lên phía bắc. Cơn bão không quá mạnh, sức gió gần tâm dao động 65-72 km/h.
+Dự báo đường đi và khu vực ảnh hưởng của áp thấp nhiệt đới lúc 10h ngày 17/9. Ảnh: NCHMF
+Ông Nguyễn Văn Hưởng, Trưởng phòng Dự báo thời tiết, Trung tâm Dự báo Khí tượng Thủy văn quốc gia, cho biết vị trí hình thành cơn áp thấp nhiệt đới mới gần giống bão Yagi. Tuy nhiên, do điều kiện môi trường không thuận lợi, phải chia sẻ năng lượng với bão Pulasan đang ở Tây Bắc Thái Bình Dương nên khi vào Biển Đông áp thấp nhiệt đới không mạnh ngay thành bão mà phải mất 1-2 ngày.Ngoài ra, do chịu ảnh hưởng của dòng dẫn đường quy mô lớn và khả năng chịu tác động của không khí lạnh vào cuối tuần, đường đi của áp thấp nhiệt đới sẽ phức tạp hơn so với bão Yagi.Theo ông Hưởng, áp thấp nhiệt đới sau khi mạnh lên thành bão có hai kịch bản di chuyển. Thứ nhất, nó sẽ đi thẳng vào Trung Trung Bộ. Thứ hai, bão sẽ đổi sang hướng tây tây bắc và khả năng ảnh hưởng tới Bắc Bộ, Bắc Trung Bộ.Do ảnh hưởng của áp thấp nhiệt đới, vùng biển phía đông khu vực Bắc Biển Đông có gió mạnh cấp 6-7, vùng gần tâm bão đi qua cấp 8, giật cấp 10, sóng biển cao 2-4 m; từ ngày 17/9 sóng biển cao 3-5 m. 
+Hàng loạt trụ điện ngã trên quốc lộ 18, TP Cẩm Phả, Quảng Ninh sau bão Yagi. Ảnh: Giang Huy
+10 ngày trước, bão Yagi đổ bộ Quảng Ninh với sức gió mạnh nhất cấp 14, các nơi khác cấp 12-13, giật cấp 17. Yagi hình thành từ áp thấp nhiệt đới ở phía đông của Philippines, sau đó vào Biển Đông, mạnh lên thành siêu bão chỉ trong 48 giờ. Vượt qua eo biển bán đảo Lôi Châu và Hải Nam (Trung Quốc) vào vịnh Bắc Bộ, sức gió chỉ giảm 1-2 cấp.Hoàn lưu sau bão Yagi kết hợp với dải hội tụ nhiệt đới có trục qua Bắc Bộ gây mưa lớn, lũ nhiều sông vượt kỷ lục tồn tại hơn 50 năm. Hơn 70.000 hộ dân ở Yên Bái, Lào Cai, Thái Nguyên, Bắc Giang, Bắc Ninh, Hà Nội bị ngập. Hiện nhiều vùng trũng ven sông Hồng, Thái Bình, sông Bùi, sông Tích nước vẫn ngập đến nóc nhà, dự kiến duy trì 7-9 ngày nếu thời tiết không xấu đi.Thống kê đến chiều 17/9, bão lũ đã làm 291 người chết, 38 người mất tích, 1.922 người bị thương. Thiệt hại vật chất khoảng 40.000 tỷ đồng khiến GDP năm nay thấp hơn 0,15% so với kịch bản trước đó.Từ đầu năm, Biển Đông đã có ba cơn bão. Cơ quan khí tượng dự báo mùa mưa bão năm nay có 9-11 cơn bão, áp thấp nhiệt đới trên Biển Đông, tập trung vào miền Trung từ nay đến tháng 11.
+Gia Chính</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Những sản phẩm dự kiến ra mắt tại sự kiện Apple Glowtime</t>
+          <t>Nhà dân ở TP HCM được xây tầng hầm trở lại</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-san-pham-du-kien-ra-mat-tai-su-kien-apple-glowtime-4790303.html</t>
+          <t>https://vnexpress.net/nha-dan-o-tp-hcm-duoc-xay-tang-ham-tro-lai-4793866.html</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ngoài bốn phiên bản iPhone 16, Apple nhiều khả năng sẽ công bố đồng hồ Watch series 10, tai nghe AirPods, iPad và máy Mac thế hệ mới.</t>
+          <t>Nhà thấp tầng, riêng lẻ ở TP HCM được xây một hầm làm bãi đậu xe, kỹ thuật, nếu muốn xây hai tầng trở lên cần lập quy hoạch chi tiết hoặc tổng mặt bằng.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sự kiện It's Glowtime của Apple sẽ bắt đầu lúc 10h ngày 9/9 (0h ngày 10/9, giờ Hà Nội) tại nhà hát Steve Jobs trong khuôn viên trụ sở Apple Park ở California (Mỹ).Trong thư mời, Apple thiết kế logo với các quầng sáng màu sắc xung quanh, khiến nhiều người liên tưởng đến bộ tính năng Apple Intelligence và biểu tượng trợ lý ảo Siri mới tích hợp trí tuệ nhân tạo.iPhone 16
-Ảnh dựng iPhone 16 Pro. Ảnh: MacRumors
-iPhone 16 là tâm điểm của sự kiện, với bốn phiên bản gồm iPhone 16, 16 Plus, 16 Pro và 16 Pro Max, trang bị nút chụp riêng với công nghệ cảm biến lực ở cạnh phải.iPhone 16 Pro dự kiến tăng kích cỡ màn hình từ 6,1 lên 6,3 inch, còn 16 Pro Max trang bị tấm nền 6,9 inch. Thay đổi này khiến sản phẩm dài hơn 3 mm và rộng hơn 1 mm so với dòng 15 Pro. Theo Ice Universe, sản phẩm cũng sẽ là smartphone có viền màn hình mỏng nhất thế giới. Máy tích hợp chip A18 Pro, nâng cấp mạnh camera, hỗ trợ kết nối Wi-Fi 7 và 5G Advance, đồng thời sử dụng hệ thống tản nhiệt với chất liệu graphene.iPhone 16 và 16 Plus cũng có một số thay đổi về thiết kế như thêm nút chụp hình điện dung ở cạnh phải, nút gạt chế độ âm thanh đổi thành nút Action. Cụm camera phía sau chuyển sang thiết kế dọc như trên iPhone X.Apple sẽ trang bị chip A18 sản xuất trên tiến trình 3 nm cho hai model tiêu chuẩn, RAM nâng lên 8 GB để hỗ trợ Apple Intelligence. Hãng cũng được cho là sẽ sử dụng công nghệ pin xếp chồng để nâng dung lượng và tuổi thọ pin cao hơn.iPad và iPad mini
-iPad Mini. Ảnh: Tuấn Hưng
-Apple có thể ra mắt iPad mới trong sự kiện này do lần nâng cấp gần nhất là vào 2 năm trước. iPad thế hệ mới dự kiến trang bị dòng chip A series mới hơn.Trong khi đó, iPad mini 6 đã ra mắt từ tháng 9/2021 nên model mới cũng có thể xuất hiện. Camera sau của máy có thể nâng lên 48 megapixel giống iPhone hiện tại.Apple Watch series 10
-Ảnh minh họa về Watch X. Ảnh: 9to5mac
-Smartwatch thế hệ mới của Apple có thể được gọi là Watch X với nâng cấp lớn nhằm kỷ niệm cột mốc 10 năm của dòng sản phẩm này. Máy sẽ được làm mỏng và lớn hơn với kích thước 45 và 49 mm.Apple được cho là sẽ thay đổi thiết kế kết nối gắn dây trên smartwatch thế hệ mới. Sản phẩm có thêm tính năng phát hiện ngưng thở khi ngủ và thông báo để người dùng sớm kiểm tra y tế. Tuy nhiên, tính năng đo nồng độ oxy trong máu vẫn không được trang bị trở lại do vụ kiện pháp lý với Masimo về bằng sáng chế.AirPods 4 và AirPods MaxApple đã công bố nhiều thay đổi về cách AirPods sẽ hoạt động trong iOS 18, nên khả năng cao sản phẩm mới sẽ có mặt trong sự kiện tới.Trong đó, AirPods 4 dự kiến có hai phiên bản, gồm một model giá rẻ với thiết kế mới và hộp sạc có cổng USB-C. Phiên bản thứ hai có giá cao hơn với tính năng ANC và Find My tích hợp trong hộp sạc. Ngoài ra, chất lượng âm thanh cũng tốt hơn thế hệ trước.AirPods Max ra mắt lần đầu vào tháng 12/2020 và chưa được nâng cấp sau 4 năm. Model thế hệ mới có thể chuyển sang dùng cổng kết nối USB-C tương tự các sản phẩm khác của Apple và nâng cấp chip xử lý H2 để cải thiện khả năng chống ồn và kéo dài thời lượng pin.Mac mini và iMacVới việc ra mắt chip xử lý M4 vào tháng 5, nhiều nguồn tin cho rằng Apple sẽ công bố bản nâng cấp của Mac mini và iMac vào ngày mai.Mac mini được cho là sẽ có thiết kế mới nhỏ gọn hơn phiên bản hiện tại, trang bị cả chip M4 và M4 Pro. Còn iMac cũng sử dụng chip M4, kích thước màn hình lên 32 inch so với 24 inch hiện tại.MacBook Pro
-MacBook Pro. Ảnh: Tuấn Hưng
-Với chu kỳ nâng cấp thường niên, nhiều khả năng hai model MacBook Pro 14 inch và MacBook Pro 16 inch sẽ xuất hiện trong sự kiện. Tuy nhiên, Macbook Pro mới sẽ không có nhiều thay đổi về thiết kế, chỉ nâng cấp phần cứng với chip M4 mới.
-Huy Đức</t>
+          <t>Nội dung nêu trong hai quyết định vừa được UBND TP HCM ban hành nhằm tháo gỡ ách tắc cấp phép xây dựng tầng hầm tại các dự án nhà ở riêng lẻ, thấp tầng trên địa bàn thành phố.Cùng với dự án nhà ở riêng lẻ, chung cư, các công trình dịch vụ, công cộng và trụ sở, công trình xây dựng trong các khu chế xuất, khu công nghiệp, khu công nghệ cao... cũng được xây tầng hầm nhưng phải phù hợp quy chuẩn, tiêu chuẩn xây dựng.
+Khu nhà phố tại phường Long Trường, TP Thủ Đức, tháng 11/2022. Ảnh: Quỳnh Trần
+Số tầng hầm và vị trí được xác định cụ thể trong đồ án quy hoạch chi tiết, bản vẽ xin phép xây dựng, thiết kế cơ sở, các quy chuẩn kỹ thuật quốc gia về quy hoạch xây dựng, tiêu chuẩn chuyên ngành, quy chế quản lý kiến trúc, thiết kế đô thị... Việc xây dựng ngầm phải đảm bảo các quy chuẩn, ranh giới, giấy phép xây dựng, đảm bảo an toàn cho cộng đồng, bản thân công trình và công trình lân cận...Trước đây, việc cấp phép xây công trình có tầng hầm chủ yếu căn cứ quy chuẩn quốc gia về quy hoạch, tiêu chuẩn thiết kế xây công trình có tầng hầm, Nghị định số 39. Tuy nhiên, hơn nửa năm qua, quận, huyện tại TP HCM không cấp phép cho công trình có tầng hầm. Nguyên nhân bắt nguồn từ việc Bộ Xây dựng "tuýt còi" hoạt động quản lý xây dựng nhà ở riêng lẻ có nhiều tầng, nhiều căn hộ trên địa bàn.Để tháo gỡ, Sở Quy hoạch - Kiến trúc đã đề nghị bổ sung nội dung quản lý xây dựng công trình có tầng hầm trong quy chế quản lý kiến trúc TP HCM và quản lý quy hoạch không gian ngầm cho các đồ án quy hoạch phân khu (1/2.000). Việc này nhằm làm cơ sở giải quyết cấp phép xây công trình có tầng hầm hoặc lập quy hoạch chi tiết xây dựng, quy hoạch tổng mặt bằng.Theo cơ quan này, nhu cầu xây dựng công trình nhà ở riêng lẻ có tầng hầm của người dân trên địa bàn rất lớn, đặc biệt là tại các quận trung tâm. Từ 2004 đến quý 1 năm nay, thành phố đã cấp giấy phép 1.600 công trình nhà ở riêng lẻ có tầng hầm.Lê Tuyết</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sa Pa dừng mọi hoạt động du lịch vì bão Yagi</t>
+          <t>Mưa suốt đêm, Phú Quốc có nơi ngập gần một mét</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/sa-pa-dung-moi-hoat-dong-du-lich-vi-bao-yagi-4790470.html</t>
+          <t>https://vnexpress.net/mua-suot-dem-phu-quoc-co-noi-ngap-gan-mot-met-4793816.html</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lào CaiSa Pa quyết định dừng mọi hoạt động tham quan, du lịch từ hôm nay, do nhiều nơi bị sạt lở trong mưa bão Yagi.</t>
+          <t>Kiên GiangNhiều đường trung tâm TP Phú Quốc ngập do mưa lớn liên tục, có nơi sâu gần một mét ảnh hưởng người dân, khách du lịch, sáng 17/9.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>UBND thị xã Sa Pa ngày 8/9 thông báo dừng các hoạt động du lịch ngoài trời; đón khách tham quan tại các điểm di tích, danh thắng trên địa bàn đến khi có thông báo mới. Do ảnh hưởng của bão Yagi, hiện nhiều tuyến đường và các đập tràn ở Sa Pa bị hư hỏng, không đảm bảo an toàn giao thông.
-Khu vực cầu 32, cửa ngõ vào Sa Pa, ngày 8/9. Ảnh: NVCC
-Ông Nguyễn Trung Kiên, đại diện khu du lịch Cát Cát, cho biết mưa lớn từ 7/9 làm đường DH92 từ thị xã xuống khu du lịch sạt lở nghiêm trọng. Đơn vị đã dừng các hoạt động tại đây vào sáng 8/9.Theo ông Kiên, bản Cát Cát vẫn an toàn nhưng lượng nước tại các suối hồ có khả năng dâng cao từ đêm nay. Đại diện UBND xã Tả Van nói đơn vị đang khắc phục các điểm sạt lở. Hiện tại, giao thông bên trong xã vẫn ổn, một số cơ sở homestay vẫn còn khách lưu trú.Nhiều du khách đã hủy dịch vụ du lịch ở Sa Pa từ 5/9 sau khi nghe thông tin về bão. Chị Phạm Thùy Giang, chủ homestay PaVi, cho biết cơ sở của mình và các khu lưu trú lân cận hầu như không có du khách. Đối với những khách đã đặt tour trước đó, homestay cũng chủ động dời ngày để khách có trải nghiệm an toàn hơn khi đến Sa Pa.
-Sạt lở ở đường vào bản Cát Cát
-Sạt lở ở đường vào bản Cát Cát ngày 8/9. Ảnh: Ban quản lý bản Cát Cát
-Nhà xe Interbuslines ghi nhận lượng hủy dịch vụ xe đưa đón từ Hà Nội lên Sa Pa gần 100% trong ngày 7/9. Trong ngày 8/9, hầu hết khách Việt đặt chỗ đều đã hủy vé hoặc báo dời ngày. Hai xe 30 chỗ từ Hà Nội lên Sa Pa chủ yếu chở khách nước ngoài đã mua tour từ trước. Đường đi có một số đoạn sạt lở, phải dừng khoảng 30 phút nhưng không gặp vấn đề lớn.Một số đơn vị lữ hành cho biết đã dừng tất cả hoạt động du lịch từ 5/9 khi được dự báo thời tiết xấu. Theo Bà Mai Thanh Hoa, Giám đốc Công ty Du lịch Tinh thần Cộng đồng, khách du lịch nước ngoài gặp hạn chế về việc tiếp cận thông tin nên đơn vị du lịch cần chủ động thông báo, đặt an toàn lên hàng đầu.Tú Nguyễn - Tuấn Anh</t>
+          <t>Chị Xuân, nhà ở đường Trần Phú, phường Dương Đông, cho biết từ tối qua xuất hiện mưa lớn kéo dài 7-8 giờ khiến nước ở khu vực lên nhanh. Nhiều tuyến đường trung tâm thành phố đều ngập sâu như: Nguyễn Trung Trực, Cách Mạng Tháng 8, Trần Hưng Đạo...
+Phú Quốc ngập
+Nước ngập sâu ở một số nhà người dân tại phường Dương Đông. Video: Người dân cung cấp
+Khu phố chỗ chị Xuân ở nhiều nơi ngập hơn nửa mét, cá biệt một số chỗ ngập khoảng một mét. Trong đêm người dân phải chạy đua di dời đồ đạc. Sáng nay, mưa giảm nhưng nước vẫn chưa rút.Đường ngập vào sáng sớm khiến đi lại của người dân và học sinh đến trường gặp khó khăn, phải bì bõm trong nước. Ông Nguyễn Văn Thế, nhà ở khu phố 10, phường Dương Đông, cho biết các tuyến đường quanh nhà đã "thất thủ" từ sáng nay và không có dấu hiệu nước rút vì mưa đang tiếp diễn.
+Mưa ngập ôtô ở khu vực đường Cách Mạng Tháng 8, phường Dương Đông. Ảnh: Người dân cung cấp
+Chính quyền Phú Quốc đã điều lực lượng quân đội, công an, dân quân tới hỗ trợ di dời người và tài sản ở một số khu vực nước lớn.Theo đài khí tượng thủy văn Kiên Giang, từ tối qua đến sáng nay TP Phú Quốc mưa rất to, nhất là khu vực Dương Đông, Cửa Cạn. Dự báo mưa còn kéo dài trong hôm nay với lượng nước từ 5-10 mm/h, có nơi lên 20 mm/h; vùng biển Kiên Giang mưa gió giật cấp 7-8, sóng cao 1,5-3 m.Hai hôm trước, tàu cao tốc từ đất liền đi Phú Quốc, đảo Nam Du ngưng chạy do thời tiết xấu, hiện chưa hoạt động lại.
+Trên đường Cách Mạng Tháng 8, người dân chế bè để chuyển đồ đạc. Ảnh: Người dân cung cấp
+Phú Quốc là thành phố thu hút nhiều du khách. Những năm qua địa phương có tốc độ đô thị hóa nhanh, nhiều nhà cửa, công trình lớn được xây dựng thu hẹp ao hồ, sông suối, hệ thống thoát nước. Do đó thành phố thường bị ngập cục bộ khi mưa lớn, ảnh hưởng đời sống người dân, kinh tế và du lịch.Tại huyện Bù Gia Mập, tỉnh Bình Phước, đêm 16 rạng sáng 17/9 có mưa lớn khiến nhiều con suối dâng cao. Nước từ thượng nguồn đổ về gây ngập các khu dân cư, nhiều tuyến đường, khiến giao thông bị chia cắt.
+Mực nước dâng cao ở cầu Đăk Ơ trên quốc lộ 14C. Ảnh: Văn Trăm
+Trên quốc lộ 14C nối Đông Nam Bộ với các tỉnh Tây Nguyên, cầu Đăk Ơ đoạn giáp ranh xã Đắk Ơ và xã Bù Gia Mập ngập khoảng một m. Lực lượng chức năng phải chốt chặn ngăn xe qua cầu, đồng thời hướng dẫn người dân đi đường vòng, đường tránh để đảm bảo an toàn.Mưa lũ cũng khiến nhiều cầu, đường liên xã Đăk Ơ, Bù Gia Mập... của huyện bị sạt lở, gây nguy hiểm cho người đi đường. Theo Ban Chỉ huy phòng chống thiên tai và tìm kiếm cứu nạn huyện Bù Gia Mập, hiện nhiều hộ dân nằm trong vùng bị ngập đã được sơ tán đến khu vực an toàn.Ngọc Tài - Văn Trăm</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Bộ đội, công an giúp dân khắc phục hậu quả bão Yagi</t>
+          <t>Đề xuất nghỉ Tết Ất Tỵ 9 ngày</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bo-doi-cong-an-giup-dan-khac-phuc-hau-qua-bao-yagi-4790269.html</t>
+          <t>https://vnexpress.net/de-xuat-nghi-tet-at-ty-9-ngay-4793734.html</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bộ đội giúp dân sơ tán đến nơi an toàn, xử lý cổ thụ gãy đổ và cùng người dân dọn dẹp phố phường, khôi phục cuộc sống bình thường sau bão.</t>
+          <t>Bộ Lao động Thương binh và Xã hội đề xuất nghỉ Tết Âm lịch từ 26 tháng chạp đến hết mùng 5 tháng giêng (25/1-2/2/2025), gồm 5 ngày nghỉ chính thức, 4 ngày nghỉ cuối tuần.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ảnh hưởng của bão Yagi, Lạng Sơn mưa lớn, một số khu vực ở huyện Bắc Sơn, Chi Lăng bị ngập. Bộ đội Biên phòng và Cảnh sát cứu hộ cứu nạn đã hỗ trợ sơ tán người dân và tài sản đến nơi an toàn từ chiều 7/9. 
-Ảnh hưởng của bão Yagi, Lạng Sơn mưa lớn, một số khu vực ở huyện Bắc Sơn, Chi Lăng bị ngập. Bộ đội Biên phòng và Cảnh sát cứu hộ cứu nạn đã hỗ trợ sơ tán người dân và tài sản đến nơi an toàn từ chiều 7/9. 
-Chiến sĩ Biên phòng cõng cụ ông tới nơi tránh trú mưa bão. Bộ đội Biên phòng Lạng Sơn cho biết hơn 150 lượt cán bộ, chiến sĩ của đơn vị đã giúp 18 hộ gia đình sơ tán và di dời tài sản gồm tivi, tủ lạnh, thóc lúa đến nơi an toàn. Bộ đội cũng giúp hơn 35 hộ dân chằng néo nhà cửa phòng chống mưa, bão; di dời cây đổ ảnh hưởng đến giao thông; bố trí người canh gác tại các điểm nguy hiểm có nguy cơ sạt lở. 
-Chiến sĩ Biên phòng cõng cụ ông tới nơi tránh trú mưa bão. Bộ đội Biên phòng Lạng Sơn cho biết hơn 150 lượt cán bộ, chiến sĩ của đơn vị đã giúp 18 hộ gia đình sơ tán và di dời tài sản gồm tivi, tủ lạnh, thóc lúa đến nơi an toàn. Bộ đội cũng giúp hơn 35 hộ dân chằng néo nhà cửa phòng chống mưa, bão; di dời cây đổ ảnh hưởng đến giao thông; bố trí người canh gác tại các điểm nguy hiểm có nguy cơ sạt lở. 
-Hàng chục cán bộ, chiến sĩ cũng được huy động xuống đồng giúp người dân gặt lúa chạy bão. 
-Hàng chục cán bộ, chiến sĩ cũng được huy động xuống đồng giúp người dân gặt lúa chạy bão. 
-Tại Hà Nội, Cảnh sát phòng cháy chữa cháy và cứu hộ cứu nạn tham gia xử lý, dọn dẹp nhiều cổ thụ gãy đổ. Số lượng cây gãy đổ của Hà Nội rất lớn, khoảng 17.000 nên cần nhiều người, nhiều thời gian thu dọn. 
-Tại Hà Nội, Cảnh sát phòng cháy chữa cháy và cứu hộ cứu nạn tham gia xử lý, dọn dẹp nhiều cổ thụ gãy đổ. Số lượng cây gãy đổ của Hà Nội rất lớn, khoảng 17.000 nên cần nhiều người, nhiều thời gian thu dọn. 
-Nhiều xe chuyên dụng được điều đến hiện trường. Thống kê sơ bộ đến sáng 8/9, Cảnh sát Phòng cháy chữa cháy và Cứu hộ cứu nạn Công an TP Hà Nội và công an quận, huyện, thị xã đã điều gần 300 lượt phương tiện cùng gần 2.000 cán bộ, chiến sĩ phối hợp cứu nạn, cứu hộ góp phần giảm thiểu thiệt hại do mưa bão. 
-Nhiều xe chuyên dụng được điều đến hiện trường. Thống kê sơ bộ đến sáng 8/9, Cảnh sát Phòng cháy chữa cháy và Cứu hộ cứu nạn Công an TP Hà Nội và công an quận, huyện, thị xã đã điều gần 300 lượt phương tiện cùng gần 2.000 cán bộ, chiến sĩ phối hợp cứu nạn, cứu hộ góp phần giảm thiểu thiệt hại do mưa bão. 
-Nhân viên Công ty Công viên cây xanh Hà Nội tất bật dọn dẹp khu vực công viên Lênin, đường Trần Phú do nhiều cây gãy đổ.
-Tối 7/9, tâm bão Yagi quét qua Thủ đô gây mưa to, gió mạnh suốt 7 tiếng. Gió bão giật cấp 10 khiến cây đổ la liệt khắp thành phố. 
-Nhân viên Công ty Công viên cây xanh Hà Nội tất bật dọn dẹp khu vực công viên Lênin, đường Trần Phú do nhiều cây gãy đổ.
-Tối 7/9, tâm bão Yagi quét qua Thủ đô gây mưa to, gió mạnh suốt 7 tiếng. Gió bão giật cấp 10 khiến cây đổ la liệt khắp thành phố. 
-Hàng trăm bộ đội công an dọn cây cối đổ trên đường Hoàng Quốc Việt
-Bộ đội, công an dọn cây đổ trên đường Hoàng Quốc Việt, quận Cầu Giấy, Hà Nội. Video: Lộc Chung 
-Tại Quảng Ninh, gió bão trưa 7/9 khiến xe tải chở hàng đang đỗ trên đường bêtông trong khu dân cư ở phường Cẩm Sơn, TP Cẩm Phả bị lật nghiêng. Sau khi bão tan, 16 người hợp sức dùng dây cáp giúp tài xế kéo ôtô đứng dậy. 
-Tại Quảng Ninh, gió bão trưa 7/9 khiến xe tải chở hàng đang đỗ trên đường bêtông trong khu dân cư ở phường Cẩm Sơn, TP Cẩm Phả bị lật nghiêng. Sau khi bão tan, 16 người hợp sức dùng dây cáp giúp tài xế kéo ôtô đứng dậy. 
-Hai người đàn ông lợp tạm mái nhà bằng bạt để phòng mưa ở TP Cẩm Phả. Do ảnh hưởng của bão Yagi, từ chiều đến tối hôm qua, tỉnh Quảng Ninh có gió bão cấp 12-13, giật cấp 17 và mưa 100-250 mm. Theo báo cáo của UBND tỉnh Quảng Ninh, toàn tỉnh có 2.083 nhà bị tốc mái, 254 cột điện bị gãy đổ. Một số nhà dân bị cột điện gãy đè trúng, hư hại. 
-Hai người đàn ông lợp tạm mái nhà bằng bạt để phòng mưa ở TP Cẩm Phả. Do ảnh hưởng của bão Yagi, từ chiều đến tối hôm qua, tỉnh Quảng Ninh có gió bão cấp 12-13, giật cấp 17 và mưa 100-250 mm. Theo báo cáo của UBND tỉnh Quảng Ninh, toàn tỉnh có 2.083 nhà bị tốc mái, 254 cột điện bị gãy đổ. Một số nhà dân bị cột điện gãy đè trúng, hư hại. 
-Chị Nguyễn Thị Chi ở phường Quang Anh, TP Cẩm Phả thu gom những vật dụng còn sót lại sau bão, sáng 8/9. Tầng 1 là quán phở bò, tầng 2 là nơi ở của 5 người trong gia đình, đã bị gió thổi bay toàn bộ mái tôn. "Chỉ trong hơn một phút, mái nhà bị cuốn bay, cả gia đình sợ hãi kéo nhau trốn trong nhà vệ sinh", chị kể, cho biết vợ chồng và 3 đứa con nhỏ phải khăn gói sang nhà người thân ở nhờ. 
-Chị Nguyễn Thị Chi ở phường Quang Anh, TP Cẩm Phả thu gom những vật dụng còn sót lại sau bão, sáng 8/9. Tầng 1 là quán phở bò, tầng 2 là nơi ở của 5 người trong gia đình, đã bị gió thổi bay toàn bộ mái tôn. "Chỉ trong hơn một phút, mái nhà bị cuốn bay, cả gia đình sợ hãi kéo nhau trốn trong nhà vệ sinh", chị kể, cho biết vợ chồng và 3 đứa con nhỏ phải khăn gói sang nhà người thân ở nhờ. 
-Chị Đỗ Thị Nhung 35 tuổi, ở xã Vũ Oai, TP Hạ Long, dọn dẹp nhà sau khi bị bão đánh sập trần. 
-Chị Đỗ Thị Nhung 35 tuổi, ở xã Vũ Oai, TP Hạ Long, dọn dẹp nhà sau khi bị bão đánh sập trần. 
-Tại thị trấn Cái Rồng, huyện Vân Đồn, từ chiều 7/9, ngay khi trời ngớt mưa, bớt gió, nhà chức trách huy động người và phương tiện cắt tỉa, giải phóng những cây bị đổ để tránh cản trở giao thông.
-Khắp các ngả đường ở thị trấn Cái Rồng, xã Hạ Long và nhiều khu vực khác của huyện Vân Đồn tan hoang trong bão. Nhiều biển quảng cáo, cột đèn, biển báo giao thông gãy gập. Hàng trăm mái tôn bị gió thổi bay văng xa hàng trăm mét. 
-Tại thị trấn Cái Rồng, huyện Vân Đồn, từ chiều 7/9, ngay khi trời ngớt mưa, bớt gió, nhà chức trách huy động người và phương tiện cắt tỉa, giải phóng những cây bị đổ để tránh cản trở giao thông.
-Khắp các ngả đường ở thị trấn Cái Rồng, xã Hạ Long và nhiều khu vực khác của huyện Vân Đồn tan hoang trong bão. Nhiều biển quảng cáo, cột đèn, biển báo giao thông gãy gập. Hàng trăm mái tôn bị gió thổi bay văng xa hàng trăm mét. 
-Những tấm tôn bị bay xuống đường được người dân thị trấn Cái Rồng thu gom, tập kết một chỗ.
-Bão Yagi quét qua nhiều tỉnh thành như Quảng Ninh, Hải Phòng, Thái Bình, Hải Dương, Hà Nội... làm 14 người chết, trong đó Hà Nội 3 người, 176 người khác bị thương. 
-Những tấm tôn bị bay xuống đường được người dân thị trấn Cái Rồng thu gom, tập kết một chỗ.
-Bão Yagi quét qua nhiều tỉnh thành như Quảng Ninh, Hải Phòng, Thái Bình, Hải Dương, Hà Nội... làm 14 người chết, trong đó Hà Nội 3 người, 176 người khác bị thương. 
-Giang Huy - Phạm Dự - Duy Anh - Phạm Chiểu</t>
+          <t>Bộ Lao động Thương binh và Xã hội vừa gửi văn bản xin ý kiến 16 cơ quan, bộ ngành về phương án nghỉ Tết Âm lịch 2025 trước khi trình Thủ tướng quyết định. Cơ quan này đề xuất nghỉ hai ngày trước và ba ngày sau Tết, từ 26 tháng chạp năm Giáp Thìn đến hết mùng 5 tháng giêng Ất Tỵ, tức từ thứ bảy ngày 25/1 đến hết chủ nhật 2/2/2025.Nếu phương án được thông qua, công chức, lao động cả nước sẽ nghỉ lễ kéo dài 9 ngày gồm 5 ngày nghỉ chính thức và 4 ngày nghỉ cuối tuần của hai tuần liên tiếp.
+Người dân Tứ Liên (Hà Nội) chăm sóc quất bán dịp Tết năm 2019. Ảnh: Giang Huy
+Dịp Quốc khánh năm 2025, Bộ Lao động Thương binh và Xã hội đề xuất hai phương án. Thứ nhất, nghỉ hai ngày gồm Quốc khánh 2/9 và một ngày liền kề trước. Công chức, lao động sẽ nghỉ từ thứ bảy 30/8/2025 đến hết thứ ba 2/9/2025. Kỳ nghỉ dài bốn ngày gồm hai ngày nghỉ chính thức và hai ngày nghỉ hàng tuần. Phương án hai là nghỉ hai ngày thứ ba và thứ tư 2-3/9/2025.Cơ quan soạn thảo chọn phương án một, nghỉ bốn ngày để kỳ lễ liên tục, kéo dài, giúp người lao động có thời gian tái tạo sức, kích cầu du lịch, thúc đẩy tăng trưởng kinh tế.
+Lịch nghỉ Tết Âm lịch theo đề xuất của Bộ Lao động Thương binh và Xã hội. Đồ họa: Đăng Hiếu
+Việc xin ý kiến các bộ ngành về phương án nghỉ Tết, Quốc khánh nhằm thực hiện theo luật. Bộ luật Lao động năm 2019 bổ sung quy định hàng năm căn cứ vào điều kiện thực tế, Thủ tướng quyết định cụ thể ngày nghỉ Tết Âm lịch và ngày Quốc khánh. Nếu ngày nghỉ chính thức trùng với ngày nghỉ hàng tuần sẽ áp dụng nguyên tắc liền kề hoặc hoán đổi để người dân có kỳ nghỉ kéo dài.Việt Nam có tổng cộng 11 ngày nghỉ lễ chính thức trong năm, gồm Tết Dương lịch một ngày, Tết Âm lịch 5 ngày, giỗ Tổ Hùng Vương một ngày, dịp 30/4-1/5 nghỉ hai ngày và Quốc khánh hai ngày.Từ năm 2021, cả nước có thêm một ngày nghỉ lễ dịp Quốc khánh, tùy từng năm mà Chính phủ chọn nghỉ vào 1/9 hoặc 3/9. Người nước ngoài làm việc tại Việt Nam được nghỉ thêm một ngày Tết cổ truyền và ngày Quốc khánh của nước họ.Hồng Chiêu</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Người dân xếp hàng mua xăng tại Quảng Ninh</t>
+          <t>Trạm BOT ở cửa ngõ TP HCM ùn ứ ngày đầu thu phí</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-dan-xep-hang-mua-xang-tai-quang-ninh-4790434.html</t>
+          <t>https://vnexpress.net/tram-bot-o-cua-ngo-tp-hcm-un-u-ngay-dau-thu-phi-4793821.html</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Nhiều cây xăng tại các địa phương bị ảnh hưởng do siêu bão Yagi, có nơi người dân phải xếp hàng, chờ gần 30 phút để mua nhiên liệu.</t>
+          <t>Nhiều tài xế chưa quen, trong khi một số người không đồng tình, dừng xe phản ứng khiến trạm BOT Phú Hữu, TP Thủ Đức, ùn ứ trong ngày đầu thu phí.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sáng 8/9, hàng trăm người dân mang chai nhựa, can, đứng xếp hàng dài ở cửa hàng 125 - Petrolimex ở phường Hà Tu, thành phố Hạ Long để mua xăng dầu. Sau một ngày bị cắt điện toàn thành phố do bão Yagi, các cây xăng cũng tạm dừng hoạt động để đảm bảo an toàn.
-Anh Hoàng Quang Huy, trú thành phố Hạ Long, cho biết xếp hàng gần 30 phút để mua 10 lít dầu về chạy máy phát điện và 5 lít xăng để đổ cho 3 xe máy của gia đình.
-Người dân xếp hàng chờ mua tại một cây xăng ở Hà Tu, Hạ Long, Quảng Ninh, sáng 8/9. Ảnh: Phạm Dự
-Theo một đại diện của Petrolimex, nhiều cửa hàng xăng dầu trên địa bàn Quảng Ninh chưa khắc phục sau bão, trong khi nhu cầu tăng. Do đó, tại các cửa hàng được mở cửa lại, lượng khách vào đông, nhiều thời điểm có thể phải xếp hàng. Tuy nhiên, ông cho biết hiện chỉ còn một số cây xăng bị thiệt hại nặng, dự kiến được khắc phục để hoạt động trở lại vào ngày mai.Báo cáo của các đơn vị chức năng tại cuộc họp của Bộ Công Thương sáng nay cũng ghi nhận nhiều cơ sở kinh doanh xăng dầu bị thiệt hại do siêu bão Yagi. Trong đó, Công ty Xăng dầu B12 (đầu mối cung cấp xăng dầu lớn nhất miền Bắc, thuộc Petrolimex) bị sạt lở 100 m bờ kè và chìm 2 tàu kéo phao khi đang neo đậu tại kho cảng. Các kho xăng dầu Cái Lân (Quảng Ninh), An Hải và Đình Vũ (Hải Phòng) cũng bị ảnh hưởng.
-Video xếp hàng mua xăng chạy máy phát Hạ Long
-Người dân xếp hàng chờ mua xăng tại Quảng Ninh, sáng 8/9. Video: Huy Mạnh
-Tại Hải Phòng và Quảng Ninh, nhiều cửa hàng xăng dầu bị tốc mái. Tình trạng mất điện diện rộng, không có kết nối Internet cũng ảnh hưởng tới các cơ sở bán hàng tự động và kết nối dữ liệu hóa đơn điện tử.Tại Bắc Giang, sáng nay các cửa hàng kinh doanh xăng dầu vẫn mở cửa bán. Hệ thống cửa hàng trên địa bàn tỉnh chưa ghi nhận thêm thiệt hại đáng kể nào. Dự kiến, hoạt động cung ứng xăng dầu diễn ra bình thường.Tại Hà Nội, báo cáo nhanh của Sở Công Thương cập nhật đến 9h cho thấy, thành phố không có thiệt hại về người và các trang thiết bị phục vụ bán hàng tại các cửa hàng xăng dầu. Đa số các cửa hàng bị hư hại như bong tróc hệ thống quảng cáo, rơi biển hiệu, vỡ cửa kính, tốc mái, đứt, chập dây điện, cây đổ gần vị trí cửa hàng. Sáng sớm, các doanh nghiệp đã dọn dẹp, khắc phục hậu quả. Hiện, cơ bản các cửa hàng hoạt động bình thường.Chỉ một số cây xăng tạm dừng do sự cố mất điện lưới, chờ cơ quan điện khắc phục, xử lý sự cố đứt đường dây, dọn dẹp cây đổ... Một số cửa hàng chỉ thanh toán được bằng tiền mặt do mất tín hiệu viễn thông.Vụ Thị trường trong nước (Bộ Công thương) đề nghị EVN, EVNNPC ưu tiên cấp điện cho xăng dầu, các hệ thống cung cấp hàng hóa thiết yếu, nhất là khắc phục điện cho khu vực B12 để bơm xăng dầu với khu vực 1 và miền Bắc.Tại cuộc họp sáng nay, Bộ trưởng Công Thương Nguyễn Hồng Diên cũng đề nghị chính quyền địa phương phối hợp với các bộ ngành chỉ đạo thương nhân đầu mối, phân phối bảo đảm duy trì nguồn cung xăng dầu trong mọi tình huống. Bộ Thông tin và Truyền thông khắc phục, khôi phục cung cấp dịch vụ viễn thông, mạng Internet để phục vụ hoạt động cung cấp điện, xăng dầu...Phạm Dự - Phương Dung</t>
+          <t>Từ 0h ngày 17/9, trạm BOT Phú Hữu bắt đầu thu phí hoàn vốn cho dự án đường nối Nguyễn Duy Trinh vào Khu công nghiệp Phú Hữu. Trạm đặt trên đường Nguyễn Thị Tư, mỗi chiều gồm hai làn thu phí tự động và một làn hỗn hợp.Phương án thu cùng mức phí (vé lượt thấp nhất 14.000 đồng, cao nhất 110.000 đồng, áp dụng đến cuối năm nay) đã được Công ty cổ phần Xi măng Vicem Hà Tiên (nhà đầu tư) công bố trước đó, song sáng nay nhiều tài xế ôtô chưa quen, bất ngờ khi tài khoản giao thông bị trừ tiền khi qua làn tự động.
+Xe chạy qua trạm BOT Phú Hữu sáng 17/9. Ảnh: Gia Minh
+Trong khi đó, một số người không đồng tình việc thu phí xe vào khu dân cư gần đó với lý do nhà họ chỉ cách trạm vài trăm mét. Mặt khác, nhiều phụ huynh phải đưa đón con đến trường mỗi ngày dẫn đến rất tốn kém khi bị thu phí. Vì vậy, họ dừng xe phản ứng khiến đường Nguyễn Thị Tư ùn ứ cục bộ.CSGT, Công an TP Thủ Đức sau đó có mặt xử lý, phân luồng tránh ùn tắc. Nhà đầu tư cũng đã huy động nhân viên phối hợp các đơn vị chức năng hướng dẫn xe qua lại và giải thích cho những trường hợp chưa đồng thuận thu phí.
+Xe ùn ứ cục bộ trước trạm BOT Phú Hữu, sáng 17/9. Ảnh: Hạ Giang
+Một lãnh đạo Sở Giao thông Vận tải TP HCM cho biết hôm nay là ngày đầu BOT Phú Hữu thu phí nên khó tránh khỏi việc tài xế chưa quen hoặc xảy ra phát sinh. Sở đã giao Trung tâm Quản lý hạ tầng giao thông đường bộ phối hợp các bên liên quan làm việc, giải quyết các bất cập nhằm đảm bảo hài hòa lợi ích giữa người dân và nhà đầu tư.Dự án đường nối Nguyễn Duy Trinh vào Khu Công nghiệp Phú Hữu được TP HCM ký hợp đồng với nhà đầu tư thực hiện theo hình thức BOT (xây dựng - kinh doanh - chuyển giao) vào năm 2012. Công trình có tổng mức đầu tư khoảng 461 tỷ đồng với quy mô xây tuyến đường dài khoảng 2,6 km, rộng 30 m.
+Vị trí trạm BOT Phú Hữu ở TP Thủ Đức. Đồ họa: Đăng Hiếu
+Theo phương án thu phí được nhà đầu tư công bố, trạm miễn, giảm cho một số nhóm gồm xe máy, ôtô chuyên dùng như cứu thương, cứu hỏa, xe cảnh sát... Ngoài ra, ôtô dưới 12 chỗ không kinh doanh, có hộ khẩu thường trú hoặc tạm trú trên 6 tháng khu vực các đường Nguyễn Thị Tư, Đặng Thanh Hiếu được miễn phí qua trạm.Từ 1/1/2025 đến 16/9/2025 xe qua trạm sẽ đóng phí cao hơn. Trong đó, vé lượt áp dụng 15.000-120.000 đồng. Vé tháng từ 450.000 đồng đến 3,6 triệu đồng. Vé quý từ 1.215.000 đồng đến 9.720.000 đồng. Tiếp đến, mức phí qua trạm tiếp tục điều chỉnh với giá vé lượt thấp nhất 17.000 đồng, cao nhất 133.000 đồng. Vé tháng 510.000 đồng đến gần 4 triệu đồng; vé quý từ 1.377.000 đồng tới 10.773.000 đồng.
+Mức phí áp dụng tại trạm Phú Hữu từ ngày 17/9 đến 31/12/2024
+STT
+Loại xe
+Mức giá
+Vé lượt
+Vé tháng
+Vé quý
+1
+Ôtô dưới 12 chỗ; ôtô tải trọng dưới 2 tấn, xe buýt
+14.000
+420.000
+1.134.000
+2
+Ôtô 12-30 chỗ; ôtô tải trọng 2-4 tấn
+21.000
+630.000
+1.701.000
+3
+Ôtô trên 31 chỗ; ôtô tải trọng 4-10 tấn
+30.000
+900.000
+2.430.000
+4
+Ôtô tải tải trọng 10-18 tấn; container 20 feet
+54.000
+1.620.000
+4.374.000
+5
+Ôtô tải tải trọng trên 18 tấn; container 40 feet
+110.000
+3.300.000
+8.910.000
+TP HCM đã triển khai 7 dự án BOT, gồm cầu đường Bình Triệu 2 (giai đoạn một) đã kết thúc thu phí hoàn vốn. Ngoài BOT Phú Hữu, ba dự án khác đang thu phí, gồm BOT An Sương - An Lạc, cầu Phú Mỹ, mở rộng xa lộ Hà Nội và quốc lộ 1. Ngoài ra, tại thành phố còn hai dự án khác đang làm thủ tục dừng hợp đồng, gồm: đường nối Võ Văn Kiệt đến cao tốc TP HCM - Trung Lương và cầu đường Bình Triệu 2 (giai đoạn hai).Gia Minh</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tháo dỡ bãi nuôi hàu trái phép trên sông Rác</t>
+          <t>Đất đấu giá huyện Phúc Thọ lên 75 triệu đồng một m2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thao-do-bai-nuoi-hau-trai-phep-tren-song-rac-4790455.html</t>
+          <t>https://vnexpress.net/dat-dau-gia-huyen-phuc-tho-len-75-trieu-dong-mot-m2-4793727.html</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hà TĩnhChính quyền huy động hơn 150 lượt người tháo dỡ hàng nghìn cọc bêtông, cọc tre, lốp xe dùng để nuôi hàu trên sông Rác ở huyện Cẩm Xuyên.</t>
+          <t>Hà NộiĐất đấu giá xã Trạch Mỹ Lộc, Phúc Thọ tiếp tục lên 75 triệu đồng một m2, trong khi hơn nửa tháng trước mới chỉ gần 60 triệu một m2.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ngày 8/9, lãnh đạo huyện Cẩm Xuyên cho biết cuối tháng 8 và đầu tháng 9 đã thành lập các đoàn liên ngành kiểm tra, rà soát, thống kê được 78 hộ dân tự ý nuôi trồng thủy sản trái phép trên sông Rác đoạn qua xã Cẩm Lĩnh và bãi bồi cửa biển. Nhà chức trách đã làm việc với các chủ bãi hàu, tuyên truyền vận động họ tháo dỡ, trả lại hiện trạng ban đầu cho sông, nhưng đa số không chấp hành.
-Nhiều lực lượng tháo dỡ bãi nuôi hàu trái phép trên sông Rác hồi cuối tháng 8. Ảnh: Hùng Lê
-Những ngày sau đó, xã Cẩm Lĩnh đã huy động 150 lượt người gồm cán bộ xã, thôn xóm, dân quân, đoàn thanh niên... xuống sông Rác tháo dỡ được hơn 2.000 cọc bêtông, cọc tre, dây néo trên diện tích 5 ha, lập biên bản xử lý 7 hộ.Lãnh đạo xã Cẩm Lĩnh cho hay việc tháo dỡ được tập trung vào các vị trí quan trọng, ảnh hưởng đến cảnh quan, dòng chảy tiêu thoát lũ, cản trở giao thông đường thủy... Quá trình làm việc gặp nhiều khó khăn do khối lượng cọc bêtông và các vật liệu khác lớn, cắm sâu dưới đáy sông nên không thể sử dụng sức người thu gom hết, huy động máy móc cũng tốn kém."Nhiều vị trí liên quan đến việc cho thuê đất trái thẩm quyền kéo dài hàng chục năm nay chưa giải quyết xong, người dân vẫn đầu tư nuôi thủy sản, vì thế gây khó khăn cho quá trình xử lý", lãnh đạo nói.
-Cọc bêtông, lốp xe dày đặc trên sông Rác đoạn tiếp giáp với cầu Cửa Nhượng, huyện Cẩm Xuyên hồi giữa tháng 8. Ảnh: Đức Hùng
-Thời gian tới, nhà chức trách huyện Cẩm Xuyên tiếp tục huy động lực lượng tháo dỡ các bãi nuôi hàu trái phép trên sông Rác, tuyên truyền người dân nuôi đúng quy hoạch, không ảnh hưởng đến dòng chảy, môi trường, cảnh quan.Sông Rác dài 35-40 km, chảy qua hai huyện Kỳ Anh và Cẩm Xuyên. Tại đoạn hai km qua xã Cẩm Lĩnh và Cẩm Trung, huyện Cẩm Xuyên, người dân cắm hàng nghìn trụ bêtông và cọc tre xuống đáy, cố định dây thừng và lốp xe để làm giá nuôi hàu khi chưa được chính quyền cho phép thuê đất, thuê mặt nước.
-Hiện trạng các bãi nuôi hàu trái phép ở huyện Cẩm Xuyên
-Bãi nuôi hàu trái phép ở huyện Cẩm Xuyên hồi giữa tháng 8. Video: Đức Hùng
-Theo thống kê, dọc bờ sông Rác đoạn qua huyện Cẩm Xuyên có gần 30 ha mặt nước bị người dân chiếm dụng để nuôi hàu tự phát. Tình trạng này xảy ra từ nhiều năm, lực lượng chức năng đã tới gặp các hộ dân tuyên truyền tháo dỡ, nhưng chưa thể chấm dứt.Theo các chủ bãi hàu, trước đây chính quyền cho họ thuê mặt nước để nuôi trồng thủy sản trên sông Rác, nhưng sau đó chấm dứt hợp đồng. Nhiều năm qua, vì "tiếc tiền" đã bỏ ra đầu tư, nhiều gia đình vẫn cố làm dù biết là không đúng.
-Đức Hùng</t>
+          <t>Trung tâm Phát triển quỹ đất huyện Phúc Thọ tổ chức bán đấu giá 13 thửa đất tại khu Dộc Tranh, xã Trạch Mỹ Lộc vào ngày 16/9. Các lô đất có ký hiệu ĐG44 đến ĐG62 với diện tích 108 - 129 m2, giá khởi điểm đều từ 23,4 triệu đồng một m2.Theo thống kê, cuộc đấu giá này có 140 hồ sơ đăng ký, tương ứng tỷ lệ gần 11 hồ sơ cùng quan tâm một lô đất. Kết thúc buổi đấu giá, 13 lô đều được bán thành công. Trong đó, lô trúng cao nhất với giá 75 triệu đồng một m2, lô thấp nhất là 28,6 triệu một m2.Như vậy, giá đất tại khu Dộc Tranh, xã Trạch Mỹ Lộc tiếp tục tạo đỉnh mới chỉ trong vòng hơn nửa tháng qua bất chấp nhiều ý kiến trái chiều về các cuộc đấu giá đất tại loạt huyện ven Hà Nội.
+Khu đất đấu giá Dộc Tranh, xã Trạch Mỹ Lộc, huyện Phúc Thọ. Ảnh: Anh Tú
+Tại phiên đấu giá hồi cuối tháng 8, 30 lô đất tại khu này được bán với giá trúng cao nhất với gần 60 triệu đồng một m2. Khi đó, nhiều nhà đầu tư cùng tham gia cho rằng mức này cao hơn nhiều so với giá trị thực tế, khi các lô đất mặt tiền ở các khu vực lân cận chỉ khoảng 40-50 triệu đồng một m2.Tuy nhiên, người đã trả mức giá gần 60 triệu một m2 này khẳng định không bỏ cọc bởi đã nghiên cứu kỹ giá thị trường, lô đất nằm ở vị trí góc đẹp, được hưởng lợi về hạ tầng giao thông trong tương lai.Đến hôm 10/9, Phúc Thọ tiếp tục tổ chức đấu giá thêm 30 lô đất cũng tại khu Dộc Tranh. Tại sự kiện có khoảng 180 khách hàng tham gia này, lô đất trúng đấu giá cao nhất là 69,8 triệu đồng một m2. Theo một số môi giới ở địa phương, lô đất này cũng đã được sang tay ngay sau đó với giá chênh hàng trăm triệu đồng.Hơn 1 tháng qua, các cuộc đấu giá đất tại loạt huyện ven như Thanh Oai, Hoài Đức đã gây xôn xao thị trường với mức trúng cao kỷ lục trên 100 triệu đồng một m2. Trong đó, một lô đất tại xã Tiền Yên, huyện Hoài Đức có mức trúng được đẩy lên tới hơn 133 triệu một m2. Sau đó, các cơ quan quản lý đã yêu cầu kiểm tra, chấn chỉnh công tác đấu giá đất trên địa bàn thành phố Hà Nội.Hiện tại, trong số 68 lô đất trúng đấu giá ở huyện Thanh Oai, mới có 13 nhà đầu tư nộp tiền dù đã hết thời hạn thanh toán. Các lô này chỉ có giá trúng từ 51,6 triệu đến 55 triệu một m2. Còn 55 lô trúng từ 80 triệu đến hơn 100 triệu đồng một m2 đều bỏ cọc, không nộp tiền.Sang tháng 10, Phúc Thọ sẽ tổ chức đấu giá 28 thửa đất tại xã Tam Hiệp và xã Thọ Lộc. Trong đó, 3 thửa đất tại khu Gạc Chợ, xã Tam Hiệp có giá khởi điểm từ 66,7 triệu đồng một m2. Tương ứng người tham gia đấu giá cần đặt trước từ gần 1,8 tỷ đến hơn 2 tỷ đồng.25 thửa đất khu Đồng Phươm, xã Lộc Thọ có giá khởi điểm 19,8 triệu đồng một m2, tương ứng tiền đặt trước từ 532 triệu - 746 triệu đồng mỗi lô (diện tích 134 - 188,4 m2). Tại phiên đấu giá ngày 10/9, 9 thửa đất ở Đồng Phươm, xã Thọ Lộc ghi nhận mức trúng cao nhất là 25,6 triệu một m2, thấp nhất 23,4 triệu đồng một m2.Phúc Thọ là huyện ngoại thành nằm ở phía Tây Bắc, cách trung tâm TP Hà Nội gần 40 km. Huyện này rộng gần 118 km2 hiện có 1 thị trấn và 20 xã, với dân số khoảng 200.000 người. Gần đây nhất hôm 9/9, Tập đoàn T&amp;T khởi công xây dựng hạ tầng kỹ thuật cụm công nghiệp Nam Phúc Thọ - giai đoạn 1. Dự án này có quy mô 41,7 ha với tổng mức đầu tư gần 780 tỷ đồng nằm ở các xã Tam Hiệp và Ngọc Tảo.Anh Tú</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Giá rau xanh tăng sau bão</t>
+          <t>Gần triệu đồng một kg muồm muỗm</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/gia-rau-xanh-tang-sau-bao-4790435.html</t>
+          <t>https://vnexpress.net/gan-trieu-dong-mot-kg-muom-muom-4793462.html</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Tại nhiều chợ dân sinh ở Hà Nội, Hải Phòng, các loại rau muống, mồng tơi, cải đều có giá 15.000 đồng một bó, tăng khoảng 30% so với hai ngày trước.</t>
+          <t>Muồm muỗm, còn gọi là "tôm bay", món ăn dân dã nay thành đặc sản có giá gần triệu đồng một kg, được nhiều người Hà Nội và TP HCM ưa chuộng.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sáng 8/9, các khu chợ ở Hà Nội, Hải Phòng, Quảng Ninh đã hoạt động lại sau cơn bão Yagi, nhưng lượng người bán và mua vắng hơn mọi ngày. Giá thực phẩm như thịt, cá không biến động nhiều, dẫu vậy rau xanh tăng mạnh. Trong đó, nhiều loại như mồng tơi, cải, ngót... đều có giá 15.000 đồng một bó.
-Một quầy rau xanh (chủ yếu củ, quả) ở Nam Từ Liêm, Hà Nội sau ngày bão tấn công. Ảnh: Anh Tú
-Theo một tiểu thương kinh doanh ở chợ Nghĩa Tân (Cầu Giấy), giá rau củ đã tăng dần từ mấy ngày trước bão khi nhu cầu tích trữ của người dân lên cao. "Giá rau hôm nay tăng tiếp 20-30% so với hai ngày trước", người này nói.Chị Thu Thanh, trú phường Kênh Dương, quận Lê Chân, Hải Phòng cho biết các chợ dân sinh ở khu vực này đã mở cửa, nhưng số lượng sản phẩm không nhiều. Nhiều loại rau xanh cũng được bán 15.000 đồng một bó, chỉ có rau dền rẻ hơn, khoảng 12.000-13.000 đồng. Các loại củ quả khác tăng nhẹ như su su, bắp cải 20.000 đồng một kg...Tại Quảng Ninh, theo báo cáo của Sở Công Thương tỉnh, một số mặt hàng rau, củ, quả cũng có xu hướng tăng 5-10% so với những ngày trước đó, tập trung tại các chợ, cửa hàng nhỏ.Lý giải giá rau tăng, các tiểu thương cho biết do giá mua vào tăng cao, việc nhập hàng, di chuyển cũng khó khăn hơn nhiều do ảnh hưởng mưa bão. Dự kiến giá rau vài ngày tới khó giảm vì mưa to, gió lớn gây thiệt hại nhiều hoa màu.
-Quầy hàng rau, củ tại một siêu thị lớn trên đường Trần Đăng Ninh, Cầu Giấy lúc 12h trưa 8/9. Ảnh: Anh Tú
-Trong khi đó tại siêu thị, giá các loại rau, củ vẫn được giữ ở mức ổn định. Ghi nhận trưa 8/9, các kệ thực phẩm, rau củ ở nhiều siêu thị Hà Nội đầy ắp, không còn cảnh cháy hàng như hai ngày trước. Tại một siêu thị lớn trên đường Trần Đăng Ninh (Cầu Giấy), các loại rau như cải, muống có giá từ 13.000-15.000 đồng một bó, nặng 0,45-0,5 kg, bắp cải từ 22.000 đồng một kg.Còn ở Hải Phòng, người dân đến các siêu thị ngay từ sáng sớm để mua bánh mỳ, nước lọc khi nhiều khu vực thành phố này vẫn chưa có điện và nước. Đến giờ trưa, một số điểm bán hết nước lọc trên kệ hàng. Đồng thời, nhiều người cũng đến siêu thị để tranh thủ sạc điện thoại, thiết bị điện tử.
-Người dân Hải Phòng đổ đến trung tâm thương mại Aeon Mall ở quận Lê Chân lúc đầu giờ chiều 8/9. Ảnh: Dương Thanh
-Đại diện Aeon Việt Nam cho biết sáng nay, sau cơn bão người dân đã bắt đầu đi mua sắm trở lại, chủ yếu vẫn là các mặt hàng thiết yếu. Hệ thống này sẽ bổ sung đầy đủ hàng hóa, ổn định giá để đáp ứng nhu cầu.Tương tự bà Nguyễn Thị Kim Dung, Giám đốc siêu thị Co.opmart Hà Nội, cho hay hiện tại hàng hóa tại siêu thị vẫn đầy đủ, giá cả ổn định. "Một số nhà cung cấp không giao hàng hôm nay nhưng chúng tôi đã có dự trữ đủ hàng để phục vụ người dân", bà Dung nói.Hôm nay, toàn bộ siêu thị WinMart hoạt động bình thường. Các cửa hàng nhỏ hơn như WinMart+/ Win cũng mở cửa trừ một số cơ sở bị thiệt hại (vỡ kính, bay mái tôn) hay nằm trong khu vực lụt, cây đổ gây cản trở giao thông.Vụ Thị trường trong nước (Bộ Công Thương) cho rằng nhu cầu tiêu dùng trên thị trường sẽ giảm do hàng hóa thiết yếu đã được mua từ ngày 6/9. Tình hình cung ứng hàng hóa, lương thực, thực phẩm, xăng dầu cơ bản đảm bảo. Bộ Công Thương sẽ tiếp tục bám sát, cập nhật tình hình để có chỉ đạo.Anh Tú - Phương Dung</t>
+          <t>Chị Hòa, ở quận Gò Vấp, TP HCM, cho biết lúc còn nhỏ ở quê, mẹ chị đi gặt về luôn mang theo một túi muồm muỗm. Khi nướng lên, chúng có mùi thơm, vị béo ngậy. "Giờ đã lớn và đang sống ở TP HCM, tôi vẫn sẵn sàng chi 400.000 đồng để mua nửa ký cho cả nhà thưởng thức lại hương vị xưa", chị nói.Trên các chợ trực tuyến, loại này được bán với giá từ 500.000-700.000 đồng một kg tùy loại. Đặc biệt, muỗm non giá tới 850.000 đồng một kg, tăng 35% so với năm ngoái và gấp đôi năm 2022.
+Muỗm xanh được chị Nga đóng gói để giao cho khách. Ảnh: Đinh Nga
+Nam Anh, người bán muồm muỗm ở TP HCM, cho biết loại này rất hiếm nên giá tăng cao. Mỗi tháng, cô chỉ nhập được hai lần, mỗi lần 6-7 kg, không đủ cho khách đặt trước. Gần đây, bão lũ tại miền Bắc khiến nguồn cung càng giảm, giá đi lên.Chuyên kinh doanh côn trùng này ở Hà Nội, chị Hoài nói loại muỗm sống có lúc giá lên đến 900.000 đồng một kg vì khan hàng, đắt hơn cấp đông từ 100.000-200.000 đồng.Tại Mường Lát (Thanh Hóa), chị Đỗ Thị Nga, đầu mối thu gom muỗm, nói mỗi ngày bán từ 10-20 kg loại tươi. "Tôi chỉ phân phối cho miền Bắc, giá sỉ khoảng 400.000 đồng một kg chưa gồm phí vận chuyển," chị cho biết.Theo chị Nga, muỗm xanh chỉ có từ tháng 8 đến tháng 9. Người dân bắt chúng vào ban đêm, dùng đèn để dụ. Sau khi bắt, chúng được sơ chế, đóng gói hút chân không. Việc sử dụng nhiều thuốc bảo vệ thực vật khiến muỗm ngày càng hiếm.
+Muỗm xanh đã cắt cánh. Ảnh: Thanh Hoài
+Nói với VnExpress, GS TS Bùi Công Hiển, Hội Côn trùng học Việt Nam, cho biết ở Việt Nam có hai loài muồm muỗm gồm loại xanh (Euconocephalus incertus) và nâu (Euconocephalus broughtoni). Đến nay, chưa có báo cáo về việc muỗm gây hại mùa màng, chỉ ghi nhận ở cào cào di cư. Dù vậy, cả hai loài này đều thuộc bộ cánh thẳng (Orthoptera).Muỗm đã được khai thác làm thực phẩm từ lâu ở Việt Nam. Tại Mù Cang Chải, chúng còn có tên "tôm bay" và được quảng bá như một đặc sản.Tuy nhiên, GS Hiển cảnh báo nếu khai thác quá mức, loài muỗm có thể suy giảm hoặc đứng trước nguy cơ tuyệt chủng. Ông đề xuất nuôi muỗm theo trang trại, giúp kiểm soát nguồn thức ăn và hạn chế nguy cơ nhiễm độc từ các cây chứa chất độc mà muỗm có thể ăn ngoài tự nhiên.Ông cũng cảnh báo rằng ăn côn trùng tự nhiên, bao gồm muỗm, có thể tiềm ẩn nguy cơ ngộ độc. Điều này có thể do côn trùng ăn phải lá độc, bị nấm hoặc vi khuẩn xâm nhập. Việc buôn bán côn trùng khai thác tự nhiên cũng thiếu kiểm soát về an toàn thực phẩm.Thi Hà</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hoàn thành nâng cấp đường nối cù lao phía Đông TP HCM</t>
+          <t>Mưa lớn 'nghìn năm có một' tấn công bang Mỹ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hoan-thanh-nang-cap-duong-noi-cu-lao-phia-dong-tp-hcm-4790430.html</t>
+          <t>https://vnexpress.net/mua-lon-nghin-nam-co-mot-tan-cong-bang-my-4793660.html</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tuyến đường 6 km kết nối cù lao Long Phước qua trung tâm Thủ Đức hoàn thành nâng cấp tạo diện mạo mới cho khu vực, người dân thuận tiện đi lại.</t>
+          <t>Lượng mưa kỷ lục trút xuống Bắc Carolina chỉ trong vài giờ, khiến nước lũ tràn vào nhà cửa, ôtô mắc kẹt.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Chiều 8/9, đại diện Ban Quản lý dự án đầu tư xây dựng khu vực TP Thủ Đức (chủ đầu tư), cho biết dự án nâng cấp đường Long Phước dài gần 6 km, thuộc phường Long Phước, đã cơ bản hoàn thành sau gần hai năm khởi động trở lại.Tuyến đường được chỉnh trang, mở rộng lên 9-12 m kết hợp các hạng mục thoát nước, chiếu sáng, vỉa hè... Trong tổng mức đầu tư hơn 260 tỷ đồng, kinh phí xây lắp của dự án chiếm phần ít với khoảng 75 tỷ đồng, còn lại chủ yếu là tiền đền bù, giải phóng mặt bằng.
-Đường Long Phước kết nối vào cầu Long Đại, phía trước là khu dân cư Vinhome Grand Park, tháng 9/2024. Ảnh: Gia Minh
-Dự án nâng cấp đường Long Phước khởi công cuối năm 2017, nhưng hai năm sau dừng do vướng mặt bằng. Thủ tục đền bù cho các hộ tiếp tục gặp khó khăn trong hai năm đại dịch, phải tới cuối năm 2022 dự án mới thi công trở lại. Đến nay, toàn bộ dự án chỉ còn một số hạng mục nhỏ như vỉa hè đang hoàn thiện.Được bao bọc bởi sông Đồng Nai, sông Tắc, vùng đất Long Phước còn được gọi là cù lao, giao thông cách trở, đi lại khó khăn. Đường Long Phước cũng là tuyến nối vào cầu Long Đại mới đưa vào khai thác cuối năm 2023. Trục đường này sau khi hoàn thành nâng cấp giúp người dân thuận tiện đi lại, rút ngắn hành trình sang phường Long Bình, vào trung tâm TP Thủ Đức còn hơn 500 m thay vì phải chạy vòng khoảng 10 km như trước.
-Đường Long Phước nằm dưới cao tốc TP HCM - Long Thành - Giây. Ảnh: Gia Minh
-Ngoài ra, đường Long Phước còn là một trong những tuyến quan trọng khi có các trục giao thông lớn cắt qua là cao tốc TP HCM - Long Thành - Dầu Giây (đã khai thác) và Vành đai 3 (đang xây dựng).Trước đó, ngành giao thông thành phố từng đề xuất xây dựng nút giao kết nối đường Long Phước với cao tốc trong phương án mở rộng tuyến đường này. Khi hai tuyến được kết nối, người dân ở khu vực thuận tiện ra vào nội thành, giảm áp lực cho trục đường hiện hữu là Long Phước - Long Thuận - Nguyễn Duy Trinh.
- Hướng tuyến đường Long Phước. Đồ hoạ: Đăng Hiếu
-Ngoài đường Long Phước, nhiều công trình giao thông trọng điểm khác ở TP Thủ Đức sau thời gian dài vướng mặt bằng được triển khai trở lại. Trong đó, tháng 9 này ở địa phương dự kiến có thêm cầu Nam Lý được thông xe, giảm ùn tắc đường Đỗ Xuân Hợp, góp phần hoàn thiện mạng lưới giao thông khu đông TP HCM.Gia Minh</t>
+          <t>Thị trấn Carolina Beach ven biển ở bang Bắc Carolina ngày 16/9 được đặt trong tình trạng khẩn cấp sau trận mưa lịch sử trút xuống 457 mm nước trong 12 giờ. Cơ quan Thời tiết Quốc gia Mỹ cho biết đây là hiện tượng "nghìn năm có một"."Đây có lẽ là trận lụt tồi tệ nhất mà dân địa phương từng chứng kiến", Bruce Oakley, quan chức thị trấn du lịch Carolina Beach, nói. "Chúng tôi phải cứu người khỏi ôtô, khỏi nhà hay nơi làm việc. Cơ quan cứu hộ tiếp nhận hàng chục cuộc gọi".
+Mưa lớn 'nghìn năm có một' tấn công bang Mỹ
+Mưa lớn gây ngập lụt nghiêm trọng ở Carolina Beach, Bắc Carolina, Mỹ. Video: X/Wright
+Trường tiểu học địa phương đã phải đóng cửa, cho học sinh ra về sớm sau khi nước tràn vào các lớp học. Giới chức cứu hộ, cứu hỏa phải đưa nhiều em về nhà vì một số tuyến đường ngập đến 91 cm.Các nơi khác trong khu vực cũng ghi nhận lượng mưa hơn 300 mm trong 12 giờ, nhiều nhất trong 200 năm.Lisa và Gary Hollon, sống ở Kure Beach, cách Carolina Beach khoảng 5 km, cho biết thị trấn này chưa từng bị ngập sau 15 năm sinh sống tại đây."Mưa gió đột ngột nổi lên vào sáng sớm. Tầng một nhà chúng tôi ngập 15 cm. Chúng tôi không chuẩn bị gì, vì khu vực chưa từng bị ngập lụt trước đây", Lisa Hollon nói.
+Một thanh niên trèo ván lướt sóng tại điểm ngập lụt ở Bắc Carolina. Ảnh: BBC
+Lượng mưa ở hạt Brunswick lân cận có lúc là hơn 127 mm một giờ. Thị trấn Sunny Point hứng lượng mưa 228 mm trong ba giờ, lớn hơn lượng mưa trung bình một tháng."Giới chức đang hỗ trợ nhiều người mắc kẹt trong xe, trong nhà", văn phòng cảnh sát khu vực thông báo.
+Ôtô bị nước lũ cuốn trôi tại hạt Brunswick, Bắc Carolina. Ảnh: Cảnh sát Brunswick
+Trận mưa lịch sử này là ảnh hưởng của khối áp thấp nằm gần bờ biển, sức gió mạnh nhất 56 km/h, chưa đủ điều kiện để được gọi là bão nhiệt đới hay cận nhiệt đới.Lũ lụt ở Carolina Beach bắt đầu rút vào chiều 16/9 khi áp thấp chuyển đến phía tây khu vực, dự kiến suy yếu và tan vào sáng 18/9.
+Đường đi của khối áp thấp gây mưa lịch sử tại Bắc Carolina, Mỹ. Đồ họa: CNN
+Đức Trung (Theo CNN, USA Today, NBC News)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hơn 20 tàu du lịch Hạ Long chìm vì bão Yagi</t>
+          <t>8 vị trí chưa thể lưu thông trên các tuyến quốc lộ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hon-20-tau-du-lich-ha-long-chim-vi-bao-yagi-4790415.html</t>
+          <t>https://vnexpress.net/8-vi-tri-chua-the-luu-thong-tren-cac-tuyen-quoc-lo-4793695.html</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quảng NinhBão Yagi đánh chìm hơn 20 tàu ở bến cảng Tuần Châu, nơi đưa khách tham quan vịnh Hạ Long, khiến chủ tàu thiệt hại hàng tỷ đồng.</t>
+          <t>8 điểm trên các tuyến quốc lộ miền núi phía Bắc bị đứt gãy do sạt lở đất khiến phương tiện chưa thể qua lại, các đơn vị đang khắc phục để sớm thông xe.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Đại diện Cảng tàu khách Quốc tế Tuần Châu cho biết hơn 20 tàu du lịch bị siêu bão Yagi đánh chìm, theo thống kê đến sáng nay. Hiện tại, công tác thống kê, xác minh chủ phương tiện vẫn chưa hoàn tất do sóng viễn thông kém, mất điện, nhiều phương tiện đi tránh trú chưa liên lạc được.Cảng Tuần Châu là một trong ba bến cảng được phép đón trả khách du lịch tham quan trên vịnh Hạ Long, diện tích hơn 1,7 triệu m2 và sức chứa trên 2.000 tàu. Đây cũng là nơi đặt nhà chờ của nhiều đơn vị kinh doanh dịch vụ du thuyền ngủ đêm trên vịnh Lan Hạ.
-video hiện trường tàu Tuần Châu
-Nhiều tàu bị đánh chìm, va đập hư hỏng tại Tuần Châu. Video: Huy Mạnh
-Theo tìm hiểu, chi phí đóng tàu du lịch chở khách tham quan vịnh trong ngày thường khoảng hai tỷ đồng, tàu ngủ đêm, vỏ thép khoảng 35 tỷ đồng. Ông Duy Anh, chủ 5 tàu du lịch hoạt động trên vịnh Lan Hạ, ước tính ban đầu đơn vị ông bị thiệt hại khoảng 5 tỷ đồng."May mắn tàu không chìm nhưng hệ thống cầu tàu, nhà chờ, kho bãi và các vật dụng phục vụ du lịch bị bão san thành bình địa", ông nói.Trước khi Hải Phòng có lệnh cấm biển, ông đã đưa hết tàu về bến, hủy tour của khách, để có chỗ neo đậu an toàn.
-Tàu chở khách tham quan trong ngày bị sóng đánh tấp vào cầu tàu của công ty ông Duy Anh và chìm sau đó, cầu tàu hư hỏng nặng. Ảnh: NVCC
-CEO Phạm Hà của Lux Group - đơn vị kinh doanh du thuyền trên vịnh Lan Hạ - nói hai xuồng chở khách từ cảng ra tàu lớn bị chìm, cần trục vớt để sửa chữa. Tàu du lịch chở khách ngủ đêm của đơn vị cũng bị gió bão đánh va đập nhưng cơ bản vẫn hoạt động được. Đại diện đơn vị này nói do cột sóng viễn thông bị đổ nên nhiều chủ tàu mất liên lạc với thuyền viên, công tác thống kê thiệt hại còn khó khăn.Tại Hạ Long, nhiều khách sạn ghi nhận thiệt hại nặng vì bão Yagi trong ngày 7/9. Khách sạn Novotel Hạ Long cho biết hàng loạt cửa kính của bị vỡ, khuôn viên cây cảnh gãy đổ. Tới sáng 8/9 Hạ Long vẫn mưa to nên khách sạn chưa thống kê được đầy đủ thiệt hại. Khách sạn Diamond ở Hạ Long cho biết "thiệt hại rất nhiều" về tài sản khi loạt cửa kính, mái hiên bị gió giật đổ.Hannah McEvoy, khách lưu trú dài hạn ở tầng cao khách sạn Best Western Premier Sapphire Halong, nói những gì đã trải qua trong ngày 7/9 "thực sự đáng sợ". Cô cảm giác tòa nhà lắc lư và phòng của mình rung lên vì gió. Do sợ cửa kính có thể vỡ, trong tối cùng ngày, cô được nhân viên khách sạn bố trí vào ở một phòng thấp hơn cùng một số khách khác còn lưu trú.Tới sáng 8/9, McEvoy mới trở lại phòng cũ, nơi chỉ bị nước tràn ướt sàn nhà. Tuy nhiên, nữ du khách cho biết khu vực sảnh và xung quanh khách sạn có nhiều kính vỡ, cây đổ.
-Bên ngoài khách sạn McEvoy thuê. Ảnh: NVCC
-Quan Lạn, Quảng Ninh, cũng là điểm chịu thiệt hại nặng nề vì bão. Tới khoảng 9h ngày 8/9, sóng viễn thông trên đảo vẫn gặp vấn đề, đường phố tan hoang vì cây đổ, nhà tốc mái. Anh Phương Nam, chủ một khách sạn trên đảo, nói cơ sở không bị tàn phá nặng nhưng bị tốc mái, khiến nước tràn ngập 5 tầng. Chủ khách sạn quan ngại khó đón khách trong tuần tới khi hệ thống điện còn gặp vấn đề và cơ sở vật chất phục vụ du lịch bị thiệt hại.Tại Đồ Sơn, Hải Phòng, hàng chục cửa hàng, nhà dân bị tốc mái, hư hỏng nặng sau bão Yagi. Cây cối, tôn, tường bao ngổn ngang khắp nơi tại bãi biển Đồ Sơn. Anh Vũ Văn Khánh, chủ kinh doanh dịch vụ ăn uống, nhà nghỉ cho biết nhà anh "gần như bị xóa sổ", thiệt hại ước tính hơn 3 tỷ đồng.Tâm bão Quảng Ninh hôm qua hứng chịu sức gió mạnh nhất ở Bãi Cháy, lên tới cấp 14, các khu vực cấp 12-13. Thống kê đến sáng nay, tỉnh có 38 tàu, thuyền bị chìm, mất tích; 1.000 lồng bè nuôi trồng thủy sản bị hư hại, chìm, mất tích. Số nhà bị tốc mái, hư hại lên đến hàng nghìn.
-Nhà nghỉ của anh Vũ Văn Khánh tại Đồ Sơn, Hải Phòng. Ảnh: Anh Phú
-Từ chiều đến tối qua, toàn tỉnh Quảng Ninh, TP Hải Phòng và Thái Bình phải cắt điện để khắc phục sự cố và đảm bảo an toàn trong mưa bão. Đến sáng nay, nhiều khu vực vẫn mất điện.Nhiều công ty lữ hành có đoàn khởi hành du lịch tuyến miền Bắc, qua Hà Nội, Hạ Long tuần tới quan ngại về khả năng cung ứng dịch vụ.Công ty CP Truyền thông Du Lịch Việt, có hai đoàn khởi hành từ phía TP HCM, tham quan tuyến du lịch miền Bắc từ 10/9, lo ngại khả năng cung ứng thực phẩm của các đối tác nhà hàng và tính khả thi của lịch trình du lịch Hạ Long - một trong những điểm chịu ảnh hưởng nặng nhất của bão Yagi. Hiện tại, các đối tác chưa thể cập nhật đủ thông tin do nhiều nhân viên còn nghỉ làm, lo dọn dẹp nhà cửa và sóng viễn thông chưa ổn định.Đại diện Vietluxtour nói theo lịch dự kiến, công ty có khoảng 10 đoàn du lịch miền Bắc và ba đoàn sẽ tới Hạ Long. Tuy nhiên, với việc các cơ sở phục vụ du lịch bị ảnh hưởng, một số đoàn có thể phải chuyển hướng tour, dời lịch khởi hành.Tuấn Anh - Tú Nguyễn</t>
+          <t>Sáng 17/9, Cục Đường bộ Việt Nam cho biết các địa phương đã xử lý được 559 điểm sạt lở, thông tuyến nhiều tuyến đường. Tuy nhiên, vẫn còn 8 vị trí, trong đó có hai điểm tại Lào Cai chưa thể thông xe do sạt lở nghiêm trọng và địa hình khó khăn. Dự kiến, các điểm này sẽ được thông xe vào ngày 30/9. 
+Tỉnh Bắc Kạn có một vị trí tắc đường trên quốc lộ 279, đoạn từ trung tâm huyện Ba Bể sang huyện Na Hang, tỉnh Tuyên Quang, do sạt lở taluy dương và taluy âm khối lượng lớn. Dự kiến vị trí này được thông xe từ 25/9.Tỉnh Tuyên Quang có một vị trí ách tắc trên quốc lộ 2C do nền đường xuất hiện cung trượt lớn, nguy cơ đá tảng sạt gây mất an toàn giao thông.Tỉnh Thái Nguyên có một vị trí sụt nền đường do mưa lũ với chiều dài 50 m, bề rộng chiếm gần hết toàn bộ nền mặt đường Hồ Chí Minh qua xã Tân Dương, huyện Định Hóa. Dự kiến hết tháng 9 đường được khôi phục tạm.Tỉnh Cao Bằng có một điểm trên quốc lộ 3 chưa thông xe do nền đường xuất hiện cung trượt lớn, nguy cơ cao về mất an toàn giao thông, có thể xử lý cho thông xe tạm trước 30/9.Tỉnh Nam Định có cầu phao Ninh Cường bị hư hỏng chưa bảo đảm an toàn khai thác sử dụng. Đơn vị quản lý sẽ đánh giá toàn bộ và sửa chữa khắc phục sau khi nước rút. Các phương tiện đã được phân luồng sang quốc lộ 21, 21B và các tuyến đường tỉnh để tránh vị trí này.Tỉnh Quảng Ninh có một đoạn trên quốc lộ 18B tại khu vực Bình Liêu bị sạt lở nền đường và trôi cống. Hiện phương tiện đã được phân luồng sáng quốc lộ 18, 18C, 4B và các tuyến đường tỉnh.
+Mưa lớn gây sạt lở cầu đường trên quốc lộ 4G qua Sơn La ngày 16/9. Ảnh: Sở GTVT Sơn La
+Phần lớn đường ngập, cầu cấm đã khai thác trở lạiSau khi khắc phục, 252/253 điểm ngập nước trên các tuyến đường đã được thông xe. Hiện chỉ còn đầu cầu Kiện Khê trên tuyến tránh thành phố Phủ Lý chưa thể thông xe do ngập lụt diện rộng. Tuy nhiên, giao thông không quá ảnh hưởng do phần lớn phương tiện đã chuyển hướng đi cao tốc Pháp Vân - Cầu Giẽ - Ninh Bình.Giao thông đã cơ bản phục hồi tại các tuyến đường huyết mạch như cầu Đoan Hùng (quốc lộ 2) và cầu Hồ (quốc lộ 38). Bến phà Cồn Nhất (Ninh Bình) cũng đã hoạt động trở lại. Tuy nhiên, do mực nước sông vẫn cao và chảy xiết, hai bến phà Đống Cao và Đại Nội (Nam Định) vẫn phải tạm ngừng khai thác.Cầu Nam Cường (cao tốc Nội Bài - Lào Cai) đang bị lún đường đầu cầu, nứt vỡ lan can cầu, lún sụt bậc lên xuống tại mố M0 và trụ T1. Đơn vị quản lý tuyến đang tiếp tục theo dõi để có giải pháp xử lý.Cao tốc Nội Bài - Lào Cai tại km 249 chiều từ Lai Châu và cửa khẩu Kim Thành về Hà Nội có cung trượt taluy âm làm khoảng nửa mặt đường bị lún sụt. Đơn vị quản lý đường đã rào chắn, cử người trực chốt, các phương tiện lưu thông chậm qua vị trí này.Tuyến Nội Bài - Bắc Ninh, cầu Đông Yên có một số cánh dầm và mối nối dọc bị rạn nứt, nhiều vị trí bong vỡ bêtông, rơi xuống gây nguy hiểm cho người và phương tiện tham gia giao thông. Đơn vị quản lý tuyến đang theo dõi, xử lý.Những ngày qua, các sở giao thông vận tải và các đơn vị ngành đường bộ đã phối hợp với chính quyền địa phương nhanh chóng khôi phục hạ tầng đường bộ để phục vụ tìm kiếm cứu nạn, bảo đảm vận chuyển hàng hóa thiết yếu phục vụ nhân dân sau mưa lũ.
+Đoàn Loan</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Khoảnh khắc rocket Hezbollah bay tới tấp vào Israel</t>
+          <t>Mỹ lần đầu công bố ảnh tàu lặn Titan bị ép nát</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/khoanh-khac-rocket-hezbollah-bay-toi-tap-vao-israel-4790405.html</t>
+          <t>https://vnexpress.net/my-lan-dau-cong-bo-anh-tau-lan-titan-bi-ep-nat-4793954.html</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Hezbollah phóng 50 rocket nhằm vào lãnh thổ Israel để đáp trả vụ ba nhân viên ứng phó khẩn cấp bị đối phương "sát hại" ở Lebanon.</t>
+          <t>Giới chức Mỹ công bố ảnh mảnh đuôi tàu lặn Titan, là hình ảnh đầu tiên về xác tàu sau vụ ép nát dưới đáy Đại Tây Dương hồi năm ngoái.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Lực lượng Phòng vệ Israel (IDF) thông báo hơn 50 rocket rạng sáng nay bay từ lãnh thổ Lebanon về hướng thành phố Kiryat Shmona ở miền bắc nước này. Khoảng 20 quả được phóng lúc 1h30 và 2h30, phần lớn bị lưới phòng không Israel đánh chặn, song một số đã gây ra thiệt hại vật chất. Một rocket đã bắn trúng một tòa nhà, còn một quả khác rơi xuống vỉa hè.Khoảng 30 quả rocket còn lại được khai hỏa vào lúc 5h30, một số bị đánh chặn, số còn lại rơi xuống khu vực trống trải. Không ai bị thương sau các vụ tấn công.Video đăng trên mạng xã hội cho thấy hàng loạt rocket bay liên tục về hướng thành phố Kiryat Shmona khi trời vẫn tối đen, tạo thành các vệt sáng lớn trên bầu trời.
-Khoảnh khắc loạt rocket Hezbollah bay tới tấp vào Israel
-Rocket Hezbollah bay vào lãnh thổ Israel rạng sáng 8/9. Video: X/OSINTdefender
-Nhóm vũ trang Hezbollah tại Lebanon ngày 8/9 thông báo sáng cùng ngày đã phóng "loạt rocket Falaq" nhằm "đáp trả các vụ tấn công của đối phương", đặc biệt là cuộc tập kích khiến các nhân viên cứu hộ thiệt mạng ở làng Froun.Bộ Y tế Lebanon cáo buộc Israel hôm 7/9 "nhắm mục tiêu vào một tổ phòng vệ dân sự đang làm nhiệm vụ dập hỏa hoạn, vốn do các cuộc tập kích gần đây của Tel Aviv gây ra tại làng Froun". Cuộc tập kích của Israel "khiến ba nhân viên ứng phó khẩn cấp thiệt mạng".Cơ quan này lên án sự việc, gọi đây là "vụ tấn công trắng trợn nhằm vào lực lượng thuộc cơ quan chính thức của nhà nước Lebanon".Phong trào Amal, đồng minh của Hezbollah, cho biết hai thành viên của nhóm nằm trong số những người chết trong vụ tập kích ngày 7/9 của Israel, thêm rằng họ "đang làm nhiệm vụ nhân đạo và quốc gia để bảo vệ Lebanon" khi thiệt mạng.Trong khi đó, Israel tuyên bố đã hạ các thành viên Amal trực thuộc "một cơ cấu quân sự của Hezbollah".Sau vụ tấn công sáng 8/9 của Hezbollah, quân đội Israel không kích đáp trả nhằm vào các cơ sở quân sự của nhóm vũ trang tại miền nam Lebanon.
-Vị trí Israel và Lebanon. Đồ họa: AFP
-Giao tranh xuyên biên giới giữa Israel và Hezbollah diễn ra gần như hàng ngày sau khi xung đột tại Dải Gaza bùng phát tháng 10 năm ngoái. Hezbollah tuyên bố họ tập kích Israel nhằm thể hiện ủng hộ với đồng minh Hamas tại Dải Gaza.Các cuộc đụng độ đã khiến 614 người thiệt mạng ở Lebanon, phần lớn là các tay súng, song cũng bao gồm 138 dân thường, theo số liệu của AFP. Bộ trưởng Y tế Lebanon Firass Abiad cho biết 27 nhân viên ứng phó khẩn cấp và nhân viên y tế đã tử vong, bên cạnh 94 người bị thương, do "hành động gây hấn của Israel".Hai bệnh viện và 21 trung tâm y tế đã bị nhắm mục tiêu, trong khi 32 xe cứu hỏa, cứu thương đã bị hư hỏng một phần hoặc không thể hoạt động tiếp, ông cho hay.Trong khi đó, giới chức Israel cho biết ít nhất 24 binh sĩ và 26 dân thường nước này đã thiệt mạng do xung đột với Hezbollah.Phạm Giang (Theo AFP, Times of Israel)</t>
+          <t>Lực lượng Tuần duyên Mỹ ngày 16/9 chia sẻ hình ảnh mảnh đuôi vỡ của tàu lặn Titan tại Bắc Đại Tây Dương dưới độ sâu gần 3.800 m, trong phiên điều trần sẽ diễn ra cho đến ngày 27/9 ở North Charleston, Nam Carolina.Trong ảnh, mảnh đuôi tách khỏi thân tàu, các cạnh nham nhở, một mảnh vỡ của tàu ở lân cận. Các điều tra viên cho biết mảnh vỡ được phát hiện cách địa điểm xác tàu Titanic vài trăm mét sau nhiều ngày tìm kiếm.
+Mảnh vỡ tàu lặn Titan ở độ sâu gần 3.800 m. Ảnh: Tuần duyên Mỹ
+Theo Ủy ban Điều tra Hàng hải, thiết bị điều khiển từ xa đã xác định được vị trí của mảnh đuôi và những mảnh vỡ khác hôm 22/6/2023, cung cấp "bằng chứng kết luận" rằng con tàu bị ép nát. Đây là hiện tượng vật thể bị phá hủy khi chịu áp suất khổng lồ bên ngoài ép vào trong, thay vì hướng ra bên ngoài như một vụ nổ.Thảm kịch cướp đi sinh mạng của Stockton Rush, người sáng lập kiêm giám đốc điều hành công ty vận hành tàu lặn OceanGate; tỷ phú kiêm nhà thám hiểm người Anh Hamish Harding, 58 tuổi; doanh nhân gốc Pakistan Shahzada Dawood, 48 tuổi cùng con trai 19 tuổi, Suleman, đều là công dân Anh; nhà hải dương học quốc tịch Pháp kiêm chuyên gia nổi tiếng về tàu Titanic Paul-Henri Nargeolet, 77 tuổi.Các phần thi thể tìm thấy khớp với 5 người trên tàu thông qua xét nghiệm và phân tích ADN. Trong phiên điều trần, ủy ban đã triệu tập các nhân chứng đầu tiên, trong đó có nhân viên cũ của OceanGate. Các nhà điều tra cũng cho biết nội dung tin nhắn cuối cùng mà tàu Titan gửi đi 6 giây trước khi mất liên lạc."Đã thả hai khối dằn tàu", là tin nhắn Titan gửi cho tàu mẹ, thông báo tàu đã giảm trọng tải để nổi lên mặt nước. Vài giây sau, Titan phát tiếng "ping" báo hiệu định vị lần cuối, tàu mẹ mất dấu Titan vào sáng 18/6/2023.Trong những ngày tiếp theo, chiến dịch tìm kiếm cứu hộ quốc tế diễn ra tại vùng biển xa xôi cách Newfoundland, Canada vài trăm km về phía đông nam.
+Tàu lặn Titan trước khi gặp thảm kịch. Ảnh: OceanGate Expeditions
+Tuần duyên Mỹ cho hay phiên điều trần sẽ cung cấp thông tin về các sự kiện xảy ra trước tai nạn, đánh giá việc tuân thủ quy định, nhiệm vụ và trình độ của người điều khiển tàu, hệ thống cơ khí và kết cấu con tàu, cơ chế ứng phó khẩn cấp và ngành công nghiệp tàu lặn.Mục đích chính của phiên điều trần là "làm sáng tỏ sự thật xung quanh tai nạn", chủ tịch Ủy ban Điều tra Hàng hải Jason Neubauer cho biết, lưu ý cơ quan này cũng có nhiệm vụ xác định "hành vi sai lầm hoặc sơ suất của các thủy thủ có chứng chỉ hành nghề"."Nếu phát hiện bất kỳ hành vi phạm tội nào, chúng tôi sẽ khuyến nghị Bộ Tư pháp hành động", ông nói.
+Tàu lặn Titan mất tích thế nào. Bấm vào hình để xem chi tiết
+Hồng Hạnh (Theo CNN, AFP)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bão Yagi làm 14 người chết</t>
+          <t>Vì sao Lào Cai, Cao Bằng, Yên Bái hứng chịu sạt lở, lũ quét?</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bao-yagi-lam-14-nguoi-chet-4790367.html</t>
+          <t>https://vnexpress.net/vi-sao-lao-cai-cao-bang-yen-bai-hung-chiu-sat-lo-lu-quet-4793081.html</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bão Yagi đổ bộ Quảng Ninh - Hải Phòng với sức gió cấp 12-13 làm 14 người chết, trong đó Quảng Ninh 4, Hà Nội 3 người, 176 người khác bị thương.</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Theo Cục Cứu hộ - Cứu nạn, Bộ Quốc phòng, tổng hợp đến 10h sáng nay bão Yagi đã làm 4 người ở Quảng Ninh, 4 người ở Hòa Bình, 3 người ở Hà Nội, Hải Phòng, Hải Dương, Quân khu 3 mỗi nơi có một người chết. Ngoài ra, 176 người, chủ yếu ở Quảng Ninh bị thương. Các nạn nhân chủ yếu do bị cây đổ đè vào người, sạt lở đất và tàu bè trôi, mất tích.Tâm bão Quảng Ninh hứng chịu sức gió mạnh nhất ở Bãi Cháy lên tới cấp 14, các khu vực cấp 12-13 chịu nhiều tổn thất nhất về tài sản. Thống kê đến sáng nay, tỉnh có 38 tàu, thuyền bị chìm, mất tích; 1.000 lồng bè nuôi trồng thủy sản bị hư hại, chìm, mất tích. Số nhà bị tốc mái, hư hại lên đến hàng nghìn.
-Cột điện gãy đổ ở Đồ Sơn, Hải Phòng. Ảnh: Anh Phú
-Mạng lưới điện chịu thiệt hại với 401 cột điện bị gãy đổ, 27 trạm biến áp hư hỏng. Từ chiều đến tối qua, toàn tỉnh Quảng Ninh, TP Hải Phòng và Thái Bình phải cắt điện để khắc phục sự cố và đảm bảo an toàn trong mưa bão, làm hơn 3 triệu khách hàng (hộ gia đình, doanh nghiệp) bị ảnh hưởng. Đến sáng nay, nhiều khu vực vẫn mất điện.Sóng di động cũng gián đoạn từ chiều qua do 7 tuyến cáp quang liên tỉnh đứt, 27 cột phát sóng gãy đổ, 6.285 trạm mất điện trong bão Yagi, theo Cục Viễn thông, Bộ Thông tin và Truyền thông. Đến sáng nay, tại một khu vực ở Hải Phòng, Quảng Ninh và Hải Dương, nhiều người phản ánh chưa bắt được sóng di động.121.500 ha lúa và hoa màu bị ngập, hư hại sau bão, tập trung tại Thái Bình, Hải Phòng, Hải Dương, Bắc Ninh, Hà Nội, Nam Định, Hưng Yên, Hà Nam. 5.000 ha cây ăn quả tại Hải Phòng, Thái Bình, Hưng Yên bị hư hại. Cây xanh ở miền Bắc gãy đổ rất nhiều, địa phương đang thống kê, riêng Hà Nội khoảng 17.000 cây.
-Một chiếc ôtô bị cây đổ đè bẹp ở bán đảo Linh Đàm, Hà Nội. Ảnh: Lộc Chung
-Sáng 8/9, Thủ tướng Phạm Minh Chính chủ trì hội nghị trực tuyến với 26 địa phương từ Thanh Hóa trở ra để đánh giá công tác chỉ đạo ứng phó, triển khai các biện pháp cấp bách khắc phục hậu quả bão Yagi.Phát biểu mở đầu hội nghị, Thủ tướng Phạm Minh Chính nói bão Yagi hoành hành trên đất liền hơn một ngày gây hậu quả nghiêm trọng. Hoàn lưu bão sẽ tiếp tục gây mưa lũ, nhất là các tỉnh miền núi phía Bắc.Thủ tướng yêu cầu cần rà soát ngay, hỗ trợ cho các địa phương bị thiệt hại, các gia đình có người thiệt mạng. Trong lúc này, người dân đang phải chịu thiệt hại, phải bàn với tinh thần khẩn trương; tiếp tục triển khai ngay các công việc khắc phục hậu quả bão; kịp thời xử lý các vấn đề liên quan tới đời sống người dân, sản xuất, kinh doanh, ứng phó sạt lở, sụt lún.Bão giảm cấp không theo quy luật thông thườngTại hội nghị, Bộ Tài nguyên và Môi trường đánh giá bão Yagi "rất đặc biệt", hình thành phía đông Philippines, mạnh lên thành siêu bão trên Biển Đông và là cơn bão mạnh nhất tại đây trong 30 năm qua. Yagi tăng cường độ rất nhanh, trong 24 giờ đã tăng 8 cấp lên cấp 16 siêu bão và duy trì cấp này trong thời gian dài. Kể cả khi đổ bộ đảo Hải Nam của Trung Quốc đêm 6/9, bão vẫn đạt cấp siêu bão.Mức độ giảm cấp trên đường đi của Yagi "không theo quy luật thông thường". Bình thường các cơn bão đi qua đảo Hải Nam vào vịnh Bắc Bộ do ma sát với đảo sẽ yếu đi nhanh, nhưng Yagi chỉ giảm 2 cấp, còn 14. Khi áp sát bờ biển Quảng Ninh - Hải Phòng vào trưa qua, bão vẫn giữ cấp 12-13.Thời gian Yagi lưu trên đất liền kéo dài 12 giờ, trong đó nhiều giờ sau khi đổ bộ Quảng Ninh - Hải Phòng bão vẫn giữ cấp 12-13. Đến 4h sáng nay, Yagi suy yếu thành áp thấp nhiệt đới ở Tây Bắc Bộ, dự báo trong 12-24 giờ tới suy yếu thành vùng thấp và tan dần.Hôm qua, lý giải vì sao bão chậm giảm cấp dù đã đổ bộ, ông Mai Văn Khiêm, Giám đốc Trung tâm Dự báo Khí tượng Thủy văn quốc gia, cho biết hoàn lưu của bão Yagi rất rộng, bao trùm cả Bắc Bộ, Bắc Trung Bộ và có tính chất đối xứng khiến việc giảm cấp nhanh rất khó. Bề mặt đệm ở Bắc Bộ nóng, ẩm, là nguồn cung cấp năng lượng cho bão.
-Người dân Hà Nội: 'Xót xa khi nghe gió bão rít, cây đổ rầm rầm'
-Hà Nội tan hoang sau bão Yagi. Video: Lộc Chung - Văn Ngọc - Bá Nam
-Bộ Tài nguyên và Môi trường đánh giá dự báo của Việt Nam về cường độ, hướng đi của bão Yagi sát với thực tế từ khi ở vịnh Bắc Bộ cũng như khi vào đất liền. Dự báo hai ngày tới hoàn lưu bão Yagi sẽ gây mưa lớn cho đồng bằng, trung du và miền núi phía Bắc, lượng mưa trung bình 24 giờ có thể lên tới 100-150 mm, có nơi lên đến hơn 200 mm.Trên các sông nhỏ ở Quảng Ninh, Lạng Sơn, Cao Bằng, Hòa Bình, lũ có thể lên mức báo động 2-3. Các tỉnh thành Quảng Ninh, Hải Phòng, Lạng Sơn, Thái Nguyên, Cao Bằng, Hà Giang, Yên Bái, Bắc Kạn, Nam Định, Thái Bình, Hà Nam, Hà Nội có nguy cơ cao ngập lụt do mưa lớn.Nhiều địa phương như Quảng Ninh, Lạng Sơn, Bắc Kạn, Thái Nguyên, Bắc Giang, Vĩnh Phúc, Hòa Bình, Phú Thọ, Tuyên Quang, Yên Bái, Sơn La, Lai Châu, Lào Cai, Thanh Hòa đối diện nguy cơ lũ ống, lũ quét, sạt lở đất.Viết Tuân - Gia Chính</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>08/09/2024</t>
-        </is>
-      </c>
+          <t>10 ngày sau bão Yagi, 80% số người chết và mất tích trên cả nước thuộc ba tỉnh Lào Cai, Cao Bằng, Yên Bái - cũng là những địa phương hứng chịu lũ quét và sạt lở nghiêm trọng nhất.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update conversation history token limit, enhance embedding input formatting, and improve README documentation
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,540 +463,311 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tuyên bố chung về việc thiết lập quan hệ Đối tác toàn diện Việt Nam - Mông Cổ</t>
+          <t>Việt Nam bình luận về việc dẫn độ kẻ chủ mưu vụ khủng bố Đăk Lăk</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://vtv.vn/chinh-tri/tuyen-bo-chung-ve-viec-thiet-lap-quan-he-doi-tac-toan-dien-viet-nam-mong-co-20241001065058779.htm</t>
+          <t>https://vnexpress.net/viet-nam-binh-luan-ve-viec-dan-do-ke-chu-muu-vu-khung-bo-dak-lak-4805424.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nhân dịp chuyến thăm cấp Nhà nước tới Mông Cổ của Tổng Bí thư, Chủ tịch nước Tô Lâm, hai bên đã ra Tuyên bố chung về việc thiết lập quan hệ Đối tác toàn diện Việt Nam - Mông Cổ.</t>
+          <t>Người phát ngôn Bộ Ngoại giao nói việc dẫn độ Y Quynh Bdap từ Thái Lan về Việt Nam là phù hợp, nhằm đảm bảo "mọi đối tượng phạm tội đều bị pháp luật xử lý".</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Trong khuôn khổ chuyến thăm cấp Nhà nước tới Mông Cổ từ ngày 30/9-1/10, Tổng Bí thư, Chủ tịch nước Tô Lâm đã hội đàm với Tổng thống Ukhnaagiin Khurelsukh, hội kiến Chủ tịch Quốc hội Dashzegviin Amarbayasgalan và Thủ tướng Luvsannamsrain Oyun-Erdene.Nhân dịp này, hai bên đã ra Tuyên bố chung về việc thiết lập quan hệ Đối tác toàn diện Việt Nam-Mông Cổ.VTV Times xin trân trọng giới thiệu toàn văn Tuyên bố chung:1. Nhân kỷ niệm 70 năm thiết lập quan hệ ngoại giao Việt Nam-Mông Cổ, nhận lời mời của Tổng thống Mông Cổ Ukhnaagiin Khurelsukh và Phu nhân, Tổng Bí thư Ban Chấp hành Trung ương Đảng Cộng sản Việt Nam, Chủ tịch nước Cộng hòa Xã hội Chủ nghĩa Việt Nam Tô Lâm đã thăm cấp Nhà nước tới Mông Cổ từ ngày 30/9-1/10/2024.Trong khuôn khổ chuyến thăm, Tổng Bí thư, Chủ tịch nước Tô Lâm đã hội đàm với Tổng thống Ukhnaagiin Khurelsukh, hội kiến Chủ tịch Quốc hội Dashzegviin Amarbayasgalan và Thủ tướng Luvsannamsrain Oyun-Erdene.2. Lãnh đạo cấp cao hai nước đánh giá cao quan hệ hữu nghị truyền thống Việt Nam-Mông Cổ tăng cường mở rộng mạnh mẽ trong suốt 70 năm qua; trao đổi ý kiến sâu rộng về phương hướng phát triển quan hệ song phương thời gian tới và các vấn đề khu vực, quốc tế cùng quan tâm.Tổng Bí thư, Chủ tịch nước Tô Lâm và Tổng thống Mông Cổ Ukhnaagiin Khurelsukh chụp ảnh chung. (Ảnh: TTXVN)3. Phía Mông Cổ khẳng định luôn coi Việt Nam là đối tác quan trọng tại khu vực Đông Nam Á, mong muốn phát triển mở rộng quan hệ hợp tác cùng có lợi trên tất cả các lĩnh vực.Việt Nam khẳng định coi trọng phát triển quan hệ với Mông Cổ, tôn trọng chính sách đối ngoại yêu chuộng hòa bình, rộng mở, tự chủ và đa trụ cột của Mông Cổ, chính sách "láng giềng thứ ba" và mong muốn thúc đẩy quan hệ hai nước phát triển hơn nữa trong thời gian tới.4. Lãnh đạo cấp cao hai nước nhất trí cho rằng việc phát triển và làm sâu sắc quan hệ giữa Việt Nam và Mông Cổ phù hợp với lợi ích chung của nhân dân hai nước, góp phần quan trọng vào việc bảo đảm hòa bình, ổn định và phát triển của khu vực và thế giới; nhất trí nâng cấp quan hệ hai nước lên "Đối tác toàn diện" và tiếp tục thúc đẩy mở rộng hợp tác, cụ thể như sau:I. Tăng cường hợp tác chính trị5. Hai bên nhất trí tăng cường hoạt động trao đổi đoàn, giao lưu, tiếp xúc cấp cao và các cấp thông qua các kênh Đảng, Nhà nước, Chính phủ, Quốc hội; nhất trí ủng hộ về mặt chính sách mở rộng quan hệ mật thiết giữa nhân dân hai nước; nghiên cứu khả năng thiết lập cơ chế hợp tác mới giữa các bộ, ngành, địa phương hai nước.6. Hai bên nhất trí tăng cường hợp tác giữa các Cơ quan lập pháp, trong đó phát triển hợp tác giữa các Ủy ban chuyên môn, nhóm nghị sỹ, nghị sỹ trẻ và nữ nghị sỹ tương xứng với khuôn khổ quan hệ mới; thúc đẩy ký mới Thỏa thuận hợp tác giữa hai Quốc hội thay thế Thỏa thuận đã ký năm 2018.Chiều 30/9, tại Cung Nhà nước ở thủ đô Ulan Bator, Tổng Bí thư, Chủ tịch nước Tô Lâm hội kiến Thủ tướng Mông Cổ Luvsannamsrain Oyun-Erdene. (Ảnh: TTXVN)7. Hai bên nhất trí duy trì hiệu quả cơ chế Tham khảo chính trị luân phiên cấp Thứ trưởng Ngoại giao; thường xuyên trao đổi về hợp tác song phương, chính sách đối ngoại, các vấn đề quốc tế và khu vực cùng quan tâm; nghiên cứu hình thức thiết lập cơ chế đàm phán đa phương.II. Mở rộng hợp tác quốc phòng, an ninh và thực thi pháp luật8. Hai bên đánh giá cao những tiến triển mới trong hợp tác quốc phòng và an ninh thời gian gần đây; nhất trí tiếp tục duy trì gặp gỡ, tiếp xúc, trao đổi đoàn các cấp.9. Hai bên nhấn mạnh tầm quan trọng của việc tiếp tục mở rộng hợp tác giữa các lực lượng vũ trang và cơ quan thực thi pháp luật hai nước.10. Hai bên nhất trí triển khai hiệu quả các thỏa thuận hợp tác đã ký, đẩy nhanh thủ tục đàm phán tiến tới ký kết các hiệp định trong lĩnh vực an ninh, phòng chống tội phạm; tăng cường hợp tác trao đổi thông tin tội phạm liên quan; phối hợp đánh giá, dự báo về các vấn đề liên quan tới lợi ích và an ninh quốc gia hai nước.Tổng Bí thư, Chủ tịch nước Tô Lâm hội đàm với Tổng thống Mông Cổ Ukhnaagiin Khurelsukh. (Ảnh: TTXVN)III. Mở rộng hợp tác kinh tế-thương mại và đầu tư11. Lãnh đạo cấp cao hai bên nhất trí thúc đẩy hợp tác kinh tế thực chất, hiệu quả và toàn diện; duy trì các cơ chế hợp tác kinh tế song phương, trong đó có cơ chế Ủy ban liên Chính phủ về hợp tác kinh tế, thương mại, khoa học và kỹ thuật; nhất trí tăng cường vai trò của Hội đồng Doanh nghiệp hai bên thông qua hỗ trợ triển khai các hoạt động xúc tiến thương mại, thúc đẩy kết nối hợp tác doanh nghiệp trong khuôn khổ Thỏa thuận hợp tác đã ký giữa Liên đoàn Thương mại và Công nghiệp Việt Nam và Phòng Thương mại và Công nghiệp Mông Cổ.12. Lãnh đạo cấp cao hai nước nhất trí nghiên cứu các giải pháp phù hợp cải thiện môi trường đầu tư; xem xét ký mới Hiệp định Khuyến khích và Bảo hộ đầu tư.IV. Thúc đẩy hợp tác thực chất về các lĩnh vực nông nghiệp, khoa học, giao thông vận tải, văn hóa, thể thao, du lịch, giáo dục, lao động, môi trường và bảo trợ xã hội13. Lãnh đạo cấp cao hai bên nhất trí đẩy mạnh hiện đại hóa chương trình hợp tác nông nghiệp trong khuôn khổ Bản ghi nhớ giữa Bộ Lương thực, Nông nghiệp và Công nghiệp nhẹ Mông Cổ và Bộ Nông nghiệp và Phát triển nông thôn Việt Nam về hợp tác trong lĩnh vực nông nghiệp ký năm 2022.14. Hai bên nhất trí tăng cường trao đổi chính sách, định hướng, giải pháp phát triển ngành nông nghiệp hai bên; tạo môi trường pháp lý xuất khẩu các sản phẩm nguồn gốc nông nghiệp có thế mạnh của hai bên; hỗ trợ nghiên cứu, ứng dụng công nghệ cao trong lĩnh vực nông nghiệp.15. Hai bên nhất trí thúc đẩy hiện thực hóa các thỏa thuận/cam kết trong khuôn khổ Ủy ban liên Chính phủ, trong đó có cơ chế Tiểu ban Khoa học và Công nghệ; tăng cường hợp tác nghiên cứu, phát triển khoa học công nghệ cao, công nghệ số, đổi mới sáng tạo và thông tin truyền thông.   Thiết lập quan hệ “Đối tác toàn diện Việt Nam - Mông Cổ” VTV.vn - Tổng Bí thư, Chủ tịch nước Tô Lâm và Tổng thống Mông Cổ bày tỏ vui mừng, hài lòng trước sự phát triển mạnh mẽ, thực chất, hiệu quả của quan hệ hữu nghị truyền thống giữa hai nước. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>"Y Quynh Bdap là đối tượng đã trực tiếp tuyển mộ, kích động và chỉ đạo thực hiện vụ khủng bố ngày 11/6/2023 tại tỉnh Đăk Lăk, gây hậu quả đặc biệt nghiêm trọng. Đối tượng này đã bị TAND tỉnh Đăk Lăk xét xử và kết án 10 năm tù về tội khủng bố", người phát ngôn Bộ Ngoại giao Phạm Thu Hằng cho biết hôm nay, khi được hỏi về thông tin tòa án Thái Lan đã quyết định dẫn độ Y Quynh Bdap về Việt Nam.Bà Hằng khẳng định việc dẫn độ Y Quynh Bdap là "phù hợp và nhằm bảo đảm mọi đối tượng phạm tội đều phải bị xử lý trước pháp luật". Các cơ quan chức năng Việt Nam sẽ tiếp tục phối hợp với các cơ quan chức năng Thái Lan để xử lý sự việc theo đúng quy định của pháp luật hai nước.
+Y Quynh Bdap khi bị bắt ở Thái Lan hồi tháng 6. Ảnh: Bangkok Post
+TAND tỉnh Đăk Lăk ngày 20/1 ra phán quyết với các bị cáo trong vụ tấn công trụ sở xã Ea Ktur và Ea Tiêu, khiến 9 cán bộ và người dân thiệt mạng ngày 11/6/2023. Y Quynh Bdap nằm trong số 6 bị cáo đang trốn truy nã ở nước ngoài và bị phạt 10 năm tù.Y Quynh Bdap sống ở Thái Lan từ năm 2018. Anh ta bị giới chức Thái Lan bắt hôm 11/6 với cáo buộc quá hạn thị thực.Truyền thông Thái Lan đưa tin Tòa án Hình sự ở Bangkok hôm 30/9 chấp thuận yêu cầu dẫn độ của Việt Nam với Y Quynh Bdap. Y Quynh Bdap đang bị giam ở nhà tù tại Bangkok và có 30 ngày để kháng án, theo Bangkok Post. Chính phủ Thái Lan có 90 ngày để thực hiện lệnh dẫn độ Y Quynh Bdap.Phạm Giang</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tổng Bí thư, Chủ tịch nước Tô Lâm thăm cấp Nhà nước tới Ireland: Đánh dấu mối quan hệ ngày càng sâu sắc giữa hai nước</t>
+          <t>Hàng từ bên kia biên giới</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://vtv.vn/chinh-tri/tong-bi-thu-chu-tich-nuoc-to-lam-tham-cap-nha-nuoc-toi-ireland-danh-dau-moi-quan-he-ngay-cang-sau-sac-giua-hai-nuoc-20240930132458974.htm</t>
+          <t>https://vnexpress.net/hang-tu-ben-kia-bien-gioi-4805058.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Chuyến thăm cấp Nhà nước của Tổng Bí thư, Chủ tịch nước Tô Lâm tới Ireland sẽ đánh dấu mối quan hệ ngày càng sâu sắc giữa hai nước.</t>
+          <t>Người dùng bây giờ ngồi ở Việt Nam, mua hàng từ Trung Quốc chỉ qua vài click, tiện và rẻ hơn bao giờ hết.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nhận lời mời của Tổng thống Ireland Michael D. Higgins, Tổng Bí thư, Chủ tịch nước Tô Lâm cùng Đoàn đại biểu cấp cao Việt Nam sẽ thăm cấp Nhà nước tới Ireland. Nhân dịp này, Đại sứ Ireland tại Việt Nam Deirdre Ní Fhallúin đã trả lời phỏng vấn về quan hệ hai nước và nội dung khác liên quan đến chuyến thăm của Tổng Bí thư, Chủ tịch nước Tô Lâm.Phóng viên: Tổng Bí thư Đảng Cộng sản Việt Nam, Chủ tịch nước Cộng hòa xã hội chủ nghĩa Việt Nam Tô Lâm sẽ có chuyến thăm cấp Nhà nước tới Cộng hòa Ireland. Xin Đại sứ cho biết ý nghĩa của chuyến thăm quan trọng này đối với quan hệ hai nước?Đại sứ Deirdre Ní Fhallúin: Kể từ khi Đại sứ quán Ireland được mở tại Việt Nam vào năm 2005, quan hệ giữa hai nước trở nên gắn bó mật thiết và được củng cố bằng nhiều chương trình hợp tác phát triển. Chúng tôi tập trung vào việc hỗ trợ cộng đồng dân tộc thiểu số tại Việt Nam; còn đối với các hoạt động hỗ trợ nhân đạo liên quan tới bom mìn, chúng tôi phối hợp với các đối tác làm sạch những vùng đất bị ô nhiễm bom mìn, vật nổ, nâng cao nhận thức về bom mìn tại các trường học và hỗ trợ nạn nhân bom mìn.Việt Nam tiếp tục ghi nhận tăng trưởng ấn tượng trong những năm qua. Cả hai nước đã tăng cường hợp tác song phương trong lĩnh vực nông nghiệp, thực phẩm và giáo dục đại học, tập trung vào hỗ trợ kỹ thuật, nâng cao năng lực và thiết lập các thể chế liên kết.Tổng thống Michael D.Higgins có chuyến thăm cấp Nhà nước tới Việt Nam vào năm 2016. Chuyến thăm này được ghi nhớ ở cả hai quốc gia, vì vậy chúng tôi rất vui mừng chào đón chuyến thăm cấp Nhà nước sắp tới của Tổng Bí thư, Chủ tịch nước Tô Lâm tới Ireland, đánh dấu mối quan hệ ngày càng sâu sắc giữa hai nước chúng ta.Phóng viên: Sau gần 30 năm thiết lập quan hệ ngoại giao, quan hệ hợp tác song phương hai nước đạt nhiều kết quả tích cực. Xin Đại sứ chia sẻ rõ hơn những dấu ấn nổi bật trong quan hệ hợp tác giữa hai nước thời gian qua cũng như triển vọng phát triển trong thời gian tới?Đại sứ Deirdre Ní Fhallúin: Chúng tôi rất tự hào về chương trình hợp tác phát triển lâu dài với Việt Nam, đặc biệt là các chương trình hỗ trợ các nhóm dân tộc thiểu số, hỗ trợ nhân đạo liên quan đến bom mìn, cũng như các chương trình về dinh dưỡng và sức khỏe bà mẹ và nỗ lực trong việc tăng cường khả năng phục hồi trước biến đổi khí hậu.Gần đây, chúng tôi viện trợ nhân đạo 250.000 Euro cho Việt Nam để khắc phục hậu quả của bão Yagi (cơn bão số 3) gây thiệt hại ở các tỉnh, thành phố phía Bắc Việt Nam. Khoản viện trợ này thông qua Quỹ Nhi đồng Liên hợp quốc (UNICEF), đã và đang hỗ trợ khẩn cấp nước sạch và vật tư vệ sinh cho các gia đình bị ảnh hưởng.Tôi rất vui mừng khi thấy mối quan hệ song phương giữa Ireland và Việt Nam phát triển trong những năm qua, kể từ khi chúng tôi mở Đại sứ quán ở Việt Nam. Chúng tôi mong muốn tăng cường hợp tác với Việt Nam trong các lĩnh vực như giáo dục và nông sản, cũng như mở rộng quan hệ thương mại giữa hai nước.Mối quan hệ giữa Ireland và Việt Nam sẽ tiếp tục phát triển và phát triển theo hướng tích cực. Chuyến thăm cấp Nhà nước của Tổng thống Michael D. Higgins tới Việt Nam gần một thập kỷ trước là một cột mốc quan trọng trong mối quan hệ song phương của chúng ta. Chuyến thăm của Tổng Bí thư, Chủ tịch nước Tô Lâm sắp tới sẽ đánh dấu một bước tiến quan trọng nữa và tôi rất vui mừng khi chuyến thăm này diễn ra. Với cương vị là Đại sứ Ireland ở Việt Nam, tôi sẽ nỗ lực để làm sâu sắc hơn và củng cố hơn nữa mối quan hệ hai nước chúng ta.Phóng viên: Việt Nam đang đẩy mạnh chuyển đổi số, chuyển đổi xanh và phát triển nền kinh tế sáng tạo, tuần hoàn. Đây cũng là những thế mạnh của Ireland. Đại sứ cho biết Ireland có kế hoạch hợp tác, hỗ trợ thế nào với Việt Nam trong các lĩnh vực này?Đại sứ Deirdre Ní Fhallúin:  Vào nửa cuối thế kỷ vừa qua, Ireland chứng kiến sự phát triển tột bậc và tăng trưởng kinh tế nhanh chóng. Đất nước chúng tôi được mệnh danh là "Thung lũng Silicon của châu Âu" và được biết đến trên toàn thế giới là một trung tâm về dược phẩm và công nghệ (Ireland là nơi đặt trụ sở của các công ty công nghệ hàng đầu thế giới như Google, Meta) và giáo dục chất lượng cao.Từ hành trình phát triển của mình, chúng tôi hiểu giáo dục có vai trò quan trọng như thế nào đối với sự phát triển của đất nước. Chúng tôi đã hỗ trợ sinh viên Việt Nam theo học các chương trình thạc sĩ toàn phần thông qua chương trình học bổng Chính phủ Ireland: "Ireland Fellows Programme". Chúng tôi hy vọng rằng du học sinh Việt Nam sau khi trở về nước sẽ trở thành cầu nối lâu dài giữa hai quốc gia.Đại sứ quán Ireland tại Việt Nam đang tăng cường hợp tác với các trường đại học, viện nghiên cứu ở cả hai nước để chia sẻ kinh nghiệm và xây dựng năng lực trong lĩnh vực ưu tiên như nông nghiệp và thực phẩm. Chương trình Đối tác nông nghiệp thực phẩm Ireland – Việt Nam (IVAP) là một ví dụ điển hình về hợp tác mạnh mẽ của chúng tôi trong lĩnh vực này.Là một quốc đảo nhỏ, Ireland cũng đối mặt với thách thức ngày càng tăng và cấp bách từ biến đổi khí hậu. Hai nước chúng ta cần hợp tác để giải quyết thách thức này. Chúng tôi đang giúp các vùng nông thôn tại Việt Nam tăng cường khả năng thích ứng với biến đổi khí hậu cũng như mở rộng hợp tác và nghiên cứu giữa các trường đại học trong các lĩnh vực biến đổi khí hậu và bền vững.Phóng viên: Trân trọng cảm ơn Đại sứ!* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Taobao, Temu, 1688 là những tên tuổi mới ở một thị trường thương mại điện tử (TMĐT) hấp dẫn và sôi nổi. Với tốc độ tăng trưởng 25% năm 2023, TMĐT Việt Nam thuộc nhóm 10 quốc gia có tốc độ tăng trưởng nhanh nhất thế giới.Theo số liệu dự đoán từ Trung tâm Thông tin Công nghiệp và Thương mại (Bộ Công Thương), tổng doanh thu TMĐT bán lẻ hàng hóa cả năm 2024 có thể tăng khoảng 45% so với 2023, lên gần 30 tỷ USD, chiếm xấp xỉ 14% tổng mức bán lẻ hàng hóa của cả nước. Miếng bánh thị trường TMĐT đang được chiếm lĩnh bởi Shopee (khoảng 67,9%) và TikTok shop (23,2%), riêng hai sàn này đã chiếm lĩnh hơn 91% thị phần, tiếp đến là Lazada, Tiki và Sendo.Các sàn TMĐT có yếu tố Việt Nam đang dần hụt hơi trong cuộc đua thị phần. Với sự gia nhập thêm của Taobao, Temu, 1688, cuộc chơi sẽ thêm phần cạnh tranh khốc liệt.Các "tay chơi" mới, với mô hình kinh doanh khác biệt, rõ ràng mang đến làn gió mới mà mỗi đối tượng tiếp nhận sẽ có những góc nhìn khác nhau.Người tiêu dùng đón nhận khá tích cực. Năm 2024, kinh tế đã khởi sắc nhưng còn nhiều khó khăn, người tiêu dùng vẫn đang thắt chặt "hầu bao". Nghiên cứu của NielsenIQ năm 2024 cho thấy 89% người tiêu dùng Việt Nam tìm kiếm mức giá thấp hơn, 72% giảm tổng chi tiêu, 62% lựa chọn nấu ăn tại nhà. Các nhóm mặt hàng không cần thiết và xa xỉ đều bị cắt giảm.Như vậy, với sự tham gia của các sàn mới, khách hàng có thêm lựa chọn. Trước đây, người dùng ở Việt Nam vẫn mua hàng trên Taobao nhưng phải đặt và nhận hàng thông qua đại lý. Do đó, trải nghiệm về giá và thời gian giao hàng chưa thật cạnh tranh so với sàn nội địa. Giờ đây, họ có thể mua được với giá tốt, giao hàng nhanh, đôi khi nhanh hơn đặt trong nước, nhờ những tổng kho tại biên giới Trung Quốc - Việt Nam.Thực tế này đặt ra cho nhà quản lý, đặc biệt là cơ quan thuế và hải quan, nhiều thách thức. Theo số liệu của Bộ Thông tin và Truyền thông, nửa đầu năm nay, mỗi ngày có 4-5 triệu đơn hàng từ Trung Quốc về Việt Nam với giá trị khoảng 50 triệu USD không phải đóng thuế. Theo Quyết định 78/2010, hàng hoá nhập khẩu gửi qua dịch vụ chuyển phát nhanh có trị giá từ 1.000.000 đồng trở xuống được miễn thuế nhập khẩu và thuế GTGT. Một container đầy hàng từ Trung Quốc sang Việt Nam, chia nhỏ có thể chứa 15.000 đơn hàng, nếu đáp ứng giá trị dưới một triệu đồng mỗi đơn, sẽ không phải thực hiện các hoạt động kiểm tra chuyên ngành hay đóng thuế.Điều này tạo ra môi trường bất bình đẳng khi các doanh nghiệp Trung Quốc được hưởng các ưu đãi cho hàng hoá xuất khẩu, trong khi nhà sản xuất, doanh nghiệp Việt Nam hoạt động trong nước phải thực hiện đầy đủ nghĩa vụ thuế nội địa. Nhiều quốc gia như Mỹ hoặc Liên minh châu Âu cũng "đau đầu" với các gói hàng giá trị thấp và cân nhắc bỏ quy định giá trị tối thiểu hàng miễn thuế. Thái Lan từ đầu 2021 đã tiến hành thu thuế giá trị gia tăng 7% với tất cả hàng hoá nhập khẩu, không phân biệt giá trị. Singapore cũng làm tương tự từ năm 2023.Quyết định miễn hay thu thuế đều rất khó khăn. Nếu tiếp tục miễn thuế sẽ khó hỗ trợ sản xuất trong nước, nhưng đánh thuế thì lại xung đột với lợi ích người tiêu dùng, hơn hết là phải có nhân sự và hệ thống để đảm nhận khối lượng công việc khổng lồ.Lo lắng và áp lực cũng là cảm xúc của các nhà thương mại, sản xuất tại Việt Nam lúc này. Hàng Trung Quốc vốn có lợi thuế về giá rẻ, mẫu mã đẹp, luôn sẵn sàng tại các tổng kho gần biên giới, lại thêm được sự "hậu thuẫn" từ các nền tảng TMĐT. Trong khi các nhà sản xuất trong nước đang gặp nhiều khó khăn: sản xuất còn phân tán, chưa có năng lực tự động hóa cao khi phải xử lý nhiều đơn hàng. Đặc biệt, chi phí logistics cao, làm cho hàng hoá sản xuất trong nước thiếu cạnh tranh với nước ngoài.Báo cáo Logistics Việt Nam 2023 cho thấy 15-20% chi phí sản xuất kinh doanh nằm ở khâu logistics, trong khi trung bình thế giới chỉ 8-10%. Không những với các doanh nghiệp sản xuất, doanh nghiệp thương mại, đại lý cũng đang dần bị loại bỏ khỏi các khâu trung gian của các nhà sản xuất Trung Quốc. Với mô hình mới của Temu D2C (Direct-to-Consumer), hàng hoá được chuyển từ nhà sản xuất đến tay khách hàng gần như trực tiếp. Đây có thể nói là biến thể hiện đại của chuỗi cung ứng, vai trò của trung gian dần bị loại bỏ, đồng nghĩa với giảm chi phí.Tổng hợp lại, Temu, Taobao, 1688 đang có tiềm năng trở thành thế lực mới của TMĐT, và hiện trạng TMĐT xuyên biên giới một chiều (từ Trung Quốc sang Việt Nam là chủ yếu) càng khẳng định điều đó. Nhưng thành quả đó không phải một sớm một chiều mà có được. Đó là cả một chiến lược phát triển tổng thể và toàn diện. Trung Quốc từ lâu được biết đến với hệ thống hạ tầng và logistics được đầu tư đồng bộ từ đường biển, đường bộ, đường sắt đến đường hàng không. Các tổng kho được xây dựng dọc biên giới theo chiến lược lâu dài cho mục tiêu thương mại xuyên biên giới; không những vậy, các nhà sản xuất nội địa Trung Quốc cũng xây dựng những tổng kho riêng với phương châm "khi cần là có".Quy mô sản xuất lớn, tự động hóa tốt, khả năng xử lý đơn hàng cực cao đã góp phần phân phối các sản phẩm sản xuất tại Trung Quốc đi khắp nơi. Không những đầu tư tốt từ phía bên kia biên giới, ngay tại Việt Nam, các đơn vị giao hàng cũng có mối liên hệ hợp tác chặt chẽ với các sàn TMĐT để thời gian giao hàng là nhanh nhất.Từ đó nhìn lại, hệ thống logistics và các dịch vụ hỗ trợ cho các doanh nghiệp Việt vẫn còn phân tán và thiếu chuẩn hoá. Hạ tầng kho bãi chưa đồng bộ, còn qua nhiều khâu trung gian. Các hình thức như tổng kho chưa nhiều, hoặc có cũng chỉ phục vụ cho một số doanh nghiệp quy mô lớn.Doanh nghiệp Việt Nam chỉ có thể gom đơn hàng 1-2 lần/ngày, dẫn đến việc chậm trễ trong giao hàng. Đóng gói và xử lý đơn hàng chưa được thực hiện với mức độ tự động và chuẩn hóa cao, cũng góp phần làm tăng chi phí giao hàng. Bên cạnh đó, các đơn vị chuyển phát nội địa có dấu hiệu hụt hơi khi cạnh tranh với các đơn vị nước ngoài vốn được đầu tư tốt và chuyển đổi công nghệ đồng bộ hơn.Thay đổi hành vi của khách hàng là không thể, vì họ được quyền lựa chọn những gì phù hợp nhất. Để thích nghi với môi trường mới, các nhà sản xuất và thương mại trong nước cần sự hỗ trợ từ các cơ quan quản lý. Phát triển một nền sản xuất mạnh mẽ và một hệ thống logistics hiệu quả không phải là việc đơn giản, nhưng là điều cần thiết để nâng cao sức cạnh tranh của hàng hóa Việt Nam trong bối cảnh thương mại toàn cầu đang ngày càng phát triển.Một cây kim, sợi chỉ được sản xuất và giao đến tay khách hàng đã là cả một quá trình phức tạp. Để cho nó cạnh tranh được, còn cần đến nỗ lực vĩ mô hơn.Nguyễn Minh Kha</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bão số 5 đi vào Bắc Biển Đông, mạnh lên thành siêu bão</t>
+          <t>Chính thức chuyển giao hai ngân hàng 0 đồng</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://vtv.vn/xa-hoi/bao-so-5-di-vao-bac-bien-dong-manh-len-thanh-sieu-bao-20241001085942471.htm</t>
+          <t>https://vnexpress.net/chinh-thuc-chuyen-giao-hai-ngan-hang-0-dong-4805009.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VTV.vn - Sáng sớm nay (1/10), bão Krathon đã đi vào vùng biển phía Đông Bắc của khu vực Bắc Biển Đông, mạnh lên cấp 16 (cấp siêu bão).</t>
+          <t>Hai ngân hàng CBBank, Oceanbank chiều nay được chuyển giao bắt buộc về Vietcombank và MB.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Theo Trung tâm Dự báo Khí tượng Thủy văn Quốc gia, hồi 7h ngày 1/10, vị trí tâm bão ở vào khoảng 20,6 độ Vĩ Bắc; 119,6 độ Kinh Đông, trên vùng biển phía Đông Bắc của khu vực Bắc Biển Đông. Sức gió mạnh nhất vùng gần tâm bão mạnh cấp 16 (184 - 201 km/h), giật trên cấp 17. Di chuyển theo hướng Tây Tây Bắc, tốc độ khoảng 5 km/h.Dự báo đến thời điểm hiện tại, bão Krathon (bão số 5) không có khả năng ảnh hưởng đến vùng ven biển và đất liền nước ta.Từ 72 đến 120 giờ tiếp theo, bão di chuyển chủ yếu theo hướng Bắc Đông Bắc, mỗi giờ đi được khoảng 10 km, cường độ tiếp tục suy yếu thêm.Do ảnh hưởng của bão Krathon, vùng biển phía Đông Bắc khu vực Bắc Biển Đông (phía Bắc vĩ tuyến 18,0N; phía Đông kinh tuyến 116,5E) gió mạnh cấp 10 - 13, vùng gần tâm bão cấp 14 - 16, giật trên cấp 17, sóng biển cao 9 - 11 m; biển động dữ dội.Tàu thuyền hoạt động trong các vùng nguy hiểm nói trên đều chịu tác động của dông, lốc, gió mạnh, sóng lớn.Với Philippines, luồng gió thổi về phía hoàn lưu của bão cũng có thể mang theo gió giật mạnh đến các khu vực ven biển và vùng cao tiếp xúc với gió như Vùng Ilocos, Vùng hành chính Cordillera, các phần phía bắc và phía đông của đất liền Cagayan, phần phía đông của Isabela, Aurora, Zambales, Bataan, Metro Manila, Calabarzon, Romblon và Camarines Norte.Cục Quản lý Thiên văn, Địa vật lý và Khí quyển Philippines (PAGASA) dự báo nguy cơ trung bình đến cao về sóng lớn đe dọa tính mạng trong 48 giờ tới ở vùng trũng thấp hoặc tiếp xúc các địa phương ven biển của Quần đảo Batanes và Babuyan.Cảnh báo về bão lớn được ban hành trên bờ biển phía bắc và phía tây của Bắc Luzon. Biển động mạnh với sóng cao lên đến 7 m trên bờ biển Batanes; 6 m trên bờ biển Quần đảo Babuyan và Ilocos Norte; 4,5 m trên bờ biển phía bắc Ilocos Sur.Bão Krathon (Julian) dự kiến ​​sẽ vòng lại về phía biển phía tây nam Đài Loan (Trung Quốc) từ ngày 1/10 đến sáng 2/10.Theo dự báo đường đi, siêu bão sẽ đổ bộ dọc theo bờ biển phía tây nam Đài Loan (Trung Quốc) vào sáng hoặc chiều 2/10. Bão sẽ băng qua địa hình gồ ghề của Đài Loan trước khi xuất hiện trên biển phía đông Đài Loan vào tối 2/10 hoặc sáng sớm thứ Năm (3/10). Sau đó, bão sẽ di chuyển về hướng đông bắc hướng tới Biển Hoa Đông, ra khỏi khu vực dự báo của Philippines (PAR) vào chiều hoặc tối 3/10, rồi chuyển hướng tây bắc vào thứ Sáu (4/10) khi đi qua Biển Hoa Đông.Bão vẫn có cơ hội tiếp tục tăng cấp trong thời gian ngắn trong 24 giờ tới. Sau đó, tương tác ngày càng tăng với địa hình đồi núi của Đài Loan (Trung Quốc) sẽ làm bão yếu đi một chút trước khi đổ bộ vào đất liền.   Bão số 5 gây sóng lớn ở Đông Bắc Biển Đông VTV.vn - Bão Krathon đã đi vào vùng biển phía Đông Bắc của khu vực Bắc Biển Đông, trở thành cơn bão số 5 trong năm 2024. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Họp báo về hoạt động ngành ngân hàng quý III, chiều 17/10, ông Nguyễn Đức Long, Phó chánh thanh tra Cơ quan Thanh tra giám sát (Ngân hàng Nhà nước), cho biết chiều nay sẽ diễn ra lễ chuyển giao hai ngân hàng bắt buộc là Ngân hàng Xây dựng (CBBank) và Ngân hàng Đại Dương (OceanBank).Trong đó, Ngân hàng Ngoại Thương Việt Nam (Vietcombank) nhận chuyển giao CBBank, còn Ngân hàng Quân Đội (MB) nhận OceanBank.Hai ngân hàng khác là Ngân hàng Dầu khí Toàn cầu (GPBank) và Ngân hàng Đông Á (DongA Bank) dự kiến sẽ tiếp tục hoàn thiện phương án và chuyển giao trong tương lai.Về quyền lợi của người gửi tiền, ông Long khẳng định sẽ được đảm bảo "trước, trong và sau quá trình chuyển giao". Mục tiêu chuyển giao để đưa các ngân hàng yếu kém quay về hoạt động bình thường, khắc phục lỗ lũy kế, đảm bảo các quy định về an toàn hoạt động.Oceanbank xuất thân là Ngân hàng nông thôn Hải Hưng. Sau khi được ông Hà Văn Thắm tham gia mua lại cổ phần, nhà băng này chuyển đổi mô hình sang ngân hàng đô thị, đổi tên thành Ngân hàng Đại Dương vào 2007. Sau sự kiện ông Thắm bị bắt, Oceanbank được Ngân hàng Nhà nước mua lại giá 0 đồng và Vietinbank hỗ trợ quản trị.
+Biển hiệu ngân hàng OceanBank sáng 17/10. Ảnh: Quỳnh Trang
+Còn CBBank tiền thân là Ngân hàng nông thôn Rạch Kiến, được chuyển đổi lên mô hình đô thị năm 2006 với tên gọi là Đại Tín (TrustBank). Năm 2013, Tập đoàn Thiên Thanh đã cùng một số cổ đông tham gia góp vốn và tái cấu trúc Trust Bank, đổi tên thành Ngân hàng Xây dựng Việt Nam (VNCB). Đến 2015, Ngân hàng Nhà nước mua lại VNCB với giá 0 đồng, được Vietcombank tham gia hỗ trợ, quản trị điều hành, sau đó đổi tên thương hiệu thành CBBank.Trước đó, tại đại hội cổ đông thường niên các năm gần đây, lãnh đạo của MB và Vietcombank từng chia sẻ, việc nhận chuyển giao bắt buộc không yêu cầu nhà băng nhận chuyển giao phải bỏ tiền mua, do đây là đơn vị yếu kém trong diện tái cơ cấu đã được mua lại 0 đồng.Để xử lý khoản lỗ lũy kế của ngân hàng 0 đồng, lãnh đạo MB nói biện pháp quan trọng nhất vẫn là sự hỗ trợ của Ngân hàng Nhà nước. Theo đó, ngân hàng nhận chuyển giao sẽ được vay với lãi suất 0% trong thời gian tái cơ cấu, được phép tăng trưởng quy mô cao hơn.Nếu tái cơ cấu không thành công, ngân hàng nhận chuyển giao không thể trả lại ngân hàng 0 đồng cho Nhà nước, nhưng có thể bán đi như một khoản đầu tư hoặc IPO chuyển thành ngân hàng cổ phần, lãnh đạo MB cũng từng chia sẻ thêm.
+Chi nhánh Ngân hàng CBBank trên đường Nguyễn Thị Minh Khai, quận 3 sáng 17/10. Ảnh: Quỳnh Trang
+Theo lãnh đạo Vietcombank, tổ chức nhận chuyển giao sẽ có quyền định đoạt, xử lý ngân hàng chuyển giao bắt buộc: nếu tìm được tổ chức nước ngoài phù hợp, có thể bán tổ chức nhận chuyển giao, duy trì hoặc có phương án khác như chuyển đổi, cải cách, chẳng hạn như chuyển sang ngân hàng số. Còn nếu tái cơ cấu thành công, ngân hàng 0 đồng có thể sáp nhập vào ngân hàng nhận chuyển giao bắt buộc là Vietcombank, MB.Oceanbank và CBBank là hai ngân hàng cùng được Ngân hàng Nhà nước mua lại giá 0 đồng trong năm 2015. Ngoài Oceanbank và CBBank, hiện còn một ngân hàng 0 đồng khác là GPBank và hai ngân hàng thuộc diện kiểm soát đặc biệt DongABank và SCB.Quỳnh Trang - Minh Sơn</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Từ hôm nay (1/10), thí điểm cấp Phiếu lý lịch tư pháp trên ứng dụng VNeID</t>
+          <t>'Việt Nam có thể tham khảo Nhật Bản khi làm đường sắt tốc độ cao Bắc Nam'</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://vtv.vn/xa-hoi/tu-hom-nay-1-10-thi-diem-cap-phieu-ly-lich-tu-phap-tren-ung-dung-vneid-20241001065750992.htm</t>
+          <t>https://vnexpress.net/viet-nam-co-the-tham-khao-nhat-ban-khi-lam-duong-sat-toc-do-cao-bac-nam-4805327.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VTV.vn - Từ 1/10/2024, người dân trên cả nước có thể đăng ký cấp Phiếu lý lịch tư pháp trên ứng dụng VNeID mà không phải đến trực tiếp Sở Tư pháp.</t>
+          <t>JICA cho biết Việt Nam có thể tham khảo kinh nghiệm Nhật Bản khi làm đường sắt tốc độ cao Bắc Nam, do nước này phát triển dự án đầu tiên trên thế giới.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Tại Công văn 656/TTg-KSTT năm 2024, Thủ tướng Chính phủ đồng ý với đề nghị của Bộ Tư pháp về việc mở rộng thí điểm cấp Phiếu lý lịch tư pháp trên ứng dụng VNeID trên toàn quốc từ ngày 1/10/2024 đến hết ngày 30/6/2025.Theo đó, Thủ tướng giao Bộ Tư pháp chủ trì, phối hợp với Bộ Công an và các địa phương có liên quan rà soát, xây dựng, ban hành quy trình nghiệp vụ cấp Phiếu lý lịch tư pháp qua ứng dụng VNeID, hoàn thành trước ngày 01/10/2024; hướng dẫn, đôn đốc, kiểm tra việc triển khai thực hiện; kịp thời xử lý các khó khăn, vướng mắc (nếu có).Bộ Tư pháp chủ trì, phối hợp với các bộ, cơ quan có liên quan rà soát, sửa đổi, bổ sung các quy định pháp luật có liên quan thuộc phạm vi quản lý nhà nước của Bộ, bảo đảm đủ cơ sở pháp lý triển khai thực hiện việc cấp Phiếu lý lịch tư pháp qua ứng dụng VNeID trên toàn quốc, hoàn thành trong Quý IV năm 2024.Đồng thời, Bộ Tư pháp chủ trì, phối hợp với Bộ Công an và các bộ, cơ quan, địa phương có liên quan tổ chức tổng kết việc thực hiện thí điểm cấp Phiếu lý lịch tư pháp qua ứng dụng VNeID trong tháng 7 năm 2025.Các bước thực hiện cấp Phiếu lý lịch tư pháp qua VNeID từ 1/10/2024Theo Quy trình 570/TTLLTPQG-QLHG năm 2024, các bước thực hiện thí điểm cấp Phiếu lý lịch tư pháp trên ứng dụng định danh quốc gia VNeID như sau: Bước 1: Công dân kê khai hồ sơ và thực hiện thanh toán phí cung cấp thông tin lý lịch tư pháp trên Ứng dụng VNeIDHồ sơ yêu cầu cấp Phiếu lý lịch tư pháp theo Quy trình thí điểm chỉ có 01 Tờ khai yêu cầu cấp Phiếu lý lịch tư pháp điện từ tương tác đã có sẵn trên Ứng dụng VNeID.Công dân truy cập vào Ứng dụng VNeID, vào mục Thủ tục hành chính/cấp Phiếu lý lịch tư pháp.- Trường hợp công dân dùng tài khoản của mình để yêu cầu cấp Phiếu LLTP thi điền thông tin theo biểu mẫu Tờ khai yêu cầu cấp Phiếu lý lịch tư pháp điện tử tương tác(Biểu mẫu số 12/2024/LLTP ban hành kèm theo Thông tư 06/2024/TT-BTP)- Trường hợp là công dân được ủy quyền yêu cầu cấp Phiếu lý lịch tư pháp thì dùng tài khoản định danh điện tử của mình đăng ký yêu cầu cấp Phiếu lý lịch tư pháp tại biểu mẫu Tờ khai yêu cầu cấp Phiếu lý lịch tư pháp điện tử tương tác trong trường hợp ủy quyền(Biểu mẫu số 13/2024/LLTP của Thông tư 06/2024/TT-BTP).- Trường hợp là trẻ chưa thành niên thì bố mẹ, người giám hộ sử dụng tài khoản định danh điện tử của mình để thực hiện đăng ký. Hệ thống định danh và xác thực điện tử tự động xác định mối quan hệ nhân thân giữa người đăng ký với trẻ chưa thành niên(Biểu mẫu số 13/2024/LLTP của Thông tư 06/2024/TT-BTP).Công dân tiến hành thanh toán trực tuyến phí cấp Phiếu lý lịch tư pháp ngay trên Ứng dụng VNeID và gửi Tờ khai yêu cầu cấp Phiếu lý lịch tư pháp.Trường hợp thuộc đối tượng miễn, giảm phí cung cấp thông tin thì người yêu cầu cấp Phiếu lý lịch tư pháp đính kèm giấy tờ chứng minh (đối tượng là trẻ em, người" cao tuổi không cần phải đính kèm giấy tờ chứng minh do đã được xác thực thông tin về độ tuổi trên Hệ thống).Lưu ý: Công dân chỉ được nộp hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp số 1 hoặc hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp số 2; không được chọn cả 02 loại Phiếu lý lịch tư pháp trong một hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp.)Bước 2: Gửi hồ sơSau khi nộp Tờ khai yêu cầu cấp Phiếu lý lịch tư pháp và nộp phí cấp Phiếu lý lịch tư pháp, thông tin của Hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp hợp lệ sẽ gửi về Hệ thống thông tin giải quyết thủ tục hành chính của địa phương.Lưu ý: Trường hợp người dân có hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp được Sở Tư pháp đang giải quyết thì người dân không thực hiện nộp hồ sơ yêu cầu Phiếu lý lịch tư pháp mới (trừ trường hợp hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp mới khác loại Phiếu với hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp đang xử lý).Bước 3: Tiếp nhận hồ sơCông chức tại Bộ phận Một cửa tiếp nhận và kiểm tra hồ sơ cấp Phiếu lý lịch tư pháp tại Hệ thống thông tin giải quyết thủ tục hành chính của địa phương và xử lý như sau:- Trường hợp hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp đầy đủ và hợp lệ, công chức tại Bộ phận Một cửa tiến hành tiếp nhận hồ sơ và gửi Phiếu giấy hẹn trả kết quả.- Trường hợp hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp chưa đầy đủ, công chức tại Bộ phận Một cửa gửi yêu cầu công dân bổ sung hồ sơ.- Trường hợp hồ sơ không đủ điều kiện, công chức tại Bộ phận Một cửa thông báo từ chối tiếp nhận. Việc hoàn phí cấp Phiếu lý lịch tư pháp cho công dân là tự động và hoàn trả về tài khoản người thanh toán sau khi nhận được thông báo Từ chối tiếp nhận Hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp.Mã số hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp thành công được lấy từ Hệ thống thông tin giải quyết thủ tục hành chính của địa phương.Ngay sau khi tiếp nhận hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp, công chức tại Bộ phận Một cửa thực hiện chuyển xử lý hồ sơ cho bộ phận chuyên môn về lý lịch tư pháp trên Hệ thống thông tin giải quyết thủ tục hành chính của tỉnh, thành phố.Bước 4: Đẩy dữ liệu sang hệ thống Phần mềm Quản lý lý lịch tư pháp  dùng chung của Bộ Tư pháp Công chức Sở Tư pháp chuyển thông tin yêu cầu cấp Phiếu lý lịch tư pháp tử Hệ thống thông tin giải quyết thủ tục hành chính của tỉnh, thành phố sang Phần mềm Quản lý lý lịch tư pháp dùng chung của Bộ Tư pháp ngay sau khi nhận được hồ sơ do Bộ phận một cửa chuyển.Bước 5: Tiếp nhận hồ sơ từ Hệ thống thông tin giải quyết thủ tục hành chính sang Phần mềm Quản lý lý lịch tư pháp  dùng chung của Bộ Tư pháp Công chức Sở Tư pháp tiếp nhận hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp trên Phần mềm Quản lý lý lịch tư pháp dùng chung của Bộ Tư pháp. Bước 6: Tra cứu, xác minh thông tin- Trường hợp 1: Tra cứu, xác minh thông tin đổi với hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp của người sinh sau ngày 01/7/1996 hoặc đã cấp Phiếu lý lịch tư pháp lần đầu kể từ ngày 01/7/2010.Công chức Sở Tư pháp thực hiện tra cứu, khai thác thông tin tại Cơ sở dữ liệu lý lịch tư pháp của Sở Tư pháp, Cơ sở dữ liệu của Trung tâm Lý lịch tư pháp quốc gia.- Trường hợp 2: Tra cứu, xác minh thông tin ủn tích đối với hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp của người sinh trước ngày 01/7/1996 và chưa cấp Phiếu lý lịch tư pháp kể từ ngày 01/7/2010.Công chức Sở Tư pháp thực hiện gửi yêu cầu tra cứu, xác minh thông tin ăn tích có trước ngày 01/7/2010 cho V06, PV06 trên Phần mềm Quản lý lý lịch tư pháp dùng chung của Bộ Tư pháp thông qua Hệ thống định danh và xác thực điện tử và thực hiện tra cứu, khai thác thông tin án tích cổ sau ngày 01/7/2010 tại Cơ sở dữ liệu lý lịch tư pháp của Sở Tư pháp, Cơ sở dữ liệu của Trung tâm Lý lịch tư pháp quốc gia.(Công chức Sở Tư pháp thực hiện các công việc từ Bước 3 đến Bước 6 trong thời hạn 1/2 ngày làm việc )Bước 7: Cơ quan Công an thực hiện tra cứu, xác minhĐối với hồ sơ yêu cầu tra cứu, xác minh của các trường hợp 2 tại bước 6, cán bộ V06, PV06 nhận yêu cầu tra cứu, xác minh của Sở Tư pháp, thực hiện tra cứu, nhập kết quả vào phần mềm, ký số và trả kết quả về Phần mềm Quản lý lý lịch tư pháp của Bộ Tư pháp qua Hệ thống định danh và xác thực điện tử.Trường hợp cần sử dụng dữ liệu sinh trắc học để thực hiện tra cứu, sẽ thực hiện thông qua kết nối nội ngành Bộ Công an.Thời gian thực hiện Bước này không quá 02 ngày làm việc, trường hợp phức tạp là 07 ngày làm việc. Trường hợp phát hiện người yêu cầu cấp Phiếu lý lịch tư pháp là đối tượng truy nã; bị can, bị cáo trong vụ án; đối tượng quản lý có thông tin trong hồ sơ, tàng thư, đối tượng thuộc diện chủ ý khi xuất, nhập cảnh, cấm đi khỏi nơi cư trú... cơ quan Hồ sơ cần phối hợp với các đơn vị liên quan xác minh, xử lý sẽ có thông báo riêng.Bước 8: Nhận, cập nhật kết quả tra cứu, xác minh- Đối với hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp tại trường hợp 1 Bước 6, công chức Sở Tư pháp cập nhật ngay kết quả tra cứu, khai thác tại Cơ sở dữ liệu lý lịch tư pháp của Sở Tư pháp, Cơ sở dữ liệu lý lịch tư pháp của Trung tâm Lý lịch tư pháp quốc gia cho từng hồ sơ yêu cầu Phiếu lý lịch tư pháp.- Đối với hồ sơ yêu cầu cấp Phiếu lý lịch tư pháp tại trường hợp 2 Bước 6, sau khi nhận kết quả tra cứu, xác minh của V06, PV06 trên Phần mềm Quản lý lý lịch tư pháp dùng chung của Bộ Tư pháp, Sở Tư pháp căn cứ vào kết quả tra cứu của V06, PV06 và kết quả tra cứu tại Cơ sở dữ liệu lý lịch tư pháp của Sở Tư pháp, Cơ sở dữ liệu lý lịch tư pháp của Trung tâm Lý lịch tư pháp quốc gia thực hiện cập nhật kết quả cho từng hồ sơ yêu cầu Phiếu lý lịch tư pháp.Trường hợp sau khi đã tra cứu thông tin lý lịch tư pháp về án tích tại cơ quan Công an mà vẫn chưa đủ căn cứ để kết luận hoặc nội dung về tình trạng án tích của người yêu cầu cấp Phiếu lý lịch tư pháp có điểm chưa rõ ràng, đầy đủ để khẳng định có hay không có án tích, Sở Tư pháp thực hiện xác minh tiếp tại các cơ quan có liên quan theo quy định.Thời gian gửi văn bản đề nghị xác minh cho các cơ quan có liên quan là 01 ngày làm việc sau khi nhận được kết quả của V06, PV06. Trường hợp các thông tin về lý lịch tư pháp từ Tòa án nhân dân tối cao, Viện kiểm sát nhân dân tối cao, Bộ Quốc phòng đã được đồng bộ về Cơ sở dữ liệu quốc gia về dân sự, các thông tin này sẽ được gửi về hệ thống của Bộ Tư pháp để các Sở Tư pháp thực hiện tra cứu, xác minh.Bước 9: Lập Phiếu lý lịch tư pháp điện tửNgay sau khi cập nhật kết quả cho từng hồ sơ yêu cầu Phiếu lý lịch tư pháp thì công chức Sở Tư pháp tiến hành lập Phiếu lý lịch tư pháp điện tử và trình người có thẩm quyền ký số Phiếu lý lịch tư pháp.Phiếu lý lịch tư pháp điện tử được ký số của người có thẩm quyền ký Phiếu lý lịch tư pháp và chữ ký của cơ quan có thẩm quyền hoặc được số hóa từ Phiếu lý lịch tư pháp bằng giấy sang bản điện tử và được ký số bởi cơ quan có thẩm quyền. Sở Tư pháp có thể ký số nhiều Phiếu lý lịch tư pháp theo hướng dẫn của Ban Cơ yếu Chính phủ.Phiếu lý lịch tư pháp điện tử sau khi được vẫn thư phát hành trên Phần mềm Quản lý lý lịch tư pháp dùng chung của Bộ Tư pháp sẽ được Hệ thống thông tin giải quyết thủ tục hành chính của tỉnh, thành phố chủ động kết nối để đồng bộ trạng thái và kết quả Phiếu lý lịch tư pháp điện tử.(Thời gian thực hiện Bước 8 và Bước 9 là 5 ngày làm việc )Bước 10: Trả kết quả cho người dânSau khi Hệ thống thông tin giải quyết thủ tục hành chính của địa phương nhận được kết quả là Phiếu lý lịch tư pháp điện tử tử Phần mềm Quản lý lý lịch tư pháp chuyển sang thì tự động cập nhật trạng thái "Đã xử lý" và kết quả là Phiếu lý lịch tư pháp điện tử, việc cập nhật trạng thái "Đã xử lý" được thực hiện cùng với Bước 9.Phiếu lý lịch tư pháp điện tử là file PDF có chữ ký số mặc định cùng trả trên Cổng dịch vụ công quốc gia, Hệ thống thông tin giải quyết thủ tục hành chính của tỉnh, thành phố và Hệ thống định danh và xác thực điện tử.Trong trường hợp công dân có nhu cầu nhận kết quả là bản giấy Phiếu lý lịch tư pháp, Công chức tại Bộ phận Một cửa tiến hành trả trực tiếp hoặc qua dịch vụ bưu chính theo quy định hiện hành.   Công dân Hà Nội có thể đề nghị cấp Phiếu Lý lịch tư pháp mọi lúc, mọi nơi VTV.vn - Hà Nội đẩy mạnh cấp Phiếu Lý lịch tư pháp qua ứng dụng VNeID, giúp công dân tiết kiệm thời gian và chi phí. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Việt Nam đang lên kế hoạch đầu tư dự án đường sắt tốc độ cao Bắc Nam, tốc độ thiết kế 350 km/h, đi qua 20 tỉnh, thành với điểm đầu tại ga Ngọc Hồi (Hà Nội), điểm cuối tại ga Thủ Thiêm (TP HCM). Tổng mức đầu tư dự án này khoảng 67,3 tỷ USD. Dự án này sẽ được Chính phủ trình Quốc hội xem xét tại kỳ họp khai mạc vào 21/10 tới.Tại họp báo ngày 17/10, ông Sugano Yuichi, Trưởng đại diện Cơ quan Hợp tác Quốc tế Nhật Bản (JICA) cho biết phía Nhật đã có nhiều cuộc làm việc với lãnh đạo Bộ Giao thông Vận tải về dự án đường sắt này.Đại diện JICA gợi ý Việt Nam có thể tham khảo kinh nghiệm từ Nhật Bản. Theo đó, trước khi nước này có tuyến đường sắt cao tốc thương mại đầu tiên trên thế giới - Shinkansen - đường sắt truyền thống trải dài khắp lãnh thổ để vận chuyển hàng hóa. Đường bộ phát triển kéo theo chuỗi logistics chuyển qua kênh này để rút ngắn thời gian.Hiện nay dù đã có đường sắt cao tốc, Nhật Bản vẫn phối hợp nhiều phương thức tùy mục đích. Nếu hàng hóa cần vận chuyển nhanh thì bằng đường bộ, còn khối lượng lớn có thể chọn đường sắt hoặc đường biển."Việt Nam có nhiều lựa chọn, có thể phát triển đường sắt tốc độ cao vận chuyển hàng khách, còn hàng hóa tận dụng tuyến đường hiện hữu. Điều này phụ thuộc vào định hướng từ Chính phủ, lợi ích kinh tế cũng như mục tiêu trung hòa CO2, hướng tới Net Zero", ông Sugano Yuichi chia sẻ.
+Ông Sugano Yuichi, Trưởng đại diện văn phòng JICA tại Việt Nam chia sẻ tại họp báo, ngày 17/10. Ảnh: JICA
+Ông cũng cho hay, nhà chức trách nước này chờ kết quả cuộc thảo luận sắp tới tại Quốc hội Việt Nam, rồi cân nhắc những khả năng hợp tác giữa hai nước trong dự án này.Dự án đường sắt tốc độ cao Bắc Nam có tốc độ thiết kế 350 km/h. Tuyến đường này sẽ vận chuyển hành khách, đáp ứng yêu cầu lưỡng dụng phục vụ quốc phòng, an ninh và có thể vận tải hàng hóa khi cần thiết. Tuyến đường sắt Bắc Nam hiện hữu sẽ vận chuyển hàng hóa và khách du lịch chặng ngắn.Trước đó, tại cuộc tiếp Thủ tướng Nhật Bản Shigeru Ishiba ngày 11/10, Thủ tướng Phạm Minh Chính đề nghị Nhật cấp khoản vay ODA mới cho dự án đường sắt tốc độ cao, đường sắt đô thị tại Việt Nam.Về định hướng hoạt động của JICA, ông Sugano Yuichi thông tin trong một năm (từ 4/2023 đến 3/2024), tổ chức này đã ký khoản vốn vay 102,2 tỷ yen (tương đương 678 triệu USD) cho Việt Nam. Số này chưa gồm tài trợ đầu tư cho khu vực tư nhân và là mức cao nhất 6 năm qua.Tới đây, vốn ODA Nhật Bản sẽ tập trung ở 3 lĩnh vực ưu tiên. Theo đó, dòng vốn này sẽ tập trung vào các dự án về tăng trưởng chất lượng cao. Hiện tổ chức này xây dựng nhà máy xử lý nước thải Yên Xá, quy mô lớn nhất tại Hà Nội, dự kiến hoàn thành thời gian tới. Bên cạnh đó, dự án tuyến Metro số 1 TP HCM đang gấp rút hoàn thiện, chạy thử để sớm đưa vào khai thác.Vốn ưu đãi của Nhật Bản cũng hỗ trợ đối tượng dễ bị tổn thương. JICA đang triển khai dự án hợp tác kỹ thuật liên quan đến các biện pháp ứng phó với sạt lở đất ở khu vực phía Bắc, nhất là những nơi chịu ảnh hưởng nặng nề bởi bão Yagi.Cuối cùng, theo đại diện JICA, họ sẽ hỗ trợ Việt Nam phát triển nguồn nhân lực, thông qua các dự án hợp tác với Trường Đại học Việt – Nhật. Họ cũng phối hợp với Viện Hàn lâm Khoa học Xã hội Việt Nam (VASS) biên soạn sách chuyên khảo cho sinh viên, cung cấp tổng quan về lịch sử quan hệ hai nước.Hiện Nhật Bản là đối tác cho vay ODA lớn nhất của Việt Nam. Sau hơn 30 năm, kể từ 1992 đến nay, nước này đã viện trợ trên 2.760 tỷ yen ODA vốn vay (bình quân mỗi năm khoảng 90 tỷ yen). Vốn vay ưu đãi của Nhật Bản chiếm trên 30% viện trợ phát triển song phương dành cho Việt Nam.JICA là cơ quan thực hiện viện trợ ODA của Chính phủ Nhật Bản thông qua 3 hình thức hợp tác, gồm kỹ thuật, vốn vay và viện trợ không hoàn lại. Việt Nam là nước đứng thứ 2 thế giới với 9 dự án thuộc chương trình "Tài trợ đầu tư cho khu vực tư nhân" của JICA, sau Brazil.
+Đức Mạnh</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bắt giam cán bộ địa chính phường “Giả mạo trong công tác”</t>
+          <t>Giá USD ngân hàng tăng mạnh</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://vtv.vn/phap-luat/bat-giam-can-bo-dia-chinh-phuong-gia-mao-trong-cong-tac-2024093016582519.htm</t>
+          <t>https://vnexpress.net/gia-usd-ngan-hang-tang-manh-4805465.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VTV.vn - Lợi dụng nhu cầu của một số người dân cần làm thủ tục cấp giấy phép xây dựng nhà ở, một cán bộ địa chính phường ở Thanh Hóa đã nhận làm hộ và thu của họ 2 - 3 triệu đồng.</t>
+          <t>Mỗi USD ngân hàng tăng gần 200 đồng trong ngày, lên sát giá đôla trên thị trường tự do.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Công an thành phố Thanh Hóa (tỉnh Thanh Hóa) vừa khởi tố vụ án, khởi tố bị can và bắt tạm giam đối với Nguyễn Ngọc Thành (sinh năm 1982, trú ở phường Đông Thọ, TP Thanh Hóa) về tội "Giả mạo trong công tác".Theo kết quả điều tra ban đầu, Cơ quan Công an an xác định, Nguyễn Ngọc Thành là cán bộ Địa chính - Xây dựng thuộc UBND phường Phú Sơn. Trong quá trình làm việc, Thành được giao nhiệm vụ tiếp nhận hồ sơ xin xác nhận của công dân trên địa bàn phường để làm thủ tục cấp giấy phép xây dựng nhà ở.Lợi dụng nhu cầu của một số người dân cần làm thủ tục cấp giấy phép xây dựng nhà ở, nhưng không thành thạo các thủ tục hành chính, không có thời gian đi làm hồ sơ nên Thành đã nhận làm hộ. Trong quá trình làm hồ sơ, các loại thuế, lệ phí, Thành sẽ thông báo để người dân đóng theo quy định, ngoài ra người dân sẽ phải hỗ trợ tiền xăng xe cho Thành đi lại làm thủ tục với mức giá từ 2 - 3 triệu đồng/bộ.Tuy nhiên, sau khi nhận hồ sơ và tiền thuế, lệ phí từ công dân, Nguyễn Ngọc Thành không liên hệ với đơn vị có thẩm quyền để làm thủ tục cấp phép theo quy định mà tự mình tải các giấy phép xây dựng do UBND TP Thanh Hóa cấp trên Cổng thông tin điện tử, sau đó cắt ghép thay đổi thông tin trong giấy phép thật, in màu và đưa cho công dân sử dụng.Với cách thức trên, Thành đã làm và cấp 4 giấy phép xây dựng giả, qua đó đã thu của người dân với tổng số tiền 85 triệu đồng.   Nữ công chức địa chính xã ở Bắc Kạn bị bắt vì nhận hối lộ VTV.vn - Thắm đã yêu cầu ông Đ. phải chi số tiền 30 triệu đồng, nếu không sẽ không tiếp nhận thực hiện thủ tục cấp sổ đỏ. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Sáng 17/10, Ngân hàng Nhà nước công bố tỷ giá trung tâm 24.199 đồng, tăng 12 đồng so với hôm qua. Với biên độ 5% so với tỷ giá trung tâm, các ngân hàng thương mại được phép mua bán USD trong vùng 22.989 - 25.409 đồng.Hôm nay, các ngân hàng thương mại điều chỉnh mạnh bảng giá USD tới gần 200 đồng so với hôm qua.Vietcombank niêm yết tỷ giá mua bán USD tại 24.960 - 25.350 đồng, tăng mạnh 180 đồng cả hai chiều. Tại BIDV, giá USD cũng lên 24.980 - 25.340 đồng. Eximbank nâng tỷ giá lên 24.980 - 25.350 đồng, Techcombank niêm yết 24.997 - 25.395 đồng.Trước đó, tỷ giá ngân hàng cũng đã có nhiều phiên liên tiếp đi lên. Trong một tuần qua, mỗi USD ngân hàng tăng khoảng 350 đồng, tương đương khoảng 1,4%. Còn so với đầu năm, hiện tỷ giá ngân hàng cao hơn khoảng 3,8% và giao dịch khá sát so với thị trường chợ đen. Chiều nay, giá USD được một số điểm thu đổi ngoại tệ neo quanh 25.250 - 25.350 đồng.  Trên thị trường quốc tế, chỉ số USD Index đo lường sức mạnh của đồng bạc xanh cũng tăng khoảng 3% từ đầu tháng, lên 103,55 điểm.Công ty chứng khoán ACB (ACBS) nhận định, dù được hưởng lợi từ quyết định cắt giảm lãi suất của Cục Dự trữ liên bang Mỹ (Fed), Ngân hàng Nhà nước cũng song song thực hiện hai đợt giảm lãi suất trên thị trường mở (OMO) nhằm duy trì nền lãi suất thấp, hỗ trợ tăng trưởng kinh tế. Vì thế, chênh lệch lãi suất VND và USD vẫn tiếp tục âm, dù mức âm không lớn.Tình trạng này theo ACBS, sẽ còn tiếp tục kéo dài ít nhất đến hết nửa đầu năm 2025. Do đó, áp lực tỷ giá có giảm bớt, nhưng vẫn dễ dàng bùng lên vào những thời điểm nhu cầu thanh toán gia tăng, đặc biệt là cuối năm.Quỳnh Trang</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Khởi tố đối tượng vận chuyển trái phép 2 kg vàng qua biên giới</t>
+          <t>87 cơ thủ Việt Nam bị cấm thi đấu 6 tháng</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://vtv.vn/phap-luat/khoi-to-doi-tuong-van-chuyen-trai-phep-2-kg-vang-qua-bien-gioi-20240930144123387.htm</t>
+          <t>https://vnexpress.net/87-co-thu-viet-nam-bi-cam-thi-dau-6-thang-4805294.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Theo kết luận giám định của Viện Khoa học hình sự Bộ Công an, 2 miếng vàng mà Hà Văn Vinh vận chuyển mỗi miếng có trọng lượng 1 kg, hàm lượng vàng tinh khiết là 99,95% và 99,94%.</t>
+          <t>Liên đoàn billiard Pool Thế giới (WPA) thông báo cấm 245 cơ thủ thi đấu sáu tháng vì dự giải Hanoi Open 2024 không được họ cấp phép.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Trưa 30/9, Đồn Biên phòng Cửa khẩu quốc tế Lào Cai thông tin, đơn vị đã ra quyết định khởi tố vụ án hình sự một đối tượng về hành vi vận chuyển trái phép 2 kg vàng từ Trung Quốc vào Việt Nam qua cửa khẩu quốc tế Lào Cai.Đối tượng Hà Văn Vinh tại Đồn cửa khẩu Quốc tế Lào Cai. Ảnh: TTXVN phátTrước đó, vào 12 giờ 5 phút ngày 25/9, tại hướng nhập cảnh, khu vực Quốc môn Cửa khẩu Quốc tế Lào Cai, trong quá trình làm nhiệm vụ, Tổ công tác Đồn Biên phòng Cửa khẩu Quốc tế Lào Cai chủ trì, phối hợp với Đoàn đặc nhiệm Phòng, chống ma túy và Tội phạm miền Bắc (thuộc Cục Phòng, chống ma túy và Tội phạm, Bộ Tư lệnh Bộ đội Biên phòng) đã phát hiện một người đàn ông đi từ Trung Quốc về Việt Nam có biểu hiện nghi vấn. Tổ công tác kiểm tra hành chính và phát hiện người đàn ông này mang theo 2 miếng kim loại màu vàng (giấu trong hai ống chân được ngụy trang cẩn thận) mỗi miếng có trọng lượng khoảng 1 kg.Qua đấu tranh ban đầu, đối tượng khai tên Hà Văn Vinh, sinh ngày 1/11/1987, trú tại xã Tam Hồng, huyện Yên Lạc, tỉnh Vĩnh Phúc. Vinh được một người đàn ông Trung Quốc thuê vận chuyển 2 miếng kim loại màu vàng trên từ Hà Khẩu - Trung Quốc về thành phố Lào Cai với giá 2 triệu đồng. Khi đang vận chuyển qua cửa khẩu đường bộ quốc tế Lào Cai thì bị lực lượng Biên phòng phát hiện, bắt giữ. Tổ công tác đã tiến hành lập biên bản bắt người phạm tội quả tang, thu giữ niêm phong vật chứng theo quy định.Theo kết luận giám định của Viện Khoa học hình sự Bộ Công an, 2 miếng vàng mà Hà Văn Vinh vận chuyển mỗi miếng có trọng lượng 1 kg, hàm lượng vàng tinh khiết là 99,95% và 99,94%.Đồn Biên phòng Cửa khẩu Quốc tế Lào Cai đã ra quyết định khởi tố vụ án hình sự “Vận chuyển trái phép hàng hóa qua biên giới”, để điều tra theo thẩm quyền.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Danh sách 245 cơ thủ được WPA công bố hôm nay có 87 đại diện Việt Nam, trong đó gồm gần như tất cả cao thủ như Dương Quốc Hoàng, Đặng Thành Kiên, Đỗ Thế Kiên, Lường Đức Thiện, Phạm Phương Nam hay Nguyễn Anh Tuấn.Một loạt cơ thủ hàng đầu thế giới cũng bị cấm, như Carlo Biado, Ko Pin Yi, Shane van Boening, Fedor Gorst, Francisco Sanchez Ruiz, David Alcaide hay Eklent Kaci. Trong top 14 cơ thủ hàng đầu World Nineball Tour (WNT) hiện tại, có tới 13 cơ thủ nằm trong danh sách bị WPA trừng phạt, ngoại trừ Joshua Filler hay Albin Ouschan vì hai cơ thủ này "quay xe" và không dự Hanoi Open.
+Dương Quốc Hoàng (giữa) cùng đội tuyển châu Á ở Reyes Cup 2024 đều nằm trong danh sách bị WPA cấm thi đấu. Ảnh: Matchroom
+"Thật không may khi ban tổ chức Hanoi Open không tìm cách để giải được WPA cấp phép, dù đã được mời", thông báo của liên đoàn có đoạn. "Chúng tôi cũng đã nhiều lần cảnh báo các cơ thủ về giải này. Họ sẽ bị cấm thi đấu trong sáu tháng kể từ khi tham dự Hanoi Open 2024".WPA thành lập năm 1987 và quản lý các giải pool, thuộc Liên đoàn thể thao billiards thế giới (WCBS). Còn WCBS là thành viên của Ủy ban Olympic Quốc tế (IOC). Các cơ thủ Việt Nam bị trừng phạt đều thuộc Liên đoàn Billiards Thể thao châu Á (ACBS), còn ACBS là thành viên của WPA.WNT ra mắt bảng thứ tự các cơ thủ cùng hệ thống giải pool 9 bi riêng năm 2023, do công ty Matchroom của Anh khởi xướng. WPA từng giao quyền tổ chức các giải 9 bi cho Matchroom năm 2019, nhưng hai bên xảy ra xung đột khiến công ty này thành lập hệ thống chuyên nghiệp WNT để đối đầu với WPA. Các giải WNT thường có tiền thưởng cao hơn hẳn WPA.Án phạt không bất ngờ, khi WPA đã nhiều lần cảnh báo từ trước, rằng giải 9 bi Hanoi Open không được liên đoàn cấp phép. Tuy nhiên, hầu hết cơ thủ hàng đầu thế giới, dù theo bảng WPA hay WNT, đều tới Hà Nội thi đấu, chấp nhận lệnh cấm. Nhóm cơ thủ như Boening, Gorst, Sanchez hay Alcaide đều từng đăng thông điệp tẩy chay WPA vì cấm các cơ thủ châu Á dự Hanoi Open. Hiện, chính nhóm cơ thủ này cũng bị WPA trừng phạt.245 cơ thủ sẽ không được phép dự các giải do liên đoàn quốc gia, châu lục của họ và WPA. Những giải này gồm vô địch quốc gia, vô địch châu Á, 8 bi, 10 bi thế giới, hay những đại hội thể thao khu vực và châu lục. Họ sẽ chỉ có thể dự các giải thuộc WNT, và những giải đấu không chính thức.Sau sáu tháng bị cấm, cơ thủ nào muốn trở lại thi đấu ở những giải này, sẽ phải nộp phạt 500 USD cho liên đoàn quốc gia.Liên đoàn Billiards &amp; Snooker Việt Nam (VBSF) là thành viên của ACBS. Trong khi, đơn vị tổ chức Hanoi Open 2024 là Liên đoàn Billiards &amp; Snooker Hà Nội, không thuộc ACBS. Trước khi nhận lệnh cấm từ WPA, các cơ thủ Việt Nam cũng từng bị ACBS trừng phạt vì dự Hanoi Open 2023, dù Liên đoàn Hà Nội cho rằng án phạt không có căn cứ.Hanoi Open 2024 diễn ra từ 8/10 đến 13/10 tại Cung Điền kinh trong nhà Hà Nội, với quỹ thưởng 200.000 USD, trong đó 30.000 USD cho nhà vô địch Johann Chua.Xuân Bình</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hàn Quốc tuyên án cảnh sát cấp cao nhất trong thảm họa giẫm đạp Itaewon</t>
+          <t>Giá xăng về dưới 21.000 đồng một lít</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://vtv.vn/the-gioi/han-quoc-tuyen-an-canh-sat-cap-cao-nhat-trong-tham-hoa-giam-dap-itaewon-20240930211732074.htm</t>
+          <t>https://vnexpress.net/gia-xang-moi-nhat-hom-nay-17-10-4805286.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>VTV.vn - Cựu cảnh sát trưởng một đồn cảnh sát địa phương ở Seoul, Hàn Quốc đã bị kết án 3 năm tù liên quan đến vụ giẫm đạp trong ngày lễ Halloween năm 2022.</t>
+          <t>Giá xăng và dầu (trừ mazut) giảm 100-180 đồng từ 15h hôm nay, sau điều chỉnh của liên Bộ Công Thương - Tài chính.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Theo đó, cựu cảnh sát trưởng trên đã trở thành viên chức thực thi pháp luật cấp cao nhất phải chịu trách nhiệm hình sự về thảm họa giẫm đạp này.Gần 160 người đã thiệt mạng trong vụ giẫm đạp tại khu phố đêm Itaewon vào ngày 29/10/2022 - một trong những thảm họa chết người nhất tại Hàn Quốc khiến cả nước bàng hoàng.Lee Im-jae - cựu cảnh sát trưởng quận Yongsan, đơn vị giám sát an toàn tại Itaewon - là một trong số nhiều cảnh sát bị truy tố vì không chuẩn bị đầy đủ để ứng phó với đám đông khổng lồ tham gia lễ Halloween tại đây.Tòa án quận phía Tây Seoul hôm 30/9 cho biết họ đã kết luận Lee Im-jae và hai cựu cảnh sát Yongsan khác có tội vì đã bỏ bê nhiệm vụ, dẫn đến hàng loạt trường hợp tử vong và thương tích trong thảm họa Itaewon. Trên thực tế, có dấu hiệu cho thấy hoàn toàn có thể dự đoán được việc đám đông tụ tập ở con dốc Itaewon, tiềm ẩn nguy cơ nghiêm trọng đe dọa tính mạng và sự an toàn của người dân. Tòa án kết tội cựu cảnh sát trưởng không ngăn chặn được vụ giẫm đạp.Ông Lee Im-jae cũng bị kết tội không thực hiện đủ biện pháp kiểm soát đám đông và cử các cảnh sát đến hiện trường. Tòa án kết luận rằng ông Lee Im-jae đã chậm trễ trong việc phản ứng với thảm họa. Ông đồng thời được xóa tội khai man.(Ảnh: AFP/Getty Images)Lee Im-jae là cảnh sát cấp cao nhất bị kết án, sau khi tòa án tuyên án một cảnh sát 18 tháng tù giam, trong khi áp dụng các bản án treo ngắn hơn đối với hai cấp dưới của ông về tội hủy bằng chứng vào đầu năm nay.Vào tháng 1, cựu cảnh sát trưởng thành phố Seoul đã bị truy tố vì tội cẩu thả liên quan đến thảm kịch giẫm đạp. Ông cũng đã bị xét xử và đang chờ phán quyết.Itaewon - nơi có một số nhà hàng và quán bar nổi tiếng tại Seoul - đã tổ chức lễ kỷ niệm Halloween trong nhiều năm.Theo nhật ký cuộc gọi khẩn cấp của cảnh sát vào ngày xảy ra vụ việc, nhiều cuộc gọi của người dân đã phản ánh về tình trạng quá tải sớm nhất là 4 giờ trước khi tình hình trở nên tồi tệ hơn.Cảnh sát sở tại đã 4 lần điều động lực lượng đến Itaewon. Tuy nhiên, số lượng người dồn vào khu vực Itaewon đã tăng lên nhanh chóng và đường phố trở nên quá đông đúc, đến nỗi những người có mặt không thể di chuyển. Một số người bị trượt chân ngã đã không đứng lên được, và nhiều người đã bị ngạt thở. Hầu hết những nạn nhân tử vong trong đêm đó là những người Hàn Quốc trẻ tuổi, phần lớn ở độ tuổi thiếu niên và trong tầm tuổi từ 20.Sự phẫn nộ của người dân Hàn Quốc đã chĩa mũi dùi vào Chính phủ của Tổng thống  Yoon Suk-yeol vào thời điểm đó, với những lời chỉ trích lên án việc lực lượng chức năng thiếu trách nhiệm.Năm 2023, chính quyền thành phố Seoul đã công bố một loạt biện pháp mới nhằm đảm bảo lễ Halloween an toàn - bao gồm một hệ thống camera giám sát an ninh mới để theo dõi số lượng người tham gia.Một số nước châu Á khác đã rút kinh nghiệm từ thảm họa Itaewon và thực hiện các biện pháp để tránh lặp lại thảm kịch. Tại Nhật Bản, năm 2023, chính quyền địa phương khuyến khích những người trẻ tuổi tránh xa các khu vực đông đúc ở quận Shibuya - một địa điểm thường tụ tập đông người vào đêm Halloween.Tại thành phố Quảng Châu ở khu vực Đông Nam Trung Quốc, công ty điều hành dịch vụ tàu điện ngầm đã cấm "hóa trang và ăn mặc đáng sợ" trên tàu để "ngăn ngừa người dân bị hoảng loạn".        Mở cuộc điều tra mới về thảm kịch Itaewon VTV.vn - Quốc hội Hàn Quốc đã thông qua một dự luật đặc biệt, yêu cầu mở cuộc điều tra mới về thảm kịch giẫm đạp tại Itaewon năm 2022.     Thảm kịch Itaewon tiếp tục nóng lên tại chính trường Hàn Quốc VTV.vn - Tổng thống Hàn Quốc Yoon Suk Yeol đang phải đối mặt với sức ép phải ký một dự luật đặc biệt kêu gọi mở cuộc điều tra mới về thảm kịch giẫm đạp tại khu phố Itaewon.     Cảnh sát trưởng Seoul bị buộc tội về thảm họa giẫm đạp Itaewon khiến 158 người chết VTV.vn - Cảnh sát trưởng thành phố Seoul, Hàn Quốc đã bị buộc tội sơ suất nghề nghiệp trong vụ giẫm đạp Halloween ở Itaewon vào năm 2022 khiến gần 160 người thiệt mạng.      * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Giá xăng RON 95-III (loại phổ biến trên thị trường) giảm 100 đồng, xuống 20.960 đồng một lít. E5 RON 92 ở mức 19.730 đồng một lít, bớt 110 đồng.Các mặt hàng dầu có giá mới 16.090-18.620 đồng một lít, kg. So với cách đây 7 ngày, dầu diesel giảm 180 đồng, xuống 18.320 đồng. Dầu hỏa hạ 170 đồng. Riêng mazut tăng 180 đồng một kg.Giá xăng, dầu thay đổi như sau:Mặt hàng
+Giá mới
+Thay đổi
+Xăng RON 95-III
+20.960
+- 100
+Xăng E5 RON 92
+19.730
+- 110
+Dầu diesel
+18.320
+- 180
+Dầu hoả
+18.620
+- 170
+Dầu mazut
+16.090
++ 180
+Đơn vị: đồng/lít hoặc kg, tùy loạiTừ đầu năm đến nay, giá xăng có 21 lần tăng, 20 đợt giảm. Còn dầu tăng 18 lần, hạ 23 lần. Liên Bộ vẫn không trích, lập Quỹ bình ổn xăng dầu, tương tự các kỳ điều hành trước đây. Tính tới hết quý II, quỹ này còn hơn 6.000 tỷ đồng, giảm khoảng 600 tỷ so với cuối 2023, theo Bộ Tài chính.Nhà điều hành cho biết giá nhiên liệu tuần qua biến động do OPEC hạ dự báo tăng trưởng nhu cầu dầu toàn cầu năm nay, căng thẳng leo thang tại khu vực Trung Đông.Bình quân 7 ngày, xăng thành phẩm giảm khoảng 1-1,1%, dầu hạ 1,4-1,5%. Riêng mazut tăng 1,1%. Theo đó, mỗi thùng xăng RON 95 xuống 87,5 USD, dầu diesel còn 88,6 USD, mazut lên 460,6 USD mỗi tấn.Phương Dung</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bão Krathon đổ bộ các đảo của Philippines</t>
+          <t>Smartphone 5G giá 30 triệu đồng nhưng chỉ dùng được 4G ở Việt Nam</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://vtv.vn/the-gioi/bao-krathon-do-bo-cac-dao-cua-philippines-20241001081205436.htm</t>
+          <t>https://vnexpress.net/smartphone-5g-gia-30-trieu-dong-nhung-chi-dung-duoc-4g-o-viet-nam-4804117.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>VTV.vn - Ngày 30/9, bão Krathon đã đổ bộ vào các đảo cực Bắc của Philippines, khiến chính quyền địa phương phải sơ tán người dân, đóng cửa trường học và dừng các tuyến phà liên đảo</t>
+          <t>Sony Xperia 1 Mark VI được trang bị phần cứng có sẵn kết nối 5G nhưng phần mềm không hỗ trợ nên chỉ sử dụng được mạng 4G tại Việt Nam.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Theo Cơ quan Khí tượng Philippines, bão Krathon, với sức gió mạnh lên tới 175 km/h và giật lên tới 215km/h, đang quét qua vùng biển ven bờ các tỉnh Cagayan và Batanes. Cơn bão di chuyển chậm về phía Tây và dự kiến sẽ mạnh lên thành siêu bão khi tiến về phía Đông Bắc vào ngày 1/10 và hướng tới Đài Loan (Trung Quốc).Bão Krathon được cảnh báo có khả năng gây thiệt hại rất lớn cho cộng đồng, đe dọa đến tính mạng của người dân trong 48 giờ tới tại làng ven biển Batanes, quần đảo Babuyan và tỉnh Cagayan. Gió mạnh có thể thổi bay mái nhà, quật đổ cây cối, phá hủy đất nông nghiệp.Đài Loan (Trung Quốc) đã phát đi cảnh báo khẩn cấp về cơn bão này. Cơn bão dự kiến sẽ mạnh lên thành bão cấp 4 trong thang 5 cấp, với sức gió vùng gần tâm bão lên tới hơn 220 km/h.        Bão Krathon giật trên cấp 17 có khả năng đi vào Biển Đông VTV.vn - Dự báo trong 24 giờ tới, bão Krathon có khả năng đi vào vùng biển phía Đông Bắc khu vực Bắc Biển Đông.     Bão Krathon tấn công các đảo phía Bắc Philippines VTV.vn - Ngày 30/9, bão mạnh Krathon đã tấn công các đảo phía Bắc của Philippines, khiến cư dân phải sơ tán, trường học và dịch vụ phà liên đảo bị đình chỉ.     Đài Loan (Trung Quốc) cảnh báo khẩn cấp về bão Krathon VTV.vn - Đài Loan (Trung Quốc) đã phát đi cảnh báo khẩn cấp về cơn bão Krathon dự kiến đổ bộ bờ biển phía Tây với mưa lớn và gió mạnh.      * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Minh Tú (Hà Nội) cho biết anh mua điện thoại Xperia với thông số kỹ thuật có 5G đầu tháng 10. Ngày 15/10, khi nhận được tin nhắn của nhà mạng thông báo điện thoại ở trong vùng phủ sóng kết nối mới, anh vào cài đặt để bật chế độ 5G nhưng không tìm thấy thông tin."Liên hệ với bộ phận chăm sóc khách hàng, họ nói thiết bị có sẵn phần cứng 5G, nhưng phần mềm không hỗ trợ do liên quan đến vấn đề giấy phép", Tú nói.Trên cộng đồng người dùng Sony Xperia tại Việt Nam, nhiều người phản ánh tình huống giống Minh Tú.Tình trạng này được ghi nhận với Xperia 1 Mark VI và 10 Mark VI, ra mắt tại Việt Nam hồi tháng 7. Hai smartphone vốn được trang bị phần cứng có sẵn kết nối 5G khi bán tại một số thị trường quốc tế. Tuy nhiên, với máy chính hãng tại Việt Nam, khi truy cập cài đặt kết nối mạng, thiết bị hiển thị lựa chọn cao nhất là LTE. Một số người mua máy "xách tay" từ Hong Kong, Đài Loan cũng gặp tình trạng tương tự.
+Phần cài đặt của một chiếc Xperia 1 Mark VI không có tùy chọn kết nối 5G. Ảnh: Hoài Anh
+Tú cho biết anh chưa có nhu cầu dùng 5G lúc này, nhưng không thể "sống mãi với 4G" trong vài năm tiếp theo. Anh bày tỏ bức xúc về thông tin mập mờ, khi website của Sony Việt Nam vẫn liệt kê băng tần 5G trong phần thông số kỹ thuật, không hề đề cập việc thiết bị có hỗ trợ 5G ở Việt Nam hay không.Đại diện Sony và hệ thống bán lẻ CellphoneS đều xác nhận máy chỉ tương thích đến 4G, không thể dùng 5G, nhưng không nêu lý do. Trên website ở Việt Nam, Sony đề cập thông số kỹ thuật gồm cả băng tần 5G, nhưng kèm ghi chú "Tình trạng có thể thay đổi theo quốc gia/khu vực, nhà mạng, phiên bản phần mềm và môi trường người dùng".Một số chuyên gia dự đoán việc cắt kết nối 5G có thể do hãng muốn giảm chi phí về thủ tục lưu hành trên thị trường. Thực tế, giá của Xperia 1 Mark VI rẻ hơn 5-6 triệu đồng so với bản tiền nhiệm. Mẫu Xperia 1 Mark V ra mắt năm ngoái có giá 36 triệu đồng tại Việt Nam, có hỗ trợ 5G.
+Xperia 1 Mark VI. Ảnh: Hoài Anh
+Hiện nhà mạng Viettel đã thương mại hóa 5G, trong khi VNPT và MobiFone đang chuẩn bị triển khai và có chương trình dùng thử. Người sở hữu thiết bị 5G có thể đăng ký và sử dụng tại những khu vực có sóng. Để tránh tình trạng mua nhầm, người dùng cần tìm hiểu và kiểm tra kết nối 5G của các nhà mạng Việt Nam trước khi mua.Bộ đôi Xperia 1 và 10 Mark VI ra mắt hồi tháng 5 và được bán tại Việt Nam từ tháng 7, với giá lần lượt 31,5 và 11,5 triệu đồng. Sản phẩm chủ yếu được mua bởi những người yêu thích thương hiệu Sony hoặc thích những mẫu đặc biệt, với đặc trưng màn hình dài, đẹp mắt. Xperia 1VI thuộc phân khúc cao cấp, cạnh tranh với Galaxy S24 Ultra. Máy trang bị chip Snapdragon 8 Gen3.Lưu Quý</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dự kiến đầu tư hơn 67 tỷ USD xây tuyến đường sắt tốc độ cao Bắc - Nam</t>
+          <t>Trung tâm hội chợ triển lãm quốc gia dự kiến hoàn thành sau 10 tháng</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://vtv.vn/kinh-te/du-kien-dau-tu-hon-67-ty-usd-xay-tuyen-duong-sat-toc-do-cao-bac-nam-20240930193437477.htm</t>
+          <t>https://vnexpress.net/trung-tam-hoi-cho-trien-lam-quoc-gia-du-kien-hoan-thanh-sau-10-thang-4805437.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>VTV.vn - Tuyến đường sắt tốc độ cao Bắc - Nam được xác định sơ bộ tổng mức đầu tư khoảng 67 tỷ USD, nếu tính theo tỷ giá hiện nay khoảng 1,7 triệu tỷ đồng.</t>
+          <t>Hà NộiVới quy mô 90 ha, Trung tâm hội chợ triển lãm quốc gia tại xã Đông Hội, Xuân Canh, huyện Đông Anh dự kiến khánh thành vào tháng 7/2025.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Nếu chỉ nhìn đơn thuần về tổng mức đầu tư của dự án, chắc chắn nhiều người sẽ không khỏi giật mình về độ lớn, nhưng với những tính toán mang tính toàn diện, khoa học và thực tiễn thì số vốn để đầu tư cho dự án, trong thời điểm này là khả quan và kiểm soát được.Gần 15 năm qua, dựa án tuyến đường sắt tốc độ cao trên trục Bắc - Nam đã được nghiên cứu. Vào năm 2010, khi quy mô GDP mới chỉ ở mức 147 tỷ USD thì với 56 tỷ USD tổng mức đầu tư cho dự án đường sắt tốc độ cao khi đó chiếm tới 38% GDP và đẩy tỷ lệ nợ công lên mức gần 57% GDP, là mức cao gần chạm ngưỡng cho phép.Tuy nhiên, với nhu cầu vận tải ngày càng tăng cao, quy mô nền kinh tế năm nay dự báo đạt trên 465 tỷ USD, tức cao gấp hơn 3 lần so với năm 2010 thì nguồn lực để đầu tư cho đường sắt tốc độ cao ở mức 67 tỷ USD đã không còn là trở ngại lớn.Ông Shantanu Chkraborty - Giám đốc Quốc gia Ngân hàng phát triển châu Á tại Việt Nam đánh giá: "Dự án này có tính chuyển đổi mang tính bước ngoặt nếu chúng được thực hiện đúng cách. Và như chúng ta thấy các dự án đường sắt tốc độ cao ở các nơi khác trên thế giới đều tạo ra động lực lớn cho tăng trưởng. Đây là dự án có tầm quan trọng chiến lược và chúng tôi rất mong đợi dự án sẽ được triển khai trong thời gian sắp tới".Dự kiến đầu tư hơn 67 tỷ USD xây tuyến đường sắt tốc độ cao Bắc - Nam. Ảnh minh họa - Ảnh: VGP.Đánh giá của Bộ Tài chính về các chỉ tiêu an toàn nợ công khi triển khai đầu tư dự án cho thấy giai đoạn đến năm 2030 cả 3 tiêu chí: nợ công, nợ Chính phủ, nợ nước ngoài quốc gia đều thấp hơn mức cho phép từ 5 đến 15%.Ông Hoàng Văn Cường - Ủy viên Ủy ban Tài chính Ngân sách của Quốc hội cho biết: "Nợ công hiện nay của chúng ta mới ở 37% và mức cho phép là 60%. Như vậy chỉ khai thác nguyên dư địa từ nợ công, chúng ta đã có thể có được gần 100 tỷ USD".Để dự án đường sắt tốc độ cao đi vào khai thác hoàn toàn phải mất khoảng chục năm. Như vậy, mỗi năm bình quân khoảng cần khoảng 5,6 tỷ USD  tương đương khoảng 145 nghìn tỷ đồng theo tỷ giá hiện hành.Con số này chiếm 24,5% vốn đầu tư công trung hạn hàng năm bố trí trong giai đoạn 2021-2025 và giảm xuống còn  khoảng 16,2% trong giai đoạn 2026-2030. Đây là những tỷ lệ chấp nhận được đối với quy mô nền kinh tế trong thời gian tới.    Kỳ vọng đường sắt tốc độ cao VTV.vn - Dự án đường sắt tốc độ cao trên trục Bắc - Nam sơ bộ có tổng mức đầu tư khoảng hơn 67 tỷ USD. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Theo đó, Vingroup hoàn thành kế hoạch đầu tư xây dựng dự án nhằm kỷ niệm 80 năm ngày Quốc khánh (2/9/1945 - 2/9/2025). Hiện tại, tập đoàn này là nhà đầu tư chiến lược sở hữu hơn 80% vốn điều lệ của Công ty cổ phần Trung tâm hội chợ triển lãm Việt Nam - chủ đầu tư Trung tâm hội chợ triển lãm quốc gia.
+Phối cảnh Trung tâm hội chợ triển lãm quốc gia. Ảnh: Vingroup
+Trung tâm hội chợ triển lãm quốc gia được khởi công xây dựng vào ngày 30/8, thuộc Top 10 các trung tâm triển lãm lớn nhất thế giới. Dự án gồm công trình triển lãm trong nhà mang hình ảnh thần Kim Quy với 9 phân khu tổng diện tích hơn 130.000 m2, 4 khu công viên triển lãm ngoài trời với tổng quy mô đến 20,6 ha, 2 nhà triển lãm trong nhà quy mô nhỏ khác cùng các công trình phụ trợ đa dạng...Với vị trí cửa ngõ Đông Bắc Hà Nội, từ đây dễ dàng di chuyển đến sân bay quốc tế Nội Bài, quận Hoàn Kiếm, Tây Hồ thông qua cầu Tứ Liên trong quy hoạch, kế cận tuyến metro tương lai kết nối Đông Anh với các địa điểm khác trong thành phố. Hiện tại, dự án kết nối vào trung tâm thông qua Quốc lộ 5 kéo dài, đường Trường Sa và cầu Đông Trù, cầu Nhật Tân.
+Khi hoàn thành, Trung tâm hội chợ triển lãm quốc gia sẽ là điểm đến của các sự kiện thương mại, triển lãm quy mô toàn cầu. Ảnh: Vingroup
+Khi đi vào hoạt động, dự án góp phần kiến tạo một điểm đến quốc tế cho các sự kiện thương mại, triển lãm quy mô toàn cầu, sánh ngang với các thành phố lớn trên thế giới như Dubai, Frankfurt hay Fiera Milano...Yên Chi</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nhiều người “sập bẫy” lãi khủng từ công ty Tikyou</t>
+          <t>Chưa phát hiện dấu hiệu án mạng vụ thi thể ở quán karaoke An Phú</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://vtv.vn/kinh-te/nhieu-nguoi-sap-bay-lai-khung-tu-cong-ty-tikyou-20241001100148248.htm</t>
+          <t>https://vnexpress.net/chua-phat-hien-dau-hieu-an-mang-vu-thi-the-o-quan-karaoke-an-phu-4805188.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>VTV.vn - Câu chuyện rủi ro từ việc đầu tư lấy lãi cao không còn là câu chuyện mới và phóng viên VTV đã phản ánh rất nhiều lần, song hiện nay câu chuyện này vẫn cứ lặp lại.</t>
+          <t>Bình DươngKhám nghiệm tử thi không nguyên vẹn trong quán karaoke, cảnh sát phát hiện có vết thương nhưng cho rằng "không phải do đâm chém, khả năng không phải án mạng".</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mới đây, đường dây nóng của VTV tiếp tục nhận được phản ánh của hàng trăm người dân khi họ đã đầu tư nhiều tỷ đồng vào công ty TNHH truyền thông văn hóa Tikyou, có địa chỉ tại quận 7, TP Hồ Chí Minh.Theo đó, công ty Tikyou đã đưa ra lời quảng cáo, mời chào rằng người dân có thể bỏ tiền vào đầu tư các gói cho thuê thiết bị phát sóng livestream trực tiếp trên Tiktok. Lãi suất được trả theo giờ, theo ngày lên tới 324%/năm, thậm chí có lúc lên tới hàng nghìn %/năm. Chỉ nghe qua về các mức lãi suất "khủng" này đã thấy rất khó tin. Thế nhưng công ty Tikyou vẫn hoạt động được gần 1 năm nay và có tới hàng nghìn người tham gia.Tikyou, Tiktok giải trí và kiếm tiền… mỗi một quảng cáo công ty Tikyou đều khéo léo gắn thêm chữ Tiktok ở bên cạnh, với giao diện gần như y hệt. Nhiều người như chị Trịnh Thị Mỹ (người tham gia đầu tư vào công ty truyền thông văn hóa Tikyou) thấy Tiktok ngày càng phát triển nên cũng tin tưởng vào việc cho thuê máy phát trực tiếp của Tikyou sẽ đem lại lợi nhuận cao, vì thế chị đã quyết định đầu tư.Thấy hợp lý thì vào tiền, công ty Tikyou lại có rất nhiều gói đầu tư, rất đa dạng dành cho nhiều đối tượng khác nhau. Người ít tiền thì có gói 500 nghìn đồng, 2 triệu đồng, người nhiều tiền thì có gói 50 triệu đồng.Ai cũng có thể tham gia, đã thế lãi suất lại còn cao ngất ngưởng. Thấp nhất là 0,4%/ngày, tương đương 144%/năm. Nhiều tiền nữa thì tham gia gói Vip lãi 0,9%/ngày, tương đương 324%/năm.Thậm chí, nếu phát triển được đội nhóm theo mô hình đa cấp thì còn được thưởng xe, được bổ nhiệm các chức vụ cao cấp. Nghe đã thấy hấp dẫn, thế là hàng nghìn người ai cũng vào tiền, thậm chí còn phát triển các chi nhánh, đội nhóm tại nhiều tỉnh, thành trên cả nước.Khi số người tham gia đầu tư ngày một nhiều lên, vào ngày 17/8 vừa qua, Công ty Tikyou tung ra "mẻ lưới" cuối cùng, với lợi nhuận cao không tưởng. Đó là đầu tư 50 triệu đồng trong 5 giờ, thu nhập mỗi giờ là 20 triệu đồng, lợi nhuận 100%.Được tiền thì rút hết ra, nhưng chưa nhà đầu tư nào kịp rút thì ứng dụng Tikyou đã sập, không còn truy cập được. Hàng nghìn người nháo nhác hỏi nhau, rủ nhau tới địa điểm đăng ký kinh doanh của công ty Tikyou tại quận Bình Thạnh, TP Hồ Chí Minh thì đã không ai còn ở đây, họ đã chuyển đi hết từ bao giờ.Trao đổi với VTVmoney, đại diện Tiktok Việt Nam, ông Nguyễn Lâm Thanh cho biết, Tiktok không hề có liên quan gì đến công ty Tikyou ở trên.Còn Đại diện Cục thuế TP Hồ Chí Minh cũng cho biết công ty Tikyou chưa đăng ký sử dụng hóa đơn, chưa phát sinh doanh thu. Ngày 13/9, cơ quan thuế đã ban hành Thông  báo về việc công ty Tikyou không còn hoạt động tại địa chỉ đăng ký kinh doanh.Vậy hàng nghìn người đã bỏ tiền đầu tư vào công ty Tikyou thì liệu họ có cách nào lấy lại được tiền? Và chủ của công ty Tikyou là ai? Phóng viên VTV sẽ tiếp tục làm rõ nội dung này.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
+          <t>Ngày 17/10, Công an Bình Dương tiếp tục điều tra vụ thi thể phân hủy trong quán karaoke An Phú (nơi từng xảy ra hỏa hoạn làm 32 người chết), nghi là người đàn ông Trung Quốc mất tích tháng trước.Bước đầu, cơ quan điều tra ghi nhận thi thể nạn nhân gồm các bộ phận cơ thể tách rời nhau. Trong đó, phần hộp sọ và cánh tay phân hủy nhiều được tìm thấy trước; phần cơ thể phân hủy ít hơn được tìm thấy sau, nằm dưới hố nước nhưng gần vị trí phát hiện hộp sọ và cánh tay. Thi thể cũng có vết thương, song không phải do bị đâm chém.Việc các bộ phận thi thể tách rời nhau, theo cơ quan điều tra, có khả năng do quá trình phân hủy tự nhiên. Ngoài ra, để có cơ sở pháp lý xác định nhân thân nạn nhân, cơ quan điều tra đang xét nghiệm ADN người thân của người đàn ông Trung Quốc.
+Hiện trường phát hiện thi thể nạn nhân. Ảnh: Phước Tuấn
+Chiều 15/10, anh Nguyễn Văn Tú, 30 tuổi, chở theo người cháu từ An Giang lên Bình Dương, đến quán karaoke An Phú - hiện trường vụ cháy 32 người chết năm 2022, đang bỏ không, với mục đích quay video đăng mạng xã hội kiểu "khám phá".Một mình anh Tú vào trong quay video. Khi đi sâu vào khu vực bãi xe trước đây của quán, anh phát hiện một bàn tay người (từ khuỷu tay đến bàn tay) đang phân huỷ cạnh thùng rác lớn màu xanh. Tại hố ga gần đó có phần đầu người nổi lên, cũng đang phân huỷ. Anh Tú sợ hãi chạy ra ngoài, cùng người cháu về quê ngay, không báo cho công an địa phương. Đến sáng nay, sau khi bình tâm, anh này đã gọi đến Công an phường An Phú trình báo.Công an Bình Dương xác định nạn nhân có thể là ông Luo Quilong (42 tuổi, quốc tịch Trung Quốc). Trước đó, gia đình có thông báo tìm người thân với nội dung ông Luo Quilong bị trầm cảm nặng, đầu óc không tỉnh táo, bỏ nhà đi từ ngày 14/9 không về; kèm một số thông tin, hình ảnh nhận dạng.Hiện, Công an Bình Dương chưa đưa ra kết luận cuối cùng về vụ việc.
+Cảnh sát khám nghiệm hiện trường phát hiện các phần thi thể, sáng 16/10. Ảnh: Yên Khánh
+Phước Tuấn</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Độc đạo - Tập 14: Quân "già" trực tiếp đàm phán với lão Cừ về việc vận chuyển hàng trắng</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/truyen-hinh/doc-dao-tap-14-quan-gia-truc-tiep-dam-phan-voi-lao-cu-ve-viec-van-chuyen-hang-trang-20241001092110654.htm</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>VTV.vn - Biết tin Lê Toàn đã chết, kế hoạch vận chuyển hàng của Quân "già" buộc phải chuyển hướng. Hắn tìm gặp "trưởng bản" Cừ để thỏa thuận.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Cũng trong tập này, Quân "già" xuất hiện trở lại, bàn việc vận chuyển hàng trắng với trưởng bản Cừ (NSND Bùi Bài Bình) sau khi Lê Toàn (NSƯT Hoàng Hải) chết. "Tôi không thích vòng vo. Tôi biết đó là hàng gì nên nói thẳng, đúng ngày đúng giờ, có người ra lấy hàng mang đến địa điểm chú chỉ sẵn, không liên hệ với chú và tôi. Nếu có bị bắt cũng không có manh mối gì. Đợt này chỉ chuyển được ít thôi vì tôi chỉ còn ít người đáng tin", ông Cừ nói.Nghe thấy trưởng bản Cừ nói thế, Quân "già" tỏ vẻ nghi ngờ: "Nghe nguy hiểm thế, không khéo lại là người của công an cài vào. Đã làm phải đến nơi đến chốn, tối thiểu cũng phải nửa tấn".Trong tập 13, Tuyết đã phần nào hiểu mình cũng chỉ là con cờ trong tay Dũng "kính". Chính vì vậy, Dũng tiếp tục "thao túng" tâm lý người tình bằng cách hứa sẽ bảo vệ Tuyết. "Vị thế của anh càng chắc thì càng bảo vệ em tốt hơn", Dũng "kính" nói. Tuyết đáp: "Em hiểu rồi, bây giờ anh cần em phải làm gì?". Dũng tiếp tục: "Anh cần em tung tin về vụ đánh bạc hôm trước. Em cần phải làm việc này thật khéo để mọi người tin những đứa đánh bạc là người của Hưng "khẹc"". Liệu Tuyết có mù quáng vì tình cảm với Dũng "kính" mà tiếp tục hi sinh bản thân để giúp hắn?Mời quý vị khán giả theo dõi chi tiết tập 14 phim Độc đạo sẽ lên sóng lúc 21h40 tối nay trên VTV3.         Độc đạo - Tập 14: Hồng - Khương liệu có thoát khỏi sự truy lùng của giới giang hồ? VTV.vn - Hai anh em Hồng - Khương chạy về bản Mộc vực sâu, để trốn sự truy lùng của giới giang hồ.     Độc đạo - Tập 13: Hai anh em Hồng - Khương bị giữ chân tại bản Mây VTV.vn - Sau khi “xử lý” Dương cơ bắp, Hồng - Khương bị chặn đường trở về nhà. Cả hai tìm đến Trưởng bản Cừ để nhờ sự giúp đỡ.     Độc đạo - Tập 12: Ông Lê Toàn chết, Hồng bắn Dương "cơ bắp" trả thù cho 2 bố? VTV.vn - Sau khi nói toàn bộ mọi bí mật, ông Lê Toàn đã chết dù Hồng và Khương nỗ lực đưa đi cấp cứu.      * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>INFOGRAPHIC: VTV phát sóng nhiều chương trình kỷ niệm 70 năm Ngày Giải phóng Thủ đô</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/truyen-hinh/infographic-vtv-phat-song-nhieu-chuong-trinh-ky-niem-70-nam-ngay-giai-phong-thu-do-20241001005845373.htm</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>VTV.vn - Đài Truyền hình Việt Nam đã có sự chuẩn bị và đầu tư công phu cho nhiều chương trình trọng điểm, phim truyền hình, phim tài liệu trên đa nền tảng của VTV.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Nhiều chương trình trọng điểm kỷ niệm 70 năm Ngày Giải phóng Thủ đô trên VTV VTV.vn - Nhân kỷ niệm 70 năm Ngày Giải phóng Thủ đô, Đài Truyền hình Việt Nam thực hiện nhiều chương trình trọng điểm, phát sóng đa nền tảng trên các kênh và nền tảng số của VTV.     20 bộ phim tài liệu về Hà Nội sẽ được công chiếu trên VTVGo VTV.vn - 20 bộ phim tài liệu đặc sắc sẽ được ra mắt khán giả trong khuôn khổ Tuần phim tài liệu Hà Nội năm nay.     Tuần phim tài liệu Hà Nội trên VTVGo: Món quà cho những người yêu Hà Nội VTV.vn - Đài Truyền hình Việt Nam sẽ tổ chức Tuần phim tài liệu Hà Nội với mong muốn tiếp cận được nhiều khán giả hơn để lan tỏa tình yêu với Hà Nội.      * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Sao "Sex and the City" từng tham gia Tiệc trắng của Sean "Diddy" Comb</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/van-hoa-giai-tri/sao-sex-and-the-city-tung-tham-gia-tiec-trang-cua-sean-diddy-comb-20241001110303881.htm</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>VTV.vn - Sean "Diddy" Combs đã chào đón hàng loạt ngôi sao lớn nhất của Hollywood đến dinh thự Hamptons của mình nhiều thập kỷ qua - trước khi bị chính quyền liên bang bắt.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Sau vụ bắt giữ của rapper tai tiếng này, những bức ảnh từ một số Bữa tiệc Trắng toàn sao của Sean "Diddy" Combs đã xuất hiện trở lại trên mạng. Qua những bức ảnh này, mọi người có thể thấy tất cả những ngôi sao hạng A của Hollywood - từ những người đẹp trai tuổi teen đến một số tên tuổi lớn nhất của làng thời trang đều tham dự các bữa tiệc trong dinh thự của Diddy ở phía Đông.Một bức ảnh chụp vào tháng 7 năm 2000 cho thấy Diddy và bạn gái khi đó là Jennifer Lopez đang nằm dài trên một chiếc giường trắng lớn phủ đầy gối. Cặp đôi này đã hẹn hò từ năm 1999 đến năm 2001. Trong cùng một bữa tiệc, cặp đôi này đã được chụp ảnh cùng Kimora Lee Simmons và chồng cô khi đó là Russell Simmons, Matthew Broderick. Người ta cũng thấy cả nữ chính đình đám của bộ phim truyền hình siêu đình đám Sex and the City là Sarah Jessica Parker cùng chồng cô Matthew Broderick, Aaliyah, Leonardo DiCaprio và nhiều người khác. Sarah Jessica Parker và Matthew Broderick đã tham dự bữa tiệc mừng ngày 4 tháng 7 của Diddy vào năm 2000. (Ảnh: Patrick McMullan)Trong nhiều năm qua, danh sách khách mời của Diddy bao gồm Paris Hilton, Kim Kardashian, Howard Stern, Kelly Osbourne, Aretha Franklin, Martha Stewart, Tommy Lee, Pamela Anderson, Regis Philbin, Vera Wange, Jay-Z, Beyonce, Mariah Carey, Nick Cannon và nhiều người khác. Sau khi chuyển đến Bờ Tây, Sean "Diddy" Comb tiếp tục truyền thống này tại ngôi nhà của mình ở Beverly Hills, nơi những ngôi sao như Ashton Kutcher và Russell Brand đã xuất hiện trong trang phục toàn màu trắng.Sean "Diddy" Combs và Kutcher thậm chí đã từng đồng tổ chức bữa tiệc vào năm 2009 để nâng cao nhận thức về Malaria No More. Tuy nhiên, không có dấu hiệu nào cho thấy bất kỳ người nổi tiếng nào tham dự có liên quan đến bất kỳ hoạt động bất hợp pháp nào bị cáo buộc tại các bữa tiệc.Ngôi sao của "Titanic" Leonardo DiCaprio lúc chụp bức ảnh này đang ở tuổi 25. Anh chụp ảnh đang ngồi cùng Diddy và một vài người bạn khi họ hút thuốc và nhâm nhi rượu sâm panh. (Ảnh: Patrick McMullan)Cùng với những người tham dự hạng A, những bức ảnh được đăng lại chia sẻ một chút thông tin chi tiết về cách mọi thứ diễn ra. Một hình ảnh được chụp vào năm 2008 cho thấy hai người phụ nữ ngực trần đang cưỡi trên một người lạ trong hồ bơi trong khi những người dự tiệc khác vẫn tiếp tục công việc của họ.Một bức ảnh khác từ năm 1998 cho thấy Sean "Diddy" đang rót rượu sâm-panh cho hai người phụ nữ gần như khỏa thân, chỉ mặc mỗi chiếc quần lọt khe màu trắng mỏng manh. Những người mẫu khác đi vòng quanh bữa tiệc chỉ với miếng dán ngực nhỏ xíu.Một cựu tay buôn ma túy của Diddy đã mô tả trải nghiệm của mình tại một trong những bữa tiệc của rapper ở Hamptons trong một cuộc phỏng vấn gần đây với The Post. Người này nói: "Những chuyện kỳ ​​lạ bắt đầu xảy ra. Những anh chàng nổi tiếng quan hệ với nhau. Có những phòng ngủ phía sau và giống như một nơi linh thiêng bên trong. Bạn sẽ thấy hai người mà bạn không nghĩ sẽ quan hệ với nhau, những tay buôn ma túy, đó là điều khiến tôi bị sốc".Theo báo cáo mới nhất, Sean đã được đưa ra khỏi danh sách theo dõi tự tử. Luật sư của ông trùm hip hop cho biết Sean sẽ ra làm chứng tại tòa để phản biện lại những cáo buộc của bản thân và rằng tại phiên tòa, Sean sẽ kể câu chuyện của mình. Tuy nhiên, theo các luật sư, việc Sean tự đứng ra làm chứng được cho là sẽ đưa Sean vào tình huống bất lợi nhiều hơn.   Sean "Diddy" Combs ra tòa làm chứng sẽ gặp nhiều bất lợi VTV.vn - Sean "Diddy" Combs dự kiến ​​sẽ làm chứng trong vụ án buôn bán tình dục và tống tiền của mình, nhưng các luật sư cho rằng động thái "táo bạo" này không tốt cho Sean. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Jennie (BLACKPINK) xuất hiện với tạo hình khác lạ, quảng bá ca khúc mới</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/van-hoa-giai-tri/jennie-blackpink-xuat-hien-voi-tao-hinh-khac-la-quang-ba-ca-khuc-moi-20241001095533901.htm</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>VTV.vn - Tạo hình mới của Jennie cho thấy cô đã sẵn sàng phá bỏ rào cản K-Pop để tiến tới thị trường âm nhạc Mỹ.</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Rạng sáng nay (ngày 1/10), Jennie - thành viên nhóm nhạc BLACKPINK - tiếp tục đăng tải những hình ảnh mới để quảng bá cho ca khúc solo sắp tới mang tên Mantra. Trong một đoạn video đăng tải trên mạng xã hội, Jennie đã hé lộ một phần ca khúc khiến những người hâm mộ vô cùng háo hức.Cụ thể, đoạn video cho thấy ngôi sao K-Pop với mái tóc hồng khác lạ cùng tông makeup đơn giản nhưng mang đậm hơi hướng US-UK. Video quảng bá sau đó đã nhận được gần 2 triệu lượt thích chỉ trong vòng 5 tiếng kể từ khi đăng tải. Những người hâm mộ và khán giả trên toàn thế giới đều có những nhận xét tích cực với hình ảnh mới lạ từ thành viên của BLACKPINK. Những hình ảnh mới nhất của Jennie trong video quảng bá ca khúc "Mantra". (Ảnh: Instagram/Jennie)Trước đó, ngôi sao xứ sở kimchi cũng được khen ngợi với cách quảng bá sáng tạo và khác biệt khi đăng tải loạt ảnh như trò chơi xếp hình, sau đó để khán giả tự lắp ghép và có những thông tin về sản phẩm âm nhạc mới.Sau màn solo của Lisa, Jennie là thành viên tiếp theo nhận được sự quan tâm của công chúng toàn thế giới với sự trở lại này. Ca khúc Mantra được dự đoán sẽ "làm mưa làm gió" trên các BXH âm nhạc sau khi ra mắt vào 11/10 tới.        Jennie (BLACKPINK) tung ảnh mới, chuẩn bị trở lại solo VTV.vn - Hình ảnh mới của Jennie khiến những người hâm mộ vô cùng háo hức, hy vọng sản phẩm solo mới sẽ là một siêu phẩm K-Pop.     Jennie (BLACKPINK) lên tiếng về lùm xùm hút thuốc, khán giả tranh cãi VTV.vn - Jennie không ngần ngại nhắc tới scandal hút thuốc, cho rằng đây là vấn đề liên quan tới quan điểm và văn hoá.     Jennie (BLACKPINK) sẽ trở lại với âm nhạc vào tháng 10 VTV.vn - Jennie đang hợp tác với hãng thu âm Colombia Records để ra mắt ca khúc solo mới vào tháng 10 tới.      * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Lý do không nên uống cà phê ngay khi thức dậy</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/doi-song/ly-do-khong-nen-uong-ca-phe-ngay-khi-thuc-day-20240930102819724.htm</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>VTV.vn - Đôi khi, một tách latte là lý do khiến chúng ta thức dậy, nhưng ngoài việc giúp chúng ta tỉnh táo hơn, liệu uống cà phê ngay khi thức dậy có tốt cho chúng ta không?</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Không gì tuyệt hơn cảm giác nhấp ngụm đầu tiên của tách cà phê mới pha vào buổi sáng, trước khi mắt bạn kịp mở ra. Bạn sẽ không bao giờ nghĩ rằng thứ gì đó có hương vị và cảm giác tuyệt vời như vậy lại có thể gây hại cho bạn, phải không?Mặc dù chúng ta có thể dựa vào một tách cà phê vào sáng sớm để bắt đầu ngày mới (thực tế là chúng ta sẽ uống một tách khác vào lúc 3 giờ chiều), nhưng các chuyên gia cho biết đó có thể không phải là cách lý tưởng nhất để bắt đầu ngày mới.Sau đây là những tác dụng của việc uống cà phê ngay khi thức dậy, cùng với lời khuyên của chuyên gia về thời điểm tốt nhất để chúng ta bổ sung caffeine vào buổi sáng.Tại sao mọi người lại uống cà phê vào sáng sớm?Cho dù bạn cảm thấy như một thây ma hay một xác sống cho đến khi caffeine phát huy tác dụng hay chỉ đơn giản là thích một tách cappuccino trước bữa sáng, thì vẫn có nhiều lý do khiến mọi người lựa chọn uống cà phê để bắt đầu ngày mới.Chuyên gia dinh dưỡng và khoa học thể dục Amelia Phillips cho biết có nhiều lý giải về mặt sinh hóa và tâm lý cho điều này, một trong những lý do là não của chúng ta liên kết cà phê với buổi sáng, do đó giải phóng phản ứng dopamine. Vì vậy, về cơ bản, cà phê khiến chúng ta vui vẻ. Nghe có vẻ đúng.Phillips nói thêm rằng lượng đường trong máu thấp tự nhiên của chúng ta sau khi nhịn ăn qua đêm có thể khiến cơ thể tìm kiếm nguồn năng lượng tăng cường nhanh chóng, và cà phê cũng cung cấp năng lượng.Uống cà phê ngay từ sáng sớm có hại gì?Bạn có thể không muốn nghe, nhưng Phillips cho biết uống cà phê vào lúc sáng sớm có thể có những nhược điểm. Bà cho biết các vấn đề tiềm ẩn bao gồm chứng ợ nóng hoặc khó tiêu do tăng sản xuất axit dạ dày, căng thẳng và mất cân bằng nội tiết tố do nồng độ cortisol bị rối loạn.Uống caffeine quá sớm cũng có thể gây lo lắng, bồn chồn và lượng đường trong máu tăng đột biến, sau đó là tình trạng tụt dốc không phanh vào cuối ngày. Và thật ngạc nhiên, uống cà phê ngay khi thức dậy cũng có thể cản trở đáng kể giấc ngủ của bạn.Phillips giải thích rằng: "Hãy nghĩ về nhịp sinh học của bạn như một dàn nhạc gồm các hormone, tất cả đều hòa hợp hoàn hảo, chơi một bản giao hưởng tinh tế nhưng phức tạp trong suốt cả ngày - việc bổ sung caffeine sẽ ảnh hưởng đến sự hòa hợp này".Chuyên gia dinh dưỡng Shivaun Conn cho biết đối với những người uống nhiều caffeine để tìm kiếm sự tỉnh táo có lẽ đã đến lúc phải tìm ra gốc rễ của vấn đề. Vậy, bạn nên uống cà phê buổi sáng khi nào?Phillips cho biết những người muốn cải thiện sức khỏe của mình nên cố gắng chống lại sự cám dỗ của cà phê trong ít nhất một giờ sau khi thức dậy. Bà cho biết: "Bằng cách đợi một giờ sau khi thức dậy, chúng ta đang cho phép các hormone đánh thức tự nhiên của cơ thể thực hiện công việc của chúng"."Bạn có thể cảm thấy rất uể oải trong vài ngày đầu nếu bạn phụ thuộc vào cà phê, nhưng cơ thể bạn sẽ sớm phục hồi sự cân bằng cần thiết để tỉnh táo".Bà nói thêm rằng trong một thế giới lý tưởng, bạn cũng nên cố gắng kết thúc việc uống cà phê vào khoảng 12 giờ trưa để đảm bảo giấc ngủ của bạn không bị cản trở.Nhưng cũng có một thông tin được đánh giá là vui vẻ cho những người yêu thích cà phê, Phillips cho biết mặc dù bà khuyên bạn chỉ nên uống một hoặc hai tách cà phê mỗi ngày, nhưng bất kỳ lượng nào từ một đến bốn tách đều có thể được coi là an toàn.Việc kiềm chế cơn thèm cà phê vào đầu ngày có thể khó khăn, nhưng Conn cho biết cách tốt nhất để bắt đầu ngày mới là bằng những thực phẩm và đồ uống cung cấp chất dinh dưỡng và bù nước cho cơ thể. Bà nói rằng: "Bắt đầu ngày mới bằng ngũ cốc nguyên hạt, nguồn protein, trái cây hoặc rau quả chất lượng và chất béo lành mạnh có thể hỗ trợ sức khỏe tối ưu và cung cấp nhiên liệu lâu dài".Và một cốc nước H20, nước dừa hoặc một tách trà thảo mộc hoặc trà xanh là ngụm đầu tiên tốt nhất.   Làm thế nào để "cai" cà phê? VTV.vn - Rất nhiều người cảm thấy một ngày chưa thể bắt đầu hứng khởi nếu thiếu đi ly cà phê. Nhưng khi cơ thể phát đi một số tín hiệu, đã đến lúc cần hạn chế thức uống yêu thích. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>30/09/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Chèo thuyền thúng ở sông Cửa Cạn</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/tin-bai-vtv/cheo-thuyen-thung-o-song-cua-can-20240923145111988.htm</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>VTV.vn - Một đảo ngọc rất lạ khi có những chiếc thuyền thúng mang đến cho du khách những trải nghiệm mới.</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Ở vùng duyên hải miền Trung, thuyền thúng là phương tiện dùng để di chuyển và đánh bắt thuỷ hải sản duy trì cuộc sống. Chèo thuyền thúng cũng là một trong những hoạt động thể thao truyền thống của người dân địa phương.Nếu như trước kia, trải nghiệm du lịch trên sông ở thuyền thúng chỉ có ở Hội An mà thôi thì bây giờ hoạt động này đã xuất hiện ở Kiên Giang. Chèo thuyền thúng trên sông Cửa Cạn, Phú Quốc hiện là một sản phẩm du lịch mới rất thú vị, thu hút rất nhiều du khách ở trong và ngoài nước đến tham quan và trải nghiệm.Phóng viên Miền Tây hôm nay (VTV Cần Thơ) đưa khán giả du lịch qua màn ảnh nhỏ đến với sông Cửa Cạn để xem hoạt động mới mẻ này. Hào hứng trong những tiếng reo hò, những tràng pháo tay khi được ngồi trên những chiếc thuyền thúng khám phá dòng sông Cửa Cạn, xem người dân địa phương đánh bắt cá, thưởng thức đờn ca tài tử… là những trải nghiệm không thể nào quên với nhiều khách du lịch.Ngoài việc chèo thuyền và múa thúng, trải nghiệm còn có những hoạt động khác gắn với đời sống của người dân miền sông nước và văn hoá Nam Bộ. Đây là điểm nhấn, nét khác biệt ở Nam Bộ và các địa phương khác. Tour chèo thuyền thúng trên sông không chỉ góp phần làm phong phú các sản phẩm du lịch mà còn tạo thêm sinh kế cho người dân trên đảo. Đây cũng là cách để quảng bá nét đẹp hình ảnh Việt Nam ra thế giới.Ngồi thuyền thúng không chỉ săn được những ảnh đẹp mà còn mãn nhãn với bức tranh văn hóa đa sắc màu của bà con tại vùng biển đảo. Chính sự sáng tạo trong du lịch đã góp phần đưa văn hóa Việt ra khơi, đến với bạn bè quốc tế.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>26/09/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>SpaceX "giải cứu" phi hành gia mắc kẹt trên ISS trở về Trái đất</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/cong-nghe/spacex-giai-cuu-phi-hanh-gia-mac-ket-tren-iss-tro-ve-trai-dat-20240930065034544.htm</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>VTV.vn - Khi trở về Trái đất vào tháng 2/2025, Crew-9 sẽ mang theo 2 phi hành gia kỳ cựu - những người buộc phải ở lại ISS lâu hơn dự kiến do sự cố với tàu Starliner của Boeing.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Ngày 28/9, công ty khai phá không gian SpaceX đã phóng thành công tên lửa Falcon 9 từ trung tâm Cape Canaveral, ở Florida (Mỹ), đưa tàu vũ trụ Dragon cùng phi hành đoàn Crew-9 lên Trạm vũ trụ quốc tế (ISS). Ngoài việc triển khai phi hành đoàn Crew-9, sứ mệnh này còn có nhiệm vụ "giải cứu" các phi hành gia Mỹ bị mắc kẹt tại ISS trở về Trái đất. Đây cũng là lần đầu tiên bệ phóng mới của Falcon 9 được sử dụng cho một sứ mệnh có người lái, đánh dấu cột mốc quan trọng trong quá trình khám phá vũ trụ.Sau vụ phóng, Giám đốc Cơ quan Hàng không Vũ trụ Mỹ (NASA) Bill Nelson đã đăng trên mạng xã hội X những chia sẻ phấn chấn: "Chúc mừng NASA và SpaceX với vụ phóng thành công. Chúng ta đang bước vào thời kỳ đầy cảm hứng của thám hiểm và đổi mới giữa các vì sao".Trên chuyến bay Crew-9 có 2 phi hành gia: Nick Hague của NASA và Alexander Gorbunov từ Nga. Theo kế hoạch, khi trở về Trái đất vào tháng 2/2025,  Crew-9 sẽ mang theo cả 2 phi hành gia kỳ cựu Butch Wilmore và Suni Williams, những người đã buộc phải ở lại ISS lâu hơn dự kiến do sự cố với tàu Starliner của Boeing.Ban đầu, hai nhà du hành Wilmore và Williams chỉ dự kiến ở lại ISS trong 8 ngày sau khi được tàu vũ trụ Starliner đưa lên trạm vào tháng 6 vừa qua. Tuy nhiên, sự cố động cơ của Starliner buộc NASA phải điều chỉnh kế hoạch và để họ ở lại ISS trong thời gian dài hơn. Sau nhiều tuần kiểm tra và đánh giá, NASA quyết định đưa Starliner trở về Trái đất mà không có phi hành đoàn, đồng thời sử dụng sứ mệnh Crew-9 của SpaceX để đưa hai phi hành gia này trở về an toàn.Ông Jim Free - Phó Giám đốc NASA - cho biết: "Đây là một sứ mệnh đặc biệt, khi chúng tôi phải điều chỉnh kế hoạch ban đầu, từ 4 phi hành gia xuống còn 2 người. Chúng tôi rất cảm kích trước sự hỗ trợ và tính linh hoạt của SpaceX trong hoạt động này".Sứ mệnh Crew-9 đã phải hoãn từ giữa tháng 8 đến cuối tháng 9 để NASA có thêm thời gian đánh giá độ tin cậy của Starliner và đưa ra quyết định cuối cùng. Ngoài ra, những ảnh hưởng từ cơn bão Helene tại Florida cũng đã khiến sứ mệnh phải lùi thêm vài ngày.Dự kiến, tàu Dragon của SpaceX sẽ ghép nối với ISS vào tối 29/9 (theo giờ GMT). Sau khi hoàn tất bàn giao nhiệm vụ, 4 thành viên của Crew-8 sẽ trở về Trái đất trên một tàu SpaceX khác.Trong sứ mệnh Crew-9, hai nhà du hành Hague và Gorbunov sẽ ở lại ISS khoảng 5 tháng, trong khi hai đồng nghiệp Wilmore và Williams đã trải qua 8 tháng trên trạm. Crew-9 sẽ thực hiện khoảng 200 thí nghiệm khoa học trong suốt thời gian làm việc trên ISS với kỳ vọng mở ra những khám phá mới cho nhân loại.   SpaceX có thể bị phạt vì phóng tên lửa đẩy không phép VTV.vn - Công ty hàng không vũ trụ tư nhân SpaceX bị cáo buộc vi phạm các quy tắc an toàn khi phóng tên lửa đẩy. * Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>30/09/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Google nâng cấp Gmail</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/hitech-cong-nghe-tuong-lai/google-nang-cap-gmail-20240928024912741.htm</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>VTV.vn - Tính năng mới trên Gmail sử dụng AI Gemini để tạo phản hồi thông minh, cá nhân hóa hơn.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Google vừa công bố một bản cập nhật lớn cho tính năng Trả Lời Thông Minh (Smart Replies) trên Gmail, với sự hỗ trợ của công nghệ trí tuệ nhân tạo Gemini. Tính năng mới này hứa hẹn sẽ mang đến cho người dùng những phản hồi tự động thông minh hơn, chính xác hơn và phù hợp hơn với ngữ cảnh của email. Điều này không chỉ giúp người dùng tiết kiệm thời gian, mà còn giúp họ giao tiếp hiệu quả hơn trong công việc qua email.Kể từ khi ra mắt tính năng Smart Replies vào năm 2017, Gmail đã trở thành một công cụ không thể thiếu trong việc quản lý email hàng ngày. Với phiên bản mới nhất này, Google đã ứng dụng Gemini – một mô hình AI tiên tiến, giúp tính năng này phân tích toàn bộ nội dung cuộc trò chuyện email để đưa ra các gợi ý phản hồi chi tiết hơn. Điều này khác biệt hoàn toàn so với các phản hồi ngắn gọn, chung chung như "Cảm ơn, tôi đã nhận được!" hay "Tôi sẽ làm việc này ngay".Nhờ Gemini, các phản hồi sẽ không chỉ đơn thuần là câu trả lời nhanh, mà còn có thể bổ sung lời chào đầu hoặc lời chúc kết thúc email. Điều này giúp phản hồi trở nên tự nhiên hơn, tạo cảm giác chuyên nghiệp và thân thiện hơn khi giao tiếp qua email.(Ảnh: Theo Google)Việc trả lời hàng chục, thậm chí hàng trăm email mỗi ngày là một thách thức lớn với nhiều người, đặc biệt là những ai thường xuyên bị "ngập" trong hộp thư. Với tính năng mới này, Google mong muốn giảm bớt gánh nặng cho người dùng, giúp họ không phải mất quá nhiều thời gian để suy nghĩ và soạn thảo từng câu trả lời.Ngoài ra, bạn cũng có thể chỉnh sửa các phản hồi được đề xuất trước khi gửi đi, giúp giữ được phong cách giao tiếp riêng. Việc chọn lọc từ các phản hồi thông minh có thể giúp bạn không chỉ tiết kiệm thời gian mà còn tạo ra những email chuyên nghiệp hơn mà không cần quá nhiều công sức.Tính năng Trả Lời Thông Minh nâng cấp này hiện đang được triển khai cho các gói đăng ký Gemini Business, Enterprise, Education, Education Premium và Google One AI Premium. Điều này có nghĩa là các doanh nghiệp, tổ chức giáo dục và người dùng trả phí sẽ là những người đầu tiên trải nghiệm sức mạnh của công nghệ AI mới này.Tuy nhiên, Google chỉ hỗ trợ tiếng Anh cho tính năng này vào thời điểm hiện tại. Đây là một điểm đáng chú ý, nhưng có thể trong tương lai, Google sẽ mở rộng hỗ trợ cho nhiều ngôn ngữ khác, bao gồm cả tiếng Việt.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>30/09/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Hà Nội tăng cường ứng dụng AI trong hoạt động dạy và học</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/giao-duc/ha-noi-tang-cuong-ung-dung-ai-trong-hoat-dong-day-va-hoc-20240930004340156.htm</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>VTV.vn - Hà Nội yêu cầu tăng cường ứng dụng trí tuệ nhân tạo trong hoạt động dạy học, nâng cao năng lực số cho người học và đội ngũ nhà giáo.</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Sở GD&amp;ĐT Hà Nội vừa có văn bản gửi các phòng GD&amp;ĐT và cơ sở giáo dục trực thuộc về thực hiện nhiệm vụ ứng dụng công nghệ thông tin, chuyển đổi số năm học 2024 - 2025.Theo đó, Sở lưu ý các đơn vị tiếp tục thực hiện việc kết nối cơ sở dữ liệu GD&amp;ĐT nhằm nâng cao tiện ích và hiệu quả cho công tác quản lý giáo dục; triển khai học bạ số; xây dựng cơ sở dữ liệu văn bằng, chứng chỉ hướng đến văn bằng số, chứng chỉ số.Các đơn vị tăng cường điều kiện bảo đảm về hạ tầng kỹ thuật và kỹ năng ứng dụng CNTT trong công tác quản lý, quản trị, dạy, học và nuôi dưỡng, chăm sóc, giáo dục trẻ em, kiểm tra, đánh giá trong giáo dục; tiếp tục xây dựng hạ tầng số quốc gia về học tập, kho học liệu số chia sẻ dùng chung toàn ngành.Tăng cường ứng dụng trí tuệ nhân tạo trong hoạt động dạy, học và quản lý giáo dục đi cùng với phát triển các giải pháp bảo đảm an toàn môi trường học tập số; nâng cao năng lực số cho người học và đội ngũ nhà giáo, cán bộ quản lý giáo dục; tiếp tục triển khai hệ thống thư viện số toàn ngành; khai thác hiệu quả kho học liệu số chia sẻ dùng chung toàn ngành và ngân hàng câu hỏi trực tuyến.Sở cũng lưu ý đảm bảo các điều kiện về hạ tầng, trang thiết bị, yêu cầu rà soát, đầu tư mới, mua sắm bổ sung máy tính dạy môn tin học tối thiểu đáp ứng mức độ cơ bản (mức độ 2 theo Quyết định số 4725/QĐ-BGDĐT ngày 30/12/2022) phục vụ dạy môn Tin học.Đảm bảo tối đa 2 học sinh học chung 1 máy tính ở cấp Tiểu học, THCS; mỗi học sinh được học 1 máy tính ở cấp THPT. Chú trọng khai thác phòng máy tính cho các hoạt động chuyên môn của nhà trường và các môn học khác ngoài môn Tin học.Tùy theo điều kiện của mỗi đơn vị, xây dựng phòng sản xuất nội dung số phục vụ xây dựng học liệu số và dạy học trực tuyến (gồm máy tính, thiết bị phụ trợ và các phần mềm cần thiết).Tăng cường đầu tư cho hạ tầng ứng dụng CNTT, chuyển đổi số của đơn vị; đảm bảo kết nối Internet (có dây hoặc không dây) đến từng phòng học; đầu tư thiết bị bảo mật (tường lửa, kiểm soát truy cập - IPS...) cho hệ thống mạng cục bộ và phần mềm bản quyền cho máy tính của các đơn vị.Khuyến khích các đơn vị sử dụng đồng thời nhiều đường truyền Internet của các nhà cung cấp khác nhau, kết hợp các phần mềm dạy học trực tuyến phổ biến, ưu tiên lựa chọn những phần mềm có nền tảng công nghệ trong nước để đảm bảo chất lượng và ổn định việc dạy, học trực tuyến.Khuyến khích các đơn vị triển khai các giải pháp bảo đảm an toàn an ninh trong môi trường giáo dục nhằm mục tiêu "Cổng trường thông minh" bằng các giải pháp kiểm soát vào ra bằng thẻ, nhận diện khuôn mặt, điểm danh tự động... Thường xuyên rà soát, khắc phục các nguy cơ mất an toàn, an ninh thông tin.Sở cũng lưu ý các đơn vị, nhà trường đẩy mạnh tuyên truyền tới toàn thể cán bộ, giáo viên và học sinh kỹ năng nhận biết, phòng tránh các nguy cơ mất an toàn thông tin khi sử dụng các phần mềm trực tuyến và thiết bị cá nhân như điện thoại thông minh, máy tính bảng, máy tính cá nhân.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>30/09/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Quảng Nam miễn học phí 2 năm cho học sinh</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://vtv.vn/giao-duc/quang-nam-mien-hoc-phi-2-nam-cho-hoc-sinh-20240926222435084.htm</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>VTV.vn - Học sinh toàn tỉnh Quảng Nam sẽ được miễn học phí trong 2 năm học 2024-2025 và 2025-2026 với tổng số tiền là hơn 158 tỷ đồng.</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Ngày 26/9, tại kỳ họp thứ 26, HĐND tỉnh Quảng Nam khóa X, nhiệm kỳ 2021 - 2026 đã thông qua Nghị quyết về việc chi hơn 158 tỷ đồng hỗ trợ học phí cho trẻ mầm non, học sinh phổ thông trong 2 năm học 2024-2025 và 2025-2026.Theo đó, đối tượng áp dụng là trẻ mầm non, học sinh các trường phổ thông công lập và tư thục, kể cả học viên tại các Trung tâm giáo dục thường xuyên theo chương trình GDPT.Chính sách miễn học phí không áp dụng đối với trẻ mầm non, học sinh tiểu học và phổ thông thuộc các cơ sở giáo dục có vốn đầu tư nước ngoài.HĐND tỉnh Quảng Nam biểu quyết thông qua Nghị quyết miễn học phí 2 năm học 2024 - 2025, 2025 - 2026. Ảnh: Báo NLĐCụ thể, tỉnh Quảng Nam hỗ trợ 100% theo mức thu học phí đối với các cơ sở giáo dục mầm non, GDPT công lập trên địa bàn.Đối với cơ sở giáo dục tư thục, Quảng Nam sẽ hỗ trợ bằng mức hỗ trợ đối với các cơ sở giáo dục công lập tương ứng theo quy định (ví dụ hiện nay, Nghị quyết 17 quy định học sinh mầm non ở thành thị nộp 105.000 đồng/tháng, nông thôn 45.000 đồng/tháng thì nhà nước sẽ hỗ trợ đóng số tiền này, phần còn lại do phụ huynh đóng theo thỏa thuận với nhà trường tư thục).Chính sách miễn học phí này không áp dụng đối với các cơ sở giáo dục có vốn đầu tư nước ngoài và học sinh tiểu học công lập, tư thục.Hiện toàn tỉnh Quảng Nam đang có 725 trường công lập, 722 cơ sở giáo dục mầm non độc lập tư thục và 72 trường ngoài công lập.Theo tính toán của UBND tỉnh Quảng Nam, kinh phí để hỗ trợ miễn giảm học phí cho trường công lập và tư thục trên địa bàn trong 2 năm học 2024-2025 và 2025-2026 là hơn 158 tỷ đồng.Trong đó, tổng kinh phí hỗ trợ các cơ sở giáo dục năm học 2024-2025 hơn 93,9 tỷ đồng, gồm kinh phí hỗ trợ các cơ sở giáo dục mầm non, giáo dục phổ thông công lập hơn 74 tỷ đồng.Về trường tư thục, năm học 2024-2025, Quảng Nam có 25.338 trẻ mầm non và 1.918 học sinh phổ thông tại các cơ sở giáo dục tư thục; với mức hỗ trợ bằng với các cơ sở giáo dục công lập tương ứng theo Nghị quyết số 17, ước tính kinh phí là hơn 19 tỷ đồng.Dự kiến năm học 2025-2026, tổng kinh phí hỗ trợ cho các cơ sở giáo dục hơn 64 tỷ đồng, gồm hơn 44 tỷ hỗ trợ các cơ sở giáo dục công lập và hơn 19 tỷ đồng hỗ trợ các cơ sở giáo dục tư thục.* Mời quý độc giả theo dõi các chương trình đã phát sóng của Đài Truyền hình Việt Nam trên TV Online và VTVGo!</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>27/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
     </row>

</xml_diff>